<commit_message>
Add "call by name" function.
</commit_message>
<xml_diff>
--- a/NCDK-Excel/ExcelNCDK-Test.xlsx
+++ b/NCDK-Excel/ExcelNCDK-Test.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE9978B-A6F9-4AF0-9DD3-74C73212D95A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{537BAFEF-8018-4242-8110-D180D9DDC2B1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="239" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,6 +12,7 @@
     <sheet name="SDF" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="165">
   <si>
     <t>CC(=O)O</t>
     <phoneticPr fontId="1"/>
@@ -1801,6 +1802,10 @@
   </si>
   <si>
     <t>Text</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MACCSFingerprinter</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2129,21 +2134,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B185B08-1BAB-4052-951E-1A2BC1F97D8F}">
-  <dimension ref="A1:BU11"/>
+  <dimension ref="A1:BV11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="3" width="11.25" customWidth="1"/>
     <col min="4" max="4" width="11.08203125" customWidth="1"/>
-    <col min="5" max="22" width="6.5" customWidth="1"/>
-    <col min="24" max="25" width="8.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21.1640625" customWidth="1"/>
+    <col min="6" max="23" width="6.5" customWidth="1"/>
+    <col min="25" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:73" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -2157,214 +2163,217 @@
         <v>84</v>
       </c>
       <c r="E1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" t="s">
         <v>67</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>68</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>69</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>70</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>71</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>72</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>73</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>74</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>75</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>76</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>77</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>78</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>79</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>80</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>81</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>82</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>83</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>66</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>1</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>50</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>51</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>2</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>3</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>4</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>5</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>6</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>7</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>8</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>9</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>10</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>11</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>12</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>13</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>14</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>15</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>16</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>17</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>18</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>19</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>20</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>21</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>22</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>23</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>24</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>25</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>26</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>27</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>28</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>29</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>30</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>31</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>61</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>32</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>33</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>34</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>35</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>36</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>37</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>38</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>39</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>40</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BO1" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BP1" t="s">
         <v>41</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BQ1" t="s">
         <v>42</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BR1" t="s">
         <v>43</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BS1" t="s">
         <v>44</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BT1" t="s">
         <v>45</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BU1" t="s">
         <v>46</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BV1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:73" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -2417,287 +2426,291 @@
 </v>
       </c>
       <c r="D2">
-        <f>_xll.NCDK_Tanimoto($G2,$G3)</f>
+        <f>_xll.NCDK_Tanimoto($H2,$H3)</f>
         <v>0</v>
       </c>
       <c r="E2" t="str">
+        <f>_xll.NCDK(E$1,$B2)</f>
+        <v>0000000000000000001000000000000000001000001000000100100000000100010000000001100100000000111100001110000001010101010011011000001110100001100001100110011001110111101110</v>
+      </c>
+      <c r="F2" t="str">
         <f>_xll.NCDK_ECFP0($B2)</f>
         <v>0000000000000010000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000100000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="F2" t="str">
+      <c r="G2" t="str">
         <f>_xll.NCDK_ECFP2($B2)</f>
         <v>0000000000000010000000001100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000100000000000000000000000000011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000010000000000000100000000000010000010000001000000000000000000000000000100</v>
       </c>
-      <c r="G2" t="str">
+      <c r="H2" t="str">
         <f>_xll.NCDK_ECFP4($B2)</f>
         <v>0000000000000010000000001100000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000010010000000000000000000000000000000000000000000000000000000000000010001000000000000010000000100000000000000000000000000011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000100000000000000000000000000000000101000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000010000010000000000000100000000000010100010000001000000000000000000000000000100</v>
       </c>
-      <c r="H2" t="str">
+      <c r="I2" t="str">
         <f>_xll.NCDK_ECFP6($B2)</f>
         <v>0000000000000010000000001100000000000000000000000000000000100010000000000000000000000000000000000000000000000000000000010000000000000100000000000000000010010000000000000000000000000000000000000000000000000000000000000010001000000000000010000000100000000000000000000000000011000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000001000000000001000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000100000000000000000000000000000000101000000000000000000000000000000000000000000000100001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000001001000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000010000010000000000000100000000000010100010000001000010000000000000000000000100</v>
       </c>
-      <c r="I2" t="str">
+      <c r="J2" t="str">
         <f>_xll.NCDK_FCFP0($B2)</f>
         <v>1011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="J2" t="str">
+      <c r="K2" t="str">
         <f>_xll.NCDK_FCFP2($B2)</f>
         <v>1011000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000010000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="K2" t="str">
+      <c r="L2" t="str">
         <f>_xll.NCDK_FCFP4($B2)</f>
         <v>1011000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000010000000000000000000000000000000010000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000001000000000000000000000000001000000001000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000001000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000100100000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000100000000000010000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="L2" t="str">
+      <c r="M2" t="str">
         <f>_xll.NCDK_FCFP0($B2)</f>
         <v>1011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="M2" t="str">
+      <c r="N2" t="str">
         <f>_xll.NCDK_AtomPairs2DFingerprinter($B2)</f>
         <v>111000000000000000000000000000000000000000000000000000000000000000000000000000111000000000110000000000000000000000000000000000000000000000000000000000000000111000000000000000000000000000000000000000000000000000000000000000000000000000111000000000010000000001000000000000000000000000000000000000000000000000000000111000000000000000000000000000000000000000000000000000000000000000000000000000111000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="N2" t="str">
+      <c r="O2" t="str">
         <f>_xll.NCDK_EStateFingerprinter($B2)</f>
         <v>0000001010100001001000010000000000100000000000000000000000000000000000000000000</v>
       </c>
-      <c r="O2" t="str">
+      <c r="P2" t="str">
         <f>_xll.NCDK_ExtendedFingerprinter($B2)</f>
         <v>000000000000001000000000000000001000000000010000000000000000001000000100000001000000000000000010000000000000000000000100000000000000000000001000001000000000000000000000000000000000100100100000000000000000000000010000000000000001010000000000000000000000010100010000000000000000000001100000000000001000000000000000000000000000010000000000000010000000000010000000000000000000000000000000000000000000000000001000011100000000000000100000000000001000001000010100000100000000000000010100000100000000000000000001000000000000000110000000000000100000000000000010000010000000000000000000010000000000001100000000010001100010100010000010000000000000000001000000000000000000000000000001000000000000000100000000000000000000000010000000001000000000000000000010000000001000100100000000100010001000000000110000000000000000000000010000000000000000000000100000000010001000000001000000000000000000100000100000000000000000000000000000000000100000000010000000000010010000010000000000101100010000000000010000000100000001000000000000011001</v>
       </c>
-      <c r="P2" t="str">
+      <c r="Q2" t="str">
         <f>_xll.NCDK_CDKFingerprinter($B2)</f>
         <v>0000010000000000010000000011000000000010000000000000000010010000000000000001010000001011000000000000000000001010000000000010010010000000000000000000100000000000000001000001000010000100000000000000000000000010100000000100000000010000000001100000000000000000000000000000000000000000000000001000000000001000000000000000000100000000000000100100000000000100000000000000001100000000000000000000000110000000000000000001000000000000000000000000000000010000100000101000000000001011001000000000000000000000000010100100000100000000001000000000000000000011010001100000000000000000000000000000000000001000000001000100000000000000000000100000000000000100000000101000000000000000000000000010000000000100000000000000000000000001000001000000000000000000000001110001000010000000100000000000000000000000000000000000000000000000000000000000000000000010000000000000001000100000000000010100000000000000000000000000000000000000000000001000000000001000000000100000000000001000010000000000000000000000000010000000000000000000110001000000001000000000</v>
       </c>
-      <c r="Q2" t="str">
+      <c r="R2" t="str">
         <f>_xll.NCDK_KlekotaRothFingerprinter($B2)</f>
         <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000010010110000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000001000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000011000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000100000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000001101000000000000000000000000000001000001000000000000000000001010000000000000000000000000000000000000000010000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000011000000001011000100010010000000000000000000011000000010000110100110000110110011001000101000010100000001000000000000000000000010000010100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000010100001000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000011000000000010001000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000010000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="R2" t="str">
+      <c r="S2" t="str">
         <f>_xll.NCDK_LingoFingerprinter($B2)</f>
         <v>0010000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000100000000100100000000000000000100000000000000000000000000000000000000000000000000000001000100000000000001000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000001000100000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000001000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000</v>
       </c>
-      <c r="S2" t="str">
+      <c r="T2" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($B2)</f>
         <v>0000000000000000001000000000000000001000001000000100100000000100010000000001100100000000111100001110000001010101010011011000001110100001100001100110011001110111101110</v>
       </c>
-      <c r="T2" t="str">
+      <c r="U2" t="str">
         <f>_xll.NCDK_ShortestPathFingerprinter($B2)</f>
         <v>0100000000000100100000000000000010000000110000000010000110000000101110100000000000100000000000000000000000100000000100001000100001000000000010000000000000001000000000000000000000000110000000000000100000000000001001000000000011000001001000000000000010000000000000001000100000000000000000010100000000000000100000000000000000000000000000000010000000000000000010000100000000000000000000000000000000000000000000110000000000000100000100000000010000000000010000000011010000000000000000000001011000000000000000010100000000000000100000000000010001001100000000000000000000000001000000000000100000000010000000000001000000000010000000000000000000000000000000000100010000000000000001000000100010000000100101001001000001001110001100010000000000000000000000000000000000000000000000100010000000000000001010000000000000000000000010000000000000000001110000000000000010000000000000100000000100100000000000000000011100000010000000000000000000000000000000000000000000000000000100000000000000100000000000000000000000101010000000101000000000000000</v>
       </c>
-      <c r="U2" t="str">
+      <c r="V2" t="str">
         <f>_xll.NCDK_SubstructureFingerprinter($B2)</f>
         <v>1101100000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000100010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000001000010100001</v>
       </c>
-      <c r="V2" t="str">
+      <c r="W2" t="str">
         <f>_xll.NCDK_PubchemFingerprinter($B2)</f>
         <v>00000000011100110011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001011000000000000000000000000000000010001000000000000000000000000000000000000000000000000000000000000000001111000000000000100000000000000000000000000000000111000000000100000011000000000000000000000110000000000000010110000000000000000000000100010000000001000100001010100100001000000000000000000000000000000000000001000000000000000000000000000000000100000000001000000000000000000001000100000000000000000011010000010001100000100000000000001000000000000000000000010001000010100100010000010000000000000000011000110001000100011000000100011110000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="W2">
+      <c r="X2">
         <f>_xll.NCDK_AcidicGroupCount(B2)</f>
         <v>0</v>
       </c>
-      <c r="X2">
+      <c r="Y2">
         <f>_xll.NCDK_ALogP(B2)</f>
         <v>-1.2114000000000014</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <f>_xll.NCDK_AMolarRefractivity(B2)</f>
         <v>59.947099999999999</v>
       </c>
-      <c r="Z2">
+      <c r="AA2">
         <f>_xll.NCDK_APol(B2)</f>
         <v>39.488274000000011</v>
       </c>
-      <c r="AA2">
+      <c r="AB2">
         <f>_xll.NCDK_AromaticAtomsCount(B2)</f>
         <v>0</v>
       </c>
-      <c r="AB2">
+      <c r="AC2">
         <f>_xll.NCDK_AromaticBondsCount(B2)</f>
         <v>0</v>
       </c>
-      <c r="AC2">
+      <c r="AD2">
         <f>_xll.NCDK_AtomCount(B2)</f>
         <v>36</v>
       </c>
-      <c r="AD2" t="str">
+      <c r="AE2" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B2)</f>
         <v>0.482364049323966, -0.239230483102807, 0.193743260003086, -0.422975414094056, 0.245070516996786</v>
       </c>
-      <c r="AE2" t="str">
+      <c r="AF2" t="str">
         <f>_xll.NCDK_AutocorrelationMass(B2)</f>
         <v>21.0433677091758, 20.6610036641195, 30.570374510169, 39.3180113704083, 36.7520657397667</v>
       </c>
-      <c r="AF2" t="str">
+      <c r="AG2" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B2)</f>
         <v>1236.72445709937, 1455.26096710327, 2067.09825744824, 2452.45202784668, 1776.45546782422</v>
       </c>
-      <c r="AG2">
+      <c r="AH2">
         <f>_xll.NCDK_BasicGroupCount(B2)</f>
         <v>0</v>
       </c>
-      <c r="AH2" t="str">
+      <c r="AI2" t="str">
         <f>_xll.NCDK_BCUT(B2)</f>
         <v>11.89, 15.9969274797474, -0.279527566151374, 0.285306450703295, 4.45516607690972, 12.225254833975</v>
       </c>
-      <c r="AI2">
+      <c r="AJ2">
         <f>_xll.NCDK_BondCount(B2)</f>
         <v>0</v>
       </c>
-      <c r="AJ2">
+      <c r="AK2">
         <f>_xll.NCDK_BPol(B2)</f>
         <v>23.871725999999995</v>
       </c>
-      <c r="AK2" t="str">
+      <c r="AL2" t="str">
         <f>_xll.NCDK_CarbonTypes(B2)</f>
         <v>0, 0, 2, 1, 1, 1, 6, 0, 1</v>
       </c>
-      <c r="AL2" t="str">
+      <c r="AM2" t="str">
         <f>_xll.NCDK_ChiChain(B2)</f>
         <v>0, 0, 0, 0.0481125224324688, 0.206136035947173, 0, 0, 0, 0.015625, 0.0379976820715334</v>
       </c>
-      <c r="AM2" t="str">
+      <c r="AN2" t="str">
         <f>_xll.NCDK_ChiCluster(B2)</f>
         <v>1.29103942781429, 0.0680413817439772, 0.635379749451514, 0.130245735736926, 0.58282022448487, 0.0441941738241592, 0.195368603605389, 0.0360843918243516</v>
       </c>
-      <c r="AN2" t="str">
+      <c r="AO2" t="str">
         <f>_xll.NCDK_ChiPathCluster(B2)</f>
         <v>3.75820832838601, 7.24003474940441, 9.47142848690227, 1.60201233255417, 2.48389505922722, 2.76623804293011</v>
       </c>
-      <c r="AO2" t="str">
+      <c r="AP2" t="str">
         <f>_xll.NCDK_ChiPath(B2)</f>
         <v>13.1733621074374, 8.60822612591632, 7.53308445980525, 6.57446305443147, 5.83502554474493, 3.66414268256136, 2.81639208561656, 1.24750715936873, 10.5447358277005, 6.47350942312757, 4.82495377161152, 3.84884458919458, 2.7963481600948, 1.78170696456175, 1.19223951604789, 0.520731228864019</v>
       </c>
-      <c r="AP2" t="str">
+      <c r="AQ2" t="str">
         <f>_xll.NCDK_CPSA(B2)</f>
         <v>#N/A</v>
       </c>
-      <c r="AQ2">
+      <c r="AR2">
         <f>_xll.NCDK_EccentricConnectivityIndex(B2)</f>
         <v>226</v>
       </c>
-      <c r="AR2">
+      <c r="AS2">
         <f>_xll.NCDK_FMF(B2)</f>
         <v>0.72222222222222221</v>
       </c>
-      <c r="AS2">
+      <c r="AT2">
         <f>_xll.NCDK_FractionalPSA(B2)</f>
         <v>0.30092142334124705</v>
       </c>
-      <c r="AT2">
+      <c r="AU2">
         <f>_xll.NCDK_FragmentComplexity(B2)</f>
         <v>1063.05</v>
       </c>
-      <c r="AU2" t="str">
+      <c r="AV2" t="str">
         <f>_xll.NCDK_GravitationalIndex(B2)</f>
         <v>#N/A</v>
       </c>
-      <c r="AV2">
+      <c r="AW2">
         <f>_xll.NCDK_HBondAcceptorCount(B2)</f>
         <v>5</v>
       </c>
-      <c r="AW2">
+      <c r="AX2">
         <f>_xll.NCDK_HBondDonorCount(B2)</f>
         <v>2</v>
       </c>
-      <c r="AX2">
+      <c r="AY2">
         <f>_xll.NCDK_HybridizationRatio(B2)</f>
         <v>0.61538461538461542</v>
       </c>
-      <c r="AY2" t="str">
+      <c r="AZ2" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B2)</f>
         <v>14.409972299169, 5.96982167352538, 2.65927977839335</v>
       </c>
-      <c r="AZ2" t="str">
+      <c r="BA2" t="str">
         <f>_xll.NCDK_KierHallSmarts(B2)</f>
         <v>0, 0, 0, 0, 0, 0, 1, 0, 6, 0, 1, 0, 0, 0, 0, 4, 0, 0, 1, 0, 0, 0, 0, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 3, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BA2">
+      <c r="BB2">
         <f>_xll.NCDK_LargestChain(B2)</f>
         <v>9</v>
       </c>
-      <c r="BB2">
+      <c r="BC2">
         <f>_xll.NCDK_LargestPiSystem(B2)</f>
         <v>8</v>
       </c>
-      <c r="BC2" t="str">
+      <c r="BD2" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B2)</f>
         <v>#N/A</v>
       </c>
-      <c r="BD2">
+      <c r="BE2">
         <f>_xll.NCDK_LongestAliphaticChain(B2)</f>
         <v>2</v>
       </c>
-      <c r="BE2">
+      <c r="BF2">
         <f>_xll.NCDK_MannholdLogP(B2)</f>
         <v>2.34</v>
       </c>
-      <c r="BF2" t="str">
+      <c r="BG2" t="str">
         <f>_xll.NCDK_MDE(B2)</f>
         <v>0, 1.78256861348341, 1.17348231572452, 0.5, 9.28105720195319, 8.27801156561087, 2.82326712400687, 2.67269615442102, 3.03934274260637, 0, 0.75, 0, 0, 0, 0, 0, 0.5, 0, 0</v>
       </c>
-      <c r="BG2" t="str">
+      <c r="BH2" t="str">
         <f>_xll.NCDK_MomentOfInertia(B2)</f>
         <v>#N/A</v>
       </c>
-      <c r="BH2">
+      <c r="BI2">
         <f>_xll.NCDK_PetitjeanNumber(B2)</f>
         <v>0.5</v>
       </c>
-      <c r="BI2" t="str">
+      <c r="BJ2" t="str">
         <f>_xll.NCDK_PetitjeanShapeIndex(B2)</f>
         <v>#N/A</v>
       </c>
-      <c r="BJ2">
+      <c r="BK2">
         <f>_xll.NCDK_RotatableBondsCount(B2)</f>
         <v>2</v>
       </c>
-      <c r="BK2">
+      <c r="BL2">
         <f>_xll.NCDK_RuleOfFive(B2)</f>
         <v>0</v>
       </c>
-      <c r="BL2" t="str">
+      <c r="BM2" t="str">
         <f>_xll.NCDK_SmallRing(B2)</f>
         <v>2, 0, 2, 0, 0, 0, 0, 1, 1, 0, 0</v>
       </c>
-      <c r="BM2">
+      <c r="BN2">
         <f>_xll.NCDK_TPSA(B2)</f>
         <v>75.27000000000001</v>
       </c>
-      <c r="BN2">
+      <c r="BO2">
         <f>_xll.NCDK_VABC(B2)</f>
         <v>246.50970715028382</v>
       </c>
-      <c r="BO2">
+      <c r="BP2">
         <f>_xll.NCDK_VAdjMa(B2)</f>
         <v>5.2479275134435852</v>
       </c>
-      <c r="BP2">
+      <c r="BQ2">
         <f>_xll.NCDK_Weight(B2)</f>
         <v>250.131742436</v>
       </c>
-      <c r="BQ2" t="str">
+      <c r="BR2" t="str">
         <f>_xll.NCDK_WeightedPath(B2)</f>
         <v>35.9822147160759, 1.99901192867088, 13.5466431850826, 7.60403910050065, 5.94260408458194</v>
       </c>
-      <c r="BR2" t="str">
+      <c r="BS2" t="str">
         <f>_xll.NCDK_WHIM(B2)</f>
         <v>#N/A</v>
       </c>
-      <c r="BS2" t="str">
+      <c r="BT2" t="str">
         <f>_xll.NCDK_WienerNumbers(B2)</f>
         <v>537, 35</v>
       </c>
-      <c r="BT2">
+      <c r="BU2">
         <f>_xll.NCDK_XLogP(B2)</f>
         <v>2.1759999999999997</v>
       </c>
-      <c r="BU2">
+      <c r="BV2">
         <f>_xll.NCDK_ZagrebIndex(B2)</f>
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:73" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -2714,287 +2727,291 @@
 </v>
       </c>
       <c r="D3">
-        <f>_xll.NCDK_Tanimoto($G3,$G4)</f>
+        <f>_xll.NCDK_Tanimoto($H3,$H4)</f>
         <v>0</v>
       </c>
       <c r="E3" t="str">
+        <f>_xll.NCDK(E$1,$B3)</f>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000</v>
+      </c>
+      <c r="F3" t="str">
         <f>_xll.NCDK_ECFP0($B3)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="F3" t="str">
+      <c r="G3" t="str">
         <f>_xll.NCDK_ECFP2($B3)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="G3" t="str">
+      <c r="H3" t="str">
         <f>_xll.NCDK_ECFP4($B3)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="H3" t="str">
+      <c r="I3" t="str">
         <f>_xll.NCDK_ECFP6($B3)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="I3" t="str">
+      <c r="J3" t="str">
         <f>_xll.NCDK_FCFP0($B3)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="J3" t="str">
+      <c r="K3" t="str">
         <f>_xll.NCDK_FCFP2($B3)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="K3" t="str">
+      <c r="L3" t="str">
         <f>_xll.NCDK_FCFP4($B3)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="L3" t="str">
+      <c r="M3" t="str">
         <f>_xll.NCDK_FCFP0($B3)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="M3" t="str">
+      <c r="N3" t="str">
         <f>_xll.NCDK_AtomPairs2DFingerprinter($B3)</f>
         <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="N3" t="str">
+      <c r="O3" t="str">
         <f>_xll.NCDK_EStateFingerprinter($B3)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="O3" t="str">
+      <c r="P3" t="str">
         <f>_xll.NCDK_ExtendedFingerprinter($B3)</f>
         <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="P3" t="str">
+      <c r="Q3" t="str">
         <f>_xll.NCDK_CDKFingerprinter($B3)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="Q3" t="str">
+      <c r="R3" t="str">
         <f>_xll.NCDK_KlekotaRothFingerprinter($B3)</f>
         <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="R3" t="str">
+      <c r="S3" t="str">
         <f>_xll.NCDK_LingoFingerprinter($B3)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="S3" t="str">
+      <c r="T3" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($B3)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000</v>
       </c>
-      <c r="T3" t="str">
+      <c r="U3" t="str">
         <f>_xll.NCDK_ShortestPathFingerprinter($B3)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="U3" t="str">
+      <c r="V3" t="str">
         <f>_xll.NCDK_SubstructureFingerprinter($B3)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="V3" t="str">
+      <c r="W3" t="str">
         <f>_xll.NCDK_PubchemFingerprinter($B3)</f>
         <v>00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="W3">
+      <c r="X3">
         <f>_xll.NCDK_AcidicGroupCount(B3)</f>
         <v>0</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <f>_xll.NCDK_ALogP(B3)</f>
         <v>0</v>
       </c>
-      <c r="Y3">
+      <c r="Z3">
         <f>_xll.NCDK_AMolarRefractivity(B3)</f>
         <v>0</v>
       </c>
-      <c r="Z3">
+      <c r="AA3">
         <f>_xll.NCDK_APol(B3)</f>
         <v>4.4271719999999997</v>
       </c>
-      <c r="AA3">
+      <c r="AB3">
         <f>_xll.NCDK_AromaticAtomsCount(B3)</f>
         <v>0</v>
       </c>
-      <c r="AB3">
+      <c r="AC3">
         <f>_xll.NCDK_AromaticBondsCount(B3)</f>
         <v>0</v>
       </c>
-      <c r="AC3">
+      <c r="AD3">
         <f>_xll.NCDK_AtomCount(B3)</f>
         <v>5</v>
       </c>
-      <c r="AD3" t="str">
+      <c r="AE3" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B3)</f>
         <v>0, 0, 0, 0, 0</v>
       </c>
-      <c r="AE3" t="str">
+      <c r="AF3" t="str">
         <f>_xll.NCDK_AutocorrelationMass(B3)</f>
         <v>1, 0, 0, 0, 0</v>
       </c>
-      <c r="AF3" t="str">
+      <c r="AG3" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B3)</f>
         <v>6.822544, 0, 0, 0, 0</v>
       </c>
-      <c r="AG3">
+      <c r="AH3">
         <f>_xll.NCDK_BasicGroupCount(B3)</f>
         <v>0</v>
       </c>
-      <c r="AH3" t="str">
+      <c r="AI3" t="str">
         <f>_xll.NCDK_BCUT(B3)</f>
         <v>12, 12, -0.0779229231460157, -0.0779229231460157, 2.612, 2.612</v>
       </c>
-      <c r="AI3">
+      <c r="AJ3">
         <f>_xll.NCDK_BondCount(B3)</f>
         <v>0</v>
       </c>
-      <c r="AJ3">
+      <c r="AK3">
         <f>_xll.NCDK_BPol(B3)</f>
         <v>4.3728280000000002</v>
       </c>
-      <c r="AK3" t="str">
+      <c r="AL3" t="str">
         <f>_xll.NCDK_CarbonTypes(B3)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AL3" t="str">
+      <c r="AM3" t="str">
         <f>_xll.NCDK_ChiChain(B3)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AM3" t="str">
+      <c r="AN3" t="str">
         <f>_xll.NCDK_ChiCluster(B3)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AN3" t="str">
+      <c r="AO3" t="str">
         <f>_xll.NCDK_ChiPathCluster(B3)</f>
         <v>0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AO3" t="str">
+      <c r="AP3" t="str">
         <f>_xll.NCDK_ChiPath(B3)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AP3" t="str">
+      <c r="AQ3" t="str">
         <f>_xll.NCDK_CPSA(B3)</f>
         <v>#N/A</v>
       </c>
-      <c r="AQ3">
+      <c r="AR3">
         <f>_xll.NCDK_EccentricConnectivityIndex(B3)</f>
         <v>0</v>
       </c>
-      <c r="AR3">
+      <c r="AS3">
         <f>_xll.NCDK_FMF(B3)</f>
         <v>0</v>
       </c>
-      <c r="AS3">
+      <c r="AT3">
         <f>_xll.NCDK_FractionalPSA(B3)</f>
         <v>0</v>
       </c>
-      <c r="AT3">
+      <c r="AU3">
         <f>_xll.NCDK_FragmentComplexity(B3)</f>
         <v>16</v>
       </c>
-      <c r="AU3" t="str">
+      <c r="AV3" t="str">
         <f>_xll.NCDK_GravitationalIndex(B3)</f>
         <v>#N/A</v>
       </c>
-      <c r="AV3">
+      <c r="AW3">
         <f>_xll.NCDK_HBondAcceptorCount(B3)</f>
         <v>0</v>
       </c>
-      <c r="AW3">
+      <c r="AX3">
         <f>_xll.NCDK_HBondDonorCount(B3)</f>
         <v>0</v>
       </c>
-      <c r="AX3">
+      <c r="AY3">
         <f>_xll.NCDK_HybridizationRatio(B3)</f>
         <v>1</v>
       </c>
-      <c r="AY3" t="str">
+      <c r="AZ3" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B3)</f>
         <v>0, 0, 0</v>
       </c>
-      <c r="AZ3" t="str">
+      <c r="BA3" t="str">
         <f>_xll.NCDK_KierHallSmarts(B3)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BA3">
+      <c r="BB3">
         <f>_xll.NCDK_LargestChain(B3)</f>
         <v>0</v>
       </c>
-      <c r="BB3">
+      <c r="BC3">
         <f>_xll.NCDK_LargestPiSystem(B3)</f>
         <v>0</v>
       </c>
-      <c r="BC3" t="str">
+      <c r="BD3" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B3)</f>
         <v>#N/A</v>
       </c>
-      <c r="BD3">
+      <c r="BE3">
         <f>_xll.NCDK_LongestAliphaticChain(B3)</f>
         <v>0</v>
       </c>
-      <c r="BE3">
+      <c r="BF3">
         <f>_xll.NCDK_MannholdLogP(B3)</f>
         <v>1.57</v>
       </c>
-      <c r="BF3" t="str">
+      <c r="BG3" t="str">
         <f>_xll.NCDK_MDE(B3)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BG3" t="str">
+      <c r="BH3" t="str">
         <f>_xll.NCDK_MomentOfInertia(B3)</f>
         <v>#N/A</v>
       </c>
-      <c r="BH3">
+      <c r="BI3">
         <f>_xll.NCDK_PetitjeanNumber(B3)</f>
         <v>0</v>
       </c>
-      <c r="BI3" t="str">
+      <c r="BJ3" t="str">
         <f>_xll.NCDK_PetitjeanShapeIndex(B3)</f>
         <v>#N/A</v>
       </c>
-      <c r="BJ3">
+      <c r="BK3">
         <f>_xll.NCDK_RotatableBondsCount(B3)</f>
         <v>0</v>
       </c>
-      <c r="BK3">
+      <c r="BL3">
         <f>_xll.NCDK_RuleOfFive(B3)</f>
         <v>0</v>
       </c>
-      <c r="BL3" t="str">
+      <c r="BM3" t="str">
         <f>_xll.NCDK_SmallRing(B3)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BM3">
+      <c r="BN3">
         <f>_xll.NCDK_TPSA(B3)</f>
         <v>0</v>
       </c>
-      <c r="BN3">
+      <c r="BO3">
         <f>_xll.NCDK_VABC(B3)</f>
         <v>25.852443326666702</v>
       </c>
-      <c r="BO3">
+      <c r="BP3">
         <f>_xll.NCDK_VAdjMa(B3)</f>
         <v>0</v>
       </c>
-      <c r="BP3">
+      <c r="BQ3">
         <f>_xll.NCDK_Weight(B3)</f>
         <v>16.031300127999998</v>
       </c>
-      <c r="BQ3" t="str">
+      <c r="BR3" t="str">
         <f>_xll.NCDK_WeightedPath(B3)</f>
         <v>1, 1, 0, 0, 0</v>
       </c>
-      <c r="BR3" t="str">
+      <c r="BS3" t="str">
         <f>_xll.NCDK_WHIM(B3)</f>
         <v>#N/A</v>
       </c>
-      <c r="BS3" t="str">
+      <c r="BT3" t="str">
         <f>_xll.NCDK_WienerNumbers(B3)</f>
         <v>0, 0</v>
       </c>
-      <c r="BT3">
+      <c r="BU3">
         <f>_xll.NCDK_XLogP(B3)</f>
         <v>0.73899999999999999</v>
       </c>
-      <c r="BU3">
+      <c r="BV3">
         <f>_xll.NCDK_ZagrebIndex(B3)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:73" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -3006,287 +3023,291 @@
         <v>InChI=1S/C2H4O2/c1-2(3)4/h1H3,(H,3,4)</v>
       </c>
       <c r="D4">
-        <f>_xll.NCDK_Tanimoto($G4,$G5)</f>
+        <f>_xll.NCDK_Tanimoto($H4,$H5)</f>
         <v>0</v>
       </c>
       <c r="E4" t="str">
+        <f>_xll.NCDK(E$1,$B4)</f>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000001000000000000001001011000100</v>
+      </c>
+      <c r="F4" t="str">
         <f>_xll.NCDK_ECFP0($B4)</f>
         <v>0000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="F4" t="str">
+      <c r="G4" t="str">
         <f>_xll.NCDK_ECFP2($B4)</f>
         <v>0000000000000000000100000000000000000000000000000000000000000000010000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="G4" t="str">
+      <c r="H4" t="str">
         <f>_xll.NCDK_ECFP4($B4)</f>
         <v>0000000000000000000100000000000000000000000000000000000000000000010000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="H4" t="str">
+      <c r="I4" t="str">
         <f>_xll.NCDK_ECFP6($B4)</f>
         <v>0000000000000000000100000000000000000000000000000000000000000000010000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="I4" t="str">
+      <c r="J4" t="str">
         <f>_xll.NCDK_FCFP0($B4)</f>
         <v>1010000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="J4" t="str">
+      <c r="K4" t="str">
         <f>_xll.NCDK_FCFP2($B4)</f>
         <v>1010000010000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="K4" t="str">
+      <c r="L4" t="str">
         <f>_xll.NCDK_FCFP4($B4)</f>
         <v>1010000010000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="L4" t="str">
+      <c r="M4" t="str">
         <f>_xll.NCDK_FCFP0($B4)</f>
         <v>1010000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="M4" t="str">
+      <c r="N4" t="str">
         <f>_xll.NCDK_AtomPairs2DFingerprinter($B4)</f>
         <v>101000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="N4" t="str">
+      <c r="O4" t="str">
         <f>_xll.NCDK_EStateFingerprinter($B4)</f>
         <v>0000001000000001000000000000000001100000000000000000000000000000000000000000000</v>
       </c>
-      <c r="O4" t="str">
+      <c r="P4" t="str">
         <f>_xll.NCDK_ExtendedFingerprinter($B4)</f>
         <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010010000000000000000000000000000000000000000001000</v>
       </c>
-      <c r="P4" t="str">
+      <c r="Q4" t="str">
         <f>_xll.NCDK_CDKFingerprinter($B4)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000001010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="Q4" t="str">
+      <c r="R4" t="str">
         <f>_xll.NCDK_KlekotaRothFingerprinter($B4)</f>
         <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000010000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="R4" t="str">
+      <c r="S4" t="str">
         <f>_xll.NCDK_LingoFingerprinter($B4)</f>
         <v>0000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="S4" t="str">
+      <c r="T4" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($B4)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000001000000000000001001011000100</v>
       </c>
-      <c r="T4" t="str">
+      <c r="U4" t="str">
         <f>_xll.NCDK_ShortestPathFingerprinter($B4)</f>
         <v>0000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000100000000100000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000010000000000000001000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000</v>
       </c>
-      <c r="U4" t="str">
+      <c r="V4" t="str">
         <f>_xll.NCDK_SubstructureFingerprinter($B4)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000010001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000010000000</v>
       </c>
-      <c r="V4" t="str">
+      <c r="W4" t="str">
         <f>_xll.NCDK_PubchemFingerprinter($B4)</f>
         <v>00000000010000000011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001101000000000000000000000100000000000000000000000000000000000100000001000000000000000000000100000100000000000000000000000001000000000000010000000000000000000100100000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <f>_xll.NCDK_AcidicGroupCount(B4)</f>
         <v>1</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <f>_xll.NCDK_ALogP(B4)</f>
         <v>-0.22990000000000016</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <f>_xll.NCDK_AMolarRefractivity(B4)</f>
         <v>12.643699999999999</v>
       </c>
-      <c r="Z4">
+      <c r="AA4">
         <f>_xll.NCDK_APol(B4)</f>
         <v>7.7911719999999995</v>
       </c>
-      <c r="AA4">
+      <c r="AB4">
         <f>_xll.NCDK_AromaticAtomsCount(B4)</f>
         <v>0</v>
       </c>
-      <c r="AB4">
+      <c r="AC4">
         <f>_xll.NCDK_AromaticBondsCount(B4)</f>
         <v>0</v>
       </c>
-      <c r="AC4">
+      <c r="AD4">
         <f>_xll.NCDK_AtomCount(B4)</f>
         <v>8</v>
       </c>
-      <c r="AD4" t="str">
+      <c r="AE4" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B4)</f>
         <v>0.194598407923705, -0.0910121789036757, -0.00628702505817703, 0, 0</v>
       </c>
-      <c r="AE4" t="str">
+      <c r="AF4" t="str">
         <f>_xll.NCDK_AutocorrelationMass(B4)</f>
         <v>5.54893807108189, 3.66418395426513, 4.43865298980608, 0, 0</v>
       </c>
-      <c r="AF4" t="str">
+      <c r="AG4" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B4)</f>
         <v>58.780575625, 47.106336, 38.8410481875, 0, 0</v>
       </c>
-      <c r="AG4">
+      <c r="AH4">
         <f>_xll.NCDK_BasicGroupCount(B4)</f>
         <v>0</v>
       </c>
-      <c r="AH4" t="str">
+      <c r="AI4" t="str">
         <f>_xll.NCDK_BCUT(B4)</f>
         <v>11.9966879762366, 15.9982572603197, -0.351666803410558, 0.275648439067482, 3.09299617864267, 4.35788090208676</v>
       </c>
-      <c r="AI4">
+      <c r="AJ4">
         <f>_xll.NCDK_BondCount(B4)</f>
         <v>0</v>
       </c>
-      <c r="AJ4">
+      <c r="AK4">
         <f>_xll.NCDK_BPol(B4)</f>
         <v>5.3308280000000003</v>
       </c>
-      <c r="AK4" t="str">
+      <c r="AL4" t="str">
         <f>_xll.NCDK_CarbonTypes(B4)</f>
         <v>0, 0, 1, 0, 0, 1, 0, 0, 0</v>
       </c>
-      <c r="AL4" t="str">
+      <c r="AM4" t="str">
         <f>_xll.NCDK_ChiChain(B4)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AM4" t="str">
+      <c r="AN4" t="str">
         <f>_xll.NCDK_ChiCluster(B4)</f>
         <v>0.577350269189626, 0, 0, 0, 0.0912870929175277, 0, 0, 0</v>
       </c>
-      <c r="AN4" t="str">
+      <c r="AO4" t="str">
         <f>_xll.NCDK_ChiPathCluster(B4)</f>
         <v>0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AO4" t="str">
+      <c r="AP4" t="str">
         <f>_xll.NCDK_ChiPath(B4)</f>
         <v>3.57735026918963, 1.73205080756888, 1.73205080756888, 0, 0, 0, 0, 0, 2.35546188596382, 0.927730942981911, 0.519018035899438, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AP4" t="str">
+      <c r="AQ4" t="str">
         <f>_xll.NCDK_CPSA(B4)</f>
         <v>#N/A</v>
       </c>
-      <c r="AQ4">
+      <c r="AR4">
         <f>_xll.NCDK_EccentricConnectivityIndex(B4)</f>
         <v>9</v>
       </c>
-      <c r="AR4">
+      <c r="AS4">
         <f>_xll.NCDK_FMF(B4)</f>
         <v>0</v>
       </c>
-      <c r="AS4">
+      <c r="AT4">
         <f>_xll.NCDK_FractionalPSA(B4)</f>
         <v>0.62144781967398288</v>
       </c>
-      <c r="AT4">
+      <c r="AU4">
         <f>_xll.NCDK_FragmentComplexity(B4)</f>
         <v>37.020000000000003</v>
       </c>
-      <c r="AU4" t="str">
+      <c r="AV4" t="str">
         <f>_xll.NCDK_GravitationalIndex(B4)</f>
         <v>#N/A</v>
       </c>
-      <c r="AV4">
+      <c r="AW4">
         <f>_xll.NCDK_HBondAcceptorCount(B4)</f>
         <v>2</v>
       </c>
-      <c r="AW4">
+      <c r="AX4">
         <f>_xll.NCDK_HBondDonorCount(B4)</f>
         <v>1</v>
       </c>
-      <c r="AX4">
+      <c r="AY4">
         <f>_xll.NCDK_HybridizationRatio(B4)</f>
         <v>0.5</v>
       </c>
-      <c r="AY4" t="str">
+      <c r="AZ4" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B4)</f>
         <v>4, 1.33333333333333, #N/A</v>
       </c>
-      <c r="AZ4" t="str">
+      <c r="BA4" t="str">
         <f>_xll.NCDK_KierHallSmarts(B4)</f>
         <v>0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BA4">
+      <c r="BB4">
         <f>_xll.NCDK_LargestChain(B4)</f>
         <v>3</v>
       </c>
-      <c r="BB4">
+      <c r="BC4">
         <f>_xll.NCDK_LargestPiSystem(B4)</f>
         <v>2</v>
       </c>
-      <c r="BC4" t="str">
+      <c r="BD4" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B4)</f>
         <v>#N/A</v>
       </c>
-      <c r="BD4">
+      <c r="BE4">
         <f>_xll.NCDK_LongestAliphaticChain(B4)</f>
         <v>2</v>
       </c>
-      <c r="BE4">
+      <c r="BF4">
         <f>_xll.NCDK_MannholdLogP(B4)</f>
         <v>1.46</v>
       </c>
-      <c r="BF4" t="str">
+      <c r="BG4" t="str">
         <f>_xll.NCDK_MDE(B4)</f>
         <v>0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0.5, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BG4" t="str">
+      <c r="BH4" t="str">
         <f>_xll.NCDK_MomentOfInertia(B4)</f>
         <v>#N/A</v>
       </c>
-      <c r="BH4">
+      <c r="BI4">
         <f>_xll.NCDK_PetitjeanNumber(B4)</f>
         <v>0.5</v>
       </c>
-      <c r="BI4" t="str">
+      <c r="BJ4" t="str">
         <f>_xll.NCDK_PetitjeanShapeIndex(B4)</f>
         <v>#N/A</v>
       </c>
-      <c r="BJ4">
+      <c r="BK4">
         <f>_xll.NCDK_RotatableBondsCount(B4)</f>
         <v>0</v>
       </c>
-      <c r="BK4">
+      <c r="BL4">
         <f>_xll.NCDK_RuleOfFive(B4)</f>
         <v>0</v>
       </c>
-      <c r="BL4" t="str">
+      <c r="BM4" t="str">
         <f>_xll.NCDK_SmallRing(B4)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BM4">
+      <c r="BN4">
         <f>_xll.NCDK_TPSA(B4)</f>
         <v>37.299999999999997</v>
       </c>
-      <c r="BN4">
+      <c r="BO4">
         <f>_xll.NCDK_VABC(B4)</f>
         <v>58.092422652855603</v>
       </c>
-      <c r="BO4">
+      <c r="BP4">
         <f>_xll.NCDK_VAdjMa(B4)</f>
         <v>2.5849625007211561</v>
       </c>
-      <c r="BP4">
+      <c r="BQ4">
         <f>_xll.NCDK_Weight(B4)</f>
         <v>60.021129368000004</v>
       </c>
-      <c r="BQ4" t="str">
+      <c r="BR4" t="str">
         <f>_xll.NCDK_WeightedPath(B4)</f>
         <v>6.73205080756888, 1.68301270189222, 4.48803387171259, 4.48803387171259, 0</v>
       </c>
-      <c r="BR4" t="str">
+      <c r="BS4" t="str">
         <f>_xll.NCDK_WHIM(B4)</f>
         <v>#N/A</v>
       </c>
-      <c r="BS4" t="str">
+      <c r="BT4" t="str">
         <f>_xll.NCDK_WienerNumbers(B4)</f>
         <v>9, 0</v>
       </c>
-      <c r="BT4">
+      <c r="BU4">
         <f>_xll.NCDK_XLogP(B4)</f>
         <v>-0.08</v>
       </c>
-      <c r="BU4">
+      <c r="BV4">
         <f>_xll.NCDK_ZagrebIndex(B4)</f>
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:73" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -3298,287 +3319,291 @@
         <v>InChI=1S/C6H6/c1-2-4-6-5-3-1/h1-6H</v>
       </c>
       <c r="D5">
-        <f>_xll.NCDK_Tanimoto($G5,$G6)</f>
+        <f>_xll.NCDK_Tanimoto($H5,$H6)</f>
         <v>0.27272727272727271</v>
       </c>
       <c r="E5" t="str">
+        <f>_xll.NCDK(E$1,$B5)</f>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000011010</v>
+      </c>
+      <c r="F5" t="str">
         <f>_xll.NCDK_ECFP0($B5)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="F5" t="str">
+      <c r="G5" t="str">
         <f>_xll.NCDK_ECFP2($B5)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="G5" t="str">
+      <c r="H5" t="str">
         <f>_xll.NCDK_ECFP4($B5)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="H5" t="str">
+      <c r="I5" t="str">
         <f>_xll.NCDK_ECFP6($B5)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="I5" t="str">
+      <c r="J5" t="str">
         <f>_xll.NCDK_FCFP0($B5)</f>
         <v>0000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="J5" t="str">
+      <c r="K5" t="str">
         <f>_xll.NCDK_FCFP2($B5)</f>
         <v>0000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="K5" t="str">
+      <c r="L5" t="str">
         <f>_xll.NCDK_FCFP4($B5)</f>
         <v>0000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="L5" t="str">
+      <c r="M5" t="str">
         <f>_xll.NCDK_FCFP0($B5)</f>
         <v>0000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="M5" t="str">
+      <c r="N5" t="str">
         <f>_xll.NCDK_AtomPairs2DFingerprinter($B5)</f>
         <v>100000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="N5" t="str">
+      <c r="O5" t="str">
         <f>_xll.NCDK_EStateFingerprinter($B5)</f>
         <v>0000000000010000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="O5" t="str">
+      <c r="P5" t="str">
         <f>_xll.NCDK_ExtendedFingerprinter($B5)</f>
         <v>000000000000000000000000000000000000000000000000000001000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000010000000000000000000000000000000000000000000000000000000000010001</v>
       </c>
-      <c r="P5" t="str">
+      <c r="Q5" t="str">
         <f>_xll.NCDK_CDKFingerprinter($B5)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="Q5" t="str">
+      <c r="R5" t="str">
         <f>_xll.NCDK_KlekotaRothFingerprinter($B5)</f>
         <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="R5" t="str">
+      <c r="S5" t="str">
         <f>_xll.NCDK_LingoFingerprinter($B5)</f>
         <v>0000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000</v>
       </c>
-      <c r="S5" t="str">
+      <c r="T5" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($B5)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000011010</v>
       </c>
-      <c r="T5" t="str">
+      <c r="U5" t="str">
         <f>_xll.NCDK_ShortestPathFingerprinter($B5)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
       </c>
-      <c r="U5" t="str">
+      <c r="V5" t="str">
         <f>_xll.NCDK_SubstructureFingerprinter($B5)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000001</v>
       </c>
-      <c r="V5" t="str">
+      <c r="W5" t="str">
         <f>_xll.NCDK_PubchemFingerprinter($B5)</f>
         <v>00000000011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000001100000000000000000000000000000000000000000000000100000000000100000000001000000000000001100000000000010000000000000000000000000000000100000000000000000100000010000100000000000000000000000100000000000000000001000000000000000000000000010001000100000000000000000000000000010001000000010000010000000100010100000000001000100010000100000000010000000000000001000001000000000000000000010001000100000000111000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <f>_xll.NCDK_AcidicGroupCount(B5)</f>
         <v>0</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <f>_xll.NCDK_ALogP(B5)</f>
         <v>1.8299999999999996</v>
       </c>
-      <c r="Y5">
+      <c r="Z5">
         <f>_xll.NCDK_AMolarRefractivity(B5)</f>
         <v>26.058</v>
       </c>
-      <c r="Z5">
+      <c r="AA5">
         <f>_xll.NCDK_APol(B5)</f>
         <v>14.560758</v>
       </c>
-      <c r="AA5">
+      <c r="AB5">
         <f>_xll.NCDK_AromaticAtomsCount(B5)</f>
         <v>6</v>
       </c>
-      <c r="AB5">
+      <c r="AC5">
         <f>_xll.NCDK_AromaticBondsCount(B5)</f>
         <v>6</v>
       </c>
-      <c r="AC5">
+      <c r="AD5">
         <f>_xll.NCDK_AtomCount(B5)</f>
         <v>12</v>
       </c>
-      <c r="AD5" t="str">
+      <c r="AE5" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B5)</f>
         <v>0, 0, 0, 0, 0</v>
       </c>
-      <c r="AE5" t="str">
+      <c r="AF5" t="str">
         <f>_xll.NCDK_AutocorrelationMass(B5)</f>
         <v>6, 6, 6, 3, 0</v>
       </c>
-      <c r="AF5" t="str">
+      <c r="AG5" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B5)</f>
         <v>233.87838834375, 233.87838834375, 233.87838834375, 116.939194171875, 0</v>
       </c>
-      <c r="AG5">
+      <c r="AH5">
         <f>_xll.NCDK_BasicGroupCount(B5)</f>
         <v>0</v>
       </c>
-      <c r="AH5" t="str">
+      <c r="AI5" t="str">
         <f>_xll.NCDK_BCUT(B5)</f>
         <v>11.85, 12.1500544016358, -0.211758152069243, 0.0882962495665529, 6.093375, 6.3934294016358</v>
       </c>
-      <c r="AI5">
+      <c r="AJ5">
         <f>_xll.NCDK_BondCount(B5)</f>
         <v>0</v>
       </c>
-      <c r="AJ5">
+      <c r="AK5">
         <f>_xll.NCDK_BPol(B5)</f>
         <v>6.5592419999999994</v>
       </c>
-      <c r="AK5" t="str">
+      <c r="AL5" t="str">
         <f>_xll.NCDK_CarbonTypes(B5)</f>
         <v>0, 0, 0, 6, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AL5" t="str">
+      <c r="AM5" t="str">
         <f>_xll.NCDK_ChiChain(B5)</f>
         <v>0, 0, 0, 0.125, 0, 0, 0, 0, 0.037037037037037, 0</v>
       </c>
-      <c r="AM5" t="str">
+      <c r="AN5" t="str">
         <f>_xll.NCDK_ChiCluster(B5)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AN5" t="str">
+      <c r="AO5" t="str">
         <f>_xll.NCDK_ChiPathCluster(B5)</f>
         <v>0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AO5" t="str">
+      <c r="AP5" t="str">
         <f>_xll.NCDK_ChiPath(B5)</f>
         <v>4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0, 3.46410161513775, 2, 1.15470053837925, 0.666666666666667, 0.384900179459751, 0.222222222222222, 0, 0</v>
       </c>
-      <c r="AP5" t="str">
+      <c r="AQ5" t="str">
         <f>_xll.NCDK_CPSA(B5)</f>
         <v>#N/A</v>
       </c>
-      <c r="AQ5">
+      <c r="AR5">
         <f>_xll.NCDK_EccentricConnectivityIndex(B5)</f>
         <v>36</v>
       </c>
-      <c r="AR5">
+      <c r="AS5">
         <f>_xll.NCDK_FMF(B5)</f>
         <v>1</v>
       </c>
-      <c r="AS5">
+      <c r="AT5">
         <f>_xll.NCDK_FractionalPSA(B5)</f>
         <v>0</v>
       </c>
-      <c r="AT5">
+      <c r="AU5">
         <f>_xll.NCDK_FragmentComplexity(B5)</f>
         <v>114</v>
       </c>
-      <c r="AU5" t="str">
+      <c r="AV5" t="str">
         <f>_xll.NCDK_GravitationalIndex(B5)</f>
         <v>#N/A</v>
       </c>
-      <c r="AV5">
+      <c r="AW5">
         <f>_xll.NCDK_HBondAcceptorCount(B5)</f>
         <v>0</v>
       </c>
-      <c r="AW5">
+      <c r="AX5">
         <f>_xll.NCDK_HBondDonorCount(B5)</f>
         <v>0</v>
       </c>
-      <c r="AX5">
+      <c r="AY5">
         <f>_xll.NCDK_HybridizationRatio(B5)</f>
         <v>0</v>
       </c>
-      <c r="AY5" t="str">
+      <c r="AZ5" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B5)</f>
         <v>4.16666666666667, 2.22222222222222, 1.33333333333333</v>
       </c>
-      <c r="AZ5" t="str">
+      <c r="BA5" t="str">
         <f>_xll.NCDK_KierHallSmarts(B5)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 6, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BA5">
+      <c r="BB5">
         <f>_xll.NCDK_LargestChain(B5)</f>
         <v>4</v>
       </c>
-      <c r="BB5">
+      <c r="BC5">
         <f>_xll.NCDK_LargestPiSystem(B5)</f>
         <v>6</v>
       </c>
-      <c r="BC5" t="str">
+      <c r="BD5" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B5)</f>
         <v>#N/A</v>
       </c>
-      <c r="BD5">
+      <c r="BE5">
         <f>_xll.NCDK_LongestAliphaticChain(B5)</f>
         <v>0</v>
       </c>
-      <c r="BE5">
+      <c r="BF5">
         <f>_xll.NCDK_MannholdLogP(B5)</f>
         <v>2.12</v>
       </c>
-      <c r="BF5" t="str">
+      <c r="BG5" t="str">
         <f>_xll.NCDK_MDE(B5)</f>
         <v>0, 0, 0, 0, 9.12546512839809, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BG5" t="str">
+      <c r="BH5" t="str">
         <f>_xll.NCDK_MomentOfInertia(B5)</f>
         <v>#N/A</v>
       </c>
-      <c r="BH5">
+      <c r="BI5">
         <f>_xll.NCDK_PetitjeanNumber(B5)</f>
         <v>0</v>
       </c>
-      <c r="BI5" t="str">
+      <c r="BJ5" t="str">
         <f>_xll.NCDK_PetitjeanShapeIndex(B5)</f>
         <v>#N/A</v>
       </c>
-      <c r="BJ5">
+      <c r="BK5">
         <f>_xll.NCDK_RotatableBondsCount(B5)</f>
         <v>0</v>
       </c>
-      <c r="BK5">
+      <c r="BL5">
         <f>_xll.NCDK_RuleOfFive(B5)</f>
         <v>0</v>
       </c>
-      <c r="BL5" t="str">
+      <c r="BM5" t="str">
         <f>_xll.NCDK_SmallRing(B5)</f>
         <v>1, 1, 1, 1, 0, 0, 0, 1, 0, 0, 0</v>
       </c>
-      <c r="BM5">
+      <c r="BN5">
         <f>_xll.NCDK_TPSA(B5)</f>
         <v>0</v>
       </c>
-      <c r="BN5">
+      <c r="BO5">
         <f>_xll.NCDK_VABC(B5)</f>
         <v>81.166531652800174</v>
       </c>
-      <c r="BO5">
+      <c r="BP5">
         <f>_xll.NCDK_VAdjMa(B5)</f>
         <v>3.5849625007211561</v>
       </c>
-      <c r="BP5">
+      <c r="BQ5">
         <f>_xll.NCDK_Weight(B5)</f>
         <v>78.046950191999997</v>
       </c>
-      <c r="BQ5" t="str">
+      <c r="BR5" t="str">
         <f>_xll.NCDK_WeightedPath(B5)</f>
         <v>11.8125, 1.96875, 0, 0, 0</v>
       </c>
-      <c r="BR5" t="str">
+      <c r="BS5" t="str">
         <f>_xll.NCDK_WHIM(B5)</f>
         <v>#N/A</v>
       </c>
-      <c r="BS5" t="str">
+      <c r="BT5" t="str">
         <f>_xll.NCDK_WienerNumbers(B5)</f>
         <v>27, 3</v>
       </c>
-      <c r="BT5">
+      <c r="BU5">
         <f>_xll.NCDK_XLogP(B5)</f>
         <v>2.0220000000000002</v>
       </c>
-      <c r="BU5">
+      <c r="BV5">
         <f>_xll.NCDK_ZagrebIndex(B5)</f>
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:73" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>85</v>
       </c>
@@ -3590,287 +3615,291 @@
         <v>InChI=1S/C7H8/c1-7-5-3-2-4-6-7/h2-6H,1H3</v>
       </c>
       <c r="D6">
-        <f>_xll.NCDK_Tanimoto($G6,$G7)</f>
+        <f>_xll.NCDK_Tanimoto($H6,$H7)</f>
         <v>0</v>
       </c>
       <c r="E6" t="str">
+        <f>_xll.NCDK(E$1,$B6)</f>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001011010</v>
+      </c>
+      <c r="F6" t="str">
         <f>_xll.NCDK_ECFP0($B6)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000100000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="F6" t="str">
+      <c r="G6" t="str">
         <f>_xll.NCDK_ECFP2($B6)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000100000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="G6" t="str">
+      <c r="H6" t="str">
         <f>_xll.NCDK_ECFP4($B6)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000100000000000000000000000000000010000000000000000000000000</v>
       </c>
-      <c r="H6" t="str">
+      <c r="I6" t="str">
         <f>_xll.NCDK_ECFP6($B6)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000010100000000001000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000100000000000000000000000000000010000000000000000000000000</v>
       </c>
-      <c r="I6" t="str">
+      <c r="J6" t="str">
         <f>_xll.NCDK_FCFP0($B6)</f>
         <v>1000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="J6" t="str">
+      <c r="K6" t="str">
         <f>_xll.NCDK_FCFP2($B6)</f>
         <v>1000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="K6" t="str">
+      <c r="L6" t="str">
         <f>_xll.NCDK_FCFP4($B6)</f>
         <v>1000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000001000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="L6" t="str">
+      <c r="M6" t="str">
         <f>_xll.NCDK_FCFP0($B6)</f>
         <v>1000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="M6" t="str">
+      <c r="N6" t="str">
         <f>_xll.NCDK_AtomPairs2DFingerprinter($B6)</f>
         <v>100000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="N6" t="str">
+      <c r="O6" t="str">
         <f>_xll.NCDK_EStateFingerprinter($B6)</f>
         <v>0000001000010000100000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="O6" t="str">
+      <c r="P6" t="str">
         <f>_xll.NCDK_ExtendedFingerprinter($B6)</f>
         <v>000000000000000000000000000000000000000001000000000001000000010000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000010000000000000000000000000000000000000000000001000000000000010001</v>
       </c>
-      <c r="P6" t="str">
+      <c r="Q6" t="str">
         <f>_xll.NCDK_CDKFingerprinter($B6)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000010010000000000000000000000000000000000000000000000000001000000001000000000000000000000000000000100000000000000000100000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="Q6" t="str">
+      <c r="R6" t="str">
         <f>_xll.NCDK_KlekotaRothFingerprinter($B6)</f>
         <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="R6" t="str">
+      <c r="S6" t="str">
         <f>_xll.NCDK_LingoFingerprinter($B6)</f>
         <v>0000000000000000000000001000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000100000000000000000000</v>
       </c>
-      <c r="S6" t="str">
+      <c r="T6" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($B6)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001011010</v>
       </c>
-      <c r="T6" t="str">
+      <c r="U6" t="str">
         <f>_xll.NCDK_ShortestPathFingerprinter($B6)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000100000000000000000100000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000001000000000001000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000101</v>
       </c>
-      <c r="U6" t="str">
+      <c r="V6" t="str">
         <f>_xll.NCDK_SubstructureFingerprinter($B6)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000001</v>
       </c>
-      <c r="V6" t="str">
+      <c r="W6" t="str">
         <f>_xll.NCDK_PubchemFingerprinter($B6)</f>
         <v>00000000011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000001100000000000000000000000000000000000000000000000110000000000100000000001100000000000001100100000000010000000000000000000000000000000100000000000001000100000010000100000000000000000000000100000000000000000001000000000000000000000000010001000100000000000000000000000000010001000000010000010000000100010100000000001000100010000100000000010000000000000001000001000000000000000000010001000100000000111000000001000000000000000000011100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="W6">
+      <c r="X6">
         <f>_xll.NCDK_AcidicGroupCount(B6)</f>
         <v>0</v>
       </c>
-      <c r="X6">
+      <c r="Y6">
         <f>_xll.NCDK_ALogP(B6)</f>
         <v>2.3162000000000003</v>
       </c>
-      <c r="Y6">
+      <c r="Z6">
         <f>_xll.NCDK_AMolarRefractivity(B6)</f>
         <v>31.0992</v>
       </c>
-      <c r="Z6">
+      <c r="AA6">
         <f>_xll.NCDK_APol(B6)</f>
         <v>17.654343999999998</v>
       </c>
-      <c r="AA6">
+      <c r="AB6">
         <f>_xll.NCDK_AromaticAtomsCount(B6)</f>
         <v>6</v>
       </c>
-      <c r="AB6">
+      <c r="AC6">
         <f>_xll.NCDK_AromaticBondsCount(B6)</f>
         <v>6</v>
       </c>
-      <c r="AC6">
+      <c r="AD6">
         <f>_xll.NCDK_AtomCount(B6)</f>
         <v>15</v>
       </c>
-      <c r="AD6" t="str">
+      <c r="AE6" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B6)</f>
         <v>0.00145821501522747, -0.000488055819316601, -0.000225165712015084, -1.53979004755717E-05, -4.88075806479512E-07</v>
       </c>
-      <c r="AE6" t="str">
+      <c r="AF6" t="str">
         <f>_xll.NCDK_AutocorrelationMass(B6)</f>
         <v>7, 7, 8, 5, 1</v>
       </c>
-      <c r="AF6" t="str">
+      <c r="AG6" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B6)</f>
         <v>310.962687273438, 320.438287539063, 355.858255328125, 213.793837835938, 36.9196446054688</v>
       </c>
-      <c r="AG6">
+      <c r="AH6">
         <f>_xll.NCDK_BasicGroupCount(B6)</f>
         <v>0</v>
       </c>
-      <c r="AH6" t="str">
+      <c r="AI6" t="str">
         <f>_xll.NCDK_BCUT(B6)</f>
         <v>11.89, 12.1100942558098, -0.155208136358149, 0.0651359477608963, 5.76122693815409, 7.50783741355056</v>
       </c>
-      <c r="AI6">
+      <c r="AJ6">
         <f>_xll.NCDK_BondCount(B6)</f>
         <v>0</v>
       </c>
-      <c r="AJ6">
+      <c r="AK6">
         <f>_xll.NCDK_BPol(B6)</f>
         <v>8.7456560000000003</v>
       </c>
-      <c r="AK6" t="str">
+      <c r="AL6" t="str">
         <f>_xll.NCDK_CarbonTypes(B6)</f>
         <v>0, 0, 0, 5, 1, 1, 0, 0, 0</v>
       </c>
-      <c r="AL6" t="str">
+      <c r="AM6" t="str">
         <f>_xll.NCDK_ChiChain(B6)</f>
         <v>0, 0, 0, 0.102062072615966, 0.102062072615966, 0, 0, 0, 0.0320750149549792, 0.0320750149549792</v>
       </c>
-      <c r="AM6" t="str">
+      <c r="AN6" t="str">
         <f>_xll.NCDK_ChiCluster(B6)</f>
         <v>0.288675134594813, 0, 0, 0, 0.166666666666667, 0, 0, 0</v>
       </c>
-      <c r="AN6" t="str">
+      <c r="AO6" t="str">
         <f>_xll.NCDK_ChiPathCluster(B6)</f>
         <v>0.408248290463863, 0.433012701892219, 0.408248290463863, 0.192450089729875, 0.166666666666667, 0.128300059819917</v>
       </c>
-      <c r="AO6" t="str">
+      <c r="AP6" t="str">
         <f>_xll.NCDK_ChiPath(B6)</f>
         <v>5.11288417512236, 3.39384685011735, 2.74318215649199, 1.89384685011735, 1.30671282224753, 0.901047570290607, 0.204124145231932, 0, 4.38675134594813, 2.41068360252296, 1.65470053837925, 0.940455735015306, 0.534377897417612, 0.303561200840986, 0.0641500299099584, 0</v>
       </c>
-      <c r="AP6" t="str">
+      <c r="AQ6" t="str">
         <f>_xll.NCDK_CPSA(B6)</f>
         <v>#N/A</v>
       </c>
-      <c r="AQ6">
+      <c r="AR6">
         <f>_xll.NCDK_EccentricConnectivityIndex(B6)</f>
         <v>45</v>
       </c>
-      <c r="AR6">
+      <c r="AS6">
         <f>_xll.NCDK_FMF(B6)</f>
         <v>0.8571428571428571</v>
       </c>
-      <c r="AS6">
+      <c r="AT6">
         <f>_xll.NCDK_FractionalPSA(B6)</f>
         <v>0</v>
       </c>
-      <c r="AT6">
+      <c r="AU6">
         <f>_xll.NCDK_FragmentComplexity(B6)</f>
         <v>183</v>
       </c>
-      <c r="AU6" t="str">
+      <c r="AV6" t="str">
         <f>_xll.NCDK_GravitationalIndex(B6)</f>
         <v>#N/A</v>
       </c>
-      <c r="AV6">
+      <c r="AW6">
         <f>_xll.NCDK_HBondAcceptorCount(B6)</f>
         <v>0</v>
       </c>
-      <c r="AW6">
+      <c r="AX6">
         <f>_xll.NCDK_HBondDonorCount(B6)</f>
         <v>0</v>
       </c>
-      <c r="AX6">
+      <c r="AY6">
         <f>_xll.NCDK_HybridizationRatio(B6)</f>
         <v>0.14285714285714285</v>
       </c>
-      <c r="AY6" t="str">
+      <c r="AZ6" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B6)</f>
         <v>5.14285714285714, 2.34375, 1.5</v>
       </c>
-      <c r="AZ6" t="str">
+      <c r="BA6" t="str">
         <f>_xll.NCDK_KierHallSmarts(B6)</f>
         <v>0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 5, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BA6">
+      <c r="BB6">
         <f>_xll.NCDK_LargestChain(B6)</f>
         <v>0</v>
       </c>
-      <c r="BB6">
+      <c r="BC6">
         <f>_xll.NCDK_LargestPiSystem(B6)</f>
         <v>6</v>
       </c>
-      <c r="BC6" t="str">
+      <c r="BD6" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B6)</f>
         <v>#N/A</v>
       </c>
-      <c r="BD6">
+      <c r="BE6">
         <f>_xll.NCDK_LongestAliphaticChain(B6)</f>
         <v>0</v>
       </c>
-      <c r="BE6">
+      <c r="BF6">
         <f>_xll.NCDK_MannholdLogP(B6)</f>
         <v>2.23</v>
       </c>
-      <c r="BF6" t="str">
+      <c r="BG6" t="str">
         <f>_xll.NCDK_MDE(B6)</f>
         <v>0, 1.85053586243577, 1, 0, 6.08364341893206, 3.04182170946603, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BG6" t="str">
+      <c r="BH6" t="str">
         <f>_xll.NCDK_MomentOfInertia(B6)</f>
         <v>#N/A</v>
       </c>
-      <c r="BH6">
+      <c r="BI6">
         <f>_xll.NCDK_PetitjeanNumber(B6)</f>
         <v>0.25</v>
       </c>
-      <c r="BI6" t="str">
+      <c r="BJ6" t="str">
         <f>_xll.NCDK_PetitjeanShapeIndex(B6)</f>
         <v>#N/A</v>
       </c>
-      <c r="BJ6">
+      <c r="BK6">
         <f>_xll.NCDK_RotatableBondsCount(B6)</f>
         <v>0</v>
       </c>
-      <c r="BK6">
+      <c r="BL6">
         <f>_xll.NCDK_RuleOfFive(B6)</f>
         <v>0</v>
       </c>
-      <c r="BL6" t="str">
+      <c r="BM6" t="str">
         <f>_xll.NCDK_SmallRing(B6)</f>
         <v>1, 1, 1, 1, 0, 0, 0, 1, 0, 0, 0</v>
       </c>
-      <c r="BM6">
+      <c r="BN6">
         <f>_xll.NCDK_TPSA(B6)</f>
         <v>0</v>
       </c>
-      <c r="BN6">
+      <c r="BO6">
         <f>_xll.NCDK_VABC(B6)</f>
         <v>98.462516278666868</v>
       </c>
-      <c r="BO6">
+      <c r="BP6">
         <f>_xll.NCDK_VAdjMa(B6)</f>
         <v>3.8073549220576042</v>
       </c>
-      <c r="BP6">
+      <c r="BQ6">
         <f>_xll.NCDK_Weight(B6)</f>
         <v>92.062600255999996</v>
       </c>
-      <c r="BQ6" t="str">
+      <c r="BR6" t="str">
         <f>_xll.NCDK_WeightedPath(B6)</f>
         <v>13.6768253204364, 1.95383218863377, 0, 0, 0</v>
       </c>
-      <c r="BR6" t="str">
+      <c r="BS6" t="str">
         <f>_xll.NCDK_WHIM(B6)</f>
         <v>#N/A</v>
       </c>
-      <c r="BS6" t="str">
+      <c r="BT6" t="str">
         <f>_xll.NCDK_WienerNumbers(B6)</f>
         <v>42, 5</v>
       </c>
-      <c r="BT6">
+      <c r="BU6">
         <f>_xll.NCDK_XLogP(B6)</f>
         <v>2.4590000000000001</v>
       </c>
-      <c r="BU6">
+      <c r="BV6">
         <f>_xll.NCDK_ZagrebIndex(B6)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:73" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -3882,287 +3911,291 @@
         <v>[C]1[C][C][C][C][C]1</v>
       </c>
       <c r="D7">
-        <f>_xll.NCDK_Tanimoto($G7,$G8)</f>
+        <f>_xll.NCDK_Tanimoto($H7,$H8)</f>
         <v>1</v>
       </c>
       <c r="E7" t="str">
+        <f>_xll.NCDK(E$1,$B7)</f>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001010</v>
+      </c>
+      <c r="F7" t="str">
         <f>_xll.NCDK_ECFP0($B7)</f>
         <v>0000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="F7" t="str">
+      <c r="G7" t="str">
         <f>_xll.NCDK_ECFP2($B7)</f>
         <v>0000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="G7" t="str">
+      <c r="H7" t="str">
         <f>_xll.NCDK_ECFP4($B7)</f>
         <v>0000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="H7" t="str">
+      <c r="I7" t="str">
         <f>_xll.NCDK_ECFP6($B7)</f>
         <v>0000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="I7" t="str">
+      <c r="J7" t="str">
         <f>_xll.NCDK_FCFP0($B7)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="J7" t="str">
+      <c r="K7" t="str">
         <f>_xll.NCDK_FCFP2($B7)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="K7" t="str">
+      <c r="L7" t="str">
         <f>_xll.NCDK_FCFP4($B7)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="L7" t="str">
+      <c r="M7" t="str">
         <f>_xll.NCDK_FCFP0($B7)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="M7" t="str">
+      <c r="N7" t="str">
         <f>_xll.NCDK_AtomPairs2DFingerprinter($B7)</f>
         <v>100000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="N7" t="str">
+      <c r="O7" t="str">
         <f>_xll.NCDK_EStateFingerprinter($B7)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="O7" t="str">
+      <c r="P7" t="str">
         <f>_xll.NCDK_ExtendedFingerprinter($B7)</f>
         <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000001000000000000010001</v>
       </c>
-      <c r="P7" t="str">
+      <c r="Q7" t="str">
         <f>_xll.NCDK_CDKFingerprinter($B7)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000010000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="Q7" t="str">
+      <c r="R7" t="str">
         <f>_xll.NCDK_KlekotaRothFingerprinter($B7)</f>
         <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000010000000000000100000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="R7" t="str">
+      <c r="S7" t="str">
         <f>_xll.NCDK_LingoFingerprinter($B7)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="S7" t="str">
+      <c r="T7" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($B7)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001010</v>
       </c>
-      <c r="T7" t="str">
+      <c r="U7" t="str">
         <f>_xll.NCDK_ShortestPathFingerprinter($B7)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="U7" t="str">
+      <c r="V7" t="str">
         <f>_xll.NCDK_SubstructureFingerprinter($B7)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="V7" t="str">
+      <c r="W7" t="str">
         <f>_xll.NCDK_PubchemFingerprinter($B7)</f>
         <v>00000000011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="W7">
+      <c r="X7">
         <f>_xll.NCDK_AcidicGroupCount(B7)</f>
         <v>0</v>
       </c>
-      <c r="X7">
+      <c r="Y7">
         <f>_xll.NCDK_ALogP(B7)</f>
         <v>-1.7280000000000006</v>
       </c>
-      <c r="Y7">
+      <c r="Z7">
         <f>_xll.NCDK_AMolarRefractivity(B7)</f>
         <v>17.4696</v>
       </c>
-      <c r="Z7">
+      <c r="AA7">
         <f>_xll.NCDK_APol(B7)</f>
         <v>10.56</v>
       </c>
-      <c r="AA7">
+      <c r="AB7">
         <f>_xll.NCDK_AromaticAtomsCount(B7)</f>
         <v>0</v>
       </c>
-      <c r="AB7">
+      <c r="AC7">
         <f>_xll.NCDK_AromaticBondsCount(B7)</f>
         <v>0</v>
       </c>
-      <c r="AC7">
+      <c r="AD7">
         <f>_xll.NCDK_AtomCount(B7)</f>
         <v>6</v>
       </c>
-      <c r="AD7" t="str">
+      <c r="AE7" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B7)</f>
         <v>0, 0, 0, 0, 0</v>
       </c>
-      <c r="AE7" t="str">
+      <c r="AF7" t="str">
         <f>_xll.NCDK_AutocorrelationMass(B7)</f>
         <v>6, 6, 6, 3, 0</v>
       </c>
-      <c r="AF7" t="str">
+      <c r="AG7" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B7)</f>
         <v>257.709834375, 257.709834375, 257.709834375, 128.8549171875, 0</v>
       </c>
-      <c r="AG7">
+      <c r="AH7">
         <f>_xll.NCDK_BasicGroupCount(B7)</f>
         <v>0</v>
       </c>
-      <c r="AH7" t="str">
+      <c r="AI7" t="str">
         <f>_xll.NCDK_BCUT(B7)</f>
         <v>11.9, 12.1000824042221, -0.15279744210896, 0.0472849621131451, 6.45375, 6.65383240422211</v>
       </c>
-      <c r="AI7">
+      <c r="AJ7">
         <f>_xll.NCDK_BondCount(B7)</f>
         <v>0</v>
       </c>
-      <c r="AJ7">
+      <c r="AK7">
         <f>_xll.NCDK_BPol(B7)</f>
         <v>0</v>
       </c>
-      <c r="AK7" t="str">
+      <c r="AL7" t="str">
         <f>_xll.NCDK_CarbonTypes(B7)</f>
         <v>0, 0, 0, 0, 0, 0, 6, 0, 0</v>
       </c>
-      <c r="AL7" t="str">
+      <c r="AM7" t="str">
         <f>_xll.NCDK_ChiChain(B7)</f>
         <v>0, 0, 0, 0.125, 0, 0, 0, 0, 0.125, 0</v>
       </c>
-      <c r="AM7" t="str">
+      <c r="AN7" t="str">
         <f>_xll.NCDK_ChiCluster(B7)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AN7" t="str">
+      <c r="AO7" t="str">
         <f>_xll.NCDK_ChiPathCluster(B7)</f>
         <v>0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AO7" t="str">
+      <c r="AP7" t="str">
         <f>_xll.NCDK_ChiPath(B7)</f>
         <v>4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0, 4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0</v>
       </c>
-      <c r="AP7" t="str">
+      <c r="AQ7" t="str">
         <f>_xll.NCDK_CPSA(B7)</f>
         <v>#N/A</v>
       </c>
-      <c r="AQ7">
+      <c r="AR7">
         <f>_xll.NCDK_EccentricConnectivityIndex(B7)</f>
         <v>36</v>
       </c>
-      <c r="AR7">
+      <c r="AS7">
         <f>_xll.NCDK_FMF(B7)</f>
         <v>1</v>
       </c>
-      <c r="AS7">
+      <c r="AT7">
         <f>_xll.NCDK_FractionalPSA(B7)</f>
         <v>0</v>
       </c>
-      <c r="AT7">
+      <c r="AU7">
         <f>_xll.NCDK_FragmentComplexity(B7)</f>
         <v>6</v>
       </c>
-      <c r="AU7" t="str">
+      <c r="AV7" t="str">
         <f>_xll.NCDK_GravitationalIndex(B7)</f>
         <v>#N/A</v>
       </c>
-      <c r="AV7">
+      <c r="AW7">
         <f>_xll.NCDK_HBondAcceptorCount(B7)</f>
         <v>0</v>
       </c>
-      <c r="AW7">
+      <c r="AX7">
         <f>_xll.NCDK_HBondDonorCount(B7)</f>
         <v>0</v>
       </c>
-      <c r="AX7">
+      <c r="AY7">
         <f>_xll.NCDK_HybridizationRatio(B7)</f>
         <v>1</v>
       </c>
-      <c r="AY7" t="str">
+      <c r="AZ7" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B7)</f>
         <v>4.16666666666667, 2.22222222222222, 1.33333333333333</v>
       </c>
-      <c r="AZ7" t="str">
+      <c r="BA7" t="str">
         <f>_xll.NCDK_KierHallSmarts(B7)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BA7">
+      <c r="BB7">
         <f>_xll.NCDK_LargestChain(B7)</f>
         <v>4</v>
       </c>
-      <c r="BB7">
+      <c r="BC7">
         <f>_xll.NCDK_LargestPiSystem(B7)</f>
         <v>0</v>
       </c>
-      <c r="BC7" t="str">
+      <c r="BD7" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B7)</f>
         <v>#N/A</v>
       </c>
-      <c r="BD7">
+      <c r="BE7">
         <f>_xll.NCDK_LongestAliphaticChain(B7)</f>
         <v>0</v>
       </c>
-      <c r="BE7">
+      <c r="BF7">
         <f>_xll.NCDK_MannholdLogP(B7)</f>
         <v>2.12</v>
       </c>
-      <c r="BF7" t="str">
+      <c r="BG7" t="str">
         <f>_xll.NCDK_MDE(B7)</f>
         <v>0, 0, 0, 0, 9.12546512839809, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BG7" t="str">
+      <c r="BH7" t="str">
         <f>_xll.NCDK_MomentOfInertia(B7)</f>
         <v>#N/A</v>
       </c>
-      <c r="BH7">
+      <c r="BI7">
         <f>_xll.NCDK_PetitjeanNumber(B7)</f>
         <v>0</v>
       </c>
-      <c r="BI7" t="str">
+      <c r="BJ7" t="str">
         <f>_xll.NCDK_PetitjeanShapeIndex(B7)</f>
         <v>#N/A</v>
       </c>
-      <c r="BJ7">
+      <c r="BK7">
         <f>_xll.NCDK_RotatableBondsCount(B7)</f>
         <v>0</v>
       </c>
-      <c r="BK7">
+      <c r="BL7">
         <f>_xll.NCDK_RuleOfFive(B7)</f>
         <v>0</v>
       </c>
-      <c r="BL7" t="str">
+      <c r="BM7" t="str">
         <f>_xll.NCDK_SmallRing(B7)</f>
         <v>1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0</v>
       </c>
-      <c r="BM7">
+      <c r="BN7">
         <f>_xll.NCDK_TPSA(B7)</f>
         <v>0</v>
       </c>
-      <c r="BN7">
+      <c r="BO7">
         <f>_xll.NCDK_VABC(B7)</f>
         <v>99.975907755200197</v>
       </c>
-      <c r="BO7">
+      <c r="BP7">
         <f>_xll.NCDK_VAdjMa(B7)</f>
         <v>3.5849625007211561</v>
       </c>
-      <c r="BP7">
+      <c r="BQ7">
         <f>_xll.NCDK_Weight(B7)</f>
         <v>72</v>
       </c>
-      <c r="BQ7" t="str">
+      <c r="BR7" t="str">
         <f>_xll.NCDK_WeightedPath(B7)</f>
         <v>11.8125, 1.96875, 0, 0, 0</v>
       </c>
-      <c r="BR7" t="str">
+      <c r="BS7" t="str">
         <f>_xll.NCDK_WHIM(B7)</f>
         <v>#N/A</v>
       </c>
-      <c r="BS7" t="str">
+      <c r="BT7" t="str">
         <f>_xll.NCDK_WienerNumbers(B7)</f>
         <v>27, 3</v>
       </c>
-      <c r="BT7">
+      <c r="BU7">
         <f>_xll.NCDK_XLogP(B7)</f>
         <v>3.4139999999999997</v>
       </c>
-      <c r="BU7">
+      <c r="BV7">
         <f>_xll.NCDK_ZagrebIndex(B7)</f>
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:73" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -4174,287 +4207,291 @@
         <v>PXCDDPIOUAJVRE-UHFFFAOYSA-N</v>
       </c>
       <c r="D8">
-        <f>_xll.NCDK_Tanimoto($G8,$G9)</f>
+        <f>_xll.NCDK_Tanimoto($H8,$H9)</f>
         <v>1</v>
       </c>
       <c r="E8" t="str">
+        <f>_xll.NCDK(E$1,$B8)</f>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001010</v>
+      </c>
+      <c r="F8" t="str">
         <f>_xll.NCDK_ECFP0($B8)</f>
         <v>0000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="F8" t="str">
+      <c r="G8" t="str">
         <f>_xll.NCDK_ECFP2($B8)</f>
         <v>0000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="G8" t="str">
+      <c r="H8" t="str">
         <f>_xll.NCDK_ECFP4($B8)</f>
         <v>0000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="H8" t="str">
+      <c r="I8" t="str">
         <f>_xll.NCDK_ECFP6($B8)</f>
         <v>0000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="I8" t="str">
+      <c r="J8" t="str">
         <f>_xll.NCDK_FCFP0($B8)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="J8" t="str">
+      <c r="K8" t="str">
         <f>_xll.NCDK_FCFP2($B8)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="K8" t="str">
+      <c r="L8" t="str">
         <f>_xll.NCDK_FCFP4($B8)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="L8" t="str">
+      <c r="M8" t="str">
         <f>_xll.NCDK_FCFP0($B8)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="M8" t="str">
+      <c r="N8" t="str">
         <f>_xll.NCDK_AtomPairs2DFingerprinter($B8)</f>
         <v>100000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="N8" t="str">
+      <c r="O8" t="str">
         <f>_xll.NCDK_EStateFingerprinter($B8)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="O8" t="str">
+      <c r="P8" t="str">
         <f>_xll.NCDK_ExtendedFingerprinter($B8)</f>
         <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000001000000000000010001</v>
       </c>
-      <c r="P8" t="str">
+      <c r="Q8" t="str">
         <f>_xll.NCDK_CDKFingerprinter($B8)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000010000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="Q8" t="str">
+      <c r="R8" t="str">
         <f>_xll.NCDK_KlekotaRothFingerprinter($B8)</f>
         <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000010000000000000100000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="R8" t="str">
+      <c r="S8" t="str">
         <f>_xll.NCDK_LingoFingerprinter($B8)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="S8" t="str">
+      <c r="T8" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($B8)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001010</v>
       </c>
-      <c r="T8" t="str">
+      <c r="U8" t="str">
         <f>_xll.NCDK_ShortestPathFingerprinter($B8)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="U8" t="str">
+      <c r="V8" t="str">
         <f>_xll.NCDK_SubstructureFingerprinter($B8)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="V8" t="str">
+      <c r="W8" t="str">
         <f>_xll.NCDK_PubchemFingerprinter($B8)</f>
         <v>00000000011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <f>_xll.NCDK_AcidicGroupCount(B8)</f>
         <v>0</v>
       </c>
-      <c r="X8">
+      <c r="Y8">
         <f>_xll.NCDK_ALogP(B8)</f>
         <v>-1.7280000000000006</v>
       </c>
-      <c r="Y8">
+      <c r="Z8">
         <f>_xll.NCDK_AMolarRefractivity(B8)</f>
         <v>17.4696</v>
       </c>
-      <c r="Z8">
+      <c r="AA8">
         <f>_xll.NCDK_APol(B8)</f>
         <v>10.56</v>
       </c>
-      <c r="AA8">
+      <c r="AB8">
         <f>_xll.NCDK_AromaticAtomsCount(B8)</f>
         <v>0</v>
       </c>
-      <c r="AB8">
+      <c r="AC8">
         <f>_xll.NCDK_AromaticBondsCount(B8)</f>
         <v>0</v>
       </c>
-      <c r="AC8">
+      <c r="AD8">
         <f>_xll.NCDK_AtomCount(B8)</f>
         <v>18</v>
       </c>
-      <c r="AD8" t="str">
+      <c r="AE8" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B8)</f>
         <v>0, 0, 0, 0, 0</v>
       </c>
-      <c r="AE8" t="str">
+      <c r="AF8" t="str">
         <f>_xll.NCDK_AutocorrelationMass(B8)</f>
         <v>6, 6, 6, 3, 0</v>
       </c>
-      <c r="AF8" t="str">
+      <c r="AG8" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B8)</f>
         <v>257.709834375, 257.709834375, 257.709834375, 128.8549171875, 0</v>
       </c>
-      <c r="AG8">
+      <c r="AH8">
         <f>_xll.NCDK_BasicGroupCount(B8)</f>
         <v>0</v>
       </c>
-      <c r="AH8" t="str">
+      <c r="AI8" t="str">
         <f>_xll.NCDK_BCUT(B8)</f>
         <v>11.9, 12.1000824042221, -0.15279744210896, 0.0472849621131451, 6.45375, 6.65383240422211</v>
       </c>
-      <c r="AI8">
+      <c r="AJ8">
         <f>_xll.NCDK_BondCount(B8)</f>
         <v>0</v>
       </c>
-      <c r="AJ8">
+      <c r="AK8">
         <f>_xll.NCDK_BPol(B8)</f>
         <v>13.118483999999999</v>
       </c>
-      <c r="AK8" t="str">
+      <c r="AL8" t="str">
         <f>_xll.NCDK_CarbonTypes(B8)</f>
         <v>0, 0, 0, 0, 0, 0, 6, 0, 0</v>
       </c>
-      <c r="AL8" t="str">
+      <c r="AM8" t="str">
         <f>_xll.NCDK_ChiChain(B8)</f>
         <v>0, 0, 0, 0.125, 0, 0, 0, 0, 0.125, 0</v>
       </c>
-      <c r="AM8" t="str">
+      <c r="AN8" t="str">
         <f>_xll.NCDK_ChiCluster(B8)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AN8" t="str">
+      <c r="AO8" t="str">
         <f>_xll.NCDK_ChiPathCluster(B8)</f>
         <v>0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AO8" t="str">
+      <c r="AP8" t="str">
         <f>_xll.NCDK_ChiPath(B8)</f>
         <v>4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0, 4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0</v>
       </c>
-      <c r="AP8" t="str">
+      <c r="AQ8" t="str">
         <f>_xll.NCDK_CPSA(B8)</f>
         <v>#N/A</v>
       </c>
-      <c r="AQ8">
+      <c r="AR8">
         <f>_xll.NCDK_EccentricConnectivityIndex(B8)</f>
         <v>36</v>
       </c>
-      <c r="AR8">
+      <c r="AS8">
         <f>_xll.NCDK_FMF(B8)</f>
         <v>1</v>
       </c>
-      <c r="AS8">
+      <c r="AT8">
         <f>_xll.NCDK_FractionalPSA(B8)</f>
         <v>0</v>
       </c>
-      <c r="AT8">
+      <c r="AU8">
         <f>_xll.NCDK_FragmentComplexity(B8)</f>
         <v>294</v>
       </c>
-      <c r="AU8" t="str">
+      <c r="AV8" t="str">
         <f>_xll.NCDK_GravitationalIndex(B8)</f>
         <v>#N/A</v>
       </c>
-      <c r="AV8">
+      <c r="AW8">
         <f>_xll.NCDK_HBondAcceptorCount(B8)</f>
         <v>0</v>
       </c>
-      <c r="AW8">
+      <c r="AX8">
         <f>_xll.NCDK_HBondDonorCount(B8)</f>
         <v>0</v>
       </c>
-      <c r="AX8">
+      <c r="AY8">
         <f>_xll.NCDK_HybridizationRatio(B8)</f>
         <v>1</v>
       </c>
-      <c r="AY8" t="str">
+      <c r="AZ8" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B8)</f>
         <v>4.16666666666667, 2.22222222222222, 1.33333333333333</v>
       </c>
-      <c r="AZ8" t="str">
+      <c r="BA8" t="str">
         <f>_xll.NCDK_KierHallSmarts(B8)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BA8">
+      <c r="BB8">
         <f>_xll.NCDK_LargestChain(B8)</f>
         <v>4</v>
       </c>
-      <c r="BB8">
+      <c r="BC8">
         <f>_xll.NCDK_LargestPiSystem(B8)</f>
         <v>0</v>
       </c>
-      <c r="BC8" t="str">
+      <c r="BD8" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B8)</f>
         <v>#N/A</v>
       </c>
-      <c r="BD8">
+      <c r="BE8">
         <f>_xll.NCDK_LongestAliphaticChain(B8)</f>
         <v>0</v>
       </c>
-      <c r="BE8">
+      <c r="BF8">
         <f>_xll.NCDK_MannholdLogP(B8)</f>
         <v>2.12</v>
       </c>
-      <c r="BF8" t="str">
+      <c r="BG8" t="str">
         <f>_xll.NCDK_MDE(B8)</f>
         <v>0, 0, 0, 0, 9.12546512839809, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BG8" t="str">
+      <c r="BH8" t="str">
         <f>_xll.NCDK_MomentOfInertia(B8)</f>
         <v>#N/A</v>
       </c>
-      <c r="BH8">
+      <c r="BI8">
         <f>_xll.NCDK_PetitjeanNumber(B8)</f>
         <v>0</v>
       </c>
-      <c r="BI8" t="str">
+      <c r="BJ8" t="str">
         <f>_xll.NCDK_PetitjeanShapeIndex(B8)</f>
         <v>#N/A</v>
       </c>
-      <c r="BJ8">
+      <c r="BK8">
         <f>_xll.NCDK_RotatableBondsCount(B8)</f>
         <v>0</v>
       </c>
-      <c r="BK8">
+      <c r="BL8">
         <f>_xll.NCDK_RuleOfFive(B8)</f>
         <v>0</v>
       </c>
-      <c r="BL8" t="str">
+      <c r="BM8" t="str">
         <f>_xll.NCDK_SmallRing(B8)</f>
         <v>1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0</v>
       </c>
-      <c r="BM8">
+      <c r="BN8">
         <f>_xll.NCDK_TPSA(B8)</f>
         <v>0</v>
       </c>
-      <c r="BN8">
+      <c r="BO8">
         <f>_xll.NCDK_VABC(B8)</f>
         <v>99.975907755200197</v>
       </c>
-      <c r="BO8">
+      <c r="BP8">
         <f>_xll.NCDK_VAdjMa(B8)</f>
         <v>3.5849625007211561</v>
       </c>
-      <c r="BP8">
+      <c r="BQ8">
         <f>_xll.NCDK_Weight(B8)</f>
         <v>84.093900383999994</v>
       </c>
-      <c r="BQ8" t="str">
+      <c r="BR8" t="str">
         <f>_xll.NCDK_WeightedPath(B8)</f>
         <v>11.8125, 1.96875, 0, 0, 0</v>
       </c>
-      <c r="BR8" t="str">
+      <c r="BS8" t="str">
         <f>_xll.NCDK_WHIM(B8)</f>
         <v>#N/A</v>
       </c>
-      <c r="BS8" t="str">
+      <c r="BT8" t="str">
         <f>_xll.NCDK_WienerNumbers(B8)</f>
         <v>27, 3</v>
       </c>
-      <c r="BT8">
+      <c r="BU8">
         <f>_xll.NCDK_XLogP(B8)</f>
         <v>3.4139999999999997</v>
       </c>
-      <c r="BU8">
+      <c r="BV8">
         <f>_xll.NCDK_ZagrebIndex(B8)</f>
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:73" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -4466,287 +4503,291 @@
         <v>PXCDDPIOUAJVRE-UHFFFAOYSA-N</v>
       </c>
       <c r="D9">
-        <f>_xll.NCDK_Tanimoto($G9,$G10)</f>
+        <f>_xll.NCDK_Tanimoto($H9,$H10)</f>
         <v>1.9607843137254902E-2</v>
       </c>
       <c r="E9" t="str">
+        <f>_xll.NCDK(E$1,$B9)</f>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001010</v>
+      </c>
+      <c r="F9" t="str">
         <f>_xll.NCDK_ECFP0($B9)</f>
         <v>0000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="F9" t="str">
+      <c r="G9" t="str">
         <f>_xll.NCDK_ECFP2($B9)</f>
         <v>0000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="G9" t="str">
+      <c r="H9" t="str">
         <f>_xll.NCDK_ECFP4($B9)</f>
         <v>0000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="H9" t="str">
+      <c r="I9" t="str">
         <f>_xll.NCDK_ECFP6($B9)</f>
         <v>0000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="I9" t="str">
+      <c r="J9" t="str">
         <f>_xll.NCDK_FCFP0($B9)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="J9" t="str">
+      <c r="K9" t="str">
         <f>_xll.NCDK_FCFP2($B9)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="K9" t="str">
+      <c r="L9" t="str">
         <f>_xll.NCDK_FCFP4($B9)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="L9" t="str">
+      <c r="M9" t="str">
         <f>_xll.NCDK_FCFP0($B9)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="M9" t="str">
+      <c r="N9" t="str">
         <f>_xll.NCDK_AtomPairs2DFingerprinter($B9)</f>
         <v>100000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="N9" t="str">
+      <c r="O9" t="str">
         <f>_xll.NCDK_EStateFingerprinter($B9)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="O9" t="str">
+      <c r="P9" t="str">
         <f>_xll.NCDK_ExtendedFingerprinter($B9)</f>
         <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000001000000000000010001</v>
       </c>
-      <c r="P9" t="str">
+      <c r="Q9" t="str">
         <f>_xll.NCDK_CDKFingerprinter($B9)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000010000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="Q9" t="str">
+      <c r="R9" t="str">
         <f>_xll.NCDK_KlekotaRothFingerprinter($B9)</f>
         <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000010000000000000100000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="R9" t="str">
+      <c r="S9" t="str">
         <f>_xll.NCDK_LingoFingerprinter($B9)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="S9" t="str">
+      <c r="T9" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($B9)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001010</v>
       </c>
-      <c r="T9" t="str">
+      <c r="U9" t="str">
         <f>_xll.NCDK_ShortestPathFingerprinter($B9)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="U9" t="str">
+      <c r="V9" t="str">
         <f>_xll.NCDK_SubstructureFingerprinter($B9)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="V9" t="str">
+      <c r="W9" t="str">
         <f>_xll.NCDK_PubchemFingerprinter($B9)</f>
         <v>00000000011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="W9">
+      <c r="X9">
         <f>_xll.NCDK_AcidicGroupCount(B9)</f>
         <v>0</v>
       </c>
-      <c r="X9">
+      <c r="Y9">
         <f>_xll.NCDK_ALogP(B9)</f>
         <v>-1.7280000000000006</v>
       </c>
-      <c r="Y9">
+      <c r="Z9">
         <f>_xll.NCDK_AMolarRefractivity(B9)</f>
         <v>17.4696</v>
       </c>
-      <c r="Z9">
+      <c r="AA9">
         <f>_xll.NCDK_APol(B9)</f>
         <v>10.56</v>
       </c>
-      <c r="AA9">
+      <c r="AB9">
         <f>_xll.NCDK_AromaticAtomsCount(B9)</f>
         <v>0</v>
       </c>
-      <c r="AB9">
+      <c r="AC9">
         <f>_xll.NCDK_AromaticBondsCount(B9)</f>
         <v>0</v>
       </c>
-      <c r="AC9">
+      <c r="AD9">
         <f>_xll.NCDK_AtomCount(B9)</f>
         <v>18</v>
       </c>
-      <c r="AD9" t="str">
+      <c r="AE9" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B9)</f>
         <v>0, 0, 0, 0, 0</v>
       </c>
-      <c r="AE9" t="str">
+      <c r="AF9" t="str">
         <f>_xll.NCDK_AutocorrelationMass(B9)</f>
         <v>6, 6, 6, 3, 0</v>
       </c>
-      <c r="AF9" t="str">
+      <c r="AG9" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B9)</f>
         <v>257.709834375, 257.709834375, 257.709834375, 128.8549171875, 0</v>
       </c>
-      <c r="AG9">
+      <c r="AH9">
         <f>_xll.NCDK_BasicGroupCount(B9)</f>
         <v>0</v>
       </c>
-      <c r="AH9" t="str">
+      <c r="AI9" t="str">
         <f>_xll.NCDK_BCUT(B9)</f>
         <v>11.9, 12.1000824042221, -0.15279744210896, 0.0472849621131451, 6.45375, 6.65383240422211</v>
       </c>
-      <c r="AI9">
+      <c r="AJ9">
         <f>_xll.NCDK_BondCount(B9)</f>
         <v>0</v>
       </c>
-      <c r="AJ9">
+      <c r="AK9">
         <f>_xll.NCDK_BPol(B9)</f>
         <v>13.118483999999999</v>
       </c>
-      <c r="AK9" t="str">
+      <c r="AL9" t="str">
         <f>_xll.NCDK_CarbonTypes(B9)</f>
         <v>0, 0, 0, 0, 0, 0, 6, 0, 0</v>
       </c>
-      <c r="AL9" t="str">
+      <c r="AM9" t="str">
         <f>_xll.NCDK_ChiChain(B9)</f>
         <v>0, 0, 0, 0.125, 0, 0, 0, 0, 0.125, 0</v>
       </c>
-      <c r="AM9" t="str">
+      <c r="AN9" t="str">
         <f>_xll.NCDK_ChiCluster(B9)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AN9" t="str">
+      <c r="AO9" t="str">
         <f>_xll.NCDK_ChiPathCluster(B9)</f>
         <v>0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AO9" t="str">
+      <c r="AP9" t="str">
         <f>_xll.NCDK_ChiPath(B9)</f>
         <v>4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0, 4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0</v>
       </c>
-      <c r="AP9" t="str">
+      <c r="AQ9" t="str">
         <f>_xll.NCDK_CPSA(B9)</f>
         <v>#N/A</v>
       </c>
-      <c r="AQ9">
+      <c r="AR9">
         <f>_xll.NCDK_EccentricConnectivityIndex(B9)</f>
         <v>36</v>
       </c>
-      <c r="AR9">
+      <c r="AS9">
         <f>_xll.NCDK_FMF(B9)</f>
         <v>1</v>
       </c>
-      <c r="AS9">
+      <c r="AT9">
         <f>_xll.NCDK_FractionalPSA(B9)</f>
         <v>0</v>
       </c>
-      <c r="AT9">
+      <c r="AU9">
         <f>_xll.NCDK_FragmentComplexity(B9)</f>
         <v>294</v>
       </c>
-      <c r="AU9" t="str">
+      <c r="AV9" t="str">
         <f>_xll.NCDK_GravitationalIndex(B9)</f>
         <v>#N/A</v>
       </c>
-      <c r="AV9">
+      <c r="AW9">
         <f>_xll.NCDK_HBondAcceptorCount(B9)</f>
         <v>0</v>
       </c>
-      <c r="AW9">
+      <c r="AX9">
         <f>_xll.NCDK_HBondDonorCount(B9)</f>
         <v>0</v>
       </c>
-      <c r="AX9">
+      <c r="AY9">
         <f>_xll.NCDK_HybridizationRatio(B9)</f>
         <v>1</v>
       </c>
-      <c r="AY9" t="str">
+      <c r="AZ9" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B9)</f>
         <v>4.16666666666667, 2.22222222222222, 1.33333333333333</v>
       </c>
-      <c r="AZ9" t="str">
+      <c r="BA9" t="str">
         <f>_xll.NCDK_KierHallSmarts(B9)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BA9">
+      <c r="BB9">
         <f>_xll.NCDK_LargestChain(B9)</f>
         <v>4</v>
       </c>
-      <c r="BB9">
+      <c r="BC9">
         <f>_xll.NCDK_LargestPiSystem(B9)</f>
         <v>0</v>
       </c>
-      <c r="BC9" t="str">
+      <c r="BD9" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B9)</f>
         <v>#N/A</v>
       </c>
-      <c r="BD9">
+      <c r="BE9">
         <f>_xll.NCDK_LongestAliphaticChain(B9)</f>
         <v>0</v>
       </c>
-      <c r="BE9">
+      <c r="BF9">
         <f>_xll.NCDK_MannholdLogP(B9)</f>
         <v>2.12</v>
       </c>
-      <c r="BF9" t="str">
+      <c r="BG9" t="str">
         <f>_xll.NCDK_MDE(B9)</f>
         <v>0, 0, 0, 0, 9.12546512839809, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BG9" t="str">
+      <c r="BH9" t="str">
         <f>_xll.NCDK_MomentOfInertia(B9)</f>
         <v>#N/A</v>
       </c>
-      <c r="BH9">
+      <c r="BI9">
         <f>_xll.NCDK_PetitjeanNumber(B9)</f>
         <v>0</v>
       </c>
-      <c r="BI9" t="str">
+      <c r="BJ9" t="str">
         <f>_xll.NCDK_PetitjeanShapeIndex(B9)</f>
         <v>#N/A</v>
       </c>
-      <c r="BJ9">
+      <c r="BK9">
         <f>_xll.NCDK_RotatableBondsCount(B9)</f>
         <v>0</v>
       </c>
-      <c r="BK9">
+      <c r="BL9">
         <f>_xll.NCDK_RuleOfFive(B9)</f>
         <v>0</v>
       </c>
-      <c r="BL9" t="str">
+      <c r="BM9" t="str">
         <f>_xll.NCDK_SmallRing(B9)</f>
         <v>1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0</v>
       </c>
-      <c r="BM9">
+      <c r="BN9">
         <f>_xll.NCDK_TPSA(B9)</f>
         <v>0</v>
       </c>
-      <c r="BN9">
+      <c r="BO9">
         <f>_xll.NCDK_VABC(B9)</f>
         <v>99.975907755200197</v>
       </c>
-      <c r="BO9">
+      <c r="BP9">
         <f>_xll.NCDK_VAdjMa(B9)</f>
         <v>3.5849625007211561</v>
       </c>
-      <c r="BP9">
+      <c r="BQ9">
         <f>_xll.NCDK_Weight(B9)</f>
         <v>84.093900383999994</v>
       </c>
-      <c r="BQ9" t="str">
+      <c r="BR9" t="str">
         <f>_xll.NCDK_WeightedPath(B9)</f>
         <v>11.8125, 1.96875, 0, 0, 0</v>
       </c>
-      <c r="BR9" t="str">
+      <c r="BS9" t="str">
         <f>_xll.NCDK_WHIM(B9)</f>
         <v>#N/A</v>
       </c>
-      <c r="BS9" t="str">
+      <c r="BT9" t="str">
         <f>_xll.NCDK_WienerNumbers(B9)</f>
         <v>27, 3</v>
       </c>
-      <c r="BT9">
+      <c r="BU9">
         <f>_xll.NCDK_XLogP(B9)</f>
         <v>3.4139999999999997</v>
       </c>
-      <c r="BU9">
+      <c r="BV9">
         <f>_xll.NCDK_ZagrebIndex(B9)</f>
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:73" ht="19" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:74" ht="19" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>63</v>
       </c>
@@ -4758,287 +4799,291 @@
         <v>[C@@]12(C(C([C@](O[H])(C(C1=C(C([C@@]3([C@]2([H])C(C([C@]4([C@@]3([H])C(C([C@]4([H])[C@](C([H])([H])[H])(C(C(C(C(C([H])([H])[H])(C([H])([H])[H])[H])([H])[H])([H])[H])([H])[H])[H])([H])[H])([H])[H])C([H])([H])[H])([H])[H])([H])[H])[H])([H])[H])[H])([H])[H])[H])([H])[H])([H])[H])C([H])([H])[H]</v>
       </c>
       <c r="D10">
-        <f>_xll.NCDK_Tanimoto($G10,$G11)</f>
+        <f>_xll.NCDK_Tanimoto($H10,$H11)</f>
         <v>0.47761194029850745</v>
       </c>
       <c r="E10" t="str">
+        <f>_xll.NCDK(E$1,$B10)</f>
+        <v>0000000000000000000000000100000000000000000000000100000000000000010000000101000000000000010000010010000110010001001101000000011110010000001010101010110100101001001110</v>
+      </c>
+      <c r="F10" t="str">
         <f>_xll.NCDK_ECFP0($B10)</f>
         <v>0000000000000010000000000100000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000100000000000000000010000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000100000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="F10" t="str">
+      <c r="G10" t="str">
         <f>_xll.NCDK_ECFP2($B10)</f>
         <v>0000000000000010000000001100000000000000000000001000000000000000000000000001000000001000100000000000000000000000000000000000000000000100000000000000000010000000000000000000000000000000000000000000000000000010000000000000010000000010000000000000000000000000000000000000000001000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000001000000000000000000000000000000000000000010000000000000000000000000100000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100010000000000001000001000000000000000000000001000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000010000000000000000000100000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="G10" t="str">
+      <c r="H10" t="str">
         <f>_xll.NCDK_ECFP4($B10)</f>
         <v>0000000000000010000000001100000000000000000100001000000000010000000000000001000000001010100000000000000000000000000000000000000000000100000000010000000010000000000000000000000000000000000000000000000000000010000000000000010000000010000000000000000000000000000000000000000001000000000010000000001000000000000000100000010000000000000000000000000000000010000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000001000100000000000100000000000000000000000010000000000000000000000000100000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000010100000000000000000000000000000000000000000000000000000000000000100010000000000001000001000000000000000000000011000000000000010100000000000000000000000000000000000000000100000000000000000000000000000100000000000001000010000000000000000000000000010000000000010000000000000000000100000001000000000000000100000000000000000000000000000000</v>
       </c>
-      <c r="H10" t="str">
+      <c r="I10" t="str">
         <f>_xll.NCDK_ECFP6($B10)</f>
         <v>0000000000001010001000001100000000000000000100001000000000010000000000000001000000001010100000000000000000000000000000000000000000000100000000010000000010000000000000000000000000000000000000000000000000001010000001100000011000000010000000000000000000000000000000000000000001000000000010000000001000000000000000110000010000000000000000000000000000000010000110000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000001000100000000000100000000000000000000000010000000000000000000000000100000000000000001000000000010000000000000000001000000000000100000000000000000000000000010000010000000000000000000000000000010100000001000000000000000000000000000000000000000000000000000000100010000000000001010001000000000000000000000011000000000000010100000000000000000000011000000010000000000100000000000000000000000000000100010000000001000010000000000000000000000000010000000000010000000000000001000100000001000000010000000100000000000000000000000000000000</v>
       </c>
-      <c r="I10" t="str">
+      <c r="J10" t="str">
         <f>_xll.NCDK_FCFP0($B10)</f>
         <v>1001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="J10" t="str">
+      <c r="K10" t="str">
         <f>_xll.NCDK_FCFP2($B10)</f>
         <v>1001000000000000000000010000000000000000000000000000000000000000000000000000000001000010000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="K10" t="str">
+      <c r="L10" t="str">
         <f>_xll.NCDK_FCFP4($B10)</f>
         <v>1001000000000000000000010000000000000000000000000000000000000000000000000000000001000010000000000000000000000000000000000000000000000000000000000000000100000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000100000000000000000000000001100000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000010000000000000000000000000000000000000000000000000001000100000000000000000000000000000000000000000000000000000000000000100000000001000000000010000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000100000000000010000000000000010000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000001000000000000000000000</v>
       </c>
-      <c r="L10" t="str">
+      <c r="M10" t="str">
         <f>_xll.NCDK_FCFP0($B10)</f>
         <v>1001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="M10" t="str">
+      <c r="N10" t="str">
         <f>_xll.NCDK_AtomPairs2DFingerprinter($B10)</f>
         <v>101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="N10" t="str">
+      <c r="O10" t="str">
         <f>_xll.NCDK_EStateFingerprinter($B10)</f>
         <v>0000000000000001001000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="O10" t="str">
+      <c r="P10" t="str">
         <f>_xll.NCDK_ExtendedFingerprinter($B10)</f>
         <v>000000000000000000001000000010000000000000000000000000000000100001000000010000000000010000000010010001010000000110001110000000000000000010000000001000001001000000000000001010000000100000000000010000000000000000000000000000000000000100000010000000000010000001010000000000010000100001000000000000101000001000000000000000001000000000000011000000000000000000000000000000000000001000100000000000000000000000001100100100000000000010000001000000101000000000000100000000000000000101000000010000000000100000000001000000000000000000000010000000000000000000000000000000000000000000101000000000000000001000000000010000100010000000000000000000000000001000010000000000000000100001000001000000000010000100000000000000001010000000000000000000010000000000000000001000001000000000111000000010000000000000010000000010000010010010010000000000010000000000010000000000101000000000000000000001000000000010100100000010000010000000100000010000000000000100000000000000000010110000000001011000010010000000000000000010000001000000000000011111111</v>
       </c>
-      <c r="P10" t="str">
+      <c r="Q10" t="str">
         <f>_xll.NCDK_CDKFingerprinter($B10)</f>
         <v>0000010000000001001000000000000000000010000000000000000000100000000000000001100000000001000000000000000000000000000000000000000100001100000000000000110000000010000000000100100000110000000000000000000000000010000000000000000000000000000000000000000000000000010000000000000000000000001010000000000001001000000000000001100000000100000000000000000100000000000000000000010000000000000000000000000010000000000001001100000000000010000000000000000000010000000010000100000000000000001000000000010000000000011011100100101000000000001000000000011010000010010000000000000000000000001000100000000000001000000000000000000000000000011001000000000000000100000010000000000000011000000000000000010000000000000000000000000000010000000000011000000000000000000001110101000010000000000000000000000000000100000000000000000000001100000000000000000000000010000000001010001000100000000100010100000010000000000000000000000000000000000000000000000010000000010000000000000000000001000000000000000000010000000000000000000000000000000000000000001000000000</v>
       </c>
-      <c r="Q10" t="str">
+      <c r="R10" t="str">
         <f>_xll.NCDK_KlekotaRothFingerprinter($B10)</f>
         <v>110000010000010011000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001111000000100000000000000000010000000000000011010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000010100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000010000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000011000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000001000000000000000000100000100000000000001000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000100000000000000001011000000010000000000000000000000010000000000000100000100000010010000100100000010000001000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="R10" t="str">
+      <c r="S10" t="str">
         <f>_xll.NCDK_LingoFingerprinter($B10)</f>
         <v>0000010000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000010000000000000000000000000000100000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000011000000000000000000000000000000010000000010000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000010000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000</v>
       </c>
-      <c r="S10" t="str">
+      <c r="T10" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($B10)</f>
         <v>0000000000000000000000000100000000000000000000000100000000000000010000000101000000000000010000010010000110010001001101000000011110010000001010101010110100101001001110</v>
       </c>
-      <c r="T10" t="str">
+      <c r="U10" t="str">
         <f>_xll.NCDK_ShortestPathFingerprinter($B10)</f>
         <v>1011001000010001010001111111000100000001000000000011011110010100101010100100000000001100000010100101000010010000011110100100000000010100010101000100000010000001000001010100000001100010000100000001100001000110100001000000001011000010101101010011010010001000010001000010001111000100011000000100101010110000110000010010110001100100010000000001000000010010110000000000010010111010010001101010010011000000101100000000100101101011000110100001100000100010010001010000000000010000010100001011001010001100010000010001111001100000101000010100010001001010000001000010011000111110010010000000110101011010001011001010000110000000000100000000010011000100000000011000010000000101000100000000100000000000010100000000010001000110100100000000000000010000001010000000010001000000101000010110000000101000011010011100011001110000000011100000001000000010101000001001001000010000111100010010010001110100100100001000010101000101000010010110010000000011001010010000000010011001101010100101001100000001011000001011001001101100000100100010000000000000</v>
       </c>
-      <c r="U10" t="str">
+      <c r="V10" t="str">
         <f>_xll.NCDK_SubstructureFingerprinter($B10)</f>
         <v>1111100000010110000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000001000000100001</v>
       </c>
-      <c r="V10" t="str">
+      <c r="W10" t="str">
         <f>_xll.NCDK_PubchemFingerprinter($B10)</f>
         <v>11110000011110000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000110000000000000000000000000000000001100100110000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001101000000000000000000000100000000000000000000000111100010100101000001000000000000010000000100000000000000000000000000000001000000000100000000000001000100000010000100000000000000000000000000000000000000000001000000000000000000000000000000000100000000000000000000000000000001000000000000001000000000010000000000000000100000000000000000100000000000000000001001100000000000000000010000000000000000011100000001100000011110000000011111000000000000000000000000000000000000000000000000000000000000000110000000000000000000100000000000000000000100000000000000000000100000000000000000000100000000000000000000</v>
       </c>
-      <c r="W10">
+      <c r="X10">
         <f>_xll.NCDK_AcidicGroupCount(B10)</f>
         <v>0</v>
       </c>
-      <c r="X10">
+      <c r="Y10">
         <f>_xll.NCDK_ALogP(B10)</f>
         <v>1.5548000000000011</v>
       </c>
-      <c r="Y10">
+      <c r="Z10">
         <f>_xll.NCDK_AMolarRefractivity(B10)</f>
         <v>115.17460000000001</v>
       </c>
-      <c r="Z10">
+      <c r="AA10">
         <f>_xll.NCDK_APol(B10)</f>
         <v>78.99447799999993</v>
       </c>
-      <c r="AA10">
+      <c r="AB10">
         <f>_xll.NCDK_AromaticAtomsCount(B10)</f>
         <v>0</v>
       </c>
-      <c r="AB10">
+      <c r="AC10">
         <f>_xll.NCDK_AromaticBondsCount(B10)</f>
         <v>0</v>
       </c>
-      <c r="AC10">
+      <c r="AD10">
         <f>_xll.NCDK_AtomCount(B10)</f>
         <v>74</v>
       </c>
-      <c r="AD10" t="str">
+      <c r="AE10" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B10)</f>
         <v>0.0827991713427503, -0.0229631507285856, -0.0270969061556759, 0.00647128770548948, 0.00909713625645344</v>
       </c>
-      <c r="AE10" t="str">
+      <c r="AF10" t="str">
         <f>_xll.NCDK_AutocorrelationMass(B10)</f>
         <v>28.7744690355409, 31.3320919771326, 48.6641839542651, 54.6641839542651, 49.6641839542651</v>
       </c>
-      <c r="AF10" t="str">
+      <c r="AG10" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B10)</f>
         <v>2589.35165284459, 3179.06049775734, 4922.9791073968, 5328.87269506555, 4616.91714731414</v>
       </c>
-      <c r="AG10">
+      <c r="AH10">
         <f>_xll.NCDK_BasicGroupCount(B10)</f>
         <v>0</v>
       </c>
-      <c r="AH10" t="str">
+      <c r="AI10" t="str">
         <f>_xll.NCDK_BCUT(B10)</f>
         <v>11.89, 15.9949214370833, -0.392219399090072, 0.0596280868632924, 5.23875003301361, 12.6475909449557</v>
       </c>
-      <c r="AI10">
+      <c r="AJ10">
         <f>_xll.NCDK_BondCount(B10)</f>
         <v>46</v>
       </c>
-      <c r="AJ10">
+      <c r="AK10">
         <f>_xll.NCDK_BPol(B10)</f>
         <v>50.287521999999989</v>
       </c>
-      <c r="AK10" t="str">
+      <c r="AL10" t="str">
         <f>_xll.NCDK_CarbonTypes(B10)</f>
         <v>0, 0, 0, 1, 1, 5, 12, 6, 2</v>
       </c>
-      <c r="AL10" t="str">
+      <c r="AM10" t="str">
         <f>_xll.NCDK_ChiChain(B10)</f>
         <v>0, 0, 0.0833333333333333, 0.393634553260967, 0.976046921839545, 0, 0, 0.0833333333333333, 0.37164819290959, 0.863165765466815</v>
       </c>
-      <c r="AM10" t="str">
+      <c r="AN10" t="str">
         <f>_xll.NCDK_ChiCluster(B10)</f>
         <v>2.9521315814894, 0.235702260395516, 1.02234106177579, 0.203263132396285, 2.68481479020038, 0.219913202813724, 0.935219433730957, 0.179558378198271</v>
       </c>
-      <c r="AN10" t="str">
+      <c r="AO10" t="str">
         <f>_xll.NCDK_ChiPathCluster(B10)</f>
         <v>6.93012787723299, 11.9183161832455, 18.084244169983, 6.31056734345633, 10.8246614459309, 15.7948474414898</v>
       </c>
-      <c r="AO10" t="str">
+      <c r="AP10" t="str">
         <f>_xll.NCDK_ChiPath(B10)</f>
         <v>20.1040835277556, 13.2536913009629, 13.0668536638687, 11.1291235227258, 9.49703814548855, 7.69096408557495, 5.93907638185732, 4.4721666474432, 19.344190342069, 12.6298450216499, 12.1863667747532, 10.2790812759586, 8.6662445789686, 6.67875288189192, 5.16344144011131, 3.80610378452706</v>
       </c>
-      <c r="AP10" t="str">
+      <c r="AQ10" t="str">
         <f>_xll.NCDK_CPSA(B10)</f>
         <v>740.518679745203, 1141.6281036277, 24.7477735904141, 216.516577646307, -333.794969260415, -24.5734427697376, 524.002102098896, 1475.42307288811, 49.3212163601517, 0.773763217212662, 1.19287988066324, 0.0258587898400593, 0.226236782787338, -0.348780221713257, -0.025676632684061, 708.702485273172, 1092.57834600072, 23.6844918679688, 207.213998617263, -319.453554322133, -23.5176511261314, 0.136302900713605, 0.25436791475781, 2.7228153119618, 9.4535627888125, 899.894129431074, 57.1411279604366, 0.940293602018195, 0.0597063979818049</v>
       </c>
-      <c r="AQ10">
+      <c r="AR10">
         <f>_xll.NCDK_EccentricConnectivityIndex(B10)</f>
         <v>669</v>
       </c>
-      <c r="AR10">
+      <c r="AS10">
         <f>_xll.NCDK_FMF(B10)</f>
         <v>0.22972972972972974</v>
       </c>
-      <c r="AS10">
+      <c r="AT10">
         <f>_xll.NCDK_FractionalPSA(B10)</f>
         <v>5.2361188574192148E-2</v>
       </c>
-      <c r="AT10">
+      <c r="AU10">
         <f>_xll.NCDK_FragmentComplexity(B10)</f>
         <v>5173.01</v>
       </c>
-      <c r="AU10" t="str">
+      <c r="AV10" t="str">
         <f>_xll.NCDK_GravitationalIndex(B10)</f>
         <v>1941.85812139388, 44.0665192793109, 12.4759176252409, 2394.88950905792, 48.9376083299737, 13.37914910667, 4535.65140656394, 67.3472449812458, 16.5531209985441</v>
       </c>
-      <c r="AV10">
+      <c r="AW10">
         <f>_xll.NCDK_HBondAcceptorCount(B10)</f>
         <v>1</v>
       </c>
-      <c r="AW10">
+      <c r="AX10">
         <f>_xll.NCDK_HBondDonorCount(B10)</f>
         <v>1</v>
       </c>
-      <c r="AX10">
+      <c r="AY10">
         <f>_xll.NCDK_HybridizationRatio(B10)</f>
         <v>0.92592592592592593</v>
       </c>
-      <c r="AY10" t="str">
+      <c r="AZ10" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B10)</f>
         <v>21.2403746097815, 7.921875, 3.65484429065744</v>
       </c>
-      <c r="AZ10" t="str">
+      <c r="BA10" t="str">
         <f>_xll.NCDK_KierHallSmarts(B10)</f>
         <v>0, 0, 0, 0, 0, 0, 5, 0, 11, 0, 1, 0, 7, 0, 0, 1, 0, 0, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BA10">
+      <c r="BB10">
         <f>_xll.NCDK_LargestChain(B10)</f>
         <v>7</v>
       </c>
-      <c r="BB10">
+      <c r="BC10">
         <f>_xll.NCDK_LargestPiSystem(B10)</f>
         <v>2</v>
       </c>
-      <c r="BC10" t="str">
+      <c r="BD10" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B10)</f>
         <v>3.502934717034, 3.502934717034</v>
       </c>
-      <c r="BD10">
+      <c r="BE10">
         <f>_xll.NCDK_LongestAliphaticChain(B10)</f>
         <v>7</v>
       </c>
-      <c r="BE10">
+      <c r="BF10">
         <f>_xll.NCDK_MannholdLogP(B10)</f>
         <v>4.3199999999999994</v>
       </c>
-      <c r="BF10" t="str">
+      <c r="BG10" t="str">
         <f>_xll.NCDK_MDE(B10)</f>
         <v>2.79346109096649, 16.5925259846737, 11.5560895487586, 3.39888423642021, 17.7527182855433, 29.2401176288661, 7.64127863367805, 8.77423090217006, 6.5802347918611, 0.5, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BG10" t="str">
+      <c r="BH10" t="str">
         <f>_xll.NCDK_MomentOfInertia(B10)</f>
         <v>10068.4095883237, 9731.07167302841, 773.613761142664, 1.03466606008362, 13.0147757111406, 12.5787210127379, 8.29661608019916</v>
       </c>
-      <c r="BH10">
+      <c r="BI10">
         <f>_xll.NCDK_PetitjeanNumber(B10)</f>
         <v>0.46666666666666667</v>
       </c>
-      <c r="BI10" t="str">
+      <c r="BJ10" t="str">
         <f>_xll.NCDK_PetitjeanShapeIndex(B10)</f>
         <v>0.875, 0.940550174456362</v>
       </c>
-      <c r="BJ10">
+      <c r="BK10">
         <f>_xll.NCDK_RotatableBondsCount(B10)</f>
         <v>5</v>
       </c>
-      <c r="BK10">
+      <c r="BL10">
         <f>_xll.NCDK_RuleOfFive(B10)</f>
         <v>1</v>
       </c>
-      <c r="BL10" t="str">
+      <c r="BM10" t="str">
         <f>_xll.NCDK_SmallRing(B10)</f>
         <v>4, 0, 1, 0, 0, 0, 1, 3, 0, 0, 0</v>
       </c>
-      <c r="BM10">
+      <c r="BN10">
         <f>_xll.NCDK_TPSA(B10)</f>
         <v>20.23</v>
       </c>
-      <c r="BN10">
+      <c r="BO10">
         <f>_xll.NCDK_VABC(B10)</f>
         <v>432.2759767957632</v>
       </c>
-      <c r="BO10">
+      <c r="BP10">
         <f>_xll.NCDK_VAdjMa(B10)</f>
         <v>5.9541963103868758</v>
       </c>
-      <c r="BP10">
+      <c r="BQ10">
         <f>_xll.NCDK_Weight(B10)</f>
         <v>386.35486609200063</v>
       </c>
-      <c r="BQ10" t="str">
+      <c r="BR10" t="str">
         <f>_xll.NCDK_WeightedPath(B10)</f>
         <v>57.2167299866347, 2.04345464237981, 2.54245315921217, 2.54245315921217, 0</v>
       </c>
-      <c r="BR10" t="str">
+      <c r="BS10" t="str">
         <f>_xll.NCDK_WHIM(B10)</f>
         <v>1.22231276339169, 2.17046945111189, 25.8559001988821, 0.0417903530188526, 0.0742074265238894, #N/A, #N/A, #N/A, 0.0962638773185697, 0.00388857657057473, 66.8991567190677, 29.2486824133857, 90.3764308473927, 188.22062289613, 0.413001665342944, #N/A, 66.9993091729568</v>
       </c>
-      <c r="BS10" t="str">
+      <c r="BT10" t="str">
         <f>_xll.NCDK_WienerNumbers(B10)</f>
         <v>2022, 54</v>
       </c>
-      <c r="BT10">
+      <c r="BU10">
         <f>_xll.NCDK_XLogP(B10)</f>
         <v>10.518000000000004</v>
       </c>
-      <c r="BU10">
+      <c r="BV10">
         <f>_xll.NCDK_ZagrebIndex(B10)</f>
         <v>158</v>
       </c>
     </row>
-    <row r="11" spans="1:73" ht="19" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:74" ht="19" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -5050,278 +5095,282 @@
         <v>InChI=1S/C27H46O/c1-18(2)7-6-8-19(3)23-11-12-24-22-10-9-20-17-21(28)13-15-26(20,4)25(22)14-16-27(23,24)5/h9,18-19,21-25,28H,6-8,10-17H2,1-5H3</v>
       </c>
       <c r="E11" t="str">
+        <f>_xll.NCDK(E$1,$B11)</f>
+        <v>0000000000000000000000000100000000000000000000000100000000000000010000000101000000000000010000010010000110010001001101000000001110010000001010101010110100101001001110</v>
+      </c>
+      <c r="F11" t="str">
         <f>_xll.NCDK_ECFP0($B11)</f>
         <v>0000000000000010000000000100000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000100000000000000000010000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000100000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="F11" t="str">
+      <c r="G11" t="str">
         <f>_xll.NCDK_ECFP2($B11)</f>
         <v>0000000000000010000000001100000000000000000000001000000000000000000000000000000000000000100000000000000000000000000000000000000000000100000000000000000010000000000000000000000000000000000000000000000000000010000001000000010000000010000000000000000000000000000000000000000001000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000010000001000000000000000000000000000000000000000010000000000000000000000000100000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000001000001000000000000000000000001000100000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000010000000000000000000100000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="G11" t="str">
+      <c r="H11" t="str">
         <f>_xll.NCDK_ECFP4($B11)</f>
         <v>0000000000000010000000001100000000000000000100001000100000010000000000000000000000000000100000000000000000000000000000000000000000000100000000010000000010000000000000000000000000000000000000000000000000000010000001000000010000000010000000000000000000000000000000000000000001000000000010010000000000000000000000000000000000000010000000000000001000000010000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000100100000000000000000010000001000000000000000100000000000000000000000010000001000000000000000000100000000000000000001000000000000000000000000000000010000000100000000000000000000000000000000000000000000000000000000000000010000000100000000000000000000000000010000000000000000000000000000001000000000000001000001000100000000000010000001000100000000000100000000000000000000000000000000000000000000000000000001000000000000000000000000000001000000000000000000000000000000010000000000010000000000000000000100000000000000000000000100000000000000000000000000000000</v>
       </c>
-      <c r="H11" t="str">
+      <c r="I11" t="str">
         <f>_xll.NCDK_ECFP6($B11)</f>
         <v>0000000000001010000000001100000000000000000100001000100000010000000000000000000000000000100000000010000000000000001000000000000000000100000000010000000010000000000000000000000000000001000000000000000000001010000001000010010000000010000000000000000000000000000000000000100001000001000010010000000000000000000000000000000000000010001000000000001000000010000000000000000000000000000000000000100000000001000000000000000000000000000000000000000000000000000000000100000000000100100000000000000000010100001000000000000000100000000000000000000000010000001000000000000000000110000000000000000001000000000000000000000000000000010000000100000000000000000000000000000000000000000000000000000000000000010000010100000000000000000000000000011000000000000000000000000000001000000000000001000001000100000000001010000001000100000000000100010000000000000000000000000000000000000000000000000001000000001000000000000000000001000000000000000000000000000000010000000100010000000000001000000100000000000000000000000100000000000000000000000000000000</v>
       </c>
-      <c r="I11" t="str">
+      <c r="J11" t="str">
         <f>_xll.NCDK_FCFP0($B11)</f>
         <v>1001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="J11" t="str">
+      <c r="K11" t="str">
         <f>_xll.NCDK_FCFP2($B11)</f>
         <v>1001000000000000000000010000000000000000000000000000000000000000000000000000000001000010000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="K11" t="str">
+      <c r="L11" t="str">
         <f>_xll.NCDK_FCFP4($B11)</f>
         <v>1001000000000000000000010000000000000000000000000000000000000000000000000000000001000010000000000000000000000000000000000000000000000000000000000000000100000001010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000100000000000000000000000001100000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000010000000000000000000010000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000010000000000000000000000000100000000000010000000000000010000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="L11" t="str">
+      <c r="M11" t="str">
         <f>_xll.NCDK_FCFP0($B11)</f>
         <v>1001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="M11" t="str">
+      <c r="N11" t="str">
         <f>_xll.NCDK_AtomPairs2DFingerprinter($B11)</f>
         <v>101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="N11" t="str">
+      <c r="O11" t="str">
         <f>_xll.NCDK_EStateFingerprinter($B11)</f>
         <v>0000001010101001001000000000000001000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="O11" t="str">
+      <c r="P11" t="str">
         <f>_xll.NCDK_ExtendedFingerprinter($B11)</f>
         <v>000000000000000000000000000000000000000000000000000000000000100001000000000000000000000000000010000000000000000000000110000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000001000001000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000001000000100000000000000000000000000101000000000000100000000000000000100000000010000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000010000100010000000000000000000000000000000000000000000000000000000000001000000000000000100000000000000000000000000000000000000000000000000000000001000001000000000010000000010000000000000010000000010000000000000010000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000110000000000001000010000000000000000000000000001000000000000011111111</v>
       </c>
-      <c r="P11" t="str">
+      <c r="Q11" t="str">
         <f>_xll.NCDK_CDKFingerprinter($B11)</f>
         <v>0000010000000000000000000000000000000010000000000000000000000000000000000001100000000001000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000001000100000000000010000000000000000000010000000000000000000000000000001000000000010000000000000000000000000000000000001000000000001000000010000000000000000000000000000000100000000000001000000000000000000000000000000001000000000000000100000010000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000001110001000010000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000001000100000000100010100000000000000000000000000000000000000000000000000000010000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000</v>
       </c>
-      <c r="Q11" t="str">
+      <c r="R11" t="str">
         <f>_xll.NCDK_KlekotaRothFingerprinter($B11)</f>
         <v>110000010000010011000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001111000000100000000000000000010000000000000011010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000010100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000010000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000011000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000001000000000000000000100000100000000000001000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000100000000000000001011000000010000000000000000000000010000000000000100000100000010010000100100000010000001000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="R11" t="str">
+      <c r="S11" t="str">
         <f>_xll.NCDK_LingoFingerprinter($B11)</f>
         <v>0010000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000110000000100100000110000000000000000000000000000000000000000000000000000000000000000001000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000010001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000</v>
       </c>
-      <c r="S11" t="str">
+      <c r="T11" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($B11)</f>
         <v>0000000000000000000000000100000000000000000000000100000000000000010000000101000000000000010000010010000110010001001101000000001110010000001010101010110100101001001110</v>
       </c>
-      <c r="T11" t="str">
+      <c r="U11" t="str">
         <f>_xll.NCDK_ShortestPathFingerprinter($B11)</f>
         <v>0000000000000000000001100001000000000000000000000001011100000100101000100000000000001000000000000000000010000000010100000000000000010100000000000100000000000000000000000000000001000000000000000001100000000000000001000000000001000000001001000001000010000000000000000010000010000000001000000100101000100000100000000000100000000000000000000000000000000000000000000000000000000000000000000010000001000000100000000000000100001011000100000001000000100000010000000000000000000000000000000001001000000100000000010000010000100000100000000000000000001010000000000000000000010100000000000000100000000010000010001000000110000000000100000000010010000000000000000000010000000100000100000000100000000000000000000000000001000010000100000000000000000000000000000000000000000000001000000100000000000000000000000000010000000000000010000000000000000010100000000000000000000000001100000000000000100100000000000000010100000000000010000000010000000000001000000000000010000001100000000000000100000000000000000000000000000100000000100000000000000000</v>
       </c>
-      <c r="U11" t="str">
+      <c r="V11" t="str">
         <f>_xll.NCDK_SubstructureFingerprinter($B11)</f>
         <v>1111100000010100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000001000000100001</v>
       </c>
-      <c r="V11" t="str">
+      <c r="W11" t="str">
         <f>_xll.NCDK_PubchemFingerprinter($B11)</f>
         <v>00000000011110000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000110000000000000000000000000000000001100100110000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001101000000000000000000000100000000000000000000000111100010100101000001000000000000010000000100000000000000000000000000000001000000000100000000000001000100000010000100000000000000000000000000000000000000000001000000000000000000000000000000000100000000000000000000000000000001000000000000001000000000010000000000000000100000000000000000100000000000000000001001100000000000000000010000000000000000011100000001100000011110000000011111000000000000000000000000000000000000000000000000000000000000000110000000000000000000100000000000000000000100000000000000000000100000000000000000000100000000000000000000</v>
       </c>
-      <c r="W11">
+      <c r="X11">
         <f>_xll.NCDK_AcidicGroupCount(B11)</f>
         <v>0</v>
       </c>
-      <c r="X11">
+      <c r="Y11">
         <f>_xll.NCDK_ALogP(B11)</f>
         <v>1.5548000000000011</v>
       </c>
-      <c r="Y11">
+      <c r="Z11">
         <f>_xll.NCDK_AMolarRefractivity(B11)</f>
         <v>115.17460000000001</v>
       </c>
-      <c r="Z11">
+      <c r="AA11">
         <f>_xll.NCDK_APol(B11)</f>
         <v>78.994478000000029</v>
       </c>
-      <c r="AA11">
+      <c r="AB11">
         <f>_xll.NCDK_AromaticAtomsCount(B11)</f>
         <v>0</v>
       </c>
-      <c r="AB11">
+      <c r="AC11">
         <f>_xll.NCDK_AromaticBondsCount(B11)</f>
         <v>0</v>
       </c>
-      <c r="AC11">
+      <c r="AD11">
         <f>_xll.NCDK_AtomCount(B11)</f>
         <v>74</v>
       </c>
-      <c r="AD11" t="str">
+      <c r="AE11" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B11)</f>
         <v>0.0827991713427503, -0.0229631507285856, -0.0270969061556759, 0.00647128770548948, 0.00909713625645344</v>
       </c>
-      <c r="AE11" t="str">
+      <c r="AF11" t="str">
         <f>_xll.NCDK_AutocorrelationMass(B11)</f>
         <v>28.7744690355409, 31.3320919771326, 48.6641839542651, 54.6641839542651, 49.6641839542651</v>
       </c>
-      <c r="AF11" t="str">
+      <c r="AG11" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B11)</f>
         <v>2589.35165284459, 3179.06049775734, 4922.9791073968, 5328.87269506555, 4616.91714731414</v>
       </c>
-      <c r="AG11">
+      <c r="AH11">
         <f>_xll.NCDK_BasicGroupCount(B11)</f>
         <v>0</v>
       </c>
-      <c r="AH11" t="str">
+      <c r="AI11" t="str">
         <f>_xll.NCDK_BCUT(B11)</f>
         <v>11.89, 15.9949214370832, -0.392219474278523, 0.0694748577202458, 5.23874992098634, 12.6503467270457</v>
       </c>
-      <c r="AI11">
+      <c r="AJ11">
         <f>_xll.NCDK_BondCount(B11)</f>
         <v>0</v>
       </c>
-      <c r="AJ11">
+      <c r="AK11">
         <f>_xll.NCDK_BPol(B11)</f>
         <v>50.287521999999989</v>
       </c>
-      <c r="AK11" t="str">
+      <c r="AL11" t="str">
         <f>_xll.NCDK_CarbonTypes(B11)</f>
         <v>0, 0, 0, 1, 1, 5, 12, 6, 2</v>
       </c>
-      <c r="AL11" t="str">
+      <c r="AM11" t="str">
         <f>_xll.NCDK_ChiChain(B11)</f>
         <v>0, 0, 0.0833333333333333, 0.393634553260967, 0.976046921839545, 0, 0, 0.0833333333333333, 0.37164819290959, 0.863165765466815</v>
       </c>
-      <c r="AM11" t="str">
+      <c r="AN11" t="str">
         <f>_xll.NCDK_ChiCluster(B11)</f>
         <v>2.9521315814894, 0.235702260395516, 1.02234106177579, 0.203263132396285, 2.68481479020038, 0.219913202813724, 0.935219433730957, 0.179558378198271</v>
       </c>
-      <c r="AN11" t="str">
+      <c r="AO11" t="str">
         <f>_xll.NCDK_ChiPathCluster(B11)</f>
         <v>6.93012787723299, 11.9183161832455, 18.084244169983, 6.31056734345633, 10.8246614459309, 15.7948474414898</v>
       </c>
-      <c r="AO11" t="str">
+      <c r="AP11" t="str">
         <f>_xll.NCDK_ChiPath(B11)</f>
         <v>20.1040835277556, 13.2536913009629, 13.0668536638687, 11.1291235227258, 9.49703814548855, 7.69096408557496, 5.93907638185732, 4.4721666474432, 19.344190342069, 12.6298450216499, 12.1863667747532, 10.2790812759586, 8.66624457896859, 6.67875288189192, 5.16344144011131, 3.80610378452706</v>
       </c>
-      <c r="AP11" t="str">
+      <c r="AQ11" t="str">
         <f>_xll.NCDK_CPSA(B11)</f>
         <v>#N/A</v>
       </c>
-      <c r="AQ11">
+      <c r="AR11">
         <f>_xll.NCDK_EccentricConnectivityIndex(B11)</f>
         <v>669</v>
       </c>
-      <c r="AR11">
+      <c r="AS11">
         <f>_xll.NCDK_FMF(B11)</f>
         <v>0.6071428571428571</v>
       </c>
-      <c r="AS11">
+      <c r="AT11">
         <f>_xll.NCDK_FractionalPSA(B11)</f>
         <v>5.2361188524318612E-2</v>
       </c>
-      <c r="AT11">
+      <c r="AU11">
         <f>_xll.NCDK_FragmentComplexity(B11)</f>
         <v>5173.01</v>
       </c>
-      <c r="AU11" t="str">
+      <c r="AV11" t="str">
         <f>_xll.NCDK_GravitationalIndex(B11)</f>
         <v>#N/A</v>
       </c>
-      <c r="AV11">
+      <c r="AW11">
         <f>_xll.NCDK_HBondAcceptorCount(B11)</f>
         <v>1</v>
       </c>
-      <c r="AW11">
+      <c r="AX11">
         <f>_xll.NCDK_HBondDonorCount(B11)</f>
         <v>1</v>
       </c>
-      <c r="AX11">
+      <c r="AY11">
         <f>_xll.NCDK_HybridizationRatio(B11)</f>
         <v>0.92592592592592593</v>
       </c>
-      <c r="AY11" t="str">
+      <c r="AZ11" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B11)</f>
         <v>21.2403746097815, 7.921875, 3.65484429065744</v>
       </c>
-      <c r="AZ11" t="str">
+      <c r="BA11" t="str">
         <f>_xll.NCDK_KierHallSmarts(B11)</f>
         <v>0, 0, 0, 0, 0, 0, 5, 0, 11, 0, 1, 0, 7, 0, 0, 1, 0, 0, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BA11">
+      <c r="BB11">
         <f>_xll.NCDK_LargestChain(B11)</f>
         <v>16</v>
       </c>
-      <c r="BB11">
+      <c r="BC11">
         <f>_xll.NCDK_LargestPiSystem(B11)</f>
         <v>2</v>
       </c>
-      <c r="BC11" t="str">
+      <c r="BD11" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B11)</f>
         <v>#N/A</v>
       </c>
-      <c r="BD11">
+      <c r="BE11">
         <f>_xll.NCDK_LongestAliphaticChain(B11)</f>
         <v>7</v>
       </c>
-      <c r="BE11">
+      <c r="BF11">
         <f>_xll.NCDK_MannholdLogP(B11)</f>
         <v>4.3199999999999994</v>
       </c>
-      <c r="BF11" t="str">
+      <c r="BG11" t="str">
         <f>_xll.NCDK_MDE(B11)</f>
         <v>1.54697174276407, 11.0054221495714, 8.10399071027919, 2.24225976804296, 15.301585299106, 26.1301405209996, 7.46130267367364, 6.99912877305946, 5.73136198628621, 0.25, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BG11" t="str">
+      <c r="BH11" t="str">
         <f>_xll.NCDK_MomentOfInertia(B11)</f>
         <v>#N/A</v>
       </c>
-      <c r="BH11">
+      <c r="BI11">
         <f>_xll.NCDK_PetitjeanNumber(B11)</f>
         <v>0.46666666666666667</v>
       </c>
-      <c r="BI11" t="str">
+      <c r="BJ11" t="str">
         <f>_xll.NCDK_PetitjeanShapeIndex(B11)</f>
         <v>#N/A</v>
       </c>
-      <c r="BJ11">
+      <c r="BK11">
         <f>_xll.NCDK_RotatableBondsCount(B11)</f>
         <v>5</v>
       </c>
-      <c r="BK11">
+      <c r="BL11">
         <f>_xll.NCDK_RuleOfFive(B11)</f>
         <v>1</v>
       </c>
-      <c r="BL11" t="str">
+      <c r="BM11" t="str">
         <f>_xll.NCDK_SmallRing(B11)</f>
         <v>4, 0, 1, 0, 0, 0, 1, 3, 0, 0, 0</v>
       </c>
-      <c r="BM11">
+      <c r="BN11">
         <f>_xll.NCDK_TPSA(B11)</f>
         <v>20.23</v>
       </c>
-      <c r="BN11">
+      <c r="BO11">
         <f>_xll.NCDK_VABC(B11)</f>
         <v>432.27597679576252</v>
       </c>
-      <c r="BO11">
+      <c r="BP11">
         <f>_xll.NCDK_VAdjMa(B11)</f>
         <v>5.9541963103868758</v>
       </c>
-      <c r="BP11">
+      <c r="BQ11">
         <f>_xll.NCDK_Weight(B11)</f>
         <v>386.35486609200007</v>
       </c>
-      <c r="BQ11" t="str">
+      <c r="BR11" t="str">
         <f>_xll.NCDK_WeightedPath(B11)</f>
         <v>57.2167299866347, 2.04345464237981, 2.54245315921218, 2.54245315921218, 0</v>
       </c>
-      <c r="BR11" t="str">
+      <c r="BS11" t="str">
         <f>_xll.NCDK_WHIM(B11)</f>
         <v>#N/A</v>
       </c>
-      <c r="BS11" t="str">
+      <c r="BT11" t="str">
         <f>_xll.NCDK_WienerNumbers(B11)</f>
         <v>2022, 54</v>
       </c>
-      <c r="BT11">
+      <c r="BU11">
         <f>_xll.NCDK_XLogP(B11)</f>
         <v>10.518000000000004</v>
       </c>
-      <c r="BU11">
+      <c r="BV11">
         <f>_xll.NCDK_ZagrebIndex(B11)</f>
         <v>158</v>
       </c>

</xml_diff>

<commit_message>
Use Dictionary rather than MemoryCache.
</commit_message>
<xml_diff>
--- a/NCDK-Excel/ExcelNCDK-Test.xlsx
+++ b/NCDK-Excel/ExcelNCDK-Test.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D614538-46CF-46F1-8122-738C3170166F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6492234-0E7F-4899-8503-90C148CA60B7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="407" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="407" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptors" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="167">
   <si>
     <t>CC(=O)O</t>
     <phoneticPr fontId="1"/>
@@ -1810,6 +1810,10 @@
   </si>
   <si>
     <t>CCCCCC(=O)O</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ECFP2</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2546,7 +2550,7 @@
   <dimension ref="A1:BV11"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -2792,7 +2796,7 @@
       <c r="C2" t="str">
         <f>_xll.NCDK_MolText(B2)</f>
         <v xml:space="preserve">
-  CDK     0603191242
+  CDK     0702190142
  18 19  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 O   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -3036,7 +3040,7 @@
       </c>
       <c r="BB2">
         <f>_xll.NCDK_LargestChain(B2)</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="BC2">
         <f>_xll.NCDK_LargestPiSystem(B2)</f>
@@ -3929,7 +3933,7 @@
       </c>
       <c r="BB5">
         <f>_xll.NCDK_LargestChain(B5)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="BC5">
         <f>_xll.NCDK_LargestPiSystem(B5)</f>
@@ -5793,86 +5797,94 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D78F5C-B236-40D1-A056-FD195DD12728}">
-  <dimension ref="A1:Q21"/>
+  <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="5" max="16" width="4.83203125" customWidth="1"/>
+    <col min="7" max="18" width="4.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>87</v>
       </c>
       <c r="B1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D1" t="s">
         <v>88</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>91</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>92</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>94</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>95</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>96</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>97</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>98</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>99</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>100</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>101</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>102</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>103</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>104</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="str">
+        <f>_xll.NCDK(B$1,$A2)</f>
+        <v>0000000000000000000000000001000000000000000000000000000000000000100000000000000000000000100000000000000000000000000000000000000000000100001000000000000010000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000001000000100000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000100000000000000000001000000000000000000100000000000000000000000010000000000000000000000000000010000000100000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000100100000000001000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000010000000000000000000100000100000000000000000000000100000000000000000000000000</v>
+      </c>
+      <c r="C2" s="1" t="str">
+        <f>_xll.NCDK_ECFP2($A2)</f>
+        <v>0000000000000000000000000001000000000000000000000000000000000000100000000000000000000000100000000000000000000000000000000000000000000100001000000000000010000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000001000000100000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000100000000000000000001000000000000000000100000000000000000000000010000000000000000000000000000010000000100000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000100100000000001000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000010000000000000000000100000100000000000000000000000100000000000000000000000000</v>
+      </c>
+      <c r="D2" t="s">
         <v>90</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>90</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>93</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
       <c r="G2">
         <v>0</v>
       </c>
@@ -5889,113 +5901,137 @@
         <v>0</v>
       </c>
       <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
         <v>1</v>
       </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
       <c r="O2">
         <v>0</v>
       </c>
-      <c r="Q2" t="str">
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="S2" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($A2)</f>
         <v>0000000000000000000000000000000000000100000000000000110010000100100000010010101101101000111110111100000010001100000010011100001000111010101101100101011110111111111110</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="str">
+        <f>_xll.NCDK(B$1,$A3)</f>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000100000000000001000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="C3" s="1" t="str">
+        <f>_xll.NCDK_ECFP2($A3)</f>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000100000000000001000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="D3" t="s">
         <v>106</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>106</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>107</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
+      <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="J3">
         <v>1</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
       <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="N3">
         <v>1</v>
       </c>
-      <c r="O3">
+      <c r="Q3">
         <v>1</v>
       </c>
-      <c r="Q3" t="str">
+      <c r="S3" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($A3)</f>
         <v>0000000000000000000000000000000000000000000000000000110000000000000000010000000000000000100000000010000000000000100000000000101000100000001100111100010100001010011110</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="str">
+        <f>_xll.NCDK(B$1,$A4)</f>
+        <v>0000000100000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000100000000000000000000000000000000000000000000000000000100000000000000000000000000000000011000000000000000000000000001000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000100000000000010000000000000000000000000000000000000010000000000000000000000000000000001000000000000000000000000000000010000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000010000000000000000000100000000000000000000000000000000000000000001000000000000</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f>_xll.NCDK_ECFP2($A4)</f>
+        <v>0000000100000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000100000000000000000000000000000000000000000000000000000100000000000000000000000000000000011000000000000000000000000001000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000100000000000010000000000000000000000000000000000000010000000000000000000000000000000001000000000000000000000000000000010000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000010000000000000000000100000000000000000000000000000000000000000001000000000000</v>
+      </c>
+      <c r="D4" t="s">
         <v>109</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>109</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>110</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
       <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="I4">
         <v>1</v>
       </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
+      <c r="J4">
+        <v>0</v>
       </c>
       <c r="M4">
         <v>1</v>
       </c>
       <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="Q4" t="str">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="S4" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($A4)</f>
         <v>0000000000000000000000000001000000000000000000001000000010000000100000010010000000101000000010011100001010001000100000011110111000000100100110111101110110011111111111</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="str">
+        <f>_xll.NCDK(B$1,$A5)</f>
+        <v>0000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000001000000000000100000000000000000000000000100000110000000000010000000000000000000000000000000000000000000000000000010000000000001000000000000000000000000000000000010000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000100000000000000000001000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000100001000000000000000000000000000000000000000000000000100000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000100000000100000000000000000000000000000000000</v>
+      </c>
+      <c r="C5" s="1" t="str">
+        <f>_xll.NCDK_ECFP2($A5)</f>
+        <v>0000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000001000000000000100000000000000000000000000100000110000000000010000000000000000000000000000000000000000000000000000010000000000001000000000000000000000000000000000010000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000100000000000000000001000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000100001000000000000000000000000000000000000000000000000100000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000100000000100000000000000000000000000000000000</v>
+      </c>
+      <c r="D5" t="s">
         <v>112</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>112</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>113</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
       <c r="G5">
         <v>0</v>
       </c>
@@ -6026,78 +6062,94 @@
       <c r="P5">
         <v>0</v>
       </c>
-      <c r="Q5" t="str">
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($A5)</f>
         <v>0000000000000000000000000000000000000000000001000000010010000000100000110000000000110000110101111000010100000110100110011011001000100100101101110100011101111111110111</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="str">
+        <f>_xll.NCDK(B$1,$A6)</f>
+        <v>0000000000000010000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000100000000000000000010000001000000000000000000000000001000000000000000000000000000000000000000000000000010000000000000000000001000000000000000000000000000000000000000000000000000000010000000000000000000000000000000100000000000000000010000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000001000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000010000000000000000000001000000000000100000000000000000000000000000000000000000000000000000000001000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="C6" s="1" t="str">
+        <f>_xll.NCDK_ECFP2($A6)</f>
+        <v>0000000000000010000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000100000000000000000010000001000000000000000000000000001000000000000000000000000000000000000000000000000010000000000000000000001000000000000000000000000000000000000000000000000000000010000000000000000000000000000000100000000000000000010000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000001000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000010000000000000000000001000000000000100000000000000000000000000000000000000000000000000000000001000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="D6" t="s">
         <v>116</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>116</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>117</v>
       </c>
-      <c r="E6">
+      <c r="G6">
         <v>1</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
+      <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
       <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
         <v>1</v>
       </c>
-      <c r="L6">
+      <c r="N6">
         <v>1</v>
       </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
       <c r="O6">
         <v>0</v>
       </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6" t="str">
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($A6)</f>
         <v>0000000000000000000000001000000000000100000000000000100000000010100000100000101100010000100101101100010001001100100011111001011110101010100001111010011010111110111110</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="str">
+        <f>_xll.NCDK(B$1,$A7)</f>
+        <v>1000000000000010000000000000000000000000010000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000100000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000100000000000000000000000001000000000000000000000000000000000000100000000000000010000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000100000000000000000000000000000000000001000001000000000000</v>
+      </c>
+      <c r="C7" s="1" t="str">
+        <f>_xll.NCDK_ECFP2($A7)</f>
+        <v>1000000000000010000000000000000000000000010000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000100000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000100000000000000000000000001000000000000000000000000000000000000100000000000000010000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000100000000000000000000000000000000000001000001000000000000</v>
+      </c>
+      <c r="D7" t="s">
         <v>119</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>119</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>120</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
       <c r="G7">
         <v>0</v>
       </c>
@@ -6128,30 +6180,38 @@
       <c r="P7">
         <v>0</v>
       </c>
-      <c r="Q7" t="str">
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($A7)</f>
         <v>0000000000000000000000000000000000000000000000000000000010000100000000010010001000001100000000111101000010001010100001011100100110011010110001011011000110011110111110</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="str">
+        <f>_xll.NCDK(B$1,$A8)</f>
+        <v>1000000000000010000000000000000000000000000000000000000000000000000000001000000000000000100000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000100000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000100000000000001000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000100000100000000000000000000000000000000001000000000000100</v>
+      </c>
+      <c r="C8" s="1" t="str">
+        <f>_xll.NCDK_ECFP2($A8)</f>
+        <v>1000000000000010000000000000000000000000000000000000000000000000000000001000000000000000100000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000100000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000100000000000001000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000100000100000000000000000000000000000000001000000000000100</v>
+      </c>
+      <c r="D8" t="s">
         <v>122</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>122</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>123</v>
       </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
       <c r="G8">
         <v>0</v>
       </c>
@@ -6179,30 +6239,38 @@
       <c r="O8">
         <v>0</v>
       </c>
-      <c r="Q8" t="str">
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="S8" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($A8)</f>
         <v>0000000000000000001000000000000000000000000000000000010000000100000000010000000001000100001000000001001110000010100000001000101110100100111000111010011110001110111111</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="str">
+        <f>_xll.NCDK(B$1,$A9)</f>
+        <v>0000000000000000000100000000000000100000000000000000100000000000000000000000000000000000000000000000000000000010000000000000000000000100000000000100000010000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000001000000000000000000000000001000000000000000000000000000000001000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="C9" s="1" t="str">
+        <f>_xll.NCDK_ECFP2($A9)</f>
+        <v>0000000000000000000100000000000000100000000000000000100000000000000000000000000000000000000000000000000000000010000000000000000000000100000000000100000010000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000001000000000000000000000000001000000000000000000000000000000001000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="D9" t="s">
         <v>125</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>125</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>126</v>
       </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
       <c r="G9">
         <v>0</v>
       </c>
@@ -6233,30 +6301,38 @@
       <c r="P9">
         <v>0</v>
       </c>
-      <c r="Q9" t="str">
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($A9)</f>
         <v>0000000000000000000000000000001000000100011000000010001001011000001000001000110000010001000000000000011001100001000000100001000001110101000001000001001010110110111111</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="str">
+        <f>_xll.NCDK(B$1,$A10)</f>
+        <v>0000000000000010000100000100000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000100000000000000000010000000000000000000001000000000000000000000000000000000000000000000010000100000000010000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000100000000000000000000000000100000000000000000000000000000000000100000000000000000001000000000000000000000000000000100000000000000000000000001000000000000000000001000000000000000100000000000000010001000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000001000000000000000000000000000000</v>
+      </c>
+      <c r="C10" s="1" t="str">
+        <f>_xll.NCDK_ECFP2($A10)</f>
+        <v>0000000000000010000100000100000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000100000000000000000010000000000000000000001000000000000000000000000000000000000000000000010000100000000010000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000100000000000000000000000000100000000000000000000000000000000000100000000000000000001000000000000000000000000000000100000000000000000000000001000000000000000000001000000000000000100000000000000010001000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000001000000000000000000000000000000</v>
+      </c>
+      <c r="D10" t="s">
         <v>128</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>128</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
         <v>129</v>
       </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
       <c r="G10">
         <v>0</v>
       </c>
@@ -6287,72 +6363,88 @@
       <c r="P10">
         <v>0</v>
       </c>
-      <c r="Q10" t="str">
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($A10)</f>
         <v>0000000000000000000000000000000000000000000000000000000010000100010000000010000000001100000000100101001000001011000001011110010110010100110000001111000011101110111111</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="str">
+        <f>_xll.NCDK(B$1,$A11)</f>
+        <v>0000000000000010000100000101000000000000000000000000000000000000000000000000000000000000100001000000100000000000000000000000000000000100000000000000000010000000000000000000000000000000000010000000000000000010000001000000010000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000001000000000000010101100001100000000000100010100000000000000000000001000000010000000000000000000000000000010001010000000000000000000000000000000000000000000000000000010000000010000000000100100000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000001000100000000000000001000000000000000000000001000000000000000000000000000001000000000000000001000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000001000100000000000000000000000000000100000000000000000000000000</v>
+      </c>
+      <c r="C11" s="1" t="str">
+        <f>_xll.NCDK_ECFP2($A11)</f>
+        <v>0000000000000010000100000101000000000000000000000000000000000000000000000000000000000000100001000000100000000000000000000000000000000100000000000000000010000000000000000000000000000000000010000000000000000010000001000000010000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000001000000000000010101100001100000000000100010100000000000000000000001000000010000000000000000000000000000010001010000000000000000000000000000000000000000000000000000010000000010000000000100100000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000001000100000000000000001000000000000000000000001000000000000000000000000000001000000000000000001000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000001000100000000000000000000000000000100000000000000000000000000</v>
+      </c>
+      <c r="D11" t="s">
         <v>131</v>
       </c>
-      <c r="C11" t="s">
+      <c r="E11" t="s">
         <v>131</v>
       </c>
-      <c r="D11" t="s">
+      <c r="F11" t="s">
         <v>132</v>
       </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="I11">
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
         <v>0</v>
       </c>
       <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11">
         <v>0</v>
       </c>
       <c r="M11">
         <v>1</v>
       </c>
       <c r="N11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O11">
         <v>1</v>
       </c>
-      <c r="Q11" t="str">
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="S11" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($A11)</f>
         <v>0000000000000000000000000000000000000000000000000000100010000000100000000000000100100000100110111100000010010111001110011010000110111011101111011110111101111111111110</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="str">
+        <f>_xll.NCDK(B$1,$A12)</f>
+        <v>0000000000000000000000000000000000000000000000000010000000100000000000000000000000000000001000000000000000000000000000000000000000000100010000000100000010000000000000000000000000000000000000000000000000000010000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000100000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000100000000000000000000000000000000011000000000000000000000000010000000000000000000000000000000000000000000000000100000000000000000000100000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000001000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000010000000100000000000000000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <f>_xll.NCDK_ECFP2($A12)</f>
+        <v>0000000000000000000000000000000000000000000000000010000000100000000000000000000000000000001000000000000000000000000000000000000000000100010000000100000010000000000000000000000000000000000000000000000000000010000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000100000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000100000000000000000000000000000000011000000000000000000000000010000000000000000000000000000000000000000000000000100000000000000000000100000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000001000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000010000000100000000000000000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="D12" t="s">
         <v>134</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
         <v>134</v>
       </c>
-      <c r="D12" t="s">
+      <c r="F12" t="s">
         <v>135</v>
       </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
       <c r="G12">
         <v>0</v>
       </c>
@@ -6383,30 +6475,38 @@
       <c r="P12">
         <v>0</v>
       </c>
-      <c r="Q12" t="str">
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($A12)</f>
         <v>0000000000000000000000000000000000100011000100011000011001011000001000011000000001000001000010000000010101001001100000000001011001110001001100110101010110101011011111</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="str">
+        <f>_xll.NCDK(B$1,$A13)</f>
+        <v>0000000000000010000100000000000000000000000000000000000000000000000000000000000000000000100001000000000000000010000000000000000000000100000000000000000010000000000000000000001000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000010000000100000000000000000000010000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000001000000000000000000000000000000000100001000000100000010100000000010000000000000011100000000000000000000000000000010000000000000000000000000000000000000000000100000000000000000000000000000000000000000000001000000000000000000001000000000000000000000000000000001000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000100000000000000000000000001000000000000000000000000000000</v>
+      </c>
+      <c r="C13" s="1" t="str">
+        <f>_xll.NCDK_ECFP2($A13)</f>
+        <v>0000000000000010000100000000000000000000000000000000000000000000000000000000000000000000100001000000000000000010000000000000000000000100000000000000000010000000000000000000001000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000010000000100000000000000000000010000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000001000000000000000000000000000000000100001000000100000010100000000010000000000000011100000000000000000000000000000010000000000000000000000000000000000000000000100000000000000000000000000000000000000000000001000000000000000000001000000000000000000000000000000001000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000100000000000000000000000001000000000000000000000000000000</v>
+      </c>
+      <c r="D13" t="s">
         <v>137</v>
       </c>
-      <c r="C13" t="s">
+      <c r="E13" t="s">
         <v>137</v>
       </c>
-      <c r="D13" t="s">
+      <c r="F13" t="s">
         <v>138</v>
       </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
       <c r="G13">
         <v>0</v>
       </c>
@@ -6428,36 +6528,44 @@
       <c r="M13">
         <v>0</v>
       </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
       <c r="O13">
         <v>0</v>
       </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-      <c r="Q13" t="str">
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($A13)</f>
         <v>0000000000000000000000100000000000000000000000000000000000000000000000000010001100101110000110010111001001110110000011011110010110110101111101011111010011111111111111</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="str">
+        <f>_xll.NCDK(B$1,$A14)</f>
+        <v>0000000000000010000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000100000000000000000000000000000000000000001000000000000000000000000000000000000000000001000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000010000000000000000000100000000000000000000000000000010000000000000000000000000000000000000000000000000000000100000000000100000000000000000000000000000000000000010000000000100000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000100000000000100000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="C14" s="1" t="str">
+        <f>_xll.NCDK_ECFP2($A14)</f>
+        <v>0000000000000010000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000100000000000000000000000000000000000000001000000000000000000000000000000000000000000001000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000010000000000000000000100000000000000000000000000000010000000000000000000000000000000000000000000000000000000100000000000100000000000000000000000000000000000000010000000000100000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000100000000000100000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="D14" t="s">
         <v>140</v>
       </c>
-      <c r="C14" t="s">
+      <c r="E14" t="s">
         <v>140</v>
       </c>
-      <c r="D14" t="s">
+      <c r="F14" t="s">
         <v>141</v>
       </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
       <c r="G14">
         <v>0</v>
       </c>
@@ -6488,30 +6596,38 @@
       <c r="P14">
         <v>0</v>
       </c>
-      <c r="Q14" t="str">
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($A14)</f>
         <v>0000000000000000000000000000000000000000000000000000000010000100100000100010000100101100000011111001011000010010001101011101000000000100100001000011110110010101110111</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="str">
+        <f>_xll.NCDK(B$1,$A15)</f>
+        <v>0000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="C15" s="1" t="str">
+        <f>_xll.NCDK_ECFP2($A15)</f>
+        <v>0000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="D15" t="s">
         <v>143</v>
       </c>
-      <c r="C15" t="s">
+      <c r="E15" t="s">
         <v>143</v>
       </c>
-      <c r="D15" t="s">
+      <c r="F15" t="s">
         <v>144</v>
       </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
       <c r="G15">
         <v>0</v>
       </c>
@@ -6542,30 +6658,38 @@
       <c r="P15">
         <v>0</v>
       </c>
-      <c r="Q15" t="str">
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($A15)</f>
         <v>0000000010000000000000000000000000000000001100001000100000000000000010000000100100000000000001001000011001000001000010000001010001100100000001000001001000010010100101</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="str">
+        <f>_xll.NCDK(B$1,$A16)</f>
+        <v>1000000000000010000000000100000000000000010000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000100000000000000000010000001000000000000001000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000100000000000000000001000000000000000000000000000000000001000000000001000000000000000000100000000000000000000000000000000000000000000100000100000000000100000000010000010000000001000000000000000000000000000000000000000000001000000000000000000000000000000100000000000001000000000000000000000100000000001000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000001000001000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100001000000000000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="C16" s="1" t="str">
+        <f>_xll.NCDK_ECFP2($A16)</f>
+        <v>1000000000000010000000000100000000000000010000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000100000000000000000010000001000000000000001000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000100000000000000000001000000000000000000000000000000000001000000000001000000000000000000100000000000000000000000000000000000000000000100000100000000000100000000010000010000000001000000000000000000000000000000000000000000001000000000000000000000000000000100000000000001000000000000000000000100000000001000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000001000001000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100001000000000000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="D16" t="s">
         <v>146</v>
       </c>
-      <c r="C16" t="s">
+      <c r="E16" t="s">
         <v>146</v>
       </c>
-      <c r="D16" t="s">
+      <c r="F16" t="s">
         <v>147</v>
       </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
       <c r="G16">
         <v>0</v>
       </c>
@@ -6596,30 +6720,38 @@
       <c r="P16">
         <v>0</v>
       </c>
-      <c r="Q16" t="str">
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($A16)</f>
         <v>0000000000000000000001000000000000000000000000000000000010000000110000010010000000101100111000110101101110000011100001011100101110110100111101111111001110111110111111</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="str">
+        <f>_xll.NCDK(B$1,$A17)</f>
+        <v>0000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000001000000000000100000000000000000000100000000000010000000000010000000000000000000000000000000000000000000000000000010000000000000000100000010000000000100000000000000001000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000011000000000000000000000000001000000010000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000001000000000001000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000010100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="C17" s="1" t="str">
+        <f>_xll.NCDK_ECFP2($A17)</f>
+        <v>0000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000001000000000000100000000000000000000100000000000010000000000010000000000000000000000000000000000000000000000000000010000000000000000100000010000000000100000000000000001000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000011000000000000000000000000001000000010000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000001000000000001000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000010100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="D17" t="s">
         <v>149</v>
       </c>
-      <c r="C17" t="s">
+      <c r="E17" t="s">
         <v>149</v>
       </c>
-      <c r="D17" t="s">
+      <c r="F17" t="s">
         <v>150</v>
       </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
       <c r="G17">
         <v>0</v>
       </c>
@@ -6650,66 +6782,82 @@
       <c r="P17">
         <v>0</v>
       </c>
-      <c r="Q17" t="str">
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($A17)</f>
         <v>0000000000000000000000000000000110000000000000000000010000000010001001100000001101010001011101100001010100000110000010100011000101110001011101000110001011111110100100</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="str">
+        <f>_xll.NCDK(B$1,$A18)</f>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000010100000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000010000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000100000</v>
+      </c>
+      <c r="C18" s="1" t="str">
+        <f>_xll.NCDK_ECFP2($A18)</f>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000010100000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000010000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000100000</v>
+      </c>
+      <c r="D18" t="s">
         <v>152</v>
       </c>
-      <c r="C18" t="s">
+      <c r="E18" t="s">
         <v>152</v>
       </c>
-      <c r="D18" t="s">
+      <c r="F18" t="s">
         <v>153</v>
       </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="I18">
         <v>0</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>0</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="Q18" t="str">
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="S18" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($A18)</f>
         <v>0000000000000000000000000000000000000000000000000000010000000000000000000000001001000000000000000001001100000010000000000000100000100100010001001010001010110100111011</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="str">
+        <f>_xll.NCDK(B$1,$A19)</f>
+        <v>0000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000100000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000100100000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000100000000000000000000000001000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000001000000000000010000000000000000000100000000000000000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="C19" s="1" t="str">
+        <f>_xll.NCDK_ECFP2($A19)</f>
+        <v>0000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000100000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000100100000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000100000000000000000000000001000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000001000000000000010000000000000000000100000000000000000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="D19" t="s">
         <v>155</v>
       </c>
-      <c r="C19" t="s">
+      <c r="E19" t="s">
         <v>155</v>
       </c>
-      <c r="D19" t="s">
+      <c r="F19" t="s">
         <v>156</v>
       </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
       <c r="G19">
         <v>0</v>
       </c>
@@ -6723,53 +6871,61 @@
         <v>0</v>
       </c>
       <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
         <v>1</v>
       </c>
-      <c r="L19">
+      <c r="N19">
         <v>1</v>
       </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
       <c r="O19">
         <v>0</v>
       </c>
-      <c r="Q19" t="str">
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="S19" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($A19)</f>
         <v>0000000000000000000000000000000110010100000001100000000000000100101000000010111110100001000011010000000001000000000000111101100000001110100001011001010000010101111011</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="str">
+        <f>_xll.NCDK(B$1,$A20)</f>
+        <v>1000000000000010000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000001000000010000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000001000000110000000100000100000000000000000001000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000001000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000100000000000000000000000000000000000001000000000000000100</v>
+      </c>
+      <c r="C20" s="1" t="str">
+        <f>_xll.NCDK_ECFP2($A20)</f>
+        <v>1000000000000010000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000001000000010000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000001000000110000000100000100000000000000000001000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000001000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000100000000000000000000000000000000000001000000000000000100</v>
+      </c>
+      <c r="D20" t="s">
         <v>158</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E20" t="s">
         <v>158</v>
       </c>
-      <c r="D20" t="s">
+      <c r="F20" t="s">
         <v>159</v>
       </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
         <v>1</v>
       </c>
-      <c r="H20">
+      <c r="J20">
         <v>1</v>
       </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
       <c r="K20">
         <v>0</v>
       </c>
@@ -6779,33 +6935,41 @@
       <c r="M20">
         <v>0</v>
       </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
       <c r="O20">
         <v>0</v>
       </c>
-      <c r="Q20" t="str">
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="S20" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($A20)</f>
         <v>0000000000000000000000000000000000001000001000000000000000000000100000000010101000101100001010010101001011010110001110011100100000101110100001011011001011010101111111</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="str">
+        <f>_xll.NCDK(B$1,$A21)</f>
+        <v>0000000000000000000000001000000000000000000000000000000001000000001000000000000000000000000000000000000000000000000000000000000001000100000000000100000010000000000000000001000000000000000000000000000000000000000000000000000000000000000100000000100000000000000000000100000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000100000000000000000000000001000000000000000000000000000000000010000000000000000010000010000010000000000100000000000000000000000000000001000000010000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000001010000000000000000000110000000000000000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="C21" s="1" t="str">
+        <f>_xll.NCDK_ECFP2($A21)</f>
+        <v>0000000000000000000000001000000000000000000000000000000001000000001000000000000000000000000000000000000000000000000000000000000001000100000000000100000010000000000000000001000000000000000000000000000000000000000000000000000000000000000100000000100000000000000000000100000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000100000000000000000000000001000000000000000000000000000000000010000000000000000010000010000010000000000100000000000000000000000000000001000000010000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000001010000000000000000000110000000000000000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="D21" t="s">
         <v>161</v>
       </c>
-      <c r="C21" t="s">
+      <c r="E21" t="s">
         <v>161</v>
       </c>
-      <c r="D21" t="s">
+      <c r="F21" t="s">
         <v>162</v>
       </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
       <c r="G21">
         <v>0</v>
       </c>
@@ -6836,7 +7000,13 @@
       <c r="P21">
         <v>0</v>
       </c>
-      <c r="Q21" t="str">
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($A21)</f>
         <v>0000000000000000000000000000000001001111000000010010001001111101101010001010101110101001100110111111010011010101100010011101101001000001101101111101110011110111111110</v>
       </c>
@@ -6851,8 +7021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1647DD59-D041-4640-9111-9E35EC2330E5}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
Add ExactMass and JPlogP.
Update NCDK 1.5.4.
</commit_message>
<xml_diff>
--- a/NCDK-Excel/ExcelNCDK-Test.xlsx
+++ b/NCDK-Excel/ExcelNCDK-Test.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6492234-0E7F-4899-8503-90C148CA60B7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BEDA7A9-1669-4197-A75D-E74459BB78A1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="407" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="407" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptors" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="173">
   <si>
     <t>CC(=O)O</t>
     <phoneticPr fontId="1"/>
@@ -155,9 +155,6 @@
   </si>
   <si>
     <t>VAdjMa</t>
-  </si>
-  <si>
-    <t>Weight</t>
   </si>
   <si>
     <t>WeightedPath</t>
@@ -1816,11 +1813,43 @@
     <t>ECFP2</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>MolecularWeight</t>
+  </si>
+  <si>
+    <t>ExactMass</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Molecular Weight</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Exact Mass</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>JPlogP</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MACCSFingerprinter</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XLogP</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="177" formatCode="0.0000_ "/>
+    <numFmt numFmtId="179" formatCode="0.0_ "/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1857,11 +1886,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1890,21 +1922,21 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1571844</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1019317</xdr:rowOff>
+      <xdr:colOff>1870283</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="75" name="NCDK-Picture 1">
+        <xdr:cNvPr id="139" name="NCDK-Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7096EE-34AB-49CC-A9FC-49D2D01851BF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{231E937A-5F92-41FF-BEB6-4D0B1F73C48E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1922,7 +1954,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="857250" y="228600"/>
-          <a:ext cx="1571844" cy="1019317"/>
+          <a:ext cx="1870283" cy="1212850"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1940,21 +1972,21 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>276264</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>190527</xdr:rowOff>
+      <xdr:colOff>543242</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="77" name="NCDK-Picture 2">
+        <xdr:cNvPr id="141" name="NCDK-Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8027696-844A-44C7-8736-8836EA959C48}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC65AF16-C184-49DA-A021-2BCAC3980BB7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1972,7 +2004,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="857250" y="1441450"/>
-          <a:ext cx="276264" cy="190527"/>
+          <a:ext cx="543242" cy="374650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1990,21 +2022,21 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1495634</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>533474</xdr:rowOff>
+      <xdr:colOff>2136324</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="79" name="NCDK-Picture 3">
+        <xdr:cNvPr id="143" name="NCDK-Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BACE9196-6F9D-4CDF-92F5-A341065F7F70}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC00FF74-C38B-42C7-8291-C82AA6BF1B1C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2022,7 +2054,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="857250" y="1816100"/>
-          <a:ext cx="1495634" cy="533474"/>
+          <a:ext cx="2136324" cy="762000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2040,21 +2072,21 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>514422</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>581106</xdr:rowOff>
+      <xdr:colOff>652073</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="81" name="NCDK-Picture 4">
+        <xdr:cNvPr id="145" name="NCDK-Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04298DA9-5207-4578-8F40-9CEA740943C3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A98053E5-E1EF-4612-9599-F3E7B9B48A29}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2072,7 +2104,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="857250" y="2578100"/>
-          <a:ext cx="514422" cy="581106"/>
+          <a:ext cx="652073" cy="736600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2090,21 +2122,21 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>514422</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>828791</xdr:rowOff>
+      <xdr:colOff>603031</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="83" name="NCDK-Picture 5">
+        <xdr:cNvPr id="147" name="NCDK-Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B956E7D0-23C2-45AB-A384-8B949E76144F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3950DC8F-1781-48BA-AF22-3EA0BE4292C2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2122,7 +2154,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="857250" y="3314700"/>
-          <a:ext cx="514422" cy="828791"/>
+          <a:ext cx="603031" cy="971550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2140,21 +2172,21 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>581106</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>657317</xdr:rowOff>
+      <xdr:colOff>785927</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="85" name="NCDK-Picture 6">
+        <xdr:cNvPr id="149" name="NCDK-Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B7BAFBE-5F5A-4D36-8443-86C1DC61A475}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7333B961-CFC0-4E84-A89A-E5AE69943850}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2172,7 +2204,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="857250" y="4286250"/>
-          <a:ext cx="581106" cy="657317"/>
+          <a:ext cx="785927" cy="889000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2186,25 +2218,25 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>127457</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>2838846</xdr:rowOff>
+      <xdr:rowOff>2728434</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="87" name="NCDK-Picture 7">
+        <xdr:cNvPr id="151" name="NCDK-Picture 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C98CBAD5-CBA1-46E7-80E2-7FF5347693DF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{087E184A-68D8-44A8-AAD3-F49AC1CA9407}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2221,8 +2253,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="857250" y="5175250"/>
-          <a:ext cx="3277057" cy="2838846"/>
+          <a:off x="857250" y="5175251"/>
+          <a:ext cx="3149600" cy="2728433"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2234,27 +2266,27 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2695951</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>1933845</xdr:rowOff>
+      <xdr:colOff>2974428</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="89" name="NCDK-Picture 8">
+        <xdr:cNvPr id="153" name="NCDK-Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB2BF226-025E-4046-814D-A60540D4F75F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42C6C754-28F1-4248-9935-72CC127F6E1B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2271,8 +2303,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="857250" y="8172450"/>
-          <a:ext cx="2695951" cy="1933845"/>
+          <a:off x="857251" y="8172450"/>
+          <a:ext cx="2974427" cy="2133600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2547,11 +2579,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B185B08-1BAB-4052-951E-1A2BC1F97D8F}">
-  <dimension ref="A1:BV11"/>
+  <dimension ref="A1:BZ11"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -2559,244 +2589,261 @@
     <col min="4" max="4" width="11.08203125" customWidth="1"/>
     <col min="5" max="5" width="21.1640625" customWidth="1"/>
     <col min="6" max="23" width="6.5" customWidth="1"/>
-    <col min="25" max="26" width="8.6640625" customWidth="1"/>
+    <col min="24" max="25" width="8.1640625" style="2" customWidth="1"/>
+    <col min="27" max="27" width="8.6640625" style="4" customWidth="1"/>
+    <col min="28" max="30" width="8.6640625" style="4"/>
+    <col min="31" max="31" width="8.6640625" customWidth="1"/>
+    <col min="73" max="73" width="8.6640625" style="2"/>
+    <col min="74" max="74" width="10.08203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:74" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:78" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" t="s">
+        <v>71</v>
+      </c>
+      <c r="L1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M1" t="s">
+        <v>73</v>
+      </c>
+      <c r="N1" t="s">
+        <v>74</v>
+      </c>
+      <c r="O1" t="s">
+        <v>75</v>
+      </c>
+      <c r="P1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>77</v>
+      </c>
+      <c r="R1" t="s">
+        <v>78</v>
+      </c>
+      <c r="S1" t="s">
+        <v>79</v>
+      </c>
+      <c r="T1" t="s">
+        <v>80</v>
+      </c>
+      <c r="U1" t="s">
+        <v>81</v>
+      </c>
+      <c r="V1" t="s">
+        <v>82</v>
+      </c>
+      <c r="W1" t="s">
+        <v>65</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E1" t="s">
-        <v>164</v>
-      </c>
-      <c r="F1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I1" t="s">
-        <v>70</v>
-      </c>
-      <c r="J1" t="s">
-        <v>71</v>
-      </c>
-      <c r="K1" t="s">
-        <v>72</v>
-      </c>
-      <c r="L1" t="s">
-        <v>73</v>
-      </c>
-      <c r="M1" t="s">
-        <v>74</v>
-      </c>
-      <c r="N1" t="s">
-        <v>75</v>
-      </c>
-      <c r="O1" t="s">
-        <v>76</v>
-      </c>
-      <c r="P1" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>78</v>
-      </c>
-      <c r="R1" t="s">
-        <v>79</v>
-      </c>
-      <c r="S1" t="s">
-        <v>80</v>
-      </c>
-      <c r="T1" t="s">
-        <v>81</v>
-      </c>
-      <c r="U1" t="s">
-        <v>82</v>
-      </c>
-      <c r="V1" t="s">
-        <v>83</v>
-      </c>
-      <c r="W1" t="s">
-        <v>66</v>
-      </c>
-      <c r="X1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y1" t="s">
+      <c r="AB1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="AE1" t="s">
         <v>50</v>
       </c>
-      <c r="Z1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA1" t="s">
+      <c r="AF1" t="s">
         <v>2</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AG1" t="s">
         <v>3</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AH1" t="s">
         <v>4</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AI1" t="s">
         <v>5</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AJ1" t="s">
         <v>6</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AK1" t="s">
         <v>7</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AL1" t="s">
         <v>8</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AM1" t="s">
         <v>9</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AN1" t="s">
         <v>10</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AO1" t="s">
         <v>11</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AP1" t="s">
         <v>12</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AQ1" t="s">
         <v>13</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AR1" t="s">
         <v>14</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AS1" t="s">
         <v>15</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AT1" t="s">
         <v>16</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AU1" t="s">
         <v>17</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AV1" t="s">
         <v>18</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AW1" t="s">
         <v>19</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AX1" t="s">
         <v>20</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AY1" t="s">
         <v>21</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AZ1" t="s">
         <v>22</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="BA1" t="s">
         <v>23</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="BB1" t="s">
         <v>24</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BC1" t="s">
         <v>25</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BD1" t="s">
         <v>26</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BE1" t="s">
         <v>27</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BF1" t="s">
         <v>28</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BG1" t="s">
         <v>29</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BH1" t="s">
         <v>30</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BI1" t="s">
         <v>31</v>
       </c>
-      <c r="BE1" t="s">
-        <v>61</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>32</v>
-      </c>
-      <c r="BG1" t="s">
+      <c r="BJ1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BK1" t="s">
         <v>33</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BL1" t="s">
         <v>34</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BM1" t="s">
         <v>35</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BN1" t="s">
         <v>36</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BO1" t="s">
         <v>37</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BP1" t="s">
         <v>38</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BQ1" t="s">
         <v>39</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BR1" t="s">
         <v>40</v>
       </c>
-      <c r="BO1" t="s">
-        <v>65</v>
-      </c>
-      <c r="BP1" t="s">
+      <c r="BS1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BT1" t="s">
         <v>41</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BU1" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="BV1" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="BW1" t="s">
         <v>42</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BX1" t="s">
         <v>43</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BY1" t="s">
         <v>44</v>
       </c>
-      <c r="BT1" t="s">
-        <v>45</v>
-      </c>
-      <c r="BU1" t="s">
+      <c r="BZ1" t="s">
         <v>46</v>
       </c>
-      <c r="BV1" t="s">
-        <v>47</v>
-      </c>
     </row>
-    <row r="2" spans="1:74" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:78" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" t="str">
         <f>_xll.NCDK_MolText(B2)</f>
         <v xml:space="preserve">
-  CDK     0702190142
+       CDK0714190307
  18 19  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 O   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -2918,222 +2965,238 @@
         <f>_xll.NCDK_PubchemFingerprinter($B2)</f>
         <v>00000000011100110011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001011000000000000000000000000000000010001000000000000000000000000000000000000000000000000000000000000000001111000000000000100000000000000000000000000000000111000000000100000011000000000000000000000110000000000000010110000000000000000000000100010000000001000100001010100100001000000000000000000000000000000000000001000000000000000000000000000000000100000000001000000000000000000001000100000000000000000011010000010001100000100000000000001000000000000000000000010001000010100100010000010000000000000000011000110001000100011000000100011110000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="X2">
+      <c r="X2" s="2">
+        <f>_xll.NCDK_MolecularWeight(B2)</f>
+        <v>250.29412142388836</v>
+      </c>
+      <c r="Y2" s="2">
+        <f>_xll.NCDK_ExactMass(B2)</f>
+        <v>250.13174243599997</v>
+      </c>
+      <c r="Z2">
         <f>_xll.NCDK_AcidicGroupCount(B2)</f>
         <v>0</v>
       </c>
-      <c r="Y2">
+      <c r="AA2" s="4">
         <f>_xll.NCDK_ALogP(B2)</f>
-        <v>-1.2114000000000014</v>
-      </c>
-      <c r="Z2">
+        <v>2.1996999999999991</v>
+      </c>
+      <c r="AB2" s="4">
+        <f>_xll.NCDK_XLogP(B2)</f>
+        <v>2.1759999999999997</v>
+      </c>
+      <c r="AC2" s="4">
+        <f>_xll.NCDK_MannholdLogP(B2)</f>
+        <v>2.34</v>
+      </c>
+      <c r="AD2" s="4">
+        <f>_xll.NCDK_JPlogP(B2)</f>
+        <v>1.7050260777332682</v>
+      </c>
+      <c r="AE2">
         <f>_xll.NCDK_AMolarRefractivity(B2)</f>
-        <v>59.947099999999999</v>
-      </c>
-      <c r="AA2">
+        <v>66.252700000000004</v>
+      </c>
+      <c r="AF2">
         <f>_xll.NCDK_APol(B2)</f>
         <v>39.488274000000011</v>
       </c>
-      <c r="AB2">
+      <c r="AG2">
         <f>_xll.NCDK_AromaticAtomsCount(B2)</f>
         <v>0</v>
       </c>
-      <c r="AC2">
+      <c r="AH2">
         <f>_xll.NCDK_AromaticBondsCount(B2)</f>
         <v>0</v>
       </c>
-      <c r="AD2">
+      <c r="AI2">
         <f>_xll.NCDK_AtomCount(B2)</f>
         <v>36</v>
       </c>
-      <c r="AE2" t="str">
+      <c r="AJ2" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B2)</f>
         <v>0.482364049323966, -0.239230483102807, 0.193743260003086, -0.422975414094056, 0.245070516996786</v>
       </c>
-      <c r="AF2" t="str">
+      <c r="AK2" t="str">
         <f>_xll.NCDK_AutocorrelationMass(B2)</f>
         <v>21.0433677091758, 20.6610036641195, 30.570374510169, 39.3180113704083, 36.7520657397667</v>
       </c>
-      <c r="AG2" t="str">
+      <c r="AL2" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B2)</f>
         <v>1236.72445709937, 1455.26096710327, 2067.09825744824, 2452.45202784668, 1776.45546782422</v>
       </c>
-      <c r="AH2">
+      <c r="AM2">
         <f>_xll.NCDK_BasicGroupCount(B2)</f>
         <v>0</v>
       </c>
-      <c r="AI2" t="str">
+      <c r="AN2" t="str">
         <f>_xll.NCDK_BCUT(B2)</f>
         <v>11.89, 15.9969274797474, -0.279527566151374, 0.285306450703295, 4.45516607690972, 12.225254833975</v>
       </c>
-      <c r="AJ2">
+      <c r="AO2">
         <f>_xll.NCDK_BondCount(B2)</f>
         <v>0</v>
       </c>
-      <c r="AK2">
+      <c r="AP2">
         <f>_xll.NCDK_BPol(B2)</f>
         <v>23.871725999999995</v>
       </c>
-      <c r="AL2" t="str">
+      <c r="AQ2" t="str">
         <f>_xll.NCDK_CarbonTypes(B2)</f>
         <v>0, 0, 2, 1, 1, 1, 6, 0, 1</v>
       </c>
-      <c r="AM2" t="str">
+      <c r="AR2" t="str">
         <f>_xll.NCDK_ChiChain(B2)</f>
         <v>0, 0, 0, 0.0481125224324688, 0.206136035947173, 0, 0, 0, 0.015625, 0.0379976820715334</v>
       </c>
-      <c r="AN2" t="str">
+      <c r="AS2" t="str">
         <f>_xll.NCDK_ChiCluster(B2)</f>
         <v>1.29103942781429, 0.0680413817439772, 0.635379749451514, 0.130245735736926, 0.58282022448487, 0.0441941738241592, 0.195368603605389, 0.0360843918243516</v>
       </c>
-      <c r="AO2" t="str">
+      <c r="AT2" t="str">
         <f>_xll.NCDK_ChiPathCluster(B2)</f>
         <v>3.75820832838601, 7.24003474940441, 9.47142848690227, 1.60201233255417, 2.48389505922722, 2.76623804293011</v>
       </c>
-      <c r="AP2" t="str">
+      <c r="AU2" t="str">
         <f>_xll.NCDK_ChiPath(B2)</f>
         <v>13.1733621074374, 8.60822612591632, 7.53308445980525, 6.57446305443147, 5.83502554474493, 3.66414268256136, 2.81639208561656, 1.24750715936873, 10.5447358277005, 6.47350942312757, 4.82495377161152, 3.84884458919458, 2.7963481600948, 1.78170696456175, 1.19223951604789, 0.520731228864019</v>
       </c>
-      <c r="AQ2" t="str">
+      <c r="AV2" t="str">
         <f>_xll.NCDK_CPSA(B2)</f>
         <v>#N/A</v>
       </c>
-      <c r="AR2">
+      <c r="AW2">
         <f>_xll.NCDK_EccentricConnectivityIndex(B2)</f>
         <v>226</v>
       </c>
-      <c r="AS2">
+      <c r="AX2">
         <f>_xll.NCDK_FMF(B2)</f>
         <v>0.72222222222222221</v>
       </c>
-      <c r="AT2">
+      <c r="AY2">
         <f>_xll.NCDK_FractionalPSA(B2)</f>
         <v>0.30092142334124705</v>
       </c>
-      <c r="AU2">
+      <c r="AZ2">
         <f>_xll.NCDK_FragmentComplexity(B2)</f>
         <v>1063.05</v>
       </c>
-      <c r="AV2" t="str">
+      <c r="BA2" t="str">
         <f>_xll.NCDK_GravitationalIndex(B2)</f>
         <v>#N/A</v>
       </c>
-      <c r="AW2">
+      <c r="BB2">
         <f>_xll.NCDK_HBondAcceptorCount(B2)</f>
         <v>5</v>
       </c>
-      <c r="AX2">
+      <c r="BC2">
         <f>_xll.NCDK_HBondDonorCount(B2)</f>
         <v>2</v>
       </c>
-      <c r="AY2">
+      <c r="BD2">
         <f>_xll.NCDK_HybridizationRatio(B2)</f>
         <v>0.61538461538461542</v>
       </c>
-      <c r="AZ2" t="str">
+      <c r="BE2" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B2)</f>
         <v>14.409972299169, 5.96982167352538, 2.65927977839335</v>
       </c>
-      <c r="BA2" t="str">
+      <c r="BF2" t="str">
         <f>_xll.NCDK_KierHallSmarts(B2)</f>
         <v>0, 0, 0, 0, 0, 0, 1, 0, 6, 0, 1, 0, 0, 0, 0, 4, 0, 0, 1, 0, 0, 0, 0, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 3, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BB2">
+      <c r="BG2">
         <f>_xll.NCDK_LargestChain(B2)</f>
         <v>2</v>
       </c>
-      <c r="BC2">
+      <c r="BH2">
         <f>_xll.NCDK_LargestPiSystem(B2)</f>
         <v>8</v>
       </c>
-      <c r="BD2" t="str">
+      <c r="BI2" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B2)</f>
         <v>#N/A</v>
       </c>
-      <c r="BE2">
+      <c r="BJ2">
         <f>_xll.NCDK_LongestAliphaticChain(B2)</f>
         <v>2</v>
       </c>
-      <c r="BF2">
-        <f>_xll.NCDK_MannholdLogP(B2)</f>
-        <v>2.34</v>
-      </c>
-      <c r="BG2" t="str">
+      <c r="BK2" t="str">
         <f>_xll.NCDK_MDE(B2)</f>
         <v>0, 1.78256861348341, 1.17348231572452, 0.5, 9.28105720195319, 8.27801156561087, 2.82326712400687, 2.67269615442102, 3.03934274260637, 0, 0.75, 0, 0, 0, 0, 0, 0.5, 0, 0</v>
       </c>
-      <c r="BH2" t="str">
+      <c r="BL2" t="str">
         <f>_xll.NCDK_MomentOfInertia(B2)</f>
         <v>#N/A</v>
       </c>
-      <c r="BI2">
+      <c r="BM2">
         <f>_xll.NCDK_PetitjeanNumber(B2)</f>
         <v>0.5</v>
       </c>
-      <c r="BJ2" t="str">
+      <c r="BN2" t="str">
         <f>_xll.NCDK_PetitjeanShapeIndex(B2)</f>
         <v>#N/A</v>
       </c>
-      <c r="BK2">
+      <c r="BO2">
         <f>_xll.NCDK_RotatableBondsCount(B2)</f>
         <v>2</v>
       </c>
-      <c r="BL2">
+      <c r="BP2">
         <f>_xll.NCDK_RuleOfFive(B2)</f>
         <v>0</v>
       </c>
-      <c r="BM2" t="str">
+      <c r="BQ2" t="str">
         <f>_xll.NCDK_SmallRing(B2)</f>
         <v>2, 0, 2, 0, 0, 0, 0, 1, 1, 0, 0</v>
       </c>
-      <c r="BN2">
+      <c r="BR2">
         <f>_xll.NCDK_TPSA(B2)</f>
         <v>75.27000000000001</v>
       </c>
-      <c r="BO2">
+      <c r="BS2">
         <f>_xll.NCDK_VABC(B2)</f>
         <v>246.50970715028382</v>
       </c>
-      <c r="BP2">
+      <c r="BT2">
         <f>_xll.NCDK_VAdjMa(B2)</f>
         <v>5.2479275134435852</v>
       </c>
-      <c r="BQ2">
-        <f>_xll.NCDK_Weight(B2)</f>
-        <v>250.131742436</v>
-      </c>
-      <c r="BR2" t="str">
+      <c r="BU2" s="2">
+        <f>_xll.NCDK_MolecularWeight(B2)</f>
+        <v>250.29412142388836</v>
+      </c>
+      <c r="BV2" s="3">
+        <f>_xll.NCDK_ExactMass(B2)</f>
+        <v>250.13174243599997</v>
+      </c>
+      <c r="BW2" t="str">
         <f>_xll.NCDK_WeightedPath(B2)</f>
         <v>35.9822147160759, 1.99901192867088, 13.5466431850826, 7.60403910050065, 5.94260408458194</v>
       </c>
-      <c r="BS2" t="str">
+      <c r="BX2" t="str">
         <f>_xll.NCDK_WHIM(B2)</f>
         <v>#N/A</v>
       </c>
-      <c r="BT2" t="str">
+      <c r="BY2" t="str">
         <f>_xll.NCDK_WienerNumbers(B2)</f>
         <v>537, 35</v>
       </c>
-      <c r="BU2">
-        <f>_xll.NCDK_XLogP(B2)</f>
-        <v>2.1759999999999997</v>
-      </c>
-      <c r="BV2">
+      <c r="BZ2">
         <f>_xll.NCDK_ZagrebIndex(B2)</f>
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:74" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:78" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" t="str">
         <f>_xll.NCDK_MolText(B3)</f>
         <v xml:space="preserve">
-  CDK     0603191242
+       CDK0714190307
   1  0  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
 M  END
@@ -3219,214 +3282,230 @@
         <f>_xll.NCDK_PubchemFingerprinter($B3)</f>
         <v>00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="X3">
+      <c r="X3" s="2">
+        <f>_xll.NCDK_MolecularWeight(B3)</f>
+        <v>16.042498912091162</v>
+      </c>
+      <c r="Y3" s="2">
+        <f>_xll.NCDK_ExactMass(B3)</f>
+        <v>16.031300127999998</v>
+      </c>
+      <c r="Z3">
         <f>_xll.NCDK_AcidicGroupCount(B3)</f>
         <v>0</v>
       </c>
-      <c r="Y3">
+      <c r="AA3" s="4">
         <f>_xll.NCDK_ALogP(B3)</f>
         <v>0</v>
       </c>
-      <c r="Z3">
+      <c r="AB3" s="4">
+        <f>_xll.NCDK_XLogP(B3)</f>
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="AC3" s="4">
+        <f>_xll.NCDK_MannholdLogP(B3)</f>
+        <v>1.57</v>
+      </c>
+      <c r="AD3" s="4" t="e">
+        <f>_xll.NCDK_JPlogP(B3)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE3">
         <f>_xll.NCDK_AMolarRefractivity(B3)</f>
         <v>0</v>
       </c>
-      <c r="AA3">
+      <c r="AF3">
         <f>_xll.NCDK_APol(B3)</f>
         <v>4.4271719999999997</v>
       </c>
-      <c r="AB3">
+      <c r="AG3">
         <f>_xll.NCDK_AromaticAtomsCount(B3)</f>
         <v>0</v>
       </c>
-      <c r="AC3">
+      <c r="AH3">
         <f>_xll.NCDK_AromaticBondsCount(B3)</f>
         <v>0</v>
       </c>
-      <c r="AD3">
+      <c r="AI3">
         <f>_xll.NCDK_AtomCount(B3)</f>
         <v>5</v>
       </c>
-      <c r="AE3" t="str">
+      <c r="AJ3" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B3)</f>
         <v>0, 0, 0, 0, 0</v>
       </c>
-      <c r="AF3" t="str">
+      <c r="AK3" t="str">
         <f>_xll.NCDK_AutocorrelationMass(B3)</f>
         <v>1, 0, 0, 0, 0</v>
       </c>
-      <c r="AG3" t="str">
+      <c r="AL3" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B3)</f>
         <v>6.822544, 0, 0, 0, 0</v>
       </c>
-      <c r="AH3">
+      <c r="AM3">
         <f>_xll.NCDK_BasicGroupCount(B3)</f>
         <v>0</v>
       </c>
-      <c r="AI3" t="str">
+      <c r="AN3" t="str">
         <f>_xll.NCDK_BCUT(B3)</f>
         <v>12, 12, -0.0779229231460157, -0.0779229231460157, 2.612, 2.612</v>
       </c>
-      <c r="AJ3">
+      <c r="AO3">
         <f>_xll.NCDK_BondCount(B3)</f>
         <v>0</v>
       </c>
-      <c r="AK3">
+      <c r="AP3">
         <f>_xll.NCDK_BPol(B3)</f>
         <v>4.3728280000000002</v>
       </c>
-      <c r="AL3" t="str">
+      <c r="AQ3" t="str">
         <f>_xll.NCDK_CarbonTypes(B3)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AM3" t="str">
+      <c r="AR3" t="str">
         <f>_xll.NCDK_ChiChain(B3)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AN3" t="str">
+      <c r="AS3" t="str">
         <f>_xll.NCDK_ChiCluster(B3)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AO3" t="str">
+      <c r="AT3" t="str">
         <f>_xll.NCDK_ChiPathCluster(B3)</f>
         <v>0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AP3" t="str">
+      <c r="AU3" t="str">
         <f>_xll.NCDK_ChiPath(B3)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AQ3" t="str">
+      <c r="AV3" t="str">
         <f>_xll.NCDK_CPSA(B3)</f>
         <v>#N/A</v>
       </c>
-      <c r="AR3">
+      <c r="AW3">
         <f>_xll.NCDK_EccentricConnectivityIndex(B3)</f>
         <v>0</v>
       </c>
-      <c r="AS3">
+      <c r="AX3">
         <f>_xll.NCDK_FMF(B3)</f>
         <v>0</v>
       </c>
-      <c r="AT3">
+      <c r="AY3">
         <f>_xll.NCDK_FractionalPSA(B3)</f>
         <v>0</v>
       </c>
-      <c r="AU3">
+      <c r="AZ3">
         <f>_xll.NCDK_FragmentComplexity(B3)</f>
         <v>16</v>
       </c>
-      <c r="AV3" t="str">
+      <c r="BA3" t="str">
         <f>_xll.NCDK_GravitationalIndex(B3)</f>
         <v>#N/A</v>
       </c>
-      <c r="AW3">
+      <c r="BB3">
         <f>_xll.NCDK_HBondAcceptorCount(B3)</f>
         <v>0</v>
       </c>
-      <c r="AX3">
+      <c r="BC3">
         <f>_xll.NCDK_HBondDonorCount(B3)</f>
         <v>0</v>
       </c>
-      <c r="AY3">
+      <c r="BD3">
         <f>_xll.NCDK_HybridizationRatio(B3)</f>
         <v>1</v>
       </c>
-      <c r="AZ3" t="str">
+      <c r="BE3" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B3)</f>
         <v>0, 0, 0</v>
       </c>
-      <c r="BA3" t="str">
+      <c r="BF3" t="str">
         <f>_xll.NCDK_KierHallSmarts(B3)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BB3">
+      <c r="BG3">
         <f>_xll.NCDK_LargestChain(B3)</f>
         <v>0</v>
       </c>
-      <c r="BC3">
+      <c r="BH3">
         <f>_xll.NCDK_LargestPiSystem(B3)</f>
         <v>0</v>
       </c>
-      <c r="BD3" t="str">
+      <c r="BI3" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B3)</f>
         <v>#N/A</v>
       </c>
-      <c r="BE3">
+      <c r="BJ3">
         <f>_xll.NCDK_LongestAliphaticChain(B3)</f>
         <v>0</v>
       </c>
-      <c r="BF3">
-        <f>_xll.NCDK_MannholdLogP(B3)</f>
-        <v>1.57</v>
-      </c>
-      <c r="BG3" t="str">
+      <c r="BK3" t="str">
         <f>_xll.NCDK_MDE(B3)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BH3" t="str">
+      <c r="BL3" t="str">
         <f>_xll.NCDK_MomentOfInertia(B3)</f>
         <v>#N/A</v>
       </c>
-      <c r="BI3">
+      <c r="BM3">
         <f>_xll.NCDK_PetitjeanNumber(B3)</f>
         <v>0</v>
       </c>
-      <c r="BJ3" t="str">
+      <c r="BN3" t="str">
         <f>_xll.NCDK_PetitjeanShapeIndex(B3)</f>
         <v>#N/A</v>
       </c>
-      <c r="BK3">
+      <c r="BO3">
         <f>_xll.NCDK_RotatableBondsCount(B3)</f>
         <v>0</v>
       </c>
-      <c r="BL3">
+      <c r="BP3">
         <f>_xll.NCDK_RuleOfFive(B3)</f>
         <v>0</v>
       </c>
-      <c r="BM3" t="str">
+      <c r="BQ3" t="str">
         <f>_xll.NCDK_SmallRing(B3)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BN3">
+      <c r="BR3">
         <f>_xll.NCDK_TPSA(B3)</f>
         <v>0</v>
       </c>
-      <c r="BO3">
+      <c r="BS3">
         <f>_xll.NCDK_VABC(B3)</f>
         <v>25.852443326666702</v>
       </c>
-      <c r="BP3">
+      <c r="BT3">
         <f>_xll.NCDK_VAdjMa(B3)</f>
         <v>0</v>
       </c>
-      <c r="BQ3">
-        <f>_xll.NCDK_Weight(B3)</f>
+      <c r="BU3" s="2">
+        <f>_xll.NCDK_MolecularWeight(B3)</f>
+        <v>16.042498912091162</v>
+      </c>
+      <c r="BV3" s="3">
+        <f>_xll.NCDK_ExactMass(B3)</f>
         <v>16.031300127999998</v>
       </c>
-      <c r="BR3" t="str">
+      <c r="BW3" t="str">
         <f>_xll.NCDK_WeightedPath(B3)</f>
         <v>1, 1, 0, 0, 0</v>
       </c>
-      <c r="BS3" t="str">
+      <c r="BX3" t="str">
         <f>_xll.NCDK_WHIM(B3)</f>
         <v>#N/A</v>
       </c>
-      <c r="BT3" t="str">
+      <c r="BY3" t="str">
         <f>_xll.NCDK_WienerNumbers(B3)</f>
         <v>0, 0</v>
       </c>
-      <c r="BU3">
-        <f>_xll.NCDK_XLogP(B3)</f>
-        <v>0.73899999999999999</v>
-      </c>
-      <c r="BV3">
+      <c r="BZ3">
         <f>_xll.NCDK_ZagrebIndex(B3)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:74" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:78" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -3515,217 +3594,233 @@
         <f>_xll.NCDK_PubchemFingerprinter($B4)</f>
         <v>00000000010000000011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001101000000000000000000000100000000000000000000000000000000000100000001000000000000000000000100000100000000000000000000000001000000000000010000000000000000000100100000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="X4">
+      <c r="X4" s="2">
+        <f>_xll.NCDK_MolecularWeight(B4)</f>
+        <v>60.052044664017956</v>
+      </c>
+      <c r="Y4" s="2">
+        <f>_xll.NCDK_ExactMass(B4)</f>
+        <v>60.021129367999997</v>
+      </c>
+      <c r="Z4">
         <f>_xll.NCDK_AcidicGroupCount(B4)</f>
         <v>1</v>
       </c>
-      <c r="Y4">
+      <c r="AA4" s="4">
         <f>_xll.NCDK_ALogP(B4)</f>
         <v>-0.22990000000000016</v>
       </c>
-      <c r="Z4">
+      <c r="AB4" s="4">
+        <f>_xll.NCDK_XLogP(B4)</f>
+        <v>-0.08</v>
+      </c>
+      <c r="AC4" s="4">
+        <f>_xll.NCDK_MannholdLogP(B4)</f>
+        <v>1.46</v>
+      </c>
+      <c r="AD4" s="4">
+        <f>_xll.NCDK_JPlogP(B4)</f>
+        <v>-0.27735415884610526</v>
+      </c>
+      <c r="AE4">
         <f>_xll.NCDK_AMolarRefractivity(B4)</f>
         <v>12.643699999999999</v>
       </c>
-      <c r="AA4">
+      <c r="AF4">
         <f>_xll.NCDK_APol(B4)</f>
         <v>7.7911719999999995</v>
       </c>
-      <c r="AB4">
+      <c r="AG4">
         <f>_xll.NCDK_AromaticAtomsCount(B4)</f>
         <v>0</v>
       </c>
-      <c r="AC4">
+      <c r="AH4">
         <f>_xll.NCDK_AromaticBondsCount(B4)</f>
         <v>0</v>
       </c>
-      <c r="AD4">
+      <c r="AI4">
         <f>_xll.NCDK_AtomCount(B4)</f>
         <v>8</v>
       </c>
-      <c r="AE4" t="str">
+      <c r="AJ4" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B4)</f>
         <v>0.194598407923705, -0.0910121789036757, -0.00628702505817703, 0, 0</v>
       </c>
-      <c r="AF4" t="str">
+      <c r="AK4" t="str">
         <f>_xll.NCDK_AutocorrelationMass(B4)</f>
         <v>5.54893807108189, 3.66418395426513, 4.43865298980608, 0, 0</v>
       </c>
-      <c r="AG4" t="str">
+      <c r="AL4" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B4)</f>
         <v>58.780575625, 47.106336, 38.8410481875, 0, 0</v>
       </c>
-      <c r="AH4">
+      <c r="AM4">
         <f>_xll.NCDK_BasicGroupCount(B4)</f>
         <v>0</v>
       </c>
-      <c r="AI4" t="str">
+      <c r="AN4" t="str">
         <f>_xll.NCDK_BCUT(B4)</f>
         <v>11.9966879762366, 15.9982572603197, -0.351666803410558, 0.275648439067482, 3.09299617864267, 4.35788090208676</v>
       </c>
-      <c r="AJ4">
+      <c r="AO4">
         <f>_xll.NCDK_BondCount(B4)</f>
         <v>0</v>
       </c>
-      <c r="AK4">
+      <c r="AP4">
         <f>_xll.NCDK_BPol(B4)</f>
         <v>5.3308280000000003</v>
       </c>
-      <c r="AL4" t="str">
+      <c r="AQ4" t="str">
         <f>_xll.NCDK_CarbonTypes(B4)</f>
         <v>0, 0, 1, 0, 0, 1, 0, 0, 0</v>
       </c>
-      <c r="AM4" t="str">
+      <c r="AR4" t="str">
         <f>_xll.NCDK_ChiChain(B4)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AN4" t="str">
+      <c r="AS4" t="str">
         <f>_xll.NCDK_ChiCluster(B4)</f>
         <v>0.577350269189626, 0, 0, 0, 0.0912870929175277, 0, 0, 0</v>
       </c>
-      <c r="AO4" t="str">
+      <c r="AT4" t="str">
         <f>_xll.NCDK_ChiPathCluster(B4)</f>
         <v>0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AP4" t="str">
+      <c r="AU4" t="str">
         <f>_xll.NCDK_ChiPath(B4)</f>
         <v>3.57735026918963, 1.73205080756888, 1.73205080756888, 0, 0, 0, 0, 0, 2.35546188596382, 0.927730942981911, 0.519018035899438, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AQ4" t="str">
+      <c r="AV4" t="str">
         <f>_xll.NCDK_CPSA(B4)</f>
         <v>#N/A</v>
       </c>
-      <c r="AR4">
+      <c r="AW4">
         <f>_xll.NCDK_EccentricConnectivityIndex(B4)</f>
         <v>9</v>
       </c>
-      <c r="AS4">
+      <c r="AX4">
         <f>_xll.NCDK_FMF(B4)</f>
         <v>0</v>
       </c>
-      <c r="AT4">
+      <c r="AY4">
         <f>_xll.NCDK_FractionalPSA(B4)</f>
         <v>0.62144781967398288</v>
       </c>
-      <c r="AU4">
+      <c r="AZ4">
         <f>_xll.NCDK_FragmentComplexity(B4)</f>
         <v>37.020000000000003</v>
       </c>
-      <c r="AV4" t="str">
+      <c r="BA4" t="str">
         <f>_xll.NCDK_GravitationalIndex(B4)</f>
         <v>#N/A</v>
       </c>
-      <c r="AW4">
+      <c r="BB4">
         <f>_xll.NCDK_HBondAcceptorCount(B4)</f>
         <v>2</v>
       </c>
-      <c r="AX4">
+      <c r="BC4">
         <f>_xll.NCDK_HBondDonorCount(B4)</f>
         <v>1</v>
       </c>
-      <c r="AY4">
+      <c r="BD4">
         <f>_xll.NCDK_HybridizationRatio(B4)</f>
         <v>0.5</v>
       </c>
-      <c r="AZ4" t="str">
+      <c r="BE4" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B4)</f>
         <v>4, 1.33333333333333, #N/A</v>
       </c>
-      <c r="BA4" t="str">
+      <c r="BF4" t="str">
         <f>_xll.NCDK_KierHallSmarts(B4)</f>
         <v>0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BB4">
+      <c r="BG4">
         <f>_xll.NCDK_LargestChain(B4)</f>
         <v>3</v>
       </c>
-      <c r="BC4">
+      <c r="BH4">
         <f>_xll.NCDK_LargestPiSystem(B4)</f>
         <v>2</v>
       </c>
-      <c r="BD4" t="str">
+      <c r="BI4" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B4)</f>
         <v>#N/A</v>
       </c>
-      <c r="BE4">
+      <c r="BJ4">
         <f>_xll.NCDK_LongestAliphaticChain(B4)</f>
         <v>2</v>
       </c>
-      <c r="BF4">
-        <f>_xll.NCDK_MannholdLogP(B4)</f>
-        <v>1.46</v>
-      </c>
-      <c r="BG4" t="str">
+      <c r="BK4" t="str">
         <f>_xll.NCDK_MDE(B4)</f>
         <v>0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0.5, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BH4" t="str">
+      <c r="BL4" t="str">
         <f>_xll.NCDK_MomentOfInertia(B4)</f>
         <v>#N/A</v>
       </c>
-      <c r="BI4">
+      <c r="BM4">
         <f>_xll.NCDK_PetitjeanNumber(B4)</f>
         <v>0.5</v>
       </c>
-      <c r="BJ4" t="str">
+      <c r="BN4" t="str">
         <f>_xll.NCDK_PetitjeanShapeIndex(B4)</f>
         <v>#N/A</v>
       </c>
-      <c r="BK4">
+      <c r="BO4">
         <f>_xll.NCDK_RotatableBondsCount(B4)</f>
         <v>0</v>
       </c>
-      <c r="BL4">
+      <c r="BP4">
         <f>_xll.NCDK_RuleOfFive(B4)</f>
         <v>0</v>
       </c>
-      <c r="BM4" t="str">
+      <c r="BQ4" t="str">
         <f>_xll.NCDK_SmallRing(B4)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BN4">
+      <c r="BR4">
         <f>_xll.NCDK_TPSA(B4)</f>
         <v>37.299999999999997</v>
       </c>
-      <c r="BO4">
+      <c r="BS4">
         <f>_xll.NCDK_VABC(B4)</f>
         <v>58.092422652855603</v>
       </c>
-      <c r="BP4">
+      <c r="BT4">
         <f>_xll.NCDK_VAdjMa(B4)</f>
         <v>2.5849625007211561</v>
       </c>
-      <c r="BQ4">
-        <f>_xll.NCDK_Weight(B4)</f>
-        <v>60.021129368000004</v>
-      </c>
-      <c r="BR4" t="str">
+      <c r="BU4" s="2">
+        <f>_xll.NCDK_MolecularWeight(B4)</f>
+        <v>60.052044664017956</v>
+      </c>
+      <c r="BV4" s="3">
+        <f>_xll.NCDK_ExactMass(B4)</f>
+        <v>60.021129367999997</v>
+      </c>
+      <c r="BW4" t="str">
         <f>_xll.NCDK_WeightedPath(B4)</f>
         <v>6.73205080756888, 1.68301270189222, 4.48803387171259, 4.48803387171259, 0</v>
       </c>
-      <c r="BS4" t="str">
+      <c r="BX4" t="str">
         <f>_xll.NCDK_WHIM(B4)</f>
         <v>#N/A</v>
       </c>
-      <c r="BT4" t="str">
+      <c r="BY4" t="str">
         <f>_xll.NCDK_WienerNumbers(B4)</f>
         <v>9, 0</v>
       </c>
-      <c r="BU4">
-        <f>_xll.NCDK_XLogP(B4)</f>
-        <v>-0.08</v>
-      </c>
-      <c r="BV4">
+      <c r="BZ4">
         <f>_xll.NCDK_ZagrebIndex(B4)</f>
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:74" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:78" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" t="str">
         <f>_xll.NCDK_InChI(B5)</f>
@@ -3811,217 +3906,233 @@
         <f>_xll.NCDK_PubchemFingerprinter($B5)</f>
         <v>00000000011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000001100000000000000000000000000000000000000000000000100000000000100000000001000000000000001100000000000010000000000000000000000000000000100000000000000000100000010000100000000000000000000000100000000000000000001000000000000000000000000010001000100000000000000000000000000010001000000010000010000000100010100000000001000100010000100000000010000000000000001000001000000000000000000010001000100000000111000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="X5">
+      <c r="X5" s="2">
+        <f>_xll.NCDK_MolecularWeight(B5)</f>
+        <v>78.112059903682749</v>
+      </c>
+      <c r="Y5" s="2">
+        <f>_xll.NCDK_ExactMass(B5)</f>
+        <v>78.046950191999997</v>
+      </c>
+      <c r="Z5">
         <f>_xll.NCDK_AcidicGroupCount(B5)</f>
         <v>0</v>
       </c>
-      <c r="Y5">
+      <c r="AA5" s="4">
         <f>_xll.NCDK_ALogP(B5)</f>
         <v>1.8299999999999996</v>
       </c>
-      <c r="Z5">
+      <c r="AB5" s="4">
+        <f>_xll.NCDK_XLogP(B5)</f>
+        <v>2.0220000000000002</v>
+      </c>
+      <c r="AC5" s="4">
+        <f>_xll.NCDK_MannholdLogP(B5)</f>
+        <v>2.12</v>
+      </c>
+      <c r="AD5" s="4">
+        <f>_xll.NCDK_JPlogP(B5)</f>
+        <v>1.8466303941078017</v>
+      </c>
+      <c r="AE5">
         <f>_xll.NCDK_AMolarRefractivity(B5)</f>
         <v>26.058</v>
       </c>
-      <c r="AA5">
+      <c r="AF5">
         <f>_xll.NCDK_APol(B5)</f>
         <v>14.560758</v>
       </c>
-      <c r="AB5">
+      <c r="AG5">
         <f>_xll.NCDK_AromaticAtomsCount(B5)</f>
         <v>6</v>
       </c>
-      <c r="AC5">
+      <c r="AH5">
         <f>_xll.NCDK_AromaticBondsCount(B5)</f>
         <v>6</v>
       </c>
-      <c r="AD5">
+      <c r="AI5">
         <f>_xll.NCDK_AtomCount(B5)</f>
         <v>12</v>
       </c>
-      <c r="AE5" t="str">
+      <c r="AJ5" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B5)</f>
         <v>0, 0, 0, 0, 0</v>
       </c>
-      <c r="AF5" t="str">
+      <c r="AK5" t="str">
         <f>_xll.NCDK_AutocorrelationMass(B5)</f>
         <v>6, 6, 6, 3, 0</v>
       </c>
-      <c r="AG5" t="str">
+      <c r="AL5" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B5)</f>
         <v>233.87838834375, 233.87838834375, 233.87838834375, 116.939194171875, 0</v>
       </c>
-      <c r="AH5">
+      <c r="AM5">
         <f>_xll.NCDK_BasicGroupCount(B5)</f>
         <v>0</v>
       </c>
-      <c r="AI5" t="str">
+      <c r="AN5" t="str">
         <f>_xll.NCDK_BCUT(B5)</f>
         <v>11.85, 12.1500544016358, -0.211758152069243, 0.0882962495665529, 6.093375, 6.3934294016358</v>
       </c>
-      <c r="AJ5">
+      <c r="AO5">
         <f>_xll.NCDK_BondCount(B5)</f>
         <v>0</v>
       </c>
-      <c r="AK5">
+      <c r="AP5">
         <f>_xll.NCDK_BPol(B5)</f>
         <v>6.5592419999999994</v>
       </c>
-      <c r="AL5" t="str">
+      <c r="AQ5" t="str">
         <f>_xll.NCDK_CarbonTypes(B5)</f>
         <v>0, 0, 0, 6, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AM5" t="str">
+      <c r="AR5" t="str">
         <f>_xll.NCDK_ChiChain(B5)</f>
         <v>0, 0, 0, 0.125, 0, 0, 0, 0, 0.037037037037037, 0</v>
       </c>
-      <c r="AN5" t="str">
+      <c r="AS5" t="str">
         <f>_xll.NCDK_ChiCluster(B5)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AO5" t="str">
+      <c r="AT5" t="str">
         <f>_xll.NCDK_ChiPathCluster(B5)</f>
         <v>0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AP5" t="str">
+      <c r="AU5" t="str">
         <f>_xll.NCDK_ChiPath(B5)</f>
         <v>4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0, 3.46410161513775, 2, 1.15470053837925, 0.666666666666667, 0.384900179459751, 0.222222222222222, 0, 0</v>
       </c>
-      <c r="AQ5" t="str">
+      <c r="AV5" t="str">
         <f>_xll.NCDK_CPSA(B5)</f>
         <v>#N/A</v>
       </c>
-      <c r="AR5">
+      <c r="AW5">
         <f>_xll.NCDK_EccentricConnectivityIndex(B5)</f>
         <v>36</v>
       </c>
-      <c r="AS5">
+      <c r="AX5">
         <f>_xll.NCDK_FMF(B5)</f>
         <v>1</v>
       </c>
-      <c r="AT5">
+      <c r="AY5">
         <f>_xll.NCDK_FractionalPSA(B5)</f>
         <v>0</v>
       </c>
-      <c r="AU5">
+      <c r="AZ5">
         <f>_xll.NCDK_FragmentComplexity(B5)</f>
         <v>114</v>
       </c>
-      <c r="AV5" t="str">
+      <c r="BA5" t="str">
         <f>_xll.NCDK_GravitationalIndex(B5)</f>
         <v>#N/A</v>
       </c>
-      <c r="AW5">
+      <c r="BB5">
         <f>_xll.NCDK_HBondAcceptorCount(B5)</f>
         <v>0</v>
       </c>
-      <c r="AX5">
+      <c r="BC5">
         <f>_xll.NCDK_HBondDonorCount(B5)</f>
         <v>0</v>
       </c>
-      <c r="AY5">
+      <c r="BD5">
         <f>_xll.NCDK_HybridizationRatio(B5)</f>
         <v>0</v>
       </c>
-      <c r="AZ5" t="str">
+      <c r="BE5" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B5)</f>
         <v>4.16666666666667, 2.22222222222222, 1.33333333333333</v>
       </c>
-      <c r="BA5" t="str">
+      <c r="BF5" t="str">
         <f>_xll.NCDK_KierHallSmarts(B5)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 6, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BB5">
+      <c r="BG5">
         <f>_xll.NCDK_LargestChain(B5)</f>
         <v>0</v>
       </c>
-      <c r="BC5">
+      <c r="BH5">
         <f>_xll.NCDK_LargestPiSystem(B5)</f>
         <v>6</v>
       </c>
-      <c r="BD5" t="str">
+      <c r="BI5" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B5)</f>
         <v>#N/A</v>
       </c>
-      <c r="BE5">
+      <c r="BJ5">
         <f>_xll.NCDK_LongestAliphaticChain(B5)</f>
         <v>0</v>
       </c>
-      <c r="BF5">
-        <f>_xll.NCDK_MannholdLogP(B5)</f>
-        <v>2.12</v>
-      </c>
-      <c r="BG5" t="str">
+      <c r="BK5" t="str">
         <f>_xll.NCDK_MDE(B5)</f>
         <v>0, 0, 0, 0, 9.12546512839809, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BH5" t="str">
+      <c r="BL5" t="str">
         <f>_xll.NCDK_MomentOfInertia(B5)</f>
         <v>#N/A</v>
       </c>
-      <c r="BI5">
+      <c r="BM5">
         <f>_xll.NCDK_PetitjeanNumber(B5)</f>
         <v>0</v>
       </c>
-      <c r="BJ5" t="str">
+      <c r="BN5" t="str">
         <f>_xll.NCDK_PetitjeanShapeIndex(B5)</f>
         <v>#N/A</v>
       </c>
-      <c r="BK5">
+      <c r="BO5">
         <f>_xll.NCDK_RotatableBondsCount(B5)</f>
         <v>0</v>
       </c>
-      <c r="BL5">
+      <c r="BP5">
         <f>_xll.NCDK_RuleOfFive(B5)</f>
         <v>0</v>
       </c>
-      <c r="BM5" t="str">
+      <c r="BQ5" t="str">
         <f>_xll.NCDK_SmallRing(B5)</f>
         <v>1, 1, 1, 1, 0, 0, 0, 1, 0, 0, 0</v>
       </c>
-      <c r="BN5">
+      <c r="BR5">
         <f>_xll.NCDK_TPSA(B5)</f>
         <v>0</v>
       </c>
-      <c r="BO5">
+      <c r="BS5">
         <f>_xll.NCDK_VABC(B5)</f>
         <v>81.166531652800174</v>
       </c>
-      <c r="BP5">
+      <c r="BT5">
         <f>_xll.NCDK_VAdjMa(B5)</f>
         <v>3.5849625007211561</v>
       </c>
-      <c r="BQ5">
-        <f>_xll.NCDK_Weight(B5)</f>
+      <c r="BU5" s="2">
+        <f>_xll.NCDK_MolecularWeight(B5)</f>
+        <v>78.112059903682749</v>
+      </c>
+      <c r="BV5" s="3">
+        <f>_xll.NCDK_ExactMass(B5)</f>
         <v>78.046950191999997</v>
       </c>
-      <c r="BR5" t="str">
+      <c r="BW5" t="str">
         <f>_xll.NCDK_WeightedPath(B5)</f>
         <v>11.8125, 1.96875, 0, 0, 0</v>
       </c>
-      <c r="BS5" t="str">
+      <c r="BX5" t="str">
         <f>_xll.NCDK_WHIM(B5)</f>
         <v>#N/A</v>
       </c>
-      <c r="BT5" t="str">
+      <c r="BY5" t="str">
         <f>_xll.NCDK_WienerNumbers(B5)</f>
         <v>27, 3</v>
       </c>
-      <c r="BU5">
-        <f>_xll.NCDK_XLogP(B5)</f>
-        <v>2.0220000000000002</v>
-      </c>
-      <c r="BV5">
+      <c r="BZ5">
         <f>_xll.NCDK_ZagrebIndex(B5)</f>
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:74" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:78" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" t="s">
         <v>85</v>
-      </c>
-      <c r="B6" t="s">
-        <v>86</v>
       </c>
       <c r="C6" t="str">
         <f>_xll.NCDK_InChI(B6)</f>
@@ -4107,221 +4218,237 @@
         <f>_xll.NCDK_PubchemFingerprinter($B6)</f>
         <v>00000000011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000001100000000000000000000000000000000000000000000000110000000000100000000001100000000000001100100000000010000000000000000000000000000000100000000000001000100000010000100000000000000000000000100000000000000000001000000000000000000000000010001000100000000000000000000000000010001000000010000010000000100010100000000001000100010000100000000010000000000000001000001000000000000000000010001000100000000111000000001000000000000000000011100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="X6">
+      <c r="X6" s="2">
+        <f>_xll.NCDK_MolecularWeight(B6)</f>
+        <v>92.13867730812234</v>
+      </c>
+      <c r="Y6" s="2">
+        <f>_xll.NCDK_ExactMass(B6)</f>
+        <v>92.062600255999996</v>
+      </c>
+      <c r="Z6">
         <f>_xll.NCDK_AcidicGroupCount(B6)</f>
         <v>0</v>
       </c>
-      <c r="Y6">
+      <c r="AA6" s="4">
         <f>_xll.NCDK_ALogP(B6)</f>
         <v>2.3162000000000003</v>
       </c>
-      <c r="Z6">
+      <c r="AB6" s="4">
+        <f>_xll.NCDK_XLogP(B6)</f>
+        <v>2.4590000000000001</v>
+      </c>
+      <c r="AC6" s="4">
+        <f>_xll.NCDK_MannholdLogP(B6)</f>
+        <v>2.23</v>
+      </c>
+      <c r="AD6" s="4">
+        <f>_xll.NCDK_JPlogP(B6)</f>
+        <v>2.3300074064489729</v>
+      </c>
+      <c r="AE6">
         <f>_xll.NCDK_AMolarRefractivity(B6)</f>
         <v>31.0992</v>
       </c>
-      <c r="AA6">
+      <c r="AF6">
         <f>_xll.NCDK_APol(B6)</f>
         <v>17.654343999999998</v>
       </c>
-      <c r="AB6">
+      <c r="AG6">
         <f>_xll.NCDK_AromaticAtomsCount(B6)</f>
         <v>6</v>
       </c>
-      <c r="AC6">
+      <c r="AH6">
         <f>_xll.NCDK_AromaticBondsCount(B6)</f>
         <v>6</v>
       </c>
-      <c r="AD6">
+      <c r="AI6">
         <f>_xll.NCDK_AtomCount(B6)</f>
         <v>15</v>
       </c>
-      <c r="AE6" t="str">
+      <c r="AJ6" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B6)</f>
         <v>0.00145821501522747, -0.000488055819316601, -0.000225165712015084, -1.53979004755717E-05, -4.88075806479512E-07</v>
       </c>
-      <c r="AF6" t="str">
+      <c r="AK6" t="str">
         <f>_xll.NCDK_AutocorrelationMass(B6)</f>
         <v>7, 7, 8, 5, 1</v>
       </c>
-      <c r="AG6" t="str">
+      <c r="AL6" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B6)</f>
         <v>310.962687273438, 320.438287539063, 355.858255328125, 213.793837835938, 36.9196446054688</v>
       </c>
-      <c r="AH6">
+      <c r="AM6">
         <f>_xll.NCDK_BasicGroupCount(B6)</f>
         <v>0</v>
       </c>
-      <c r="AI6" t="str">
+      <c r="AN6" t="str">
         <f>_xll.NCDK_BCUT(B6)</f>
         <v>11.89, 12.1100942558098, -0.155208136358149, 0.0651359477608963, 5.76122693815409, 7.50783741355056</v>
       </c>
-      <c r="AJ6">
+      <c r="AO6">
         <f>_xll.NCDK_BondCount(B6)</f>
         <v>0</v>
       </c>
-      <c r="AK6">
+      <c r="AP6">
         <f>_xll.NCDK_BPol(B6)</f>
         <v>8.7456560000000003</v>
       </c>
-      <c r="AL6" t="str">
+      <c r="AQ6" t="str">
         <f>_xll.NCDK_CarbonTypes(B6)</f>
         <v>0, 0, 0, 5, 1, 1, 0, 0, 0</v>
       </c>
-      <c r="AM6" t="str">
+      <c r="AR6" t="str">
         <f>_xll.NCDK_ChiChain(B6)</f>
         <v>0, 0, 0, 0.102062072615966, 0.102062072615966, 0, 0, 0, 0.0320750149549792, 0.0320750149549792</v>
       </c>
-      <c r="AN6" t="str">
+      <c r="AS6" t="str">
         <f>_xll.NCDK_ChiCluster(B6)</f>
         <v>0.288675134594813, 0, 0, 0, 0.166666666666667, 0, 0, 0</v>
       </c>
-      <c r="AO6" t="str">
+      <c r="AT6" t="str">
         <f>_xll.NCDK_ChiPathCluster(B6)</f>
         <v>0.408248290463863, 0.433012701892219, 0.408248290463863, 0.192450089729875, 0.166666666666667, 0.128300059819917</v>
       </c>
-      <c r="AP6" t="str">
+      <c r="AU6" t="str">
         <f>_xll.NCDK_ChiPath(B6)</f>
         <v>5.11288417512236, 3.39384685011735, 2.74318215649199, 1.89384685011735, 1.30671282224753, 0.901047570290607, 0.204124145231932, 0, 4.38675134594813, 2.41068360252296, 1.65470053837925, 0.940455735015306, 0.534377897417612, 0.303561200840986, 0.0641500299099584, 0</v>
       </c>
-      <c r="AQ6" t="str">
+      <c r="AV6" t="str">
         <f>_xll.NCDK_CPSA(B6)</f>
         <v>#N/A</v>
       </c>
-      <c r="AR6">
+      <c r="AW6">
         <f>_xll.NCDK_EccentricConnectivityIndex(B6)</f>
         <v>45</v>
       </c>
-      <c r="AS6">
+      <c r="AX6">
         <f>_xll.NCDK_FMF(B6)</f>
         <v>0.8571428571428571</v>
       </c>
-      <c r="AT6">
+      <c r="AY6">
         <f>_xll.NCDK_FractionalPSA(B6)</f>
         <v>0</v>
       </c>
-      <c r="AU6">
+      <c r="AZ6">
         <f>_xll.NCDK_FragmentComplexity(B6)</f>
         <v>183</v>
       </c>
-      <c r="AV6" t="str">
+      <c r="BA6" t="str">
         <f>_xll.NCDK_GravitationalIndex(B6)</f>
         <v>#N/A</v>
       </c>
-      <c r="AW6">
+      <c r="BB6">
         <f>_xll.NCDK_HBondAcceptorCount(B6)</f>
         <v>0</v>
       </c>
-      <c r="AX6">
+      <c r="BC6">
         <f>_xll.NCDK_HBondDonorCount(B6)</f>
         <v>0</v>
       </c>
-      <c r="AY6">
+      <c r="BD6">
         <f>_xll.NCDK_HybridizationRatio(B6)</f>
         <v>0.14285714285714285</v>
       </c>
-      <c r="AZ6" t="str">
+      <c r="BE6" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B6)</f>
         <v>5.14285714285714, 2.34375, 1.5</v>
       </c>
-      <c r="BA6" t="str">
+      <c r="BF6" t="str">
         <f>_xll.NCDK_KierHallSmarts(B6)</f>
         <v>0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 5, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BB6">
+      <c r="BG6">
         <f>_xll.NCDK_LargestChain(B6)</f>
         <v>0</v>
       </c>
-      <c r="BC6">
+      <c r="BH6">
         <f>_xll.NCDK_LargestPiSystem(B6)</f>
         <v>6</v>
       </c>
-      <c r="BD6" t="str">
+      <c r="BI6" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B6)</f>
         <v>#N/A</v>
       </c>
-      <c r="BE6">
+      <c r="BJ6">
         <f>_xll.NCDK_LongestAliphaticChain(B6)</f>
         <v>0</v>
       </c>
-      <c r="BF6">
-        <f>_xll.NCDK_MannholdLogP(B6)</f>
-        <v>2.23</v>
-      </c>
-      <c r="BG6" t="str">
+      <c r="BK6" t="str">
         <f>_xll.NCDK_MDE(B6)</f>
         <v>0, 1.85053586243577, 1, 0, 6.08364341893206, 3.04182170946603, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BH6" t="str">
+      <c r="BL6" t="str">
         <f>_xll.NCDK_MomentOfInertia(B6)</f>
         <v>#N/A</v>
       </c>
-      <c r="BI6">
+      <c r="BM6">
         <f>_xll.NCDK_PetitjeanNumber(B6)</f>
         <v>0.25</v>
       </c>
-      <c r="BJ6" t="str">
+      <c r="BN6" t="str">
         <f>_xll.NCDK_PetitjeanShapeIndex(B6)</f>
         <v>#N/A</v>
       </c>
-      <c r="BK6">
+      <c r="BO6">
         <f>_xll.NCDK_RotatableBondsCount(B6)</f>
         <v>0</v>
       </c>
-      <c r="BL6">
+      <c r="BP6">
         <f>_xll.NCDK_RuleOfFive(B6)</f>
         <v>0</v>
       </c>
-      <c r="BM6" t="str">
+      <c r="BQ6" t="str">
         <f>_xll.NCDK_SmallRing(B6)</f>
         <v>1, 1, 1, 1, 0, 0, 0, 1, 0, 0, 0</v>
       </c>
-      <c r="BN6">
+      <c r="BR6">
         <f>_xll.NCDK_TPSA(B6)</f>
         <v>0</v>
       </c>
-      <c r="BO6">
+      <c r="BS6">
         <f>_xll.NCDK_VABC(B6)</f>
         <v>98.462516278666868</v>
       </c>
-      <c r="BP6">
+      <c r="BT6">
         <f>_xll.NCDK_VAdjMa(B6)</f>
         <v>3.8073549220576042</v>
       </c>
-      <c r="BQ6">
-        <f>_xll.NCDK_Weight(B6)</f>
+      <c r="BU6" s="2">
+        <f>_xll.NCDK_MolecularWeight(B6)</f>
+        <v>92.13867730812234</v>
+      </c>
+      <c r="BV6" s="3">
+        <f>_xll.NCDK_ExactMass(B6)</f>
         <v>92.062600255999996</v>
       </c>
-      <c r="BR6" t="str">
+      <c r="BW6" t="str">
         <f>_xll.NCDK_WeightedPath(B6)</f>
         <v>13.6768253204364, 1.95383218863377, 0, 0, 0</v>
       </c>
-      <c r="BS6" t="str">
+      <c r="BX6" t="str">
         <f>_xll.NCDK_WHIM(B6)</f>
         <v>#N/A</v>
       </c>
-      <c r="BT6" t="str">
+      <c r="BY6" t="str">
         <f>_xll.NCDK_WienerNumbers(B6)</f>
         <v>42, 5</v>
       </c>
-      <c r="BU6">
-        <f>_xll.NCDK_XLogP(B6)</f>
-        <v>2.4590000000000001</v>
-      </c>
-      <c r="BV6">
+      <c r="BZ6">
         <f>_xll.NCDK_ZagrebIndex(B6)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:74" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:78" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
         <v>56</v>
-      </c>
-      <c r="B7" t="s">
-        <v>57</v>
       </c>
       <c r="C7" t="str">
         <f>_xll.NCDK_SMILES(B7)</f>
-        <v>[C]1[C][C][C][C][C]1</v>
+        <v>C1CCCCC1</v>
       </c>
       <c r="D7">
         <f>_xll.NCDK_Tanimoto($H7,$H8)</f>
@@ -4329,7 +4456,7 @@
       </c>
       <c r="E7" t="str">
         <f>_xll.NCDK(E$1,$B7)</f>
-        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001010</v>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000010000000000000000010000000000000001010</v>
       </c>
       <c r="F7" t="str">
         <f>_xll.NCDK_ECFP0($B7)</f>
@@ -4369,7 +4496,7 @@
       </c>
       <c r="O7" t="str">
         <f>_xll.NCDK_EStateFingerprinter($B7)</f>
-        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>0000000010000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="P7" t="str">
         <f>_xll.NCDK_ExtendedFingerprinter($B7)</f>
@@ -4385,11 +4512,11 @@
       </c>
       <c r="S7" t="str">
         <f>_xll.NCDK_LingoFingerprinter($B7)</f>
-        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="T7" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($B7)</f>
-        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001010</v>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000010000000000000000010000000000000001010</v>
       </c>
       <c r="U7" t="str">
         <f>_xll.NCDK_ShortestPathFingerprinter($B7)</f>
@@ -4397,227 +4524,243 @@
       </c>
       <c r="V7" t="str">
         <f>_xll.NCDK_SubstructureFingerprinter($B7)</f>
-        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>0100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="W7" t="str">
         <f>_xll.NCDK_PubchemFingerprinter($B7)</f>
         <v>00000000011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="X7">
+      <c r="X7" s="2">
+        <f>_xll.NCDK_MolecularWeight(B7)</f>
+        <v>72.064415380728008</v>
+      </c>
+      <c r="Y7" s="2">
+        <f>_xll.NCDK_ExactMass(B7)</f>
+        <v>72</v>
+      </c>
+      <c r="Z7">
         <f>_xll.NCDK_AcidicGroupCount(B7)</f>
         <v>0</v>
       </c>
-      <c r="Y7">
+      <c r="AA7" s="4">
         <f>_xll.NCDK_ALogP(B7)</f>
-        <v>-1.7280000000000006</v>
-      </c>
-      <c r="Z7">
+        <v>2.7372000000000005</v>
+      </c>
+      <c r="AB7" s="4">
+        <f>_xll.NCDK_XLogP(B7)</f>
+        <v>3.4139999999999997</v>
+      </c>
+      <c r="AC7" s="4">
+        <f>_xll.NCDK_MannholdLogP(B7)</f>
+        <v>2.12</v>
+      </c>
+      <c r="AD7" s="4">
+        <f>_xll.NCDK_JPlogP(B7)</f>
+        <v>2.6952762459207973</v>
+      </c>
+      <c r="AE7">
         <f>_xll.NCDK_AMolarRefractivity(B7)</f>
-        <v>17.4696</v>
-      </c>
-      <c r="AA7">
+        <v>27.606000000000002</v>
+      </c>
+      <c r="AF7">
         <f>_xll.NCDK_APol(B7)</f>
-        <v>10.56</v>
-      </c>
-      <c r="AB7">
+        <v>18.561516000000001</v>
+      </c>
+      <c r="AG7">
         <f>_xll.NCDK_AromaticAtomsCount(B7)</f>
         <v>0</v>
       </c>
-      <c r="AC7">
+      <c r="AH7">
         <f>_xll.NCDK_AromaticBondsCount(B7)</f>
         <v>0</v>
       </c>
-      <c r="AD7">
+      <c r="AI7">
         <f>_xll.NCDK_AtomCount(B7)</f>
-        <v>6</v>
-      </c>
-      <c r="AE7" t="str">
+        <v>18</v>
+      </c>
+      <c r="AJ7" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B7)</f>
         <v>0, 0, 0, 0, 0</v>
       </c>
-      <c r="AF7" t="str">
+      <c r="AK7" t="str">
         <f>_xll.NCDK_AutocorrelationMass(B7)</f>
         <v>6, 6, 6, 3, 0</v>
       </c>
-      <c r="AG7" t="str">
+      <c r="AL7" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B7)</f>
         <v>257.709834375, 257.709834375, 257.709834375, 128.8549171875, 0</v>
       </c>
-      <c r="AH7">
+      <c r="AM7">
         <f>_xll.NCDK_BasicGroupCount(B7)</f>
         <v>0</v>
       </c>
-      <c r="AI7" t="str">
+      <c r="AN7" t="str">
         <f>_xll.NCDK_BCUT(B7)</f>
         <v>11.9, 12.1000824042221, -0.15279744210896, 0.0472849621131451, 6.45375, 6.65383240422211</v>
       </c>
-      <c r="AJ7">
+      <c r="AO7">
         <f>_xll.NCDK_BondCount(B7)</f>
         <v>0</v>
       </c>
-      <c r="AK7">
+      <c r="AP7">
         <f>_xll.NCDK_BPol(B7)</f>
-        <v>0</v>
-      </c>
-      <c r="AL7" t="str">
+        <v>13.118483999999999</v>
+      </c>
+      <c r="AQ7" t="str">
         <f>_xll.NCDK_CarbonTypes(B7)</f>
         <v>0, 0, 0, 0, 0, 0, 6, 0, 0</v>
       </c>
-      <c r="AM7" t="str">
+      <c r="AR7" t="str">
         <f>_xll.NCDK_ChiChain(B7)</f>
         <v>0, 0, 0, 0.125, 0, 0, 0, 0, 0.125, 0</v>
       </c>
-      <c r="AN7" t="str">
+      <c r="AS7" t="str">
         <f>_xll.NCDK_ChiCluster(B7)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AO7" t="str">
+      <c r="AT7" t="str">
         <f>_xll.NCDK_ChiPathCluster(B7)</f>
         <v>0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AP7" t="str">
+      <c r="AU7" t="str">
         <f>_xll.NCDK_ChiPath(B7)</f>
         <v>4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0, 4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0</v>
       </c>
-      <c r="AQ7" t="str">
+      <c r="AV7" t="str">
         <f>_xll.NCDK_CPSA(B7)</f>
         <v>#N/A</v>
       </c>
-      <c r="AR7">
+      <c r="AW7">
         <f>_xll.NCDK_EccentricConnectivityIndex(B7)</f>
         <v>36</v>
       </c>
-      <c r="AS7">
+      <c r="AX7">
         <f>_xll.NCDK_FMF(B7)</f>
         <v>1</v>
       </c>
-      <c r="AT7">
+      <c r="AY7">
         <f>_xll.NCDK_FractionalPSA(B7)</f>
         <v>0</v>
       </c>
-      <c r="AU7">
+      <c r="AZ7">
         <f>_xll.NCDK_FragmentComplexity(B7)</f>
         <v>6</v>
       </c>
-      <c r="AV7" t="str">
+      <c r="BA7" t="str">
         <f>_xll.NCDK_GravitationalIndex(B7)</f>
         <v>#N/A</v>
       </c>
-      <c r="AW7">
+      <c r="BB7">
         <f>_xll.NCDK_HBondAcceptorCount(B7)</f>
         <v>0</v>
       </c>
-      <c r="AX7">
+      <c r="BC7">
         <f>_xll.NCDK_HBondDonorCount(B7)</f>
         <v>0</v>
       </c>
-      <c r="AY7">
+      <c r="BD7">
         <f>_xll.NCDK_HybridizationRatio(B7)</f>
         <v>1</v>
       </c>
-      <c r="AZ7" t="str">
+      <c r="BE7" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B7)</f>
         <v>4.16666666666667, 2.22222222222222, 1.33333333333333</v>
       </c>
-      <c r="BA7" t="str">
+      <c r="BF7" t="str">
         <f>_xll.NCDK_KierHallSmarts(B7)</f>
-        <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
-      </c>
-      <c r="BB7">
+        <v>0, 0, 0, 0, 0, 0, 0, 0, 6, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
+      </c>
+      <c r="BG7">
         <f>_xll.NCDK_LargestChain(B7)</f>
-        <v>4</v>
-      </c>
-      <c r="BC7">
+        <v>0</v>
+      </c>
+      <c r="BH7">
         <f>_xll.NCDK_LargestPiSystem(B7)</f>
         <v>0</v>
       </c>
-      <c r="BD7" t="str">
+      <c r="BI7" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B7)</f>
         <v>#N/A</v>
       </c>
-      <c r="BE7">
+      <c r="BJ7">
         <f>_xll.NCDK_LongestAliphaticChain(B7)</f>
         <v>0</v>
       </c>
-      <c r="BF7">
-        <f>_xll.NCDK_MannholdLogP(B7)</f>
-        <v>2.12</v>
-      </c>
-      <c r="BG7" t="str">
+      <c r="BK7" t="str">
         <f>_xll.NCDK_MDE(B7)</f>
         <v>0, 0, 0, 0, 9.12546512839809, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BH7" t="str">
+      <c r="BL7" t="str">
         <f>_xll.NCDK_MomentOfInertia(B7)</f>
         <v>#N/A</v>
       </c>
-      <c r="BI7">
+      <c r="BM7">
         <f>_xll.NCDK_PetitjeanNumber(B7)</f>
         <v>0</v>
       </c>
-      <c r="BJ7" t="str">
+      <c r="BN7" t="str">
         <f>_xll.NCDK_PetitjeanShapeIndex(B7)</f>
         <v>#N/A</v>
       </c>
-      <c r="BK7">
+      <c r="BO7">
         <f>_xll.NCDK_RotatableBondsCount(B7)</f>
         <v>0</v>
       </c>
-      <c r="BL7">
+      <c r="BP7">
         <f>_xll.NCDK_RuleOfFive(B7)</f>
         <v>0</v>
       </c>
-      <c r="BM7" t="str">
+      <c r="BQ7" t="str">
         <f>_xll.NCDK_SmallRing(B7)</f>
         <v>1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0</v>
       </c>
-      <c r="BN7">
+      <c r="BR7">
         <f>_xll.NCDK_TPSA(B7)</f>
         <v>0</v>
       </c>
-      <c r="BO7">
+      <c r="BS7">
         <f>_xll.NCDK_VABC(B7)</f>
         <v>99.975907755200197</v>
       </c>
-      <c r="BP7">
+      <c r="BT7">
         <f>_xll.NCDK_VAdjMa(B7)</f>
         <v>3.5849625007211561</v>
       </c>
-      <c r="BQ7">
-        <f>_xll.NCDK_Weight(B7)</f>
+      <c r="BU7" s="2">
+        <f>_xll.NCDK_MolecularWeight(B7)</f>
+        <v>72.064415380728008</v>
+      </c>
+      <c r="BV7" s="3">
+        <f>_xll.NCDK_ExactMass(B7)</f>
         <v>72</v>
       </c>
-      <c r="BR7" t="str">
+      <c r="BW7" t="str">
         <f>_xll.NCDK_WeightedPath(B7)</f>
         <v>11.8125, 1.96875, 0, 0, 0</v>
       </c>
-      <c r="BS7" t="str">
+      <c r="BX7" t="str">
         <f>_xll.NCDK_WHIM(B7)</f>
         <v>#N/A</v>
       </c>
-      <c r="BT7" t="str">
+      <c r="BY7" t="str">
         <f>_xll.NCDK_WienerNumbers(B7)</f>
         <v>27, 3</v>
       </c>
-      <c r="BU7">
-        <f>_xll.NCDK_XLogP(B7)</f>
-        <v>3.4139999999999997</v>
-      </c>
-      <c r="BV7">
+      <c r="BZ7">
         <f>_xll.NCDK_ZagrebIndex(B7)</f>
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:74" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:78" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C8" t="str">
         <f>_xll.NCDK_InChIKey(B8)</f>
-        <v>PXCDDPIOUAJVRE-UHFFFAOYSA-N</v>
+        <v>XDTMQSROBMDMFD-UHFFFAOYSA-N</v>
       </c>
       <c r="D8">
         <f>_xll.NCDK_Tanimoto($H8,$H9)</f>
@@ -4625,7 +4768,7 @@
       </c>
       <c r="E8" t="str">
         <f>_xll.NCDK(E$1,$B8)</f>
-        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001010</v>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000010000000000000000010000000000000001010</v>
       </c>
       <c r="F8" t="str">
         <f>_xll.NCDK_ECFP0($B8)</f>
@@ -4665,7 +4808,7 @@
       </c>
       <c r="O8" t="str">
         <f>_xll.NCDK_EStateFingerprinter($B8)</f>
-        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>0000000010000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="P8" t="str">
         <f>_xll.NCDK_ExtendedFingerprinter($B8)</f>
@@ -4685,7 +4828,7 @@
       </c>
       <c r="T8" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($B8)</f>
-        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001010</v>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000010000000000000000010000000000000001010</v>
       </c>
       <c r="U8" t="str">
         <f>_xll.NCDK_ShortestPathFingerprinter($B8)</f>
@@ -4693,227 +4836,243 @@
       </c>
       <c r="V8" t="str">
         <f>_xll.NCDK_SubstructureFingerprinter($B8)</f>
-        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>0100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="W8" t="str">
         <f>_xll.NCDK_PubchemFingerprinter($B8)</f>
-        <v>00000000011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
-      </c>
-      <c r="X8">
+        <v>00000000011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000100000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="X8" s="2">
+        <f>_xll.NCDK_MolecularWeight(B8)</f>
+        <v>72.064415380728008</v>
+      </c>
+      <c r="Y8" s="2">
+        <f>_xll.NCDK_ExactMass(B8)</f>
+        <v>72</v>
+      </c>
+      <c r="Z8">
         <f>_xll.NCDK_AcidicGroupCount(B8)</f>
         <v>0</v>
       </c>
-      <c r="Y8">
+      <c r="AA8" s="4">
         <f>_xll.NCDK_ALogP(B8)</f>
-        <v>-1.7280000000000006</v>
-      </c>
-      <c r="Z8">
+        <v>2.7372000000000005</v>
+      </c>
+      <c r="AB8" s="4">
+        <f>_xll.NCDK_XLogP(B8)</f>
+        <v>3.4139999999999997</v>
+      </c>
+      <c r="AC8" s="4">
+        <f>_xll.NCDK_MannholdLogP(B8)</f>
+        <v>2.12</v>
+      </c>
+      <c r="AD8" s="4">
+        <f>_xll.NCDK_JPlogP(B8)</f>
+        <v>2.6952762459207973</v>
+      </c>
+      <c r="AE8">
         <f>_xll.NCDK_AMolarRefractivity(B8)</f>
-        <v>17.4696</v>
-      </c>
-      <c r="AA8">
+        <v>27.606000000000002</v>
+      </c>
+      <c r="AF8">
         <f>_xll.NCDK_APol(B8)</f>
-        <v>10.56</v>
-      </c>
-      <c r="AB8">
+        <v>18.561516000000001</v>
+      </c>
+      <c r="AG8">
         <f>_xll.NCDK_AromaticAtomsCount(B8)</f>
         <v>0</v>
       </c>
-      <c r="AC8">
+      <c r="AH8">
         <f>_xll.NCDK_AromaticBondsCount(B8)</f>
         <v>0</v>
       </c>
-      <c r="AD8">
+      <c r="AI8">
         <f>_xll.NCDK_AtomCount(B8)</f>
-        <v>18</v>
-      </c>
-      <c r="AE8" t="str">
+        <v>6</v>
+      </c>
+      <c r="AJ8" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B8)</f>
         <v>0, 0, 0, 0, 0</v>
       </c>
-      <c r="AF8" t="str">
+      <c r="AK8" t="str">
         <f>_xll.NCDK_AutocorrelationMass(B8)</f>
         <v>6, 6, 6, 3, 0</v>
       </c>
-      <c r="AG8" t="str">
+      <c r="AL8" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B8)</f>
         <v>257.709834375, 257.709834375, 257.709834375, 128.8549171875, 0</v>
       </c>
-      <c r="AH8">
+      <c r="AM8">
         <f>_xll.NCDK_BasicGroupCount(B8)</f>
         <v>0</v>
       </c>
-      <c r="AI8" t="str">
+      <c r="AN8" t="str">
         <f>_xll.NCDK_BCUT(B8)</f>
         <v>11.9, 12.1000824042221, -0.15279744210896, 0.0472849621131451, 6.45375, 6.65383240422211</v>
       </c>
-      <c r="AJ8">
+      <c r="AO8">
         <f>_xll.NCDK_BondCount(B8)</f>
         <v>0</v>
       </c>
-      <c r="AK8">
+      <c r="AP8">
         <f>_xll.NCDK_BPol(B8)</f>
-        <v>13.118483999999999</v>
-      </c>
-      <c r="AL8" t="str">
+        <v>0</v>
+      </c>
+      <c r="AQ8" t="str">
         <f>_xll.NCDK_CarbonTypes(B8)</f>
         <v>0, 0, 0, 0, 0, 0, 6, 0, 0</v>
       </c>
-      <c r="AM8" t="str">
+      <c r="AR8" t="str">
         <f>_xll.NCDK_ChiChain(B8)</f>
         <v>0, 0, 0, 0.125, 0, 0, 0, 0, 0.125, 0</v>
       </c>
-      <c r="AN8" t="str">
+      <c r="AS8" t="str">
         <f>_xll.NCDK_ChiCluster(B8)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AO8" t="str">
+      <c r="AT8" t="str">
         <f>_xll.NCDK_ChiPathCluster(B8)</f>
         <v>0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AP8" t="str">
+      <c r="AU8" t="str">
         <f>_xll.NCDK_ChiPath(B8)</f>
         <v>4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0, 4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0</v>
       </c>
-      <c r="AQ8" t="str">
+      <c r="AV8" t="str">
         <f>_xll.NCDK_CPSA(B8)</f>
         <v>#N/A</v>
       </c>
-      <c r="AR8">
+      <c r="AW8">
         <f>_xll.NCDK_EccentricConnectivityIndex(B8)</f>
         <v>36</v>
       </c>
-      <c r="AS8">
+      <c r="AX8">
         <f>_xll.NCDK_FMF(B8)</f>
         <v>1</v>
       </c>
-      <c r="AT8">
+      <c r="AY8">
         <f>_xll.NCDK_FractionalPSA(B8)</f>
         <v>0</v>
       </c>
-      <c r="AU8">
+      <c r="AZ8">
         <f>_xll.NCDK_FragmentComplexity(B8)</f>
         <v>294</v>
       </c>
-      <c r="AV8" t="str">
+      <c r="BA8" t="str">
         <f>_xll.NCDK_GravitationalIndex(B8)</f>
         <v>#N/A</v>
       </c>
-      <c r="AW8">
+      <c r="BB8">
         <f>_xll.NCDK_HBondAcceptorCount(B8)</f>
         <v>0</v>
       </c>
-      <c r="AX8">
+      <c r="BC8">
         <f>_xll.NCDK_HBondDonorCount(B8)</f>
         <v>0</v>
       </c>
-      <c r="AY8">
+      <c r="BD8">
         <f>_xll.NCDK_HybridizationRatio(B8)</f>
         <v>1</v>
       </c>
-      <c r="AZ8" t="str">
+      <c r="BE8" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B8)</f>
         <v>4.16666666666667, 2.22222222222222, 1.33333333333333</v>
       </c>
-      <c r="BA8" t="str">
+      <c r="BF8" t="str">
         <f>_xll.NCDK_KierHallSmarts(B8)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BB8">
+      <c r="BG8">
         <f>_xll.NCDK_LargestChain(B8)</f>
-        <v>4</v>
-      </c>
-      <c r="BC8">
+        <v>0</v>
+      </c>
+      <c r="BH8">
         <f>_xll.NCDK_LargestPiSystem(B8)</f>
         <v>0</v>
       </c>
-      <c r="BD8" t="str">
+      <c r="BI8" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B8)</f>
         <v>#N/A</v>
       </c>
-      <c r="BE8">
+      <c r="BJ8">
         <f>_xll.NCDK_LongestAliphaticChain(B8)</f>
         <v>0</v>
       </c>
-      <c r="BF8">
-        <f>_xll.NCDK_MannholdLogP(B8)</f>
-        <v>2.12</v>
-      </c>
-      <c r="BG8" t="str">
+      <c r="BK8" t="str">
         <f>_xll.NCDK_MDE(B8)</f>
         <v>0, 0, 0, 0, 9.12546512839809, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BH8" t="str">
+      <c r="BL8" t="str">
         <f>_xll.NCDK_MomentOfInertia(B8)</f>
         <v>#N/A</v>
       </c>
-      <c r="BI8">
+      <c r="BM8">
         <f>_xll.NCDK_PetitjeanNumber(B8)</f>
         <v>0</v>
       </c>
-      <c r="BJ8" t="str">
+      <c r="BN8" t="str">
         <f>_xll.NCDK_PetitjeanShapeIndex(B8)</f>
         <v>#N/A</v>
       </c>
-      <c r="BK8">
+      <c r="BO8">
         <f>_xll.NCDK_RotatableBondsCount(B8)</f>
         <v>0</v>
       </c>
-      <c r="BL8">
+      <c r="BP8">
         <f>_xll.NCDK_RuleOfFive(B8)</f>
         <v>0</v>
       </c>
-      <c r="BM8" t="str">
+      <c r="BQ8" t="str">
         <f>_xll.NCDK_SmallRing(B8)</f>
         <v>1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0</v>
       </c>
-      <c r="BN8">
+      <c r="BR8">
         <f>_xll.NCDK_TPSA(B8)</f>
         <v>0</v>
       </c>
-      <c r="BO8">
+      <c r="BS8">
         <f>_xll.NCDK_VABC(B8)</f>
         <v>99.975907755200197</v>
       </c>
-      <c r="BP8">
+      <c r="BT8">
         <f>_xll.NCDK_VAdjMa(B8)</f>
         <v>3.5849625007211561</v>
       </c>
-      <c r="BQ8">
-        <f>_xll.NCDK_Weight(B8)</f>
-        <v>84.093900383999994</v>
-      </c>
-      <c r="BR8" t="str">
+      <c r="BU8" s="2">
+        <f>_xll.NCDK_MolecularWeight(B8)</f>
+        <v>72.064415380728008</v>
+      </c>
+      <c r="BV8" s="3">
+        <f>_xll.NCDK_ExactMass(B8)</f>
+        <v>72</v>
+      </c>
+      <c r="BW8" t="str">
         <f>_xll.NCDK_WeightedPath(B8)</f>
         <v>11.8125, 1.96875, 0, 0, 0</v>
       </c>
-      <c r="BS8" t="str">
+      <c r="BX8" t="str">
         <f>_xll.NCDK_WHIM(B8)</f>
         <v>#N/A</v>
       </c>
-      <c r="BT8" t="str">
+      <c r="BY8" t="str">
         <f>_xll.NCDK_WienerNumbers(B8)</f>
         <v>27, 3</v>
       </c>
-      <c r="BU8">
-        <f>_xll.NCDK_XLogP(B8)</f>
-        <v>3.4139999999999997</v>
-      </c>
-      <c r="BV8">
+      <c r="BZ8">
         <f>_xll.NCDK_ZagrebIndex(B8)</f>
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:74" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:78" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" t="str">
         <f>_xll.NCDK_InChIKey(B9)</f>
-        <v>PXCDDPIOUAJVRE-UHFFFAOYSA-N</v>
+        <v>XDTMQSROBMDMFD-UHFFFAOYSA-N</v>
       </c>
       <c r="D9">
         <f>_xll.NCDK_Tanimoto($H9,$H10)</f>
@@ -4921,7 +5080,7 @@
       </c>
       <c r="E9" t="str">
         <f>_xll.NCDK(E$1,$B9)</f>
-        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001010</v>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000010000000000000000010000000000000001010</v>
       </c>
       <c r="F9" t="str">
         <f>_xll.NCDK_ECFP0($B9)</f>
@@ -4961,7 +5120,7 @@
       </c>
       <c r="O9" t="str">
         <f>_xll.NCDK_EStateFingerprinter($B9)</f>
-        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>0000000010000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="P9" t="str">
         <f>_xll.NCDK_ExtendedFingerprinter($B9)</f>
@@ -4981,7 +5140,7 @@
       </c>
       <c r="T9" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($B9)</f>
-        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001010</v>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000010000000000000000010000000000000001010</v>
       </c>
       <c r="U9" t="str">
         <f>_xll.NCDK_ShortestPathFingerprinter($B9)</f>
@@ -4989,223 +5148,239 @@
       </c>
       <c r="V9" t="str">
         <f>_xll.NCDK_SubstructureFingerprinter($B9)</f>
-        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>0100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="W9" t="str">
         <f>_xll.NCDK_PubchemFingerprinter($B9)</f>
-        <v>00000000011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
-      </c>
-      <c r="X9">
+        <v>00000000011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000100000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="X9" s="2">
+        <f>_xll.NCDK_MolecularWeight(B9)</f>
+        <v>72.064415380728008</v>
+      </c>
+      <c r="Y9" s="2">
+        <f>_xll.NCDK_ExactMass(B9)</f>
+        <v>72</v>
+      </c>
+      <c r="Z9">
         <f>_xll.NCDK_AcidicGroupCount(B9)</f>
         <v>0</v>
       </c>
-      <c r="Y9">
+      <c r="AA9" s="4">
         <f>_xll.NCDK_ALogP(B9)</f>
-        <v>-1.7280000000000006</v>
-      </c>
-      <c r="Z9">
+        <v>2.7372000000000005</v>
+      </c>
+      <c r="AB9" s="4">
+        <f>_xll.NCDK_XLogP(B9)</f>
+        <v>3.4139999999999997</v>
+      </c>
+      <c r="AC9" s="4">
+        <f>_xll.NCDK_MannholdLogP(B9)</f>
+        <v>2.12</v>
+      </c>
+      <c r="AD9" s="4">
+        <f>_xll.NCDK_JPlogP(B9)</f>
+        <v>2.6952762459207973</v>
+      </c>
+      <c r="AE9">
         <f>_xll.NCDK_AMolarRefractivity(B9)</f>
-        <v>17.4696</v>
-      </c>
-      <c r="AA9">
+        <v>27.606000000000002</v>
+      </c>
+      <c r="AF9">
         <f>_xll.NCDK_APol(B9)</f>
-        <v>10.56</v>
-      </c>
-      <c r="AB9">
+        <v>18.561516000000001</v>
+      </c>
+      <c r="AG9">
         <f>_xll.NCDK_AromaticAtomsCount(B9)</f>
         <v>0</v>
       </c>
-      <c r="AC9">
+      <c r="AH9">
         <f>_xll.NCDK_AromaticBondsCount(B9)</f>
         <v>0</v>
       </c>
-      <c r="AD9">
+      <c r="AI9">
         <f>_xll.NCDK_AtomCount(B9)</f>
-        <v>18</v>
-      </c>
-      <c r="AE9" t="str">
+        <v>6</v>
+      </c>
+      <c r="AJ9" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B9)</f>
         <v>0, 0, 0, 0, 0</v>
       </c>
-      <c r="AF9" t="str">
+      <c r="AK9" t="str">
         <f>_xll.NCDK_AutocorrelationMass(B9)</f>
         <v>6, 6, 6, 3, 0</v>
       </c>
-      <c r="AG9" t="str">
+      <c r="AL9" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B9)</f>
         <v>257.709834375, 257.709834375, 257.709834375, 128.8549171875, 0</v>
       </c>
-      <c r="AH9">
+      <c r="AM9">
         <f>_xll.NCDK_BasicGroupCount(B9)</f>
         <v>0</v>
       </c>
-      <c r="AI9" t="str">
+      <c r="AN9" t="str">
         <f>_xll.NCDK_BCUT(B9)</f>
         <v>11.9, 12.1000824042221, -0.15279744210896, 0.0472849621131451, 6.45375, 6.65383240422211</v>
       </c>
-      <c r="AJ9">
+      <c r="AO9">
         <f>_xll.NCDK_BondCount(B9)</f>
         <v>0</v>
       </c>
-      <c r="AK9">
+      <c r="AP9">
         <f>_xll.NCDK_BPol(B9)</f>
-        <v>13.118483999999999</v>
-      </c>
-      <c r="AL9" t="str">
+        <v>0</v>
+      </c>
+      <c r="AQ9" t="str">
         <f>_xll.NCDK_CarbonTypes(B9)</f>
         <v>0, 0, 0, 0, 0, 0, 6, 0, 0</v>
       </c>
-      <c r="AM9" t="str">
+      <c r="AR9" t="str">
         <f>_xll.NCDK_ChiChain(B9)</f>
         <v>0, 0, 0, 0.125, 0, 0, 0, 0, 0.125, 0</v>
       </c>
-      <c r="AN9" t="str">
+      <c r="AS9" t="str">
         <f>_xll.NCDK_ChiCluster(B9)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AO9" t="str">
+      <c r="AT9" t="str">
         <f>_xll.NCDK_ChiPathCluster(B9)</f>
         <v>0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AP9" t="str">
+      <c r="AU9" t="str">
         <f>_xll.NCDK_ChiPath(B9)</f>
         <v>4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0, 4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0</v>
       </c>
-      <c r="AQ9" t="str">
+      <c r="AV9" t="str">
         <f>_xll.NCDK_CPSA(B9)</f>
         <v>#N/A</v>
       </c>
-      <c r="AR9">
+      <c r="AW9">
         <f>_xll.NCDK_EccentricConnectivityIndex(B9)</f>
         <v>36</v>
       </c>
-      <c r="AS9">
+      <c r="AX9">
         <f>_xll.NCDK_FMF(B9)</f>
         <v>1</v>
       </c>
-      <c r="AT9">
+      <c r="AY9">
         <f>_xll.NCDK_FractionalPSA(B9)</f>
         <v>0</v>
       </c>
-      <c r="AU9">
+      <c r="AZ9">
         <f>_xll.NCDK_FragmentComplexity(B9)</f>
         <v>294</v>
       </c>
-      <c r="AV9" t="str">
+      <c r="BA9" t="str">
         <f>_xll.NCDK_GravitationalIndex(B9)</f>
         <v>#N/A</v>
       </c>
-      <c r="AW9">
+      <c r="BB9">
         <f>_xll.NCDK_HBondAcceptorCount(B9)</f>
         <v>0</v>
       </c>
-      <c r="AX9">
+      <c r="BC9">
         <f>_xll.NCDK_HBondDonorCount(B9)</f>
         <v>0</v>
       </c>
-      <c r="AY9">
+      <c r="BD9">
         <f>_xll.NCDK_HybridizationRatio(B9)</f>
         <v>1</v>
       </c>
-      <c r="AZ9" t="str">
+      <c r="BE9" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B9)</f>
         <v>4.16666666666667, 2.22222222222222, 1.33333333333333</v>
       </c>
-      <c r="BA9" t="str">
+      <c r="BF9" t="str">
         <f>_xll.NCDK_KierHallSmarts(B9)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BB9">
+      <c r="BG9">
         <f>_xll.NCDK_LargestChain(B9)</f>
-        <v>4</v>
-      </c>
-      <c r="BC9">
+        <v>0</v>
+      </c>
+      <c r="BH9">
         <f>_xll.NCDK_LargestPiSystem(B9)</f>
         <v>0</v>
       </c>
-      <c r="BD9" t="str">
+      <c r="BI9" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B9)</f>
         <v>#N/A</v>
       </c>
-      <c r="BE9">
+      <c r="BJ9">
         <f>_xll.NCDK_LongestAliphaticChain(B9)</f>
         <v>0</v>
       </c>
-      <c r="BF9">
-        <f>_xll.NCDK_MannholdLogP(B9)</f>
-        <v>2.12</v>
-      </c>
-      <c r="BG9" t="str">
+      <c r="BK9" t="str">
         <f>_xll.NCDK_MDE(B9)</f>
         <v>0, 0, 0, 0, 9.12546512839809, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BH9" t="str">
+      <c r="BL9" t="str">
         <f>_xll.NCDK_MomentOfInertia(B9)</f>
         <v>#N/A</v>
       </c>
-      <c r="BI9">
+      <c r="BM9">
         <f>_xll.NCDK_PetitjeanNumber(B9)</f>
         <v>0</v>
       </c>
-      <c r="BJ9" t="str">
+      <c r="BN9" t="str">
         <f>_xll.NCDK_PetitjeanShapeIndex(B9)</f>
         <v>#N/A</v>
       </c>
-      <c r="BK9">
+      <c r="BO9">
         <f>_xll.NCDK_RotatableBondsCount(B9)</f>
         <v>0</v>
       </c>
-      <c r="BL9">
+      <c r="BP9">
         <f>_xll.NCDK_RuleOfFive(B9)</f>
         <v>0</v>
       </c>
-      <c r="BM9" t="str">
+      <c r="BQ9" t="str">
         <f>_xll.NCDK_SmallRing(B9)</f>
         <v>1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0</v>
       </c>
-      <c r="BN9">
+      <c r="BR9">
         <f>_xll.NCDK_TPSA(B9)</f>
         <v>0</v>
       </c>
-      <c r="BO9">
+      <c r="BS9">
         <f>_xll.NCDK_VABC(B9)</f>
         <v>99.975907755200197</v>
       </c>
-      <c r="BP9">
+      <c r="BT9">
         <f>_xll.NCDK_VAdjMa(B9)</f>
         <v>3.5849625007211561</v>
       </c>
-      <c r="BQ9">
-        <f>_xll.NCDK_Weight(B9)</f>
-        <v>84.093900383999994</v>
-      </c>
-      <c r="BR9" t="str">
+      <c r="BU9" s="2">
+        <f>_xll.NCDK_MolecularWeight(B9)</f>
+        <v>72.064415380728008</v>
+      </c>
+      <c r="BV9" s="3">
+        <f>_xll.NCDK_ExactMass(B9)</f>
+        <v>72</v>
+      </c>
+      <c r="BW9" t="str">
         <f>_xll.NCDK_WeightedPath(B9)</f>
         <v>11.8125, 1.96875, 0, 0, 0</v>
       </c>
-      <c r="BS9" t="str">
+      <c r="BX9" t="str">
         <f>_xll.NCDK_WHIM(B9)</f>
         <v>#N/A</v>
       </c>
-      <c r="BT9" t="str">
+      <c r="BY9" t="str">
         <f>_xll.NCDK_WienerNumbers(B9)</f>
         <v>27, 3</v>
       </c>
-      <c r="BU9">
-        <f>_xll.NCDK_XLogP(B9)</f>
-        <v>3.4139999999999997</v>
-      </c>
-      <c r="BV9">
+      <c r="BZ9">
         <f>_xll.NCDK_ZagrebIndex(B9)</f>
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:74" ht="19" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:78" ht="19" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" t="str">
         <f>_xll.NCDK_SMILES(B10)</f>
@@ -5291,217 +5466,233 @@
         <f>_xll.NCDK_PubchemFingerprinter($B10)</f>
         <v>11110000011110000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000110000000000000000000000000000000001100100110000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001101000000000000000000000100000000000000000000000111100010100101000001000000000000010000000100000000000000000000000000000001000000000100000000000001000100000010000100000000000000000000000000000000000000000001000000000000000000000000000000000100000000000000000000000000000001000000000000001000000000010000000000000000100000000000000000100000000000000000001001100000000000000000010000000000000000011100000001100000011110000000011111000000000000000000000000000000000000000000000000000000000000000110000000000000000000100000000000000000000100000000000000000000100000000000000000000100000000000000000000</v>
       </c>
-      <c r="X10">
+      <c r="X10" s="2">
+        <f>_xll.NCDK_MolecularWeight(B10)</f>
+        <v>386.65454881683121</v>
+      </c>
+      <c r="Y10" s="2">
+        <f>_xll.NCDK_ExactMass(B10)</f>
+        <v>386.35486609199995</v>
+      </c>
+      <c r="Z10">
         <f>_xll.NCDK_AcidicGroupCount(B10)</f>
         <v>0</v>
       </c>
-      <c r="Y10">
+      <c r="AA10" s="4">
         <f>_xll.NCDK_ALogP(B10)</f>
-        <v>1.5548000000000011</v>
-      </c>
-      <c r="Z10">
+        <v>7.376100000000001</v>
+      </c>
+      <c r="AB10" s="4">
+        <f>_xll.NCDK_XLogP(B10)</f>
+        <v>10.518000000000004</v>
+      </c>
+      <c r="AC10" s="4">
+        <f>_xll.NCDK_MannholdLogP(B10)</f>
+        <v>4.3199999999999994</v>
+      </c>
+      <c r="AD10" s="4">
+        <f>_xll.NCDK_JPlogP(B10)</f>
+        <v>7.8290832169857083</v>
+      </c>
+      <c r="AE10">
         <f>_xll.NCDK_AMolarRefractivity(B10)</f>
-        <v>115.17460000000001</v>
-      </c>
-      <c r="AA10">
+        <v>120.6157</v>
+      </c>
+      <c r="AF10">
         <f>_xll.NCDK_APol(B10)</f>
         <v>78.99447799999993</v>
       </c>
-      <c r="AB10">
+      <c r="AG10">
         <f>_xll.NCDK_AromaticAtomsCount(B10)</f>
         <v>0</v>
       </c>
-      <c r="AC10">
+      <c r="AH10">
         <f>_xll.NCDK_AromaticBondsCount(B10)</f>
         <v>0</v>
       </c>
-      <c r="AD10">
+      <c r="AI10">
         <f>_xll.NCDK_AtomCount(B10)</f>
         <v>74</v>
       </c>
-      <c r="AE10" t="str">
+      <c r="AJ10" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B10)</f>
         <v>0.0827991713427503, -0.0229631507285856, -0.0270969061556759, 0.00647128770548948, 0.00909713625645344</v>
       </c>
-      <c r="AF10" t="str">
+      <c r="AK10" t="str">
         <f>_xll.NCDK_AutocorrelationMass(B10)</f>
         <v>28.7744690355409, 31.3320919771326, 48.6641839542651, 54.6641839542651, 49.6641839542651</v>
       </c>
-      <c r="AG10" t="str">
+      <c r="AL10" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B10)</f>
         <v>2589.35165284459, 3179.06049775734, 4922.9791073968, 5328.87269506555, 4616.91714731414</v>
       </c>
-      <c r="AH10">
+      <c r="AM10">
         <f>_xll.NCDK_BasicGroupCount(B10)</f>
         <v>0</v>
       </c>
-      <c r="AI10" t="str">
+      <c r="AN10" t="str">
         <f>_xll.NCDK_BCUT(B10)</f>
         <v>11.89, 15.9949214370833, -0.392219399090072, 0.0596280868632924, 5.23875003301361, 12.6475909449557</v>
       </c>
-      <c r="AJ10">
+      <c r="AO10">
         <f>_xll.NCDK_BondCount(B10)</f>
         <v>46</v>
       </c>
-      <c r="AK10">
+      <c r="AP10">
         <f>_xll.NCDK_BPol(B10)</f>
         <v>50.287521999999989</v>
       </c>
-      <c r="AL10" t="str">
+      <c r="AQ10" t="str">
         <f>_xll.NCDK_CarbonTypes(B10)</f>
         <v>0, 0, 0, 1, 1, 5, 12, 6, 2</v>
       </c>
-      <c r="AM10" t="str">
+      <c r="AR10" t="str">
         <f>_xll.NCDK_ChiChain(B10)</f>
         <v>0, 0, 0.0833333333333333, 0.393634553260967, 0.976046921839545, 0, 0, 0.0833333333333333, 0.37164819290959, 0.863165765466815</v>
       </c>
-      <c r="AN10" t="str">
+      <c r="AS10" t="str">
         <f>_xll.NCDK_ChiCluster(B10)</f>
         <v>2.9521315814894, 0.235702260395516, 1.02234106177579, 0.203263132396285, 2.68481479020038, 0.219913202813724, 0.935219433730957, 0.179558378198271</v>
       </c>
-      <c r="AO10" t="str">
+      <c r="AT10" t="str">
         <f>_xll.NCDK_ChiPathCluster(B10)</f>
         <v>6.93012787723299, 11.9183161832455, 18.084244169983, 6.31056734345633, 10.8246614459309, 15.7948474414898</v>
       </c>
-      <c r="AP10" t="str">
+      <c r="AU10" t="str">
         <f>_xll.NCDK_ChiPath(B10)</f>
         <v>20.1040835277556, 13.2536913009629, 13.0668536638687, 11.1291235227258, 9.49703814548855, 7.69096408557495, 5.93907638185732, 4.4721666474432, 19.344190342069, 12.6298450216499, 12.1863667747532, 10.2790812759586, 8.6662445789686, 6.67875288189192, 5.16344144011131, 3.80610378452706</v>
       </c>
-      <c r="AQ10" t="str">
+      <c r="AV10" t="str">
         <f>_xll.NCDK_CPSA(B10)</f>
         <v>740.518679745203, 1141.6281036277, 24.7477735904141, 216.516577646307, -333.794969260415, -24.5734427697376, 524.002102098896, 1475.42307288811, 49.3212163601517, 0.773763217212662, 1.19287988066324, 0.0258587898400593, 0.226236782787338, -0.348780221713257, -0.025676632684061, 708.702485273172, 1092.57834600072, 23.6844918679688, 207.213998617263, -319.453554322133, -23.5176511261314, 0.136302900713605, 0.25436791475781, 2.7228153119618, 9.4535627888125, 899.894129431074, 57.1411279604366, 0.940293602018195, 0.0597063979818049</v>
       </c>
-      <c r="AR10">
+      <c r="AW10">
         <f>_xll.NCDK_EccentricConnectivityIndex(B10)</f>
         <v>669</v>
       </c>
-      <c r="AS10">
+      <c r="AX10">
         <f>_xll.NCDK_FMF(B10)</f>
         <v>0.22972972972972974</v>
       </c>
-      <c r="AT10">
+      <c r="AY10">
         <f>_xll.NCDK_FractionalPSA(B10)</f>
         <v>5.2361188574192148E-2</v>
       </c>
-      <c r="AU10">
+      <c r="AZ10">
         <f>_xll.NCDK_FragmentComplexity(B10)</f>
         <v>5173.01</v>
       </c>
-      <c r="AV10" t="str">
+      <c r="BA10" t="str">
         <f>_xll.NCDK_GravitationalIndex(B10)</f>
         <v>1941.85812139388, 44.0665192793109, 12.4759176252409, 2394.88950905792, 48.9376083299737, 13.37914910667, 4535.65140656394, 67.3472449812458, 16.5531209985441</v>
       </c>
-      <c r="AW10">
+      <c r="BB10">
         <f>_xll.NCDK_HBondAcceptorCount(B10)</f>
         <v>1</v>
       </c>
-      <c r="AX10">
+      <c r="BC10">
         <f>_xll.NCDK_HBondDonorCount(B10)</f>
         <v>1</v>
       </c>
-      <c r="AY10">
+      <c r="BD10">
         <f>_xll.NCDK_HybridizationRatio(B10)</f>
         <v>0.92592592592592593</v>
       </c>
-      <c r="AZ10" t="str">
+      <c r="BE10" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B10)</f>
         <v>21.2403746097815, 7.921875, 3.65484429065744</v>
       </c>
-      <c r="BA10" t="str">
+      <c r="BF10" t="str">
         <f>_xll.NCDK_KierHallSmarts(B10)</f>
         <v>0, 0, 0, 0, 0, 0, 5, 0, 11, 0, 1, 0, 7, 0, 0, 1, 0, 0, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BB10">
+      <c r="BG10">
         <f>_xll.NCDK_LargestChain(B10)</f>
         <v>7</v>
       </c>
-      <c r="BC10">
+      <c r="BH10">
         <f>_xll.NCDK_LargestPiSystem(B10)</f>
         <v>2</v>
       </c>
-      <c r="BD10" t="str">
+      <c r="BI10" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B10)</f>
         <v>3.502934717034, 3.502934717034</v>
       </c>
-      <c r="BE10">
+      <c r="BJ10">
         <f>_xll.NCDK_LongestAliphaticChain(B10)</f>
         <v>7</v>
       </c>
-      <c r="BF10">
-        <f>_xll.NCDK_MannholdLogP(B10)</f>
-        <v>4.3199999999999994</v>
-      </c>
-      <c r="BG10" t="str">
+      <c r="BK10" t="str">
         <f>_xll.NCDK_MDE(B10)</f>
         <v>2.79346109096649, 16.5925259846737, 11.5560895487586, 3.39888423642021, 17.7527182855433, 29.2401176288661, 7.64127863367805, 8.77423090217006, 6.5802347918611, 0.5, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BH10" t="str">
+      <c r="BL10" t="str">
         <f>_xll.NCDK_MomentOfInertia(B10)</f>
         <v>10068.4095883237, 9731.07167302841, 773.613761142664, 1.03466606008362, 13.0147757111406, 12.5787210127379, 8.29661608019916</v>
       </c>
-      <c r="BI10">
+      <c r="BM10">
         <f>_xll.NCDK_PetitjeanNumber(B10)</f>
         <v>0.46666666666666667</v>
       </c>
-      <c r="BJ10" t="str">
+      <c r="BN10" t="str">
         <f>_xll.NCDK_PetitjeanShapeIndex(B10)</f>
         <v>0.875, 0.940550174456362</v>
       </c>
-      <c r="BK10">
+      <c r="BO10">
         <f>_xll.NCDK_RotatableBondsCount(B10)</f>
         <v>5</v>
       </c>
-      <c r="BL10">
+      <c r="BP10">
         <f>_xll.NCDK_RuleOfFive(B10)</f>
         <v>1</v>
       </c>
-      <c r="BM10" t="str">
+      <c r="BQ10" t="str">
         <f>_xll.NCDK_SmallRing(B10)</f>
         <v>4, 0, 1, 0, 0, 0, 1, 3, 0, 0, 0</v>
       </c>
-      <c r="BN10">
+      <c r="BR10">
         <f>_xll.NCDK_TPSA(B10)</f>
         <v>20.23</v>
       </c>
-      <c r="BO10">
+      <c r="BS10">
         <f>_xll.NCDK_VABC(B10)</f>
         <v>432.2759767957632</v>
       </c>
-      <c r="BP10">
+      <c r="BT10">
         <f>_xll.NCDK_VAdjMa(B10)</f>
         <v>5.9541963103868758</v>
       </c>
-      <c r="BQ10">
-        <f>_xll.NCDK_Weight(B10)</f>
-        <v>386.35486609200063</v>
-      </c>
-      <c r="BR10" t="str">
+      <c r="BU10" s="2">
+        <f>_xll.NCDK_MolecularWeight(B10)</f>
+        <v>386.65454881683121</v>
+      </c>
+      <c r="BV10" s="3">
+        <f>_xll.NCDK_ExactMass(B10)</f>
+        <v>386.35486609199995</v>
+      </c>
+      <c r="BW10" t="str">
         <f>_xll.NCDK_WeightedPath(B10)</f>
         <v>57.2167299866347, 2.04345464237981, 2.54245315921217, 2.54245315921217, 0</v>
       </c>
-      <c r="BS10" t="str">
+      <c r="BX10" t="str">
         <f>_xll.NCDK_WHIM(B10)</f>
         <v>1.22231276339169, 2.17046945111189, 25.8559001988821, 0.0417903530188526, 0.0742074265238894, #N/A, #N/A, #N/A, 0.0962638773185697, 0.00388857657057473, 66.8991567190677, 29.2486824133857, 90.3764308473927, 188.22062289613, 0.413001665342944, #N/A, 66.9993091729568</v>
       </c>
-      <c r="BT10" t="str">
+      <c r="BY10" t="str">
         <f>_xll.NCDK_WienerNumbers(B10)</f>
         <v>2022, 54</v>
       </c>
-      <c r="BU10">
-        <f>_xll.NCDK_XLogP(B10)</f>
-        <v>10.518000000000004</v>
-      </c>
-      <c r="BV10">
+      <c r="BZ10">
         <f>_xll.NCDK_ZagrebIndex(B10)</f>
         <v>158</v>
       </c>
     </row>
-    <row r="11" spans="1:74" ht="19" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:78" ht="19" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" t="s">
         <v>63</v>
-      </c>
-      <c r="B11" t="s">
-        <v>64</v>
       </c>
       <c r="C11" t="str">
         <f>_xll.NCDK_InChI(B11)</f>
@@ -5583,207 +5774,223 @@
         <f>_xll.NCDK_PubchemFingerprinter($B11)</f>
         <v>00000000011110000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000110000000000000000000000000000000001100100110000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001101000000000000000000000100000000000000000000000111100010100101000001000000000000010000000100000000000000000000000000000001000000000100000000000001000100000010000100000000000000000000000000000000000000000001000000000000000000000000000000000100000000000000000000000000000001000000000000001000000000010000000000000000100000000000000000100000000000000000001001100000000000000000010000000000000000011100000001100000011110000000011111000000000000000000000000000000000000000000000000000000000000000110000000000000000000100000000000000000000100000000000000000000100000000000000000000100000000000000000000</v>
       </c>
-      <c r="X11">
+      <c r="X11" s="2">
+        <f>_xll.NCDK_MolecularWeight(B11)</f>
+        <v>386.65454881683161</v>
+      </c>
+      <c r="Y11" s="2">
+        <f>_xll.NCDK_ExactMass(B11)</f>
+        <v>386.35486609199995</v>
+      </c>
+      <c r="Z11">
         <f>_xll.NCDK_AcidicGroupCount(B11)</f>
         <v>0</v>
       </c>
-      <c r="Y11">
+      <c r="AA11" s="4">
         <f>_xll.NCDK_ALogP(B11)</f>
-        <v>1.5548000000000011</v>
-      </c>
-      <c r="Z11">
+        <v>7.376100000000001</v>
+      </c>
+      <c r="AB11" s="4">
+        <f>_xll.NCDK_XLogP(B11)</f>
+        <v>10.518000000000004</v>
+      </c>
+      <c r="AC11" s="4">
+        <f>_xll.NCDK_MannholdLogP(B11)</f>
+        <v>4.3199999999999994</v>
+      </c>
+      <c r="AD11" s="4">
+        <f>_xll.NCDK_JPlogP(B11)</f>
+        <v>7.8290832169857199</v>
+      </c>
+      <c r="AE11">
         <f>_xll.NCDK_AMolarRefractivity(B11)</f>
-        <v>115.17460000000001</v>
-      </c>
-      <c r="AA11">
+        <v>120.6157</v>
+      </c>
+      <c r="AF11">
         <f>_xll.NCDK_APol(B11)</f>
         <v>78.994478000000029</v>
       </c>
-      <c r="AB11">
+      <c r="AG11">
         <f>_xll.NCDK_AromaticAtomsCount(B11)</f>
         <v>0</v>
       </c>
-      <c r="AC11">
+      <c r="AH11">
         <f>_xll.NCDK_AromaticBondsCount(B11)</f>
         <v>0</v>
       </c>
-      <c r="AD11">
+      <c r="AI11">
         <f>_xll.NCDK_AtomCount(B11)</f>
         <v>74</v>
       </c>
-      <c r="AE11" t="str">
+      <c r="AJ11" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B11)</f>
         <v>0.0827991713427503, -0.0229631507285856, -0.0270969061556759, 0.00647128770548948, 0.00909713625645344</v>
       </c>
-      <c r="AF11" t="str">
+      <c r="AK11" t="str">
         <f>_xll.NCDK_AutocorrelationMass(B11)</f>
         <v>28.7744690355409, 31.3320919771326, 48.6641839542651, 54.6641839542651, 49.6641839542651</v>
       </c>
-      <c r="AG11" t="str">
+      <c r="AL11" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B11)</f>
         <v>2589.35165284459, 3179.06049775734, 4922.9791073968, 5328.87269506555, 4616.91714731414</v>
       </c>
-      <c r="AH11">
+      <c r="AM11">
         <f>_xll.NCDK_BasicGroupCount(B11)</f>
         <v>0</v>
       </c>
-      <c r="AI11" t="str">
+      <c r="AN11" t="str">
         <f>_xll.NCDK_BCUT(B11)</f>
         <v>11.89, 15.9949214370832, -0.392219474278523, 0.0694748577202458, 5.23874992098634, 12.6503467270457</v>
       </c>
-      <c r="AJ11">
+      <c r="AO11">
         <f>_xll.NCDK_BondCount(B11)</f>
         <v>0</v>
       </c>
-      <c r="AK11">
+      <c r="AP11">
         <f>_xll.NCDK_BPol(B11)</f>
         <v>50.287521999999989</v>
       </c>
-      <c r="AL11" t="str">
+      <c r="AQ11" t="str">
         <f>_xll.NCDK_CarbonTypes(B11)</f>
         <v>0, 0, 0, 1, 1, 5, 12, 6, 2</v>
       </c>
-      <c r="AM11" t="str">
+      <c r="AR11" t="str">
         <f>_xll.NCDK_ChiChain(B11)</f>
         <v>0, 0, 0.0833333333333333, 0.393634553260967, 0.976046921839545, 0, 0, 0.0833333333333333, 0.37164819290959, 0.863165765466815</v>
       </c>
-      <c r="AN11" t="str">
+      <c r="AS11" t="str">
         <f>_xll.NCDK_ChiCluster(B11)</f>
         <v>2.9521315814894, 0.235702260395516, 1.02234106177579, 0.203263132396285, 2.68481479020038, 0.219913202813724, 0.935219433730957, 0.179558378198271</v>
       </c>
-      <c r="AO11" t="str">
+      <c r="AT11" t="str">
         <f>_xll.NCDK_ChiPathCluster(B11)</f>
         <v>6.93012787723299, 11.9183161832455, 18.084244169983, 6.31056734345633, 10.8246614459309, 15.7948474414898</v>
       </c>
-      <c r="AP11" t="str">
+      <c r="AU11" t="str">
         <f>_xll.NCDK_ChiPath(B11)</f>
         <v>20.1040835277556, 13.2536913009629, 13.0668536638687, 11.1291235227258, 9.49703814548855, 7.69096408557496, 5.93907638185732, 4.4721666474432, 19.344190342069, 12.6298450216499, 12.1863667747532, 10.2790812759586, 8.66624457896859, 6.67875288189192, 5.16344144011131, 3.80610378452706</v>
       </c>
-      <c r="AQ11" t="str">
+      <c r="AV11" t="str">
         <f>_xll.NCDK_CPSA(B11)</f>
         <v>#N/A</v>
       </c>
-      <c r="AR11">
+      <c r="AW11">
         <f>_xll.NCDK_EccentricConnectivityIndex(B11)</f>
         <v>669</v>
       </c>
-      <c r="AS11">
+      <c r="AX11">
         <f>_xll.NCDK_FMF(B11)</f>
         <v>0.6071428571428571</v>
       </c>
-      <c r="AT11">
+      <c r="AY11">
         <f>_xll.NCDK_FractionalPSA(B11)</f>
         <v>5.2361188524318612E-2</v>
       </c>
-      <c r="AU11">
+      <c r="AZ11">
         <f>_xll.NCDK_FragmentComplexity(B11)</f>
         <v>5173.01</v>
       </c>
-      <c r="AV11" t="str">
+      <c r="BA11" t="str">
         <f>_xll.NCDK_GravitationalIndex(B11)</f>
         <v>#N/A</v>
       </c>
-      <c r="AW11">
+      <c r="BB11">
         <f>_xll.NCDK_HBondAcceptorCount(B11)</f>
         <v>1</v>
       </c>
-      <c r="AX11">
+      <c r="BC11">
         <f>_xll.NCDK_HBondDonorCount(B11)</f>
         <v>1</v>
       </c>
-      <c r="AY11">
+      <c r="BD11">
         <f>_xll.NCDK_HybridizationRatio(B11)</f>
         <v>0.92592592592592593</v>
       </c>
-      <c r="AZ11" t="str">
+      <c r="BE11" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B11)</f>
         <v>21.2403746097815, 7.921875, 3.65484429065744</v>
       </c>
-      <c r="BA11" t="str">
+      <c r="BF11" t="str">
         <f>_xll.NCDK_KierHallSmarts(B11)</f>
         <v>0, 0, 0, 0, 0, 0, 5, 0, 11, 0, 1, 0, 7, 0, 0, 1, 0, 0, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BB11">
+      <c r="BG11">
         <f>_xll.NCDK_LargestChain(B11)</f>
         <v>16</v>
       </c>
-      <c r="BC11">
+      <c r="BH11">
         <f>_xll.NCDK_LargestPiSystem(B11)</f>
         <v>2</v>
       </c>
-      <c r="BD11" t="str">
+      <c r="BI11" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B11)</f>
         <v>#N/A</v>
       </c>
-      <c r="BE11">
+      <c r="BJ11">
         <f>_xll.NCDK_LongestAliphaticChain(B11)</f>
         <v>7</v>
       </c>
-      <c r="BF11">
-        <f>_xll.NCDK_MannholdLogP(B11)</f>
-        <v>4.3199999999999994</v>
-      </c>
-      <c r="BG11" t="str">
+      <c r="BK11" t="str">
         <f>_xll.NCDK_MDE(B11)</f>
         <v>1.54697174276407, 11.0054221495714, 8.10399071027919, 2.24225976804296, 15.301585299106, 26.1301405209996, 7.46130267367364, 6.99912877305946, 5.73136198628621, 0.25, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BH11" t="str">
+      <c r="BL11" t="str">
         <f>_xll.NCDK_MomentOfInertia(B11)</f>
         <v>#N/A</v>
       </c>
-      <c r="BI11">
+      <c r="BM11">
         <f>_xll.NCDK_PetitjeanNumber(B11)</f>
         <v>0.46666666666666667</v>
       </c>
-      <c r="BJ11" t="str">
+      <c r="BN11" t="str">
         <f>_xll.NCDK_PetitjeanShapeIndex(B11)</f>
         <v>#N/A</v>
       </c>
-      <c r="BK11">
+      <c r="BO11">
         <f>_xll.NCDK_RotatableBondsCount(B11)</f>
         <v>5</v>
       </c>
-      <c r="BL11">
+      <c r="BP11">
         <f>_xll.NCDK_RuleOfFive(B11)</f>
         <v>1</v>
       </c>
-      <c r="BM11" t="str">
+      <c r="BQ11" t="str">
         <f>_xll.NCDK_SmallRing(B11)</f>
         <v>4, 0, 1, 0, 0, 0, 1, 3, 0, 0, 0</v>
       </c>
-      <c r="BN11">
+      <c r="BR11">
         <f>_xll.NCDK_TPSA(B11)</f>
         <v>20.23</v>
       </c>
-      <c r="BO11">
+      <c r="BS11">
         <f>_xll.NCDK_VABC(B11)</f>
         <v>432.27597679576252</v>
       </c>
-      <c r="BP11">
+      <c r="BT11">
         <f>_xll.NCDK_VAdjMa(B11)</f>
         <v>5.9541963103868758</v>
       </c>
-      <c r="BQ11">
-        <f>_xll.NCDK_Weight(B11)</f>
-        <v>386.35486609200007</v>
-      </c>
-      <c r="BR11" t="str">
+      <c r="BU11" s="2">
+        <f>_xll.NCDK_MolecularWeight(B11)</f>
+        <v>386.65454881683161</v>
+      </c>
+      <c r="BV11" s="3">
+        <f>_xll.NCDK_ExactMass(B11)</f>
+        <v>386.35486609199995</v>
+      </c>
+      <c r="BW11" t="str">
         <f>_xll.NCDK_WeightedPath(B11)</f>
         <v>57.2167299866347, 2.04345464237981, 2.54245315921218, 2.54245315921218, 0</v>
       </c>
-      <c r="BS11" t="str">
+      <c r="BX11" t="str">
         <f>_xll.NCDK_WHIM(B11)</f>
         <v>#N/A</v>
       </c>
-      <c r="BT11" t="str">
+      <c r="BY11" t="str">
         <f>_xll.NCDK_WienerNumbers(B11)</f>
         <v>2022, 54</v>
       </c>
-      <c r="BU11">
-        <f>_xll.NCDK_XLogP(B11)</f>
-        <v>10.518000000000004</v>
-      </c>
-      <c r="BV11">
+      <c r="BZ11">
         <f>_xll.NCDK_ZagrebIndex(B11)</f>
         <v>158</v>
       </c>
@@ -5797,76 +6004,83 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D78F5C-B236-40D1-A056-FD195DD12728}">
-  <dimension ref="A1:S21"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="7" max="18" width="4.83203125" customWidth="1"/>
+    <col min="20" max="20" width="8.6640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1" t="s">
         <v>87</v>
       </c>
-      <c r="B1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J1" t="s">
+        <v>96</v>
+      </c>
+      <c r="K1" t="s">
+        <v>97</v>
+      </c>
+      <c r="L1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M1" t="s">
+        <v>99</v>
+      </c>
+      <c r="N1" t="s">
+        <v>100</v>
+      </c>
+      <c r="O1" t="s">
+        <v>101</v>
+      </c>
+      <c r="P1" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>103</v>
+      </c>
+      <c r="R1" t="s">
+        <v>113</v>
+      </c>
+      <c r="S1" t="s">
+        <v>171</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="E1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G1" t="s">
-        <v>94</v>
-      </c>
-      <c r="H1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I1" t="s">
-        <v>96</v>
-      </c>
-      <c r="J1" t="s">
-        <v>97</v>
-      </c>
-      <c r="K1" t="s">
-        <v>98</v>
-      </c>
-      <c r="L1" t="s">
-        <v>99</v>
-      </c>
-      <c r="M1" t="s">
-        <v>100</v>
-      </c>
-      <c r="N1" t="s">
-        <v>101</v>
-      </c>
-      <c r="O1" t="s">
-        <v>102</v>
-      </c>
-      <c r="P1" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>104</v>
-      </c>
-      <c r="R1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="B2" s="1" t="str">
         <f>_xll.NCDK(B$1,$A2)</f>
@@ -5877,13 +6091,13 @@
         <v>0000000000000000000000000001000000000000000000000000000000000000100000000000000000000000100000000000000000000000000000000000000000000100001000000000000010000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000001000000100000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000100000000000000000001000000000000000000100000000000000000000000010000000000000000000000000000010000000100000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000100100000000001000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000010000000000000000000100000100000000000000000000000100000000000000000000000000</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -5922,10 +6136,14 @@
         <f>_xll.NCDK_MACCSFingerprinter($A2)</f>
         <v>0000000000000000000000000000000000000100000000000000110010000100100000010010101101101000111110111100000010001100000010011100001000111010101101100101011110111111111110</v>
       </c>
+      <c r="T2" s="4">
+        <f>_xll.NCDK_XLogP(A2)</f>
+        <v>-1.9040000000000001</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B3" s="1" t="str">
         <f>_xll.NCDK(B$1,$A3)</f>
@@ -5936,13 +6154,13 @@
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000100000000000001000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="D3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F3" t="s">
         <v>106</v>
-      </c>
-      <c r="E3" t="s">
-        <v>106</v>
-      </c>
-      <c r="F3" t="s">
-        <v>107</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -5966,10 +6184,14 @@
         <f>_xll.NCDK_MACCSFingerprinter($A3)</f>
         <v>0000000000000000000000000000000000000000000000000000110000000000000000010000000000000000100000000010000000000000100000000000101000100000001100111100010100001010011110</v>
       </c>
+      <c r="T3" s="4">
+        <f>_xll.NCDK_XLogP(A3)</f>
+        <v>1.9170000000000009</v>
+      </c>
     </row>
-    <row r="4" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B4" s="1" t="str">
         <f>_xll.NCDK(B$1,$A4)</f>
@@ -5980,13 +6202,13 @@
         <v>0000000100000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000100000000000000000000000000000000000000000000000000000100000000000000000000000000000000011000000000000000000000000001000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000100000000000010000000000000000000000000000000000000010000000000000000000000000000000001000000000000000000000000000000010000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000010000000000000000000100000000000000000000000000000000000000000001000000000000</v>
       </c>
       <c r="D4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4" t="s">
         <v>109</v>
-      </c>
-      <c r="E4" t="s">
-        <v>109</v>
-      </c>
-      <c r="F4" t="s">
-        <v>110</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -6010,10 +6232,14 @@
         <f>_xll.NCDK_MACCSFingerprinter($A4)</f>
         <v>0000000000000000000000000001000000000000000000001000000010000000100000010010000000101000000010011100001010001000100000011110111000000100100110111101110110011111111111</v>
       </c>
+      <c r="T4" s="4">
+        <f>_xll.NCDK_XLogP(A4)</f>
+        <v>3.7249999999999996</v>
+      </c>
     </row>
-    <row r="5" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5" s="1" t="str">
         <f>_xll.NCDK(B$1,$A5)</f>
@@ -6024,13 +6250,13 @@
         <v>0000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000001000000000000100000000000000000000000000100000110000000000010000000000000000000000000000000000000000000000000000010000000000001000000000000000000000000000000000010000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000100000000000000000001000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000100001000000000000000000000000000000000000000000000000100000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000100000000100000000000000000000000000000000000</v>
       </c>
       <c r="D5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F5" t="s">
         <v>112</v>
-      </c>
-      <c r="E5" t="s">
-        <v>112</v>
-      </c>
-      <c r="F5" t="s">
-        <v>113</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -6072,10 +6298,14 @@
         <f>_xll.NCDK_MACCSFingerprinter($A5)</f>
         <v>0000000000000000000000000000000000000000000001000000010010000000100000110000000000110000110101111000010100000110100110011011001000100100101101110100011101111111110111</v>
       </c>
+      <c r="T5" s="4">
+        <f>_xll.NCDK_XLogP(A5)</f>
+        <v>-1.6970000000000001</v>
+      </c>
     </row>
-    <row r="6" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B6" s="1" t="str">
         <f>_xll.NCDK(B$1,$A6)</f>
@@ -6086,13 +6316,13 @@
         <v>0000000000000010000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000100000000000000000010000001000000000000000000000000001000000000000000000000000000000000000000000000000010000000000000000000001000000000000000000000000000000000000000000000000000000010000000000000000000000000000000100000000000000000010000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000001000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000010000000000000000000001000000000000100000000000000000000000000000000000000000000000000000000001000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="D6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F6" t="s">
         <v>116</v>
-      </c>
-      <c r="E6" t="s">
-        <v>116</v>
-      </c>
-      <c r="F6" t="s">
-        <v>117</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -6128,10 +6358,14 @@
         <f>_xll.NCDK_MACCSFingerprinter($A6)</f>
         <v>0000000000000000000000001000000000000100000000000000100000000010100000100000101100010000100101101100010001001100100011111001011110101010100001111010011010111110111110</v>
       </c>
+      <c r="T6" s="4">
+        <f>_xll.NCDK_XLogP(A6)</f>
+        <v>1.413</v>
+      </c>
     </row>
-    <row r="7" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B7" s="1" t="str">
         <f>_xll.NCDK(B$1,$A7)</f>
@@ -6142,13 +6376,13 @@
         <v>1000000000000010000000000000000000000000010000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000100000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000100000000000000000000000001000000000000000000000000000000000000100000000000000010000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000100000000000000000000000000000000000001000001000000000000</v>
       </c>
       <c r="D7" t="s">
+        <v>118</v>
+      </c>
+      <c r="E7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F7" t="s">
         <v>119</v>
-      </c>
-      <c r="E7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F7" t="s">
-        <v>120</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -6190,10 +6424,14 @@
         <f>_xll.NCDK_MACCSFingerprinter($A7)</f>
         <v>0000000000000000000000000000000000000000000000000000000010000100000000010010001000001100000000111101000010001010100001011100100110011010110001011011000110011110111110</v>
       </c>
+      <c r="T7" s="4">
+        <f>_xll.NCDK_XLogP(A7)</f>
+        <v>2.4140000000000006</v>
+      </c>
     </row>
-    <row r="8" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B8" s="1" t="str">
         <f>_xll.NCDK(B$1,$A8)</f>
@@ -6204,13 +6442,13 @@
         <v>1000000000000010000000000000000000000000000000000000000000000000000000001000000000000000100000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000100000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000100000000000001000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000100000100000000000000000000000000000000001000000000000100</v>
       </c>
       <c r="D8" t="s">
+        <v>121</v>
+      </c>
+      <c r="E8" t="s">
+        <v>121</v>
+      </c>
+      <c r="F8" t="s">
         <v>122</v>
-      </c>
-      <c r="E8" t="s">
-        <v>122</v>
-      </c>
-      <c r="F8" t="s">
-        <v>123</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -6249,10 +6487,14 @@
         <f>_xll.NCDK_MACCSFingerprinter($A8)</f>
         <v>0000000000000000001000000000000000000000000000000000010000000100000000010000000001000100001000000001001110000010100000001000101110100100111000111010011110001110111111</v>
       </c>
+      <c r="T8" s="4">
+        <f>_xll.NCDK_XLogP(A8)</f>
+        <v>2.0469999999999997</v>
+      </c>
     </row>
-    <row r="9" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B9" s="1" t="str">
         <f>_xll.NCDK(B$1,$A9)</f>
@@ -6263,13 +6505,13 @@
         <v>0000000000000000000100000000000000100000000000000000100000000000000000000000000000000000000000000000000000000010000000000000000000000100000000000100000010000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000001000000000000000000000000001000000000000000000000000000000001000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="D9" t="s">
+        <v>124</v>
+      </c>
+      <c r="E9" t="s">
+        <v>124</v>
+      </c>
+      <c r="F9" t="s">
         <v>125</v>
-      </c>
-      <c r="E9" t="s">
-        <v>125</v>
-      </c>
-      <c r="F9" t="s">
-        <v>126</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -6311,10 +6553,14 @@
         <f>_xll.NCDK_MACCSFingerprinter($A9)</f>
         <v>0000000000000000000000000000001000000100011000000010001001011000001000001000110000010001000000000000011001100001000000100001000001110101000001000001001010110110111111</v>
       </c>
+      <c r="T9" s="4">
+        <f>_xll.NCDK_XLogP(A9)</f>
+        <v>0.17100000000000004</v>
+      </c>
     </row>
-    <row r="10" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B10" s="1" t="str">
         <f>_xll.NCDK(B$1,$A10)</f>
@@ -6325,13 +6571,13 @@
         <v>0000000000000010000100000100000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000100000000000000000010000000000000000000001000000000000000000000000000000000000000000000010000100000000010000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000100000000000000000000000000100000000000000000000000000000000000100000000000000000001000000000000000000000000000000100000000000000000000000001000000000000000000001000000000000000100000000000000010001000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000001000000000000000000000000000000</v>
       </c>
       <c r="D10" t="s">
+        <v>127</v>
+      </c>
+      <c r="E10" t="s">
+        <v>127</v>
+      </c>
+      <c r="F10" t="s">
         <v>128</v>
-      </c>
-      <c r="E10" t="s">
-        <v>128</v>
-      </c>
-      <c r="F10" t="s">
-        <v>129</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -6373,10 +6619,14 @@
         <f>_xll.NCDK_MACCSFingerprinter($A10)</f>
         <v>0000000000000000000000000000000000000000000000000000000010000100010000000010000000001100000000100101001000001011000001011110010110010100110000001111000011101110111111</v>
       </c>
+      <c r="T10" s="4">
+        <f>_xll.NCDK_XLogP(A10)</f>
+        <v>3.8299999999999996</v>
+      </c>
     </row>
-    <row r="11" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B11" s="1" t="str">
         <f>_xll.NCDK(B$1,$A11)</f>
@@ -6387,13 +6637,13 @@
         <v>0000000000000010000100000101000000000000000000000000000000000000000000000000000000000000100001000000100000000000000000000000000000000100000000000000000010000000000000000000000000000000000010000000000000000010000001000000010000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000001000000000000010101100001100000000000100010100000000000000000000001000000010000000000000000000000000000010001010000000000000000000000000000000000000000000000000000010000000010000000000100100000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000001000100000000000000001000000000000000000000001000000000000000000000000000001000000000000000001000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000001000100000000000000000000000000000100000000000000000000000000</v>
       </c>
       <c r="D11" t="s">
+        <v>130</v>
+      </c>
+      <c r="E11" t="s">
+        <v>130</v>
+      </c>
+      <c r="F11" t="s">
         <v>131</v>
-      </c>
-      <c r="E11" t="s">
-        <v>131</v>
-      </c>
-      <c r="F11" t="s">
-        <v>132</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -6423,10 +6673,14 @@
         <f>_xll.NCDK_MACCSFingerprinter($A11)</f>
         <v>0000000000000000000000000000000000000000000000000000100010000000100000000000000100100000100110111100000010010111001110011010000110111011101111011110111101111111111110</v>
       </c>
+      <c r="T11" s="4">
+        <f>_xll.NCDK_XLogP(A11)</f>
+        <v>3.7529999999999997</v>
+      </c>
     </row>
-    <row r="12" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B12" s="1" t="str">
         <f>_xll.NCDK(B$1,$A12)</f>
@@ -6437,13 +6691,13 @@
         <v>0000000000000000000000000000000000000000000000000010000000100000000000000000000000000000001000000000000000000000000000000000000000000100010000000100000010000000000000000000000000000000000000000000000000000010000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000100000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000100000000000000000000000000000000011000000000000000000000000010000000000000000000000000000000000000000000000000100000000000000000000100000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000001000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000010000000100000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="D12" t="s">
+        <v>133</v>
+      </c>
+      <c r="E12" t="s">
+        <v>133</v>
+      </c>
+      <c r="F12" t="s">
         <v>134</v>
-      </c>
-      <c r="E12" t="s">
-        <v>134</v>
-      </c>
-      <c r="F12" t="s">
-        <v>135</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -6485,10 +6739,14 @@
         <f>_xll.NCDK_MACCSFingerprinter($A12)</f>
         <v>0000000000000000000000000000000000100011000100011000011001011000001000011000000001000001000010000000010101001001100000000001011001110001001100110101010110101011011111</v>
       </c>
+      <c r="T12" s="4">
+        <f>_xll.NCDK_XLogP(A12)</f>
+        <v>-2.601</v>
+      </c>
     </row>
-    <row r="13" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B13" s="1" t="str">
         <f>_xll.NCDK(B$1,$A13)</f>
@@ -6499,13 +6757,13 @@
         <v>0000000000000010000100000000000000000000000000000000000000000000000000000000000000000000100001000000000000000010000000000000000000000100000000000000000010000000000000000000001000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000010000000100000000000000000000010000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000001000000000000000000000000000000000100001000000100000010100000000010000000000000011100000000000000000000000000000010000000000000000000000000000000000000000000100000000000000000000000000000000000000000000001000000000000000000001000000000000000000000000000000001000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000100000000000000000000000001000000000000000000000000000000</v>
       </c>
       <c r="D13" t="s">
+        <v>136</v>
+      </c>
+      <c r="E13" t="s">
+        <v>136</v>
+      </c>
+      <c r="F13" t="s">
         <v>137</v>
-      </c>
-      <c r="E13" t="s">
-        <v>137</v>
-      </c>
-      <c r="F13" t="s">
-        <v>138</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -6544,10 +6802,14 @@
         <f>_xll.NCDK_MACCSFingerprinter($A13)</f>
         <v>0000000000000000000000100000000000000000000000000000000000000000000000000010001100101110000110010111001001110110000011011110010110110101111101011111010011111111111111</v>
       </c>
+      <c r="T13" s="4">
+        <f>_xll.NCDK_XLogP(A13)</f>
+        <v>0.8670000000000001</v>
+      </c>
     </row>
-    <row r="14" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B14" s="1" t="str">
         <f>_xll.NCDK(B$1,$A14)</f>
@@ -6558,13 +6820,13 @@
         <v>0000000000000010000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000100000000000000000000000000000000000000001000000000000000000000000000000000000000000001000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000010000000000000000000100000000000000000000000000000010000000000000000000000000000000000000000000000000000000100000000000100000000000000000000000000000000000000010000000000100000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000100000000000100000000000000000000000000000000000000000000</v>
       </c>
       <c r="D14" t="s">
+        <v>139</v>
+      </c>
+      <c r="E14" t="s">
+        <v>139</v>
+      </c>
+      <c r="F14" t="s">
         <v>140</v>
-      </c>
-      <c r="E14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F14" t="s">
-        <v>141</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -6606,10 +6868,14 @@
         <f>_xll.NCDK_MACCSFingerprinter($A14)</f>
         <v>0000000000000000000000000000000000000000000000000000000010000100100000100010000100101100000011111001011000010010001101011101000000000100100001000011110110010101110111</v>
       </c>
+      <c r="T14" s="4">
+        <f>_xll.NCDK_XLogP(A14)</f>
+        <v>1.8070000000000004</v>
+      </c>
     </row>
-    <row r="15" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B15" s="1" t="str">
         <f>_xll.NCDK(B$1,$A15)</f>
@@ -6620,13 +6886,13 @@
         <v>0000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="D15" t="s">
+        <v>142</v>
+      </c>
+      <c r="E15" t="s">
+        <v>142</v>
+      </c>
+      <c r="F15" t="s">
         <v>143</v>
-      </c>
-      <c r="E15" t="s">
-        <v>143</v>
-      </c>
-      <c r="F15" t="s">
-        <v>144</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -6668,10 +6934,14 @@
         <f>_xll.NCDK_MACCSFingerprinter($A15)</f>
         <v>0000000010000000000000000000000000000000001100001000100000000000000010000000100100000000000001001000011001000001000010000001010001100100000001000001001000010010100101</v>
       </c>
+      <c r="T15" s="4">
+        <f>_xll.NCDK_XLogP(A15)</f>
+        <v>3.24</v>
+      </c>
     </row>
-    <row r="16" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B16" s="1" t="str">
         <f>_xll.NCDK(B$1,$A16)</f>
@@ -6682,13 +6952,13 @@
         <v>1000000000000010000000000100000000000000010000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000100000000000000000010000001000000000000001000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000100000000000000000001000000000000000000000000000000000001000000000001000000000000000000100000000000000000000000000000000000000000000100000100000000000100000000010000010000000001000000000000000000000000000000000000000000001000000000000000000000000000000100000000000001000000000000000000000100000000001000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000001000001000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100001000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="D16" t="s">
+        <v>145</v>
+      </c>
+      <c r="E16" t="s">
+        <v>145</v>
+      </c>
+      <c r="F16" t="s">
         <v>146</v>
-      </c>
-      <c r="E16" t="s">
-        <v>146</v>
-      </c>
-      <c r="F16" t="s">
-        <v>147</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -6730,10 +7000,14 @@
         <f>_xll.NCDK_MACCSFingerprinter($A16)</f>
         <v>0000000000000000000001000000000000000000000000000000000010000000110000010010000000101100111000110101101110000011100001011100101110110100111101111111001110111110111111</v>
       </c>
+      <c r="T16" s="4">
+        <f>_xll.NCDK_XLogP(A16)</f>
+        <v>1.4250000000000014</v>
+      </c>
     </row>
-    <row r="17" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B17" s="1" t="str">
         <f>_xll.NCDK(B$1,$A17)</f>
@@ -6744,13 +7018,13 @@
         <v>0000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000001000000000000100000000000000000000100000000000010000000000010000000000000000000000000000000000000000000000000000010000000000000000100000010000000000100000000000000001000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000011000000000000000000000000001000000010000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000001000000000001000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000010100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="D17" t="s">
+        <v>148</v>
+      </c>
+      <c r="E17" t="s">
+        <v>148</v>
+      </c>
+      <c r="F17" t="s">
         <v>149</v>
-      </c>
-      <c r="E17" t="s">
-        <v>149</v>
-      </c>
-      <c r="F17" t="s">
-        <v>150</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -6792,10 +7066,14 @@
         <f>_xll.NCDK_MACCSFingerprinter($A17)</f>
         <v>0000000000000000000000000000000110000000000000000000010000000010001001100000001101010001011101100001010100000110000010100011000101110001011101000110001011111110100100</v>
       </c>
+      <c r="T17" s="4">
+        <f>_xll.NCDK_XLogP(A17)</f>
+        <v>-4.3659999999999997</v>
+      </c>
     </row>
-    <row r="18" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B18" s="1" t="str">
         <f>_xll.NCDK(B$1,$A18)</f>
@@ -6806,13 +7084,13 @@
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000010100000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000010000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000100000</v>
       </c>
       <c r="D18" t="s">
+        <v>151</v>
+      </c>
+      <c r="E18" t="s">
+        <v>151</v>
+      </c>
+      <c r="F18" t="s">
         <v>152</v>
-      </c>
-      <c r="E18" t="s">
-        <v>152</v>
-      </c>
-      <c r="F18" t="s">
-        <v>153</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -6836,10 +7114,14 @@
         <f>_xll.NCDK_MACCSFingerprinter($A18)</f>
         <v>0000000000000000000000000000000000000000000000000000010000000000000000000000001001000000000000000001001100000010000000000000100000100100010001001010001010110100111011</v>
       </c>
+      <c r="T18" s="4">
+        <f>_xll.NCDK_XLogP(A18)</f>
+        <v>4.5600000000000005</v>
+      </c>
     </row>
-    <row r="19" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B19" s="1" t="str">
         <f>_xll.NCDK(B$1,$A19)</f>
@@ -6850,13 +7132,13 @@
         <v>0000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000100000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000100100000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000100000000000000000000000001000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000001000000000000010000000000000000000100000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="D19" t="s">
+        <v>154</v>
+      </c>
+      <c r="E19" t="s">
+        <v>154</v>
+      </c>
+      <c r="F19" t="s">
         <v>155</v>
-      </c>
-      <c r="E19" t="s">
-        <v>155</v>
-      </c>
-      <c r="F19" t="s">
-        <v>156</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -6895,10 +7177,14 @@
         <f>_xll.NCDK_MACCSFingerprinter($A19)</f>
         <v>0000000000000000000000000000000110010100000001100000000000000100101000000010111110100001000011010000000001000000000000111101100000001110100001011001010000010101111011</v>
       </c>
+      <c r="T19" s="4">
+        <f>_xll.NCDK_XLogP(A19)</f>
+        <v>3.8220000000000005</v>
+      </c>
     </row>
-    <row r="20" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B20" s="1" t="str">
         <f>_xll.NCDK(B$1,$A20)</f>
@@ -6909,13 +7195,13 @@
         <v>1000000000000010000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000001000000010000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000001000000110000000100000100000000000000000001000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000001000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000100000000000000000000000000000000000001000000000000000100</v>
       </c>
       <c r="D20" t="s">
+        <v>157</v>
+      </c>
+      <c r="E20" t="s">
+        <v>157</v>
+      </c>
+      <c r="F20" t="s">
         <v>158</v>
-      </c>
-      <c r="E20" t="s">
-        <v>158</v>
-      </c>
-      <c r="F20" t="s">
-        <v>159</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -6948,10 +7234,14 @@
         <f>_xll.NCDK_MACCSFingerprinter($A20)</f>
         <v>0000000000000000000000000000000000001000001000000000000000000000100000000010101000101100001010010101001011010110001110011100100000101110100001011011001011010101111111</v>
       </c>
+      <c r="T20" s="4">
+        <f>_xll.NCDK_XLogP(A20)</f>
+        <v>0.83</v>
+      </c>
     </row>
-    <row r="21" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B21" s="1" t="str">
         <f>_xll.NCDK(B$1,$A21)</f>
@@ -6962,13 +7252,13 @@
         <v>0000000000000000000000001000000000000000000000000000000001000000001000000000000000000000000000000000000000000000000000000000000001000100000000000100000010000000000000000001000000000000000000000000000000000000000000000000000000000000000100000000100000000000000000000100000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000100000000000000000000000001000000000000000000000000000000000010000000000000000010000010000010000000000100000000000000000000000000000001000000010000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000001010000000000000000000110000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="D21" t="s">
+        <v>160</v>
+      </c>
+      <c r="E21" t="s">
+        <v>160</v>
+      </c>
+      <c r="F21" t="s">
         <v>161</v>
-      </c>
-      <c r="E21" t="s">
-        <v>161</v>
-      </c>
-      <c r="F21" t="s">
-        <v>162</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -7009,6 +7299,10 @@
       <c r="S21" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($A21)</f>
         <v>0000000000000000000000000000000001001111000000010010001001111101101010001010101110101001100110111111010011010101100010011101101001000001101101111101110011110111111110</v>
+      </c>
+      <c r="T21" s="4">
+        <f>_xll.NCDK_XLogP(A21)</f>
+        <v>-0.66600000000000015</v>
       </c>
     </row>
   </sheetData>
@@ -7022,7 +7316,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -7033,74 +7327,74 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="95.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="29.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="58" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="76.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" t="s">
         <v>85</v>
-      </c>
-      <c r="B6" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="70" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
         <v>56</v>
-      </c>
-      <c r="B7" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="236" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="168" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" t="s">
         <v>63</v>
-      </c>
-      <c r="B9" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RDKit support. MACCSFingerprint is implemented.
</commit_message>
<xml_diff>
--- a/NCDK-Excel/ExcelNCDK-Test.xlsx
+++ b/NCDK-Excel/ExcelNCDK-Test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B248AA19-3655-4424-9214-4C217F8A0064}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46825268-6CF2-4CF2-ACE3-0F9C1177A419}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="407" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="173">
   <si>
     <t>CC(=O)O</t>
     <phoneticPr fontId="1"/>
@@ -2579,26 +2579,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B185B08-1BAB-4052-951E-1A2BC1F97D8F}">
-  <dimension ref="A1:BZ11"/>
+  <dimension ref="A1:CA11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="3" width="11.25" customWidth="1"/>
     <col min="4" max="4" width="11.08203125" customWidth="1"/>
-    <col min="5" max="5" width="21.1640625" customWidth="1"/>
-    <col min="6" max="23" width="6.5" customWidth="1"/>
-    <col min="24" max="25" width="8.1640625" style="2" customWidth="1"/>
-    <col min="27" max="27" width="8.6640625" style="4" customWidth="1"/>
-    <col min="28" max="30" width="8.6640625" style="4"/>
-    <col min="31" max="31" width="8.6640625" customWidth="1"/>
-    <col min="53" max="53" width="14.83203125" customWidth="1"/>
-    <col min="73" max="73" width="8.6640625" style="2"/>
-    <col min="74" max="74" width="10.08203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="29.25" customWidth="1"/>
+    <col min="7" max="24" width="6.5" customWidth="1"/>
+    <col min="25" max="26" width="8.1640625" style="2" customWidth="1"/>
+    <col min="28" max="28" width="8.6640625" style="4" customWidth="1"/>
+    <col min="29" max="31" width="8.6640625" style="4"/>
+    <col min="32" max="32" width="8.6640625" customWidth="1"/>
+    <col min="54" max="54" width="14.83203125" customWidth="1"/>
+    <col min="74" max="74" width="8.6640625" style="2"/>
+    <col min="75" max="75" width="10.08203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:79" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -2615,226 +2617,229 @@
         <v>163</v>
       </c>
       <c r="F1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" t="s">
         <v>66</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>67</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>68</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>69</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>70</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>71</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>72</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>73</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>74</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>75</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>76</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>77</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>78</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>79</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>80</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>81</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>82</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>65</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>1</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>50</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>2</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>3</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>4</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>5</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>6</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>7</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>8</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>9</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>10</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>11</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>12</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>13</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>14</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>15</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>16</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>17</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>18</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>19</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>20</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>21</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>22</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>23</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>24</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>25</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>26</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>27</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>28</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>29</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>30</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>31</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>60</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>33</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>34</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>35</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BO1" t="s">
         <v>36</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BP1" t="s">
         <v>37</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BQ1" t="s">
         <v>38</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BR1" t="s">
         <v>39</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BS1" t="s">
         <v>40</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BT1" t="s">
         <v>64</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BU1" t="s">
         <v>41</v>
       </c>
-      <c r="BU1" s="2" t="s">
+      <c r="BV1" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="BV1" s="3" t="s">
+      <c r="BW1" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BX1" t="s">
         <v>42</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="BY1" t="s">
         <v>43</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="BZ1" t="s">
         <v>44</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CA1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:78" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:79" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -2887,7 +2892,7 @@
 </v>
       </c>
       <c r="D2">
-        <f>_xll.NCDK_Tanimoto($H2,$H3)</f>
+        <f>_xll.NCDK_Tanimoto($I2,$I3)</f>
         <v>0</v>
       </c>
       <c r="E2" t="str">
@@ -2895,299 +2900,303 @@
         <v>0000000000000000001000000000000000001000001000000100100000000100010000000001100100000000111100001110000001010101010011011000001110100001100001100110011001110111101110</v>
       </c>
       <c r="F2" t="str">
+        <f>_xll.RDKit_MACCSFingerprint(B2)</f>
+        <v>00000000000000000001000000000000000001000001000000100100000000100010000000001100100000000111100001110000001010101010011011000001110100001100001100110011001110111101110</v>
+      </c>
+      <c r="G2" t="str">
         <f>_xll.NCDK_ECFP0($B2)</f>
         <v>0000000000000010000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000100000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="G2" t="str">
+      <c r="H2" t="str">
         <f>_xll.NCDK_ECFP2($B2)</f>
         <v>0000000000000010000000001100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000100000000000000000000000000011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000010000000000000100000000000010000010000001000000000000000000000000000100</v>
       </c>
-      <c r="H2" t="str">
+      <c r="I2" t="str">
         <f>_xll.NCDK_ECFP4($B2)</f>
         <v>0000000000000010000000001100000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000010010000000000000000000000000000000000000000000000000000000000000010001000000000000010000000100000000000000000000000000011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000100000000000000000000000000000000101000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000010000010000000000000100000000000010100010000001000000000000000000000000000100</v>
       </c>
-      <c r="I2" t="str">
+      <c r="J2" t="str">
         <f>_xll.NCDK_ECFP6($B2)</f>
         <v>0000000000000010000000001100000000000000000000000000000000100010000000000000000000000000000000000000000000000000000000010000000000000100000000000000000010010000000000000000000000000000000000000000000000000000000000000010001000000000000010000000100000000000000000000000000011000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000001000000000001000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000100000000000000000000000000000000101000000000000000000000000000000000000000000000100001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000001001000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000010000010000000000000100000000000010100010000001000010000000000000000000000100</v>
       </c>
-      <c r="J2" t="str">
+      <c r="K2" t="str">
         <f>_xll.NCDK_FCFP0($B2)</f>
         <v>1011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="K2" t="str">
+      <c r="L2" t="str">
         <f>_xll.NCDK_FCFP2($B2)</f>
         <v>1011000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000010000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="L2" t="str">
+      <c r="M2" t="str">
         <f>_xll.NCDK_FCFP4($B2)</f>
         <v>1011000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000010000000000000000000000000000000010000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000001000000000000000000000000001000000001000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000001000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000100100000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000100000000000010000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="M2" t="str">
+      <c r="N2" t="str">
         <f>_xll.NCDK_FCFP0($B2)</f>
         <v>1011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="N2" t="str">
+      <c r="O2" t="str">
         <f>_xll.NCDK_AtomPairs2DFingerprinter($B2)</f>
         <v>111000000000000000000000000000000000000000000000000000000000000000000000000000111000000000110000000000000000000000000000000000000000000000000000000000000000111000000000000000000000000000000000000000000000000000000000000000000000000000111000000000010000000001000000000000000000000000000000000000000000000000000000111000000000000000000000000000000000000000000000000000000000000000000000000000111000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="O2" t="str">
+      <c r="P2" t="str">
         <f>_xll.NCDK_EStateFingerprinter($B2)</f>
         <v>0000001010100001001000010000000000100000000000000000000000000000000000000000000</v>
       </c>
-      <c r="P2" t="str">
+      <c r="Q2" t="str">
         <f>_xll.NCDK_ExtendedFingerprinter($B2)</f>
         <v>000000000000001000000000000000001000000000010000000000000000001000000100000001000000000000000010000000000000000000000100000000000000000000001000001000000000000000000000000000000000100100100000000000000000000000010000000000000001010000000000000000000000010100010000000000000000000001100000000000001000000000000000000000000000010000000000000010000000000010000000000000000000000000000000000000000000000000001000011100000000000000100000000000001000001000010100000100000000000000010100000100000000000000000001000000000000000110000000000000100000000000000010000010000000000000000000010000000000001100000000010001100010100010000010000000000000000001000000000000000000000000000001000000000000000100000000000000000000000010000000001000000000000000000010000000001000100100000000100010001000000000110000000000000000000000010000000000000000000000100000000010001000000001000000000000000000100000100000000000000000000000000000000000100000000010000000000010010000010000000000101100010000000000010000000100000001000000000000011001</v>
       </c>
-      <c r="Q2" t="str">
+      <c r="R2" t="str">
         <f>_xll.NCDK_CDKFingerprinter($B2)</f>
         <v>0000010000000000010000000011000000000010000000000000000010010000000000000001010000001011000000000000000000001010000000000010010010000000000000000000100000000000000001000001000010000100000000000000000000000010100000000100000000010000000001100000000000000000000000000000000000000000000000001000000000001000000000000000000100000000000000100100000000000100000000000000001100000000000000000000000110000000000000000001000000000000000000000000000000010000100000101000000000001011001000000000000000000000000010100100000100000000001000000000000000000011010001100000000000000000000000000000000000001000000001000100000000000000000000100000000000000100000000101000000000000000000000000010000000000100000000000000000000000001000001000000000000000000000001110001000010000000100000000000000000000000000000000000000000000000000000000000000000000010000000000000001000100000000000010100000000000000000000000000000000000000000000001000000000001000000000100000000000001000010000000000000000000000000010000000000000000000110001000000001000000000</v>
       </c>
-      <c r="R2" t="str">
+      <c r="S2" t="str">
         <f>_xll.NCDK_KlekotaRothFingerprinter($B2)</f>
         <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000010010110000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000001000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000011000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000100000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000001101000000000000000000000000000001000001000000000000000000001010000000000000000000000000000000000000000010000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000011000000001011000100010010000000000000000000011000000010000110100110000110110011001000101000010100000001000000000000000000000010000010100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000010100001000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000011000000000010001000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000010000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="S2" t="str">
+      <c r="T2" t="str">
         <f>_xll.NCDK_LingoFingerprinter($B2)</f>
         <v>0010000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000100000000100100000000000000000100000000000000000000000000000000000000000000000000000001000100000000000001000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000001000100000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000001000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000</v>
       </c>
-      <c r="T2" t="str">
+      <c r="U2" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($B2)</f>
         <v>0000000000000000001000000000000000001000001000000100100000000100010000000001100100000000111100001110000001010101010011011000001110100001100001100110011001110111101110</v>
       </c>
-      <c r="U2" t="str">
+      <c r="V2" t="str">
         <f>_xll.NCDK_ShortestPathFingerprinter($B2)</f>
         <v>0100000000000100100000000000000010000000110000000010000110000000101110100000000000100000000000000000000000100000000100001000100001000000000010000000000000001000000000000000000000000110000000000000100000000000001001000000000011000001001000000000000010000000000000001000100000000000000000010100000000000000100000000000000000000000000000000010000000000000000010000100000000000000000000000000000000000000000000110000000000000100000100000000010000000000010000000011010000000000000000000001011000000000000000010100000000000000100000000000010001001100000000000000000000000001000000000000100000000010000000000001000000000010000000000000000000000000000000000100010000000000000001000000100010000000100101001001000001001110001100010000000000000000000000000000000000000000000000100010000000000000001010000000000000000000000010000000000000000001110000000000000010000000000000100000000100100000000000000000011100000010000000000000000000000000000000000000000000000000000100000000000000100000000000000000000000101010000000101000000000000000</v>
       </c>
-      <c r="V2" t="str">
+      <c r="W2" t="str">
         <f>_xll.NCDK_SubstructureFingerprinter($B2)</f>
         <v>1101100000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000100010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000001000010100001</v>
       </c>
-      <c r="W2" t="str">
+      <c r="X2" t="str">
         <f>_xll.NCDK_PubchemFingerprinter($B2)</f>
         <v>00000000011100110011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001011000000000000000000000000000000010001000000000000000000000000000000000000000000000000000000000000000001111000000000000100000000000000000000000000000000111000000000100000011000000000000000000000110000000000000010110000000000000000000000100010000000001000100001010100100001000000000000000000000000000000000000001000000000000000000000000000000000100000000001000000000000000000001000100000000000000000011010000010001100000100000000000001000000000000000000000010001000010100100010000010000000000000000011000110001000100011000000100011110000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="X2" s="2">
+      <c r="Y2" s="2">
         <f>_xll.NCDK_MolecularWeight(B2)</f>
         <v>250.29412142388836</v>
       </c>
-      <c r="Y2" s="2">
+      <c r="Z2" s="2">
         <f>_xll.NCDK_ExactMass(B2)</f>
         <v>250.13174243599997</v>
       </c>
-      <c r="Z2">
+      <c r="AA2">
         <f>_xll.NCDK_AcidicGroupCount(B2)</f>
         <v>0</v>
       </c>
-      <c r="AA2" s="4">
+      <c r="AB2" s="4">
         <f>_xll.NCDK_ALogP(B2)</f>
         <v>2.1996999999999991</v>
       </c>
-      <c r="AB2" s="4">
+      <c r="AC2" s="4">
         <f>_xll.NCDK_XLogP(B2)</f>
         <v>2.1759999999999997</v>
       </c>
-      <c r="AC2" s="4">
+      <c r="AD2" s="4">
         <f>_xll.NCDK_MannholdLogP(B2)</f>
         <v>2.34</v>
       </c>
-      <c r="AD2" s="4">
+      <c r="AE2" s="4">
         <f>_xll.NCDK_JPlogP(B2)</f>
         <v>1.7050260777332682</v>
       </c>
-      <c r="AE2">
+      <c r="AF2">
         <f>_xll.NCDK_AMolarRefractivity(B2)</f>
         <v>66.252700000000004</v>
       </c>
-      <c r="AF2">
+      <c r="AG2">
         <f>_xll.NCDK_APol(B2)</f>
         <v>39.488274000000011</v>
       </c>
-      <c r="AG2">
+      <c r="AH2">
         <f>_xll.NCDK_AromaticAtomsCount(B2)</f>
         <v>0</v>
       </c>
-      <c r="AH2">
+      <c r="AI2">
         <f>_xll.NCDK_AromaticBondsCount(B2)</f>
         <v>0</v>
       </c>
-      <c r="AI2">
+      <c r="AJ2">
         <f>_xll.NCDK_AtomCount(B2)</f>
         <v>36</v>
       </c>
-      <c r="AJ2" t="str">
+      <c r="AK2" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B2)</f>
         <v>0.482364049323966, -0.239230483102807, 0.193743260003086, -0.422975414094056, 0.245070516996786</v>
       </c>
-      <c r="AK2" t="str">
+      <c r="AL2" t="str">
         <f>_xll.NCDK_AutocorrelationMass(B2)</f>
         <v>21.0433677091758, 20.6610036641195, 30.570374510169, 39.3180113704083, 36.7520657397667</v>
       </c>
-      <c r="AL2" t="str">
+      <c r="AM2" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B2)</f>
         <v>1236.72445709937, 1455.26096710327, 2067.09825744824, 2452.45202784668, 1776.45546782422</v>
       </c>
-      <c r="AM2">
+      <c r="AN2">
         <f>_xll.NCDK_BasicGroupCount(B2)</f>
         <v>0</v>
       </c>
-      <c r="AN2" t="str">
+      <c r="AO2" t="str">
         <f>_xll.NCDK_BCUT(B2)</f>
         <v>11.89, 15.9969274797474, -0.279527566151374, 0.285306450703295, 4.45516607690972, 12.225254833975</v>
       </c>
-      <c r="AO2">
+      <c r="AP2">
         <f>_xll.NCDK_BondCount(B2)</f>
         <v>0</v>
       </c>
-      <c r="AP2">
+      <c r="AQ2">
         <f>_xll.NCDK_BPol(B2)</f>
         <v>23.871725999999995</v>
       </c>
-      <c r="AQ2" t="str">
+      <c r="AR2" t="str">
         <f>_xll.NCDK_CarbonTypes(B2)</f>
         <v>0, 0, 2, 1, 1, 1, 6, 0, 1</v>
       </c>
-      <c r="AR2" t="str">
+      <c r="AS2" t="str">
         <f>_xll.NCDK_ChiChain(B2)</f>
         <v>0, 0, 0, 0.0481125224324688, 0.206136035947173, 0, 0, 0, 0.015625, 0.0379976820715334</v>
       </c>
-      <c r="AS2" t="str">
+      <c r="AT2" t="str">
         <f>_xll.NCDK_ChiCluster(B2)</f>
         <v>1.29103942781429, 0.0680413817439772, 0.635379749451514, 0.130245735736926, 0.58282022448487, 0.0441941738241592, 0.195368603605389, 0.0360843918243516</v>
       </c>
-      <c r="AT2" t="str">
+      <c r="AU2" t="str">
         <f>_xll.NCDK_ChiPathCluster(B2)</f>
         <v>3.75820832838601, 7.24003474940441, 9.47142848690227, 1.60201233255417, 2.48389505922722, 2.76623804293011</v>
       </c>
-      <c r="AU2" t="str">
+      <c r="AV2" t="str">
         <f>_xll.NCDK_ChiPath(B2)</f>
         <v>13.1733621074374, 8.60822612591632, 7.53308445980525, 6.57446305443147, 5.83502554474493, 3.66414268256136, 2.81639208561656, 1.24750715936873, 10.5447358277005, 6.47350942312757, 4.82495377161152, 3.84884458919458, 2.7963481600948, 1.78170696456175, 1.19223951604789, 0.520731228864019</v>
       </c>
-      <c r="AV2" t="str">
+      <c r="AW2" t="str">
         <f>_xll.NCDK_CPSA(B2)</f>
         <v>#N/A</v>
       </c>
-      <c r="AW2">
+      <c r="AX2">
         <f>_xll.NCDK_EccentricConnectivityIndex(B2)</f>
         <v>226</v>
       </c>
-      <c r="AX2">
+      <c r="AY2">
         <f>_xll.NCDK_FMF(B2)</f>
         <v>0.72222222222222221</v>
       </c>
-      <c r="AY2">
+      <c r="AZ2">
         <f>_xll.NCDK_FractionalPSA(B2)</f>
         <v>0.30092142334124705</v>
       </c>
-      <c r="AZ2">
+      <c r="BA2">
         <f>_xll.NCDK_FragmentComplexity(B2)</f>
         <v>1063.05</v>
       </c>
-      <c r="BA2" t="str">
+      <c r="BB2" t="str">
         <f>_xll.NCDK_GravitationalIndex(B2)</f>
         <v>#N/A</v>
       </c>
-      <c r="BB2">
+      <c r="BC2">
         <f>_xll.NCDK_HBondAcceptorCount(B2)</f>
         <v>5</v>
       </c>
-      <c r="BC2">
+      <c r="BD2">
         <f>_xll.NCDK_HBondDonorCount(B2)</f>
         <v>2</v>
       </c>
-      <c r="BD2">
+      <c r="BE2">
         <f>_xll.NCDK_HybridizationRatio(B2)</f>
         <v>0.61538461538461542</v>
       </c>
-      <c r="BE2" t="str">
+      <c r="BF2" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B2)</f>
         <v>14.409972299169, 5.96982167352538, 2.65927977839335</v>
       </c>
-      <c r="BF2" t="str">
+      <c r="BG2" t="str">
         <f>_xll.NCDK_KierHallSmarts(B2)</f>
         <v>0, 0, 0, 0, 0, 0, 1, 0, 6, 0, 1, 0, 0, 0, 0, 4, 0, 0, 1, 0, 0, 0, 0, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 3, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BG2">
+      <c r="BH2">
         <f>_xll.NCDK_LargestChain(B2)</f>
         <v>2</v>
       </c>
-      <c r="BH2">
+      <c r="BI2">
         <f>_xll.NCDK_LargestPiSystem(B2)</f>
         <v>8</v>
       </c>
-      <c r="BI2" t="str">
+      <c r="BJ2" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B2)</f>
         <v>#N/A</v>
       </c>
-      <c r="BJ2">
+      <c r="BK2">
         <f>_xll.NCDK_LongestAliphaticChain(B2)</f>
         <v>2</v>
       </c>
-      <c r="BK2" t="str">
+      <c r="BL2" t="str">
         <f>_xll.NCDK_MDE(B2)</f>
         <v>0, 1.78256861348341, 1.17348231572452, 0.5, 9.28105720195319, 8.27801156561087, 2.82326712400687, 2.67269615442102, 3.03934274260637, 0, 0.75, 0, 0, 0, 0, 0, 0.5, 0, 0</v>
       </c>
-      <c r="BL2" t="str">
+      <c r="BM2" t="str">
         <f>_xll.NCDK_MomentOfInertia(B2)</f>
         <v>#N/A</v>
       </c>
-      <c r="BM2">
+      <c r="BN2">
         <f>_xll.NCDK_PetitjeanNumber(B2)</f>
         <v>0.5</v>
       </c>
-      <c r="BN2" t="str">
+      <c r="BO2" t="str">
         <f>_xll.NCDK_PetitjeanShapeIndex(B2)</f>
         <v>#N/A</v>
       </c>
-      <c r="BO2">
+      <c r="BP2">
         <f>_xll.NCDK_RotatableBondsCount(B2)</f>
         <v>2</v>
       </c>
-      <c r="BP2">
+      <c r="BQ2">
         <f>_xll.NCDK_RuleOfFive(B2)</f>
         <v>0</v>
       </c>
-      <c r="BQ2" t="str">
+      <c r="BR2" t="str">
         <f>_xll.NCDK_SmallRing(B2)</f>
         <v>2, 0, 2, 0, 0, 0, 0, 1, 1, 0, 0</v>
       </c>
-      <c r="BR2">
+      <c r="BS2">
         <f>_xll.NCDK_TPSA(B2)</f>
         <v>75.27000000000001</v>
       </c>
-      <c r="BS2">
+      <c r="BT2">
         <f>_xll.NCDK_VABC(B2)</f>
         <v>246.50970715028382</v>
       </c>
-      <c r="BT2">
+      <c r="BU2">
         <f>_xll.NCDK_VAdjMa(B2)</f>
         <v>5.2479275134435852</v>
       </c>
-      <c r="BU2" s="2">
+      <c r="BV2" s="2">
         <f>_xll.NCDK_MolecularWeight(B2)</f>
         <v>250.29412142388836</v>
       </c>
-      <c r="BV2" s="3">
+      <c r="BW2" s="3">
         <f>_xll.NCDK_ExactMass(B2)</f>
         <v>250.13174243599997</v>
       </c>
-      <c r="BW2" t="str">
+      <c r="BX2" t="str">
         <f>_xll.NCDK_WeightedPath(B2)</f>
         <v>35.9822147160759, 1.99901192867088, 13.5466431850826, 7.60403910050065, 5.94260408458194</v>
       </c>
-      <c r="BX2" t="str">
+      <c r="BY2" t="str">
         <f>_xll.NCDK_WHIM(B2)</f>
         <v>#N/A</v>
       </c>
-      <c r="BY2" t="str">
+      <c r="BZ2" t="str">
         <f>_xll.NCDK_WienerNumbers(B2)</f>
         <v>537, 35</v>
       </c>
-      <c r="BZ2">
+      <c r="CA2">
         <f>_xll.NCDK_ZagrebIndex(B2)</f>
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:78" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:79" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -3204,7 +3213,7 @@
 </v>
       </c>
       <c r="D3">
-        <f>_xll.NCDK_Tanimoto($H3,$H4)</f>
+        <f>_xll.NCDK_Tanimoto($I3,$I4)</f>
         <v>0</v>
       </c>
       <c r="E3" t="str">
@@ -3212,299 +3221,303 @@
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000</v>
       </c>
       <c r="F3" t="str">
+        <f>_xll.RDKit_MACCSFingerprint(B3)</f>
+        <v>00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000</v>
+      </c>
+      <c r="G3" t="str">
         <f>_xll.NCDK_ECFP0($B3)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="G3" t="str">
+      <c r="H3" t="str">
         <f>_xll.NCDK_ECFP2($B3)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="H3" t="str">
+      <c r="I3" t="str">
         <f>_xll.NCDK_ECFP4($B3)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="I3" t="str">
+      <c r="J3" t="str">
         <f>_xll.NCDK_ECFP6($B3)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="J3" t="str">
+      <c r="K3" t="str">
         <f>_xll.NCDK_FCFP0($B3)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="K3" t="str">
+      <c r="L3" t="str">
         <f>_xll.NCDK_FCFP2($B3)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="L3" t="str">
+      <c r="M3" t="str">
         <f>_xll.NCDK_FCFP4($B3)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="M3" t="str">
+      <c r="N3" t="str">
         <f>_xll.NCDK_FCFP0($B3)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="N3" t="str">
+      <c r="O3" t="str">
         <f>_xll.NCDK_AtomPairs2DFingerprinter($B3)</f>
         <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="O3" t="str">
+      <c r="P3" t="str">
         <f>_xll.NCDK_EStateFingerprinter($B3)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="P3" t="str">
+      <c r="Q3" t="str">
         <f>_xll.NCDK_ExtendedFingerprinter($B3)</f>
         <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="Q3" t="str">
+      <c r="R3" t="str">
         <f>_xll.NCDK_CDKFingerprinter($B3)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="R3" t="str">
+      <c r="S3" t="str">
         <f>_xll.NCDK_KlekotaRothFingerprinter($B3)</f>
         <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="S3" t="str">
+      <c r="T3" t="str">
         <f>_xll.NCDK_LingoFingerprinter($B3)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="T3" t="str">
+      <c r="U3" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($B3)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000</v>
       </c>
-      <c r="U3" t="str">
+      <c r="V3" t="str">
         <f>_xll.NCDK_ShortestPathFingerprinter($B3)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="V3" t="str">
+      <c r="W3" t="str">
         <f>_xll.NCDK_SubstructureFingerprinter($B3)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="W3" t="str">
+      <c r="X3" t="str">
         <f>_xll.NCDK_PubchemFingerprinter($B3)</f>
         <v>00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="X3" s="2">
+      <c r="Y3" s="2">
         <f>_xll.NCDK_MolecularWeight(B3)</f>
         <v>16.042498912091162</v>
       </c>
-      <c r="Y3" s="2">
+      <c r="Z3" s="2">
         <f>_xll.NCDK_ExactMass(B3)</f>
         <v>16.031300127999998</v>
       </c>
-      <c r="Z3">
+      <c r="AA3">
         <f>_xll.NCDK_AcidicGroupCount(B3)</f>
         <v>0</v>
       </c>
-      <c r="AA3" s="4">
+      <c r="AB3" s="4">
         <f>_xll.NCDK_ALogP(B3)</f>
         <v>0</v>
       </c>
-      <c r="AB3" s="4">
+      <c r="AC3" s="4">
         <f>_xll.NCDK_XLogP(B3)</f>
         <v>0.73899999999999999</v>
       </c>
-      <c r="AC3" s="4">
+      <c r="AD3" s="4">
         <f>_xll.NCDK_MannholdLogP(B3)</f>
         <v>1.57</v>
       </c>
-      <c r="AD3" s="4" t="e">
+      <c r="AE3" s="4" t="e">
         <f>_xll.NCDK_JPlogP(B3)</f>
         <v>#NUM!</v>
       </c>
-      <c r="AE3">
+      <c r="AF3">
         <f>_xll.NCDK_AMolarRefractivity(B3)</f>
         <v>0</v>
       </c>
-      <c r="AF3">
+      <c r="AG3">
         <f>_xll.NCDK_APol(B3)</f>
         <v>4.4271719999999997</v>
       </c>
-      <c r="AG3">
+      <c r="AH3">
         <f>_xll.NCDK_AromaticAtomsCount(B3)</f>
         <v>0</v>
       </c>
-      <c r="AH3">
+      <c r="AI3">
         <f>_xll.NCDK_AromaticBondsCount(B3)</f>
         <v>0</v>
       </c>
-      <c r="AI3">
+      <c r="AJ3">
         <f>_xll.NCDK_AtomCount(B3)</f>
         <v>5</v>
       </c>
-      <c r="AJ3" t="str">
+      <c r="AK3" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B3)</f>
         <v>0, 0, 0, 0, 0</v>
       </c>
-      <c r="AK3" t="str">
+      <c r="AL3" t="str">
         <f>_xll.NCDK_AutocorrelationMass(B3)</f>
         <v>1, 0, 0, 0, 0</v>
       </c>
-      <c r="AL3" t="str">
+      <c r="AM3" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B3)</f>
         <v>6.822544, 0, 0, 0, 0</v>
       </c>
-      <c r="AM3">
+      <c r="AN3">
         <f>_xll.NCDK_BasicGroupCount(B3)</f>
         <v>0</v>
       </c>
-      <c r="AN3" t="str">
+      <c r="AO3" t="str">
         <f>_xll.NCDK_BCUT(B3)</f>
         <v>12, 12, -0.0779229231460157, -0.0779229231460157, 2.612, 2.612</v>
       </c>
-      <c r="AO3">
+      <c r="AP3">
         <f>_xll.NCDK_BondCount(B3)</f>
         <v>0</v>
       </c>
-      <c r="AP3">
+      <c r="AQ3">
         <f>_xll.NCDK_BPol(B3)</f>
         <v>4.3728280000000002</v>
       </c>
-      <c r="AQ3" t="str">
+      <c r="AR3" t="str">
         <f>_xll.NCDK_CarbonTypes(B3)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AR3" t="str">
+      <c r="AS3" t="str">
         <f>_xll.NCDK_ChiChain(B3)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AS3" t="str">
+      <c r="AT3" t="str">
         <f>_xll.NCDK_ChiCluster(B3)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AT3" t="str">
+      <c r="AU3" t="str">
         <f>_xll.NCDK_ChiPathCluster(B3)</f>
         <v>0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AU3" t="str">
+      <c r="AV3" t="str">
         <f>_xll.NCDK_ChiPath(B3)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AV3" t="str">
+      <c r="AW3" t="str">
         <f>_xll.NCDK_CPSA(B3)</f>
         <v>#N/A</v>
       </c>
-      <c r="AW3">
+      <c r="AX3">
         <f>_xll.NCDK_EccentricConnectivityIndex(B3)</f>
         <v>0</v>
       </c>
-      <c r="AX3">
+      <c r="AY3">
         <f>_xll.NCDK_FMF(B3)</f>
         <v>0</v>
       </c>
-      <c r="AY3">
+      <c r="AZ3">
         <f>_xll.NCDK_FractionalPSA(B3)</f>
         <v>0</v>
       </c>
-      <c r="AZ3">
+      <c r="BA3">
         <f>_xll.NCDK_FragmentComplexity(B3)</f>
         <v>16</v>
       </c>
-      <c r="BA3" t="str">
+      <c r="BB3" t="str">
         <f>_xll.NCDK_GravitationalIndex(B3)</f>
         <v>#N/A</v>
       </c>
-      <c r="BB3">
+      <c r="BC3">
         <f>_xll.NCDK_HBondAcceptorCount(B3)</f>
         <v>0</v>
       </c>
-      <c r="BC3">
+      <c r="BD3">
         <f>_xll.NCDK_HBondDonorCount(B3)</f>
         <v>0</v>
       </c>
-      <c r="BD3">
+      <c r="BE3">
         <f>_xll.NCDK_HybridizationRatio(B3)</f>
         <v>1</v>
       </c>
-      <c r="BE3" t="str">
+      <c r="BF3" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B3)</f>
         <v>0, 0, 0</v>
       </c>
-      <c r="BF3" t="str">
+      <c r="BG3" t="str">
         <f>_xll.NCDK_KierHallSmarts(B3)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BG3">
+      <c r="BH3">
         <f>_xll.NCDK_LargestChain(B3)</f>
         <v>0</v>
       </c>
-      <c r="BH3">
+      <c r="BI3">
         <f>_xll.NCDK_LargestPiSystem(B3)</f>
         <v>0</v>
       </c>
-      <c r="BI3" t="str">
+      <c r="BJ3" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B3)</f>
         <v>#N/A</v>
       </c>
-      <c r="BJ3">
+      <c r="BK3">
         <f>_xll.NCDK_LongestAliphaticChain(B3)</f>
         <v>0</v>
       </c>
-      <c r="BK3" t="str">
+      <c r="BL3" t="str">
         <f>_xll.NCDK_MDE(B3)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BL3" t="str">
+      <c r="BM3" t="str">
         <f>_xll.NCDK_MomentOfInertia(B3)</f>
         <v>#N/A</v>
       </c>
-      <c r="BM3">
+      <c r="BN3">
         <f>_xll.NCDK_PetitjeanNumber(B3)</f>
         <v>0</v>
       </c>
-      <c r="BN3" t="str">
+      <c r="BO3" t="str">
         <f>_xll.NCDK_PetitjeanShapeIndex(B3)</f>
         <v>#N/A</v>
       </c>
-      <c r="BO3">
+      <c r="BP3">
         <f>_xll.NCDK_RotatableBondsCount(B3)</f>
         <v>0</v>
       </c>
-      <c r="BP3">
+      <c r="BQ3">
         <f>_xll.NCDK_RuleOfFive(B3)</f>
         <v>0</v>
       </c>
-      <c r="BQ3" t="str">
+      <c r="BR3" t="str">
         <f>_xll.NCDK_SmallRing(B3)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BR3">
+      <c r="BS3">
         <f>_xll.NCDK_TPSA(B3)</f>
         <v>0</v>
       </c>
-      <c r="BS3">
+      <c r="BT3">
         <f>_xll.NCDK_VABC(B3)</f>
         <v>25.852443326666702</v>
       </c>
-      <c r="BT3">
+      <c r="BU3">
         <f>_xll.NCDK_VAdjMa(B3)</f>
         <v>0</v>
       </c>
-      <c r="BU3" s="2">
+      <c r="BV3" s="2">
         <f>_xll.NCDK_MolecularWeight(B3)</f>
         <v>16.042498912091162</v>
       </c>
-      <c r="BV3" s="3">
+      <c r="BW3" s="3">
         <f>_xll.NCDK_ExactMass(B3)</f>
         <v>16.031300127999998</v>
       </c>
-      <c r="BW3" t="str">
+      <c r="BX3" t="str">
         <f>_xll.NCDK_WeightedPath(B3)</f>
         <v>1, 1, 0, 0, 0</v>
       </c>
-      <c r="BX3" t="str">
+      <c r="BY3" t="str">
         <f>_xll.NCDK_WHIM(B3)</f>
         <v>#N/A</v>
       </c>
-      <c r="BY3" t="str">
+      <c r="BZ3" t="str">
         <f>_xll.NCDK_WienerNumbers(B3)</f>
         <v>0, 0</v>
       </c>
-      <c r="BZ3">
+      <c r="CA3">
         <f>_xll.NCDK_ZagrebIndex(B3)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:78" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:79" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -3516,7 +3529,7 @@
         <v>InChI=1S/C2H4O2/c1-2(3)4/h1H3,(H,3,4)</v>
       </c>
       <c r="D4">
-        <f>_xll.NCDK_Tanimoto($H4,$H5)</f>
+        <f>_xll.NCDK_Tanimoto($I4,$I5)</f>
         <v>0</v>
       </c>
       <c r="E4" t="str">
@@ -3524,299 +3537,303 @@
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000001000000000000001001011000100</v>
       </c>
       <c r="F4" t="str">
+        <f>_xll.RDKit_MACCSFingerprint(B4)</f>
+        <v>00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000001000000000000001001011000100</v>
+      </c>
+      <c r="G4" t="str">
         <f>_xll.NCDK_ECFP0($B4)</f>
         <v>0000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="G4" t="str">
+      <c r="H4" t="str">
         <f>_xll.NCDK_ECFP2($B4)</f>
         <v>0000000000000000000100000000000000000000000000000000000000000000010000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="H4" t="str">
+      <c r="I4" t="str">
         <f>_xll.NCDK_ECFP4($B4)</f>
         <v>0000000000000000000100000000000000000000000000000000000000000000010000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="I4" t="str">
+      <c r="J4" t="str">
         <f>_xll.NCDK_ECFP6($B4)</f>
         <v>0000000000000000000100000000000000000000000000000000000000000000010000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="J4" t="str">
+      <c r="K4" t="str">
         <f>_xll.NCDK_FCFP0($B4)</f>
         <v>1010000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="K4" t="str">
+      <c r="L4" t="str">
         <f>_xll.NCDK_FCFP2($B4)</f>
         <v>1010000010000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="L4" t="str">
+      <c r="M4" t="str">
         <f>_xll.NCDK_FCFP4($B4)</f>
         <v>1010000010000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="M4" t="str">
+      <c r="N4" t="str">
         <f>_xll.NCDK_FCFP0($B4)</f>
         <v>1010000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="N4" t="str">
+      <c r="O4" t="str">
         <f>_xll.NCDK_AtomPairs2DFingerprinter($B4)</f>
         <v>101000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="O4" t="str">
+      <c r="P4" t="str">
         <f>_xll.NCDK_EStateFingerprinter($B4)</f>
         <v>0000001000000001000000000000000001100000000000000000000000000000000000000000000</v>
       </c>
-      <c r="P4" t="str">
+      <c r="Q4" t="str">
         <f>_xll.NCDK_ExtendedFingerprinter($B4)</f>
         <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010010000000000000000000000000000000000000000001000</v>
       </c>
-      <c r="Q4" t="str">
+      <c r="R4" t="str">
         <f>_xll.NCDK_CDKFingerprinter($B4)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000001010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="R4" t="str">
+      <c r="S4" t="str">
         <f>_xll.NCDK_KlekotaRothFingerprinter($B4)</f>
         <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000010000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="S4" t="str">
+      <c r="T4" t="str">
         <f>_xll.NCDK_LingoFingerprinter($B4)</f>
         <v>0000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="T4" t="str">
+      <c r="U4" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($B4)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000001000000000000001001011000100</v>
       </c>
-      <c r="U4" t="str">
+      <c r="V4" t="str">
         <f>_xll.NCDK_ShortestPathFingerprinter($B4)</f>
         <v>0000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000100000000100000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000010000000000000001000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000</v>
       </c>
-      <c r="V4" t="str">
+      <c r="W4" t="str">
         <f>_xll.NCDK_SubstructureFingerprinter($B4)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000010001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000010000000</v>
       </c>
-      <c r="W4" t="str">
+      <c r="X4" t="str">
         <f>_xll.NCDK_PubchemFingerprinter($B4)</f>
         <v>00000000010000000011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001101000000000000000000000100000000000000000000000000000000000100000001000000000000000000000100000100000000000000000000000001000000000000010000000000000000000100100000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="X4" s="2">
+      <c r="Y4" s="2">
         <f>_xll.NCDK_MolecularWeight(B4)</f>
         <v>60.052044664017956</v>
       </c>
-      <c r="Y4" s="2">
+      <c r="Z4" s="2">
         <f>_xll.NCDK_ExactMass(B4)</f>
         <v>60.021129367999997</v>
       </c>
-      <c r="Z4">
+      <c r="AA4">
         <f>_xll.NCDK_AcidicGroupCount(B4)</f>
         <v>1</v>
       </c>
-      <c r="AA4" s="4">
+      <c r="AB4" s="4">
         <f>_xll.NCDK_ALogP(B4)</f>
         <v>-0.22990000000000016</v>
       </c>
-      <c r="AB4" s="4">
+      <c r="AC4" s="4">
         <f>_xll.NCDK_XLogP(B4)</f>
         <v>-0.08</v>
       </c>
-      <c r="AC4" s="4">
+      <c r="AD4" s="4">
         <f>_xll.NCDK_MannholdLogP(B4)</f>
         <v>1.46</v>
       </c>
-      <c r="AD4" s="4">
+      <c r="AE4" s="4">
         <f>_xll.NCDK_JPlogP(B4)</f>
         <v>-0.27735415884610526</v>
       </c>
-      <c r="AE4">
+      <c r="AF4">
         <f>_xll.NCDK_AMolarRefractivity(B4)</f>
         <v>12.643699999999999</v>
       </c>
-      <c r="AF4">
+      <c r="AG4">
         <f>_xll.NCDK_APol(B4)</f>
         <v>7.7911719999999995</v>
       </c>
-      <c r="AG4">
+      <c r="AH4">
         <f>_xll.NCDK_AromaticAtomsCount(B4)</f>
         <v>0</v>
       </c>
-      <c r="AH4">
+      <c r="AI4">
         <f>_xll.NCDK_AromaticBondsCount(B4)</f>
         <v>0</v>
       </c>
-      <c r="AI4">
+      <c r="AJ4">
         <f>_xll.NCDK_AtomCount(B4)</f>
         <v>8</v>
       </c>
-      <c r="AJ4" t="str">
+      <c r="AK4" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B4)</f>
         <v>0.194598407923705, -0.0910121789036757, -0.00628702505817703, 0, 0</v>
       </c>
-      <c r="AK4" t="str">
+      <c r="AL4" t="str">
         <f>_xll.NCDK_AutocorrelationMass(B4)</f>
         <v>5.54893807108189, 3.66418395426513, 4.43865298980608, 0, 0</v>
       </c>
-      <c r="AL4" t="str">
+      <c r="AM4" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B4)</f>
         <v>58.780575625, 47.106336, 38.8410481875, 0, 0</v>
       </c>
-      <c r="AM4">
+      <c r="AN4">
         <f>_xll.NCDK_BasicGroupCount(B4)</f>
         <v>0</v>
       </c>
-      <c r="AN4" t="str">
+      <c r="AO4" t="str">
         <f>_xll.NCDK_BCUT(B4)</f>
         <v>11.9966879762366, 15.9982572603197, -0.351666803410558, 0.275648439067482, 3.09299617864267, 4.35788090208676</v>
       </c>
-      <c r="AO4">
+      <c r="AP4">
         <f>_xll.NCDK_BondCount(B4)</f>
         <v>0</v>
       </c>
-      <c r="AP4">
+      <c r="AQ4">
         <f>_xll.NCDK_BPol(B4)</f>
         <v>5.3308280000000003</v>
       </c>
-      <c r="AQ4" t="str">
+      <c r="AR4" t="str">
         <f>_xll.NCDK_CarbonTypes(B4)</f>
         <v>0, 0, 1, 0, 0, 1, 0, 0, 0</v>
       </c>
-      <c r="AR4" t="str">
+      <c r="AS4" t="str">
         <f>_xll.NCDK_ChiChain(B4)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AS4" t="str">
+      <c r="AT4" t="str">
         <f>_xll.NCDK_ChiCluster(B4)</f>
         <v>0.577350269189626, 0, 0, 0, 0.0912870929175277, 0, 0, 0</v>
       </c>
-      <c r="AT4" t="str">
+      <c r="AU4" t="str">
         <f>_xll.NCDK_ChiPathCluster(B4)</f>
         <v>0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AU4" t="str">
+      <c r="AV4" t="str">
         <f>_xll.NCDK_ChiPath(B4)</f>
         <v>3.57735026918963, 1.73205080756888, 1.73205080756888, 0, 0, 0, 0, 0, 2.35546188596382, 0.927730942981911, 0.519018035899438, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AV4" t="str">
+      <c r="AW4" t="str">
         <f>_xll.NCDK_CPSA(B4)</f>
         <v>#N/A</v>
       </c>
-      <c r="AW4">
+      <c r="AX4">
         <f>_xll.NCDK_EccentricConnectivityIndex(B4)</f>
         <v>9</v>
       </c>
-      <c r="AX4">
+      <c r="AY4">
         <f>_xll.NCDK_FMF(B4)</f>
         <v>0</v>
       </c>
-      <c r="AY4">
+      <c r="AZ4">
         <f>_xll.NCDK_FractionalPSA(B4)</f>
         <v>0.62144781967398288</v>
       </c>
-      <c r="AZ4">
+      <c r="BA4">
         <f>_xll.NCDK_FragmentComplexity(B4)</f>
         <v>37.020000000000003</v>
       </c>
-      <c r="BA4" t="str">
+      <c r="BB4" t="str">
         <f>_xll.NCDK_GravitationalIndex(B4)</f>
         <v>#N/A</v>
       </c>
-      <c r="BB4">
+      <c r="BC4">
         <f>_xll.NCDK_HBondAcceptorCount(B4)</f>
         <v>2</v>
       </c>
-      <c r="BC4">
+      <c r="BD4">
         <f>_xll.NCDK_HBondDonorCount(B4)</f>
         <v>1</v>
       </c>
-      <c r="BD4">
+      <c r="BE4">
         <f>_xll.NCDK_HybridizationRatio(B4)</f>
         <v>0.5</v>
       </c>
-      <c r="BE4" t="str">
+      <c r="BF4" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B4)</f>
         <v>4, 1.33333333333333, #N/A</v>
       </c>
-      <c r="BF4" t="str">
+      <c r="BG4" t="str">
         <f>_xll.NCDK_KierHallSmarts(B4)</f>
         <v>0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BG4">
+      <c r="BH4">
         <f>_xll.NCDK_LargestChain(B4)</f>
         <v>3</v>
       </c>
-      <c r="BH4">
+      <c r="BI4">
         <f>_xll.NCDK_LargestPiSystem(B4)</f>
         <v>2</v>
       </c>
-      <c r="BI4" t="str">
+      <c r="BJ4" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B4)</f>
         <v>#N/A</v>
       </c>
-      <c r="BJ4">
+      <c r="BK4">
         <f>_xll.NCDK_LongestAliphaticChain(B4)</f>
         <v>2</v>
       </c>
-      <c r="BK4" t="str">
+      <c r="BL4" t="str">
         <f>_xll.NCDK_MDE(B4)</f>
         <v>0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0.5, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BL4" t="str">
+      <c r="BM4" t="str">
         <f>_xll.NCDK_MomentOfInertia(B4)</f>
         <v>#N/A</v>
       </c>
-      <c r="BM4">
+      <c r="BN4">
         <f>_xll.NCDK_PetitjeanNumber(B4)</f>
         <v>0.5</v>
       </c>
-      <c r="BN4" t="str">
+      <c r="BO4" t="str">
         <f>_xll.NCDK_PetitjeanShapeIndex(B4)</f>
         <v>#N/A</v>
       </c>
-      <c r="BO4">
+      <c r="BP4">
         <f>_xll.NCDK_RotatableBondsCount(B4)</f>
         <v>0</v>
       </c>
-      <c r="BP4">
+      <c r="BQ4">
         <f>_xll.NCDK_RuleOfFive(B4)</f>
         <v>0</v>
       </c>
-      <c r="BQ4" t="str">
+      <c r="BR4" t="str">
         <f>_xll.NCDK_SmallRing(B4)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BR4">
+      <c r="BS4">
         <f>_xll.NCDK_TPSA(B4)</f>
         <v>37.299999999999997</v>
       </c>
-      <c r="BS4">
+      <c r="BT4">
         <f>_xll.NCDK_VABC(B4)</f>
         <v>58.092422652855603</v>
       </c>
-      <c r="BT4">
+      <c r="BU4">
         <f>_xll.NCDK_VAdjMa(B4)</f>
         <v>2.5849625007211561</v>
       </c>
-      <c r="BU4" s="2">
+      <c r="BV4" s="2">
         <f>_xll.NCDK_MolecularWeight(B4)</f>
         <v>60.052044664017956</v>
       </c>
-      <c r="BV4" s="3">
+      <c r="BW4" s="3">
         <f>_xll.NCDK_ExactMass(B4)</f>
         <v>60.021129367999997</v>
       </c>
-      <c r="BW4" t="str">
+      <c r="BX4" t="str">
         <f>_xll.NCDK_WeightedPath(B4)</f>
         <v>6.73205080756888, 1.68301270189222, 4.48803387171259, 4.48803387171259, 0</v>
       </c>
-      <c r="BX4" t="str">
+      <c r="BY4" t="str">
         <f>_xll.NCDK_WHIM(B4)</f>
         <v>#N/A</v>
       </c>
-      <c r="BY4" t="str">
+      <c r="BZ4" t="str">
         <f>_xll.NCDK_WienerNumbers(B4)</f>
         <v>9, 0</v>
       </c>
-      <c r="BZ4">
+      <c r="CA4">
         <f>_xll.NCDK_ZagrebIndex(B4)</f>
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:78" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:79" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -3828,7 +3845,7 @@
         <v>InChI=1S/C6H6/c1-2-4-6-5-3-1/h1-6H</v>
       </c>
       <c r="D5">
-        <f>_xll.NCDK_Tanimoto($H5,$H6)</f>
+        <f>_xll.NCDK_Tanimoto($I5,$I6)</f>
         <v>0.27272727272727271</v>
       </c>
       <c r="E5" t="str">
@@ -3836,299 +3853,303 @@
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000011010</v>
       </c>
       <c r="F5" t="str">
+        <f>_xll.RDKit_MACCSFingerprint(B5)</f>
+        <v>00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000011010</v>
+      </c>
+      <c r="G5" t="str">
         <f>_xll.NCDK_ECFP0($B5)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="G5" t="str">
+      <c r="H5" t="str">
         <f>_xll.NCDK_ECFP2($B5)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="H5" t="str">
+      <c r="I5" t="str">
         <f>_xll.NCDK_ECFP4($B5)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="I5" t="str">
+      <c r="J5" t="str">
         <f>_xll.NCDK_ECFP6($B5)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="J5" t="str">
+      <c r="K5" t="str">
         <f>_xll.NCDK_FCFP0($B5)</f>
         <v>0000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="K5" t="str">
+      <c r="L5" t="str">
         <f>_xll.NCDK_FCFP2($B5)</f>
         <v>0000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="L5" t="str">
+      <c r="M5" t="str">
         <f>_xll.NCDK_FCFP4($B5)</f>
         <v>0000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="M5" t="str">
+      <c r="N5" t="str">
         <f>_xll.NCDK_FCFP0($B5)</f>
         <v>0000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="N5" t="str">
+      <c r="O5" t="str">
         <f>_xll.NCDK_AtomPairs2DFingerprinter($B5)</f>
         <v>100000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="O5" t="str">
+      <c r="P5" t="str">
         <f>_xll.NCDK_EStateFingerprinter($B5)</f>
         <v>0000000000010000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="P5" t="str">
+      <c r="Q5" t="str">
         <f>_xll.NCDK_ExtendedFingerprinter($B5)</f>
         <v>000000000000000000000000000000000000000000000000000001000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000010000000000000000000000000000000000000000000000000000000000010001</v>
       </c>
-      <c r="Q5" t="str">
+      <c r="R5" t="str">
         <f>_xll.NCDK_CDKFingerprinter($B5)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="R5" t="str">
+      <c r="S5" t="str">
         <f>_xll.NCDK_KlekotaRothFingerprinter($B5)</f>
         <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="S5" t="str">
+      <c r="T5" t="str">
         <f>_xll.NCDK_LingoFingerprinter($B5)</f>
         <v>0000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000</v>
       </c>
-      <c r="T5" t="str">
+      <c r="U5" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($B5)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000011010</v>
       </c>
-      <c r="U5" t="str">
+      <c r="V5" t="str">
         <f>_xll.NCDK_ShortestPathFingerprinter($B5)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
       </c>
-      <c r="V5" t="str">
+      <c r="W5" t="str">
         <f>_xll.NCDK_SubstructureFingerprinter($B5)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000001</v>
       </c>
-      <c r="W5" t="str">
+      <c r="X5" t="str">
         <f>_xll.NCDK_PubchemFingerprinter($B5)</f>
         <v>00000000011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000001100000000000000000000000000000000000000000000000100000000000100000000001000000000000001100000000000010000000000000000000000000000000100000000000000000100000010000100000000000000000000000100000000000000000001000000000000000000000000010001000100000000000000000000000000010001000000010000010000000100010100000000001000100010000100000000010000000000000001000001000000000000000000010001000100000000111000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="X5" s="2">
+      <c r="Y5" s="2">
         <f>_xll.NCDK_MolecularWeight(B5)</f>
         <v>78.112059903682749</v>
       </c>
-      <c r="Y5" s="2">
+      <c r="Z5" s="2">
         <f>_xll.NCDK_ExactMass(B5)</f>
         <v>78.046950191999997</v>
       </c>
-      <c r="Z5">
+      <c r="AA5">
         <f>_xll.NCDK_AcidicGroupCount(B5)</f>
         <v>0</v>
       </c>
-      <c r="AA5" s="4">
+      <c r="AB5" s="4">
         <f>_xll.NCDK_ALogP(B5)</f>
         <v>1.8299999999999996</v>
       </c>
-      <c r="AB5" s="4">
+      <c r="AC5" s="4">
         <f>_xll.NCDK_XLogP(B5)</f>
         <v>2.0220000000000002</v>
       </c>
-      <c r="AC5" s="4">
+      <c r="AD5" s="4">
         <f>_xll.NCDK_MannholdLogP(B5)</f>
         <v>2.12</v>
       </c>
-      <c r="AD5" s="4">
+      <c r="AE5" s="4">
         <f>_xll.NCDK_JPlogP(B5)</f>
         <v>1.8466303941078017</v>
       </c>
-      <c r="AE5">
+      <c r="AF5">
         <f>_xll.NCDK_AMolarRefractivity(B5)</f>
         <v>26.058</v>
       </c>
-      <c r="AF5">
+      <c r="AG5">
         <f>_xll.NCDK_APol(B5)</f>
         <v>14.560758</v>
       </c>
-      <c r="AG5">
+      <c r="AH5">
         <f>_xll.NCDK_AromaticAtomsCount(B5)</f>
         <v>6</v>
       </c>
-      <c r="AH5">
+      <c r="AI5">
         <f>_xll.NCDK_AromaticBondsCount(B5)</f>
         <v>6</v>
       </c>
-      <c r="AI5">
+      <c r="AJ5">
         <f>_xll.NCDK_AtomCount(B5)</f>
         <v>12</v>
       </c>
-      <c r="AJ5" t="str">
+      <c r="AK5" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B5)</f>
         <v>0, 0, 0, 0, 0</v>
       </c>
-      <c r="AK5" t="str">
+      <c r="AL5" t="str">
         <f>_xll.NCDK_AutocorrelationMass(B5)</f>
         <v>6, 6, 6, 3, 0</v>
       </c>
-      <c r="AL5" t="str">
+      <c r="AM5" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B5)</f>
         <v>233.87838834375, 233.87838834375, 233.87838834375, 116.939194171875, 0</v>
       </c>
-      <c r="AM5">
+      <c r="AN5">
         <f>_xll.NCDK_BasicGroupCount(B5)</f>
         <v>0</v>
       </c>
-      <c r="AN5" t="str">
+      <c r="AO5" t="str">
         <f>_xll.NCDK_BCUT(B5)</f>
         <v>11.85, 12.1500544016358, -0.211758152069243, 0.0882962495665529, 6.093375, 6.3934294016358</v>
       </c>
-      <c r="AO5">
+      <c r="AP5">
         <f>_xll.NCDK_BondCount(B5)</f>
         <v>0</v>
       </c>
-      <c r="AP5">
+      <c r="AQ5">
         <f>_xll.NCDK_BPol(B5)</f>
         <v>6.5592419999999994</v>
       </c>
-      <c r="AQ5" t="str">
+      <c r="AR5" t="str">
         <f>_xll.NCDK_CarbonTypes(B5)</f>
         <v>0, 0, 0, 6, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AR5" t="str">
+      <c r="AS5" t="str">
         <f>_xll.NCDK_ChiChain(B5)</f>
         <v>0, 0, 0, 0.125, 0, 0, 0, 0, 0.037037037037037, 0</v>
       </c>
-      <c r="AS5" t="str">
+      <c r="AT5" t="str">
         <f>_xll.NCDK_ChiCluster(B5)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AT5" t="str">
+      <c r="AU5" t="str">
         <f>_xll.NCDK_ChiPathCluster(B5)</f>
         <v>0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AU5" t="str">
+      <c r="AV5" t="str">
         <f>_xll.NCDK_ChiPath(B5)</f>
         <v>4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0, 3.46410161513775, 2, 1.15470053837925, 0.666666666666667, 0.384900179459751, 0.222222222222222, 0, 0</v>
       </c>
-      <c r="AV5" t="str">
+      <c r="AW5" t="str">
         <f>_xll.NCDK_CPSA(B5)</f>
         <v>#N/A</v>
       </c>
-      <c r="AW5">
+      <c r="AX5">
         <f>_xll.NCDK_EccentricConnectivityIndex(B5)</f>
         <v>36</v>
       </c>
-      <c r="AX5">
+      <c r="AY5">
         <f>_xll.NCDK_FMF(B5)</f>
         <v>1</v>
       </c>
-      <c r="AY5">
+      <c r="AZ5">
         <f>_xll.NCDK_FractionalPSA(B5)</f>
         <v>0</v>
       </c>
-      <c r="AZ5">
+      <c r="BA5">
         <f>_xll.NCDK_FragmentComplexity(B5)</f>
         <v>114</v>
       </c>
-      <c r="BA5" t="str">
+      <c r="BB5" t="str">
         <f>_xll.NCDK_GravitationalIndex(B5)</f>
         <v>#N/A</v>
       </c>
-      <c r="BB5">
+      <c r="BC5">
         <f>_xll.NCDK_HBondAcceptorCount(B5)</f>
         <v>0</v>
       </c>
-      <c r="BC5">
+      <c r="BD5">
         <f>_xll.NCDK_HBondDonorCount(B5)</f>
         <v>0</v>
       </c>
-      <c r="BD5">
+      <c r="BE5">
         <f>_xll.NCDK_HybridizationRatio(B5)</f>
         <v>0</v>
       </c>
-      <c r="BE5" t="str">
+      <c r="BF5" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B5)</f>
         <v>4.16666666666667, 2.22222222222222, 1.33333333333333</v>
       </c>
-      <c r="BF5" t="str">
+      <c r="BG5" t="str">
         <f>_xll.NCDK_KierHallSmarts(B5)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 6, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BG5">
+      <c r="BH5">
         <f>_xll.NCDK_LargestChain(B5)</f>
         <v>0</v>
       </c>
-      <c r="BH5">
+      <c r="BI5">
         <f>_xll.NCDK_LargestPiSystem(B5)</f>
         <v>6</v>
       </c>
-      <c r="BI5" t="str">
+      <c r="BJ5" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B5)</f>
         <v>#N/A</v>
       </c>
-      <c r="BJ5">
+      <c r="BK5">
         <f>_xll.NCDK_LongestAliphaticChain(B5)</f>
         <v>0</v>
       </c>
-      <c r="BK5" t="str">
+      <c r="BL5" t="str">
         <f>_xll.NCDK_MDE(B5)</f>
         <v>0, 0, 0, 0, 9.12546512839809, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BL5" t="str">
+      <c r="BM5" t="str">
         <f>_xll.NCDK_MomentOfInertia(B5)</f>
         <v>#N/A</v>
       </c>
-      <c r="BM5">
+      <c r="BN5">
         <f>_xll.NCDK_PetitjeanNumber(B5)</f>
         <v>0</v>
       </c>
-      <c r="BN5" t="str">
+      <c r="BO5" t="str">
         <f>_xll.NCDK_PetitjeanShapeIndex(B5)</f>
         <v>#N/A</v>
       </c>
-      <c r="BO5">
+      <c r="BP5">
         <f>_xll.NCDK_RotatableBondsCount(B5)</f>
         <v>0</v>
       </c>
-      <c r="BP5">
+      <c r="BQ5">
         <f>_xll.NCDK_RuleOfFive(B5)</f>
         <v>0</v>
       </c>
-      <c r="BQ5" t="str">
+      <c r="BR5" t="str">
         <f>_xll.NCDK_SmallRing(B5)</f>
         <v>1, 1, 1, 1, 0, 0, 0, 1, 0, 0, 0</v>
       </c>
-      <c r="BR5">
+      <c r="BS5">
         <f>_xll.NCDK_TPSA(B5)</f>
         <v>0</v>
       </c>
-      <c r="BS5">
+      <c r="BT5">
         <f>_xll.NCDK_VABC(B5)</f>
         <v>81.166531652800174</v>
       </c>
-      <c r="BT5">
+      <c r="BU5">
         <f>_xll.NCDK_VAdjMa(B5)</f>
         <v>3.5849625007211561</v>
       </c>
-      <c r="BU5" s="2">
+      <c r="BV5" s="2">
         <f>_xll.NCDK_MolecularWeight(B5)</f>
         <v>78.112059903682749</v>
       </c>
-      <c r="BV5" s="3">
+      <c r="BW5" s="3">
         <f>_xll.NCDK_ExactMass(B5)</f>
         <v>78.046950191999997</v>
       </c>
-      <c r="BW5" t="str">
+      <c r="BX5" t="str">
         <f>_xll.NCDK_WeightedPath(B5)</f>
         <v>11.8125, 1.96875, 0, 0, 0</v>
       </c>
-      <c r="BX5" t="str">
+      <c r="BY5" t="str">
         <f>_xll.NCDK_WHIM(B5)</f>
         <v>#N/A</v>
       </c>
-      <c r="BY5" t="str">
+      <c r="BZ5" t="str">
         <f>_xll.NCDK_WienerNumbers(B5)</f>
         <v>27, 3</v>
       </c>
-      <c r="BZ5">
+      <c r="CA5">
         <f>_xll.NCDK_ZagrebIndex(B5)</f>
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:78" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:79" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>84</v>
       </c>
@@ -4140,7 +4161,7 @@
         <v>InChI=1S/C7H8/c1-7-5-3-2-4-6-7/h2-6H,1H3</v>
       </c>
       <c r="D6">
-        <f>_xll.NCDK_Tanimoto($H6,$H7)</f>
+        <f>_xll.NCDK_Tanimoto($I6,$I7)</f>
         <v>0</v>
       </c>
       <c r="E6" t="str">
@@ -4148,299 +4169,303 @@
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001011010</v>
       </c>
       <c r="F6" t="str">
+        <f>_xll.RDKit_MACCSFingerprint(B6)</f>
+        <v>00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001011010</v>
+      </c>
+      <c r="G6" t="str">
         <f>_xll.NCDK_ECFP0($B6)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000100000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="G6" t="str">
+      <c r="H6" t="str">
         <f>_xll.NCDK_ECFP2($B6)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000100000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="H6" t="str">
+      <c r="I6" t="str">
         <f>_xll.NCDK_ECFP4($B6)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000100000000000000000000000000000010000000000000000000000000</v>
       </c>
-      <c r="I6" t="str">
+      <c r="J6" t="str">
         <f>_xll.NCDK_ECFP6($B6)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000010100000000001000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000100000000000000000000000000000010000000000000000000000000</v>
       </c>
-      <c r="J6" t="str">
+      <c r="K6" t="str">
         <f>_xll.NCDK_FCFP0($B6)</f>
         <v>1000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="K6" t="str">
+      <c r="L6" t="str">
         <f>_xll.NCDK_FCFP2($B6)</f>
         <v>1000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="L6" t="str">
+      <c r="M6" t="str">
         <f>_xll.NCDK_FCFP4($B6)</f>
         <v>1000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000001000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="M6" t="str">
+      <c r="N6" t="str">
         <f>_xll.NCDK_FCFP0($B6)</f>
         <v>1000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="N6" t="str">
+      <c r="O6" t="str">
         <f>_xll.NCDK_AtomPairs2DFingerprinter($B6)</f>
         <v>100000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="O6" t="str">
+      <c r="P6" t="str">
         <f>_xll.NCDK_EStateFingerprinter($B6)</f>
         <v>0000001000010000100000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="P6" t="str">
+      <c r="Q6" t="str">
         <f>_xll.NCDK_ExtendedFingerprinter($B6)</f>
         <v>000000000000000000000000000000000000000001000000000001000000010000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000010000000000000000000000000000000000000000000001000000000000010001</v>
       </c>
-      <c r="Q6" t="str">
+      <c r="R6" t="str">
         <f>_xll.NCDK_CDKFingerprinter($B6)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000010010000000000000000000000000000000000000000000000000001000000001000000000000000000000000000000100000000000000000100000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="R6" t="str">
+      <c r="S6" t="str">
         <f>_xll.NCDK_KlekotaRothFingerprinter($B6)</f>
         <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="S6" t="str">
+      <c r="T6" t="str">
         <f>_xll.NCDK_LingoFingerprinter($B6)</f>
         <v>0000000000000000000000001000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000100000000000000000000</v>
       </c>
-      <c r="T6" t="str">
+      <c r="U6" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($B6)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001011010</v>
       </c>
-      <c r="U6" t="str">
+      <c r="V6" t="str">
         <f>_xll.NCDK_ShortestPathFingerprinter($B6)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000100000000000000000100000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000001000000000001000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000101</v>
       </c>
-      <c r="V6" t="str">
+      <c r="W6" t="str">
         <f>_xll.NCDK_SubstructureFingerprinter($B6)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000001</v>
       </c>
-      <c r="W6" t="str">
+      <c r="X6" t="str">
         <f>_xll.NCDK_PubchemFingerprinter($B6)</f>
         <v>00000000011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000001100000000000000000000000000000000000000000000000110000000000100000000001100000000000001100100000000010000000000000000000000000000000100000000000001000100000010000100000000000000000000000100000000000000000001000000000000000000000000010001000100000000000000000000000000010001000000010000010000000100010100000000001000100010000100000000010000000000000001000001000000000000000000010001000100000000111000000001000000000000000000011100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="X6" s="2">
+      <c r="Y6" s="2">
         <f>_xll.NCDK_MolecularWeight(B6)</f>
         <v>92.13867730812234</v>
       </c>
-      <c r="Y6" s="2">
+      <c r="Z6" s="2">
         <f>_xll.NCDK_ExactMass(B6)</f>
         <v>92.062600255999996</v>
       </c>
-      <c r="Z6">
+      <c r="AA6">
         <f>_xll.NCDK_AcidicGroupCount(B6)</f>
         <v>0</v>
       </c>
-      <c r="AA6" s="4">
+      <c r="AB6" s="4">
         <f>_xll.NCDK_ALogP(B6)</f>
         <v>2.3162000000000003</v>
       </c>
-      <c r="AB6" s="4">
+      <c r="AC6" s="4">
         <f>_xll.NCDK_XLogP(B6)</f>
         <v>2.4590000000000001</v>
       </c>
-      <c r="AC6" s="4">
+      <c r="AD6" s="4">
         <f>_xll.NCDK_MannholdLogP(B6)</f>
         <v>2.23</v>
       </c>
-      <c r="AD6" s="4">
+      <c r="AE6" s="4">
         <f>_xll.NCDK_JPlogP(B6)</f>
         <v>2.3300074064489729</v>
       </c>
-      <c r="AE6">
+      <c r="AF6">
         <f>_xll.NCDK_AMolarRefractivity(B6)</f>
         <v>31.0992</v>
       </c>
-      <c r="AF6">
+      <c r="AG6">
         <f>_xll.NCDK_APol(B6)</f>
         <v>17.654343999999998</v>
       </c>
-      <c r="AG6">
+      <c r="AH6">
         <f>_xll.NCDK_AromaticAtomsCount(B6)</f>
         <v>6</v>
       </c>
-      <c r="AH6">
+      <c r="AI6">
         <f>_xll.NCDK_AromaticBondsCount(B6)</f>
         <v>6</v>
       </c>
-      <c r="AI6">
+      <c r="AJ6">
         <f>_xll.NCDK_AtomCount(B6)</f>
         <v>15</v>
       </c>
-      <c r="AJ6" t="str">
+      <c r="AK6" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B6)</f>
         <v>0.00145821501522747, -0.000488055819316601, -0.000225165712015084, -1.53979004755717E-05, -4.88075806479512E-07</v>
       </c>
-      <c r="AK6" t="str">
+      <c r="AL6" t="str">
         <f>_xll.NCDK_AutocorrelationMass(B6)</f>
         <v>7, 7, 8, 5, 1</v>
       </c>
-      <c r="AL6" t="str">
+      <c r="AM6" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B6)</f>
         <v>310.962687273438, 320.438287539063, 355.858255328125, 213.793837835938, 36.9196446054688</v>
       </c>
-      <c r="AM6">
+      <c r="AN6">
         <f>_xll.NCDK_BasicGroupCount(B6)</f>
         <v>0</v>
       </c>
-      <c r="AN6" t="str">
+      <c r="AO6" t="str">
         <f>_xll.NCDK_BCUT(B6)</f>
         <v>11.89, 12.1100942558098, -0.155208136358149, 0.0651359477608963, 5.76122693815409, 7.50783741355056</v>
       </c>
-      <c r="AO6">
+      <c r="AP6">
         <f>_xll.NCDK_BondCount(B6)</f>
         <v>0</v>
       </c>
-      <c r="AP6">
+      <c r="AQ6">
         <f>_xll.NCDK_BPol(B6)</f>
         <v>8.7456560000000003</v>
       </c>
-      <c r="AQ6" t="str">
+      <c r="AR6" t="str">
         <f>_xll.NCDK_CarbonTypes(B6)</f>
         <v>0, 0, 0, 5, 1, 1, 0, 0, 0</v>
       </c>
-      <c r="AR6" t="str">
+      <c r="AS6" t="str">
         <f>_xll.NCDK_ChiChain(B6)</f>
         <v>0, 0, 0, 0.102062072615966, 0.102062072615966, 0, 0, 0, 0.0320750149549792, 0.0320750149549792</v>
       </c>
-      <c r="AS6" t="str">
+      <c r="AT6" t="str">
         <f>_xll.NCDK_ChiCluster(B6)</f>
         <v>0.288675134594813, 0, 0, 0, 0.166666666666667, 0, 0, 0</v>
       </c>
-      <c r="AT6" t="str">
+      <c r="AU6" t="str">
         <f>_xll.NCDK_ChiPathCluster(B6)</f>
         <v>0.408248290463863, 0.433012701892219, 0.408248290463863, 0.192450089729875, 0.166666666666667, 0.128300059819917</v>
       </c>
-      <c r="AU6" t="str">
+      <c r="AV6" t="str">
         <f>_xll.NCDK_ChiPath(B6)</f>
         <v>5.11288417512236, 3.39384685011735, 2.74318215649199, 1.89384685011735, 1.30671282224753, 0.901047570290607, 0.204124145231932, 0, 4.38675134594813, 2.41068360252296, 1.65470053837925, 0.940455735015306, 0.534377897417612, 0.303561200840986, 0.0641500299099584, 0</v>
       </c>
-      <c r="AV6" t="str">
+      <c r="AW6" t="str">
         <f>_xll.NCDK_CPSA(B6)</f>
         <v>#N/A</v>
       </c>
-      <c r="AW6">
+      <c r="AX6">
         <f>_xll.NCDK_EccentricConnectivityIndex(B6)</f>
         <v>45</v>
       </c>
-      <c r="AX6">
+      <c r="AY6">
         <f>_xll.NCDK_FMF(B6)</f>
         <v>0.8571428571428571</v>
       </c>
-      <c r="AY6">
+      <c r="AZ6">
         <f>_xll.NCDK_FractionalPSA(B6)</f>
         <v>0</v>
       </c>
-      <c r="AZ6">
+      <c r="BA6">
         <f>_xll.NCDK_FragmentComplexity(B6)</f>
         <v>183</v>
       </c>
-      <c r="BA6" t="str">
+      <c r="BB6" t="str">
         <f>_xll.NCDK_GravitationalIndex(B6)</f>
         <v>#N/A</v>
       </c>
-      <c r="BB6">
+      <c r="BC6">
         <f>_xll.NCDK_HBondAcceptorCount(B6)</f>
         <v>0</v>
       </c>
-      <c r="BC6">
+      <c r="BD6">
         <f>_xll.NCDK_HBondDonorCount(B6)</f>
         <v>0</v>
       </c>
-      <c r="BD6">
+      <c r="BE6">
         <f>_xll.NCDK_HybridizationRatio(B6)</f>
         <v>0.14285714285714285</v>
       </c>
-      <c r="BE6" t="str">
+      <c r="BF6" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B6)</f>
         <v>5.14285714285714, 2.34375, 1.5</v>
       </c>
-      <c r="BF6" t="str">
+      <c r="BG6" t="str">
         <f>_xll.NCDK_KierHallSmarts(B6)</f>
         <v>0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 5, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BG6">
+      <c r="BH6">
         <f>_xll.NCDK_LargestChain(B6)</f>
         <v>0</v>
       </c>
-      <c r="BH6">
+      <c r="BI6">
         <f>_xll.NCDK_LargestPiSystem(B6)</f>
         <v>6</v>
       </c>
-      <c r="BI6" t="str">
+      <c r="BJ6" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B6)</f>
         <v>#N/A</v>
       </c>
-      <c r="BJ6">
+      <c r="BK6">
         <f>_xll.NCDK_LongestAliphaticChain(B6)</f>
         <v>0</v>
       </c>
-      <c r="BK6" t="str">
+      <c r="BL6" t="str">
         <f>_xll.NCDK_MDE(B6)</f>
         <v>0, 1.85053586243577, 1, 0, 6.08364341893206, 3.04182170946603, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BL6" t="str">
+      <c r="BM6" t="str">
         <f>_xll.NCDK_MomentOfInertia(B6)</f>
         <v>#N/A</v>
       </c>
-      <c r="BM6">
+      <c r="BN6">
         <f>_xll.NCDK_PetitjeanNumber(B6)</f>
         <v>0.25</v>
       </c>
-      <c r="BN6" t="str">
+      <c r="BO6" t="str">
         <f>_xll.NCDK_PetitjeanShapeIndex(B6)</f>
         <v>#N/A</v>
       </c>
-      <c r="BO6">
+      <c r="BP6">
         <f>_xll.NCDK_RotatableBondsCount(B6)</f>
         <v>0</v>
       </c>
-      <c r="BP6">
+      <c r="BQ6">
         <f>_xll.NCDK_RuleOfFive(B6)</f>
         <v>0</v>
       </c>
-      <c r="BQ6" t="str">
+      <c r="BR6" t="str">
         <f>_xll.NCDK_SmallRing(B6)</f>
         <v>1, 1, 1, 1, 0, 0, 0, 1, 0, 0, 0</v>
       </c>
-      <c r="BR6">
+      <c r="BS6">
         <f>_xll.NCDK_TPSA(B6)</f>
         <v>0</v>
       </c>
-      <c r="BS6">
+      <c r="BT6">
         <f>_xll.NCDK_VABC(B6)</f>
         <v>98.462516278666868</v>
       </c>
-      <c r="BT6">
+      <c r="BU6">
         <f>_xll.NCDK_VAdjMa(B6)</f>
         <v>3.8073549220576042</v>
       </c>
-      <c r="BU6" s="2">
+      <c r="BV6" s="2">
         <f>_xll.NCDK_MolecularWeight(B6)</f>
         <v>92.13867730812234</v>
       </c>
-      <c r="BV6" s="3">
+      <c r="BW6" s="3">
         <f>_xll.NCDK_ExactMass(B6)</f>
         <v>92.062600255999996</v>
       </c>
-      <c r="BW6" t="str">
+      <c r="BX6" t="str">
         <f>_xll.NCDK_WeightedPath(B6)</f>
         <v>13.6768253204364, 1.95383218863377, 0, 0, 0</v>
       </c>
-      <c r="BX6" t="str">
+      <c r="BY6" t="str">
         <f>_xll.NCDK_WHIM(B6)</f>
         <v>#N/A</v>
       </c>
-      <c r="BY6" t="str">
+      <c r="BZ6" t="str">
         <f>_xll.NCDK_WienerNumbers(B6)</f>
         <v>42, 5</v>
       </c>
-      <c r="BZ6">
+      <c r="CA6">
         <f>_xll.NCDK_ZagrebIndex(B6)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:78" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:79" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -4452,7 +4477,7 @@
         <v>C1CCCCC1</v>
       </c>
       <c r="D7">
-        <f>_xll.NCDK_Tanimoto($H7,$H8)</f>
+        <f>_xll.NCDK_Tanimoto($I7,$I8)</f>
         <v>1</v>
       </c>
       <c r="E7" t="str">
@@ -4460,299 +4485,303 @@
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000010000000000000000010000000000000001010</v>
       </c>
       <c r="F7" t="str">
+        <f>_xll.RDKit_MACCSFingerprint(B7)</f>
+        <v>00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="G7" t="str">
         <f>_xll.NCDK_ECFP0($B7)</f>
         <v>0000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="G7" t="str">
+      <c r="H7" t="str">
         <f>_xll.NCDK_ECFP2($B7)</f>
         <v>0000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="H7" t="str">
+      <c r="I7" t="str">
         <f>_xll.NCDK_ECFP4($B7)</f>
         <v>0000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="I7" t="str">
+      <c r="J7" t="str">
         <f>_xll.NCDK_ECFP6($B7)</f>
         <v>0000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="J7" t="str">
+      <c r="K7" t="str">
         <f>_xll.NCDK_FCFP0($B7)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="K7" t="str">
+      <c r="L7" t="str">
         <f>_xll.NCDK_FCFP2($B7)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="L7" t="str">
+      <c r="M7" t="str">
         <f>_xll.NCDK_FCFP4($B7)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="M7" t="str">
+      <c r="N7" t="str">
         <f>_xll.NCDK_FCFP0($B7)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="N7" t="str">
+      <c r="O7" t="str">
         <f>_xll.NCDK_AtomPairs2DFingerprinter($B7)</f>
         <v>100000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="O7" t="str">
+      <c r="P7" t="str">
         <f>_xll.NCDK_EStateFingerprinter($B7)</f>
         <v>0000000010000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="P7" t="str">
+      <c r="Q7" t="str">
         <f>_xll.NCDK_ExtendedFingerprinter($B7)</f>
         <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000001000000000000010001</v>
       </c>
-      <c r="Q7" t="str">
+      <c r="R7" t="str">
         <f>_xll.NCDK_CDKFingerprinter($B7)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000010000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="R7" t="str">
+      <c r="S7" t="str">
         <f>_xll.NCDK_KlekotaRothFingerprinter($B7)</f>
         <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000010000000000000100000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="S7" t="str">
+      <c r="T7" t="str">
         <f>_xll.NCDK_LingoFingerprinter($B7)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="T7" t="str">
+      <c r="U7" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($B7)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000010000000000000000010000000000000001010</v>
       </c>
-      <c r="U7" t="str">
+      <c r="V7" t="str">
         <f>_xll.NCDK_ShortestPathFingerprinter($B7)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="V7" t="str">
+      <c r="W7" t="str">
         <f>_xll.NCDK_SubstructureFingerprinter($B7)</f>
         <v>0100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="W7" t="str">
+      <c r="X7" t="str">
         <f>_xll.NCDK_PubchemFingerprinter($B7)</f>
         <v>00000000011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="X7" s="2">
+      <c r="Y7" s="2">
         <f>_xll.NCDK_MolecularWeight(B7)</f>
         <v>72.064415380728008</v>
       </c>
-      <c r="Y7" s="2">
+      <c r="Z7" s="2">
         <f>_xll.NCDK_ExactMass(B7)</f>
         <v>72</v>
       </c>
-      <c r="Z7">
+      <c r="AA7">
         <f>_xll.NCDK_AcidicGroupCount(B7)</f>
         <v>0</v>
       </c>
-      <c r="AA7" s="4">
+      <c r="AB7" s="4">
         <f>_xll.NCDK_ALogP(B7)</f>
         <v>2.7372000000000005</v>
       </c>
-      <c r="AB7" s="4">
+      <c r="AC7" s="4">
         <f>_xll.NCDK_XLogP(B7)</f>
         <v>3.4139999999999997</v>
       </c>
-      <c r="AC7" s="4">
+      <c r="AD7" s="4">
         <f>_xll.NCDK_MannholdLogP(B7)</f>
         <v>2.12</v>
       </c>
-      <c r="AD7" s="4">
+      <c r="AE7" s="4">
         <f>_xll.NCDK_JPlogP(B7)</f>
         <v>2.6952762459207973</v>
       </c>
-      <c r="AE7">
+      <c r="AF7">
         <f>_xll.NCDK_AMolarRefractivity(B7)</f>
         <v>27.606000000000002</v>
       </c>
-      <c r="AF7">
+      <c r="AG7">
         <f>_xll.NCDK_APol(B7)</f>
         <v>18.561516000000001</v>
       </c>
-      <c r="AG7">
+      <c r="AH7">
         <f>_xll.NCDK_AromaticAtomsCount(B7)</f>
         <v>0</v>
       </c>
-      <c r="AH7">
+      <c r="AI7">
         <f>_xll.NCDK_AromaticBondsCount(B7)</f>
         <v>0</v>
       </c>
-      <c r="AI7">
+      <c r="AJ7">
         <f>_xll.NCDK_AtomCount(B7)</f>
         <v>18</v>
       </c>
-      <c r="AJ7" t="str">
+      <c r="AK7" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B7)</f>
         <v>0, 0, 0, 0, 0</v>
       </c>
-      <c r="AK7" t="str">
+      <c r="AL7" t="str">
         <f>_xll.NCDK_AutocorrelationMass(B7)</f>
         <v>6, 6, 6, 3, 0</v>
       </c>
-      <c r="AL7" t="str">
+      <c r="AM7" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B7)</f>
         <v>257.709834375, 257.709834375, 257.709834375, 128.8549171875, 0</v>
       </c>
-      <c r="AM7">
+      <c r="AN7">
         <f>_xll.NCDK_BasicGroupCount(B7)</f>
         <v>0</v>
       </c>
-      <c r="AN7" t="str">
+      <c r="AO7" t="str">
         <f>_xll.NCDK_BCUT(B7)</f>
         <v>11.9, 12.1000824042221, -0.15279744210896, 0.0472849621131451, 6.45375, 6.65383240422211</v>
       </c>
-      <c r="AO7">
+      <c r="AP7">
         <f>_xll.NCDK_BondCount(B7)</f>
         <v>0</v>
       </c>
-      <c r="AP7">
+      <c r="AQ7">
         <f>_xll.NCDK_BPol(B7)</f>
         <v>13.118483999999999</v>
       </c>
-      <c r="AQ7" t="str">
+      <c r="AR7" t="str">
         <f>_xll.NCDK_CarbonTypes(B7)</f>
         <v>0, 0, 0, 0, 0, 0, 6, 0, 0</v>
       </c>
-      <c r="AR7" t="str">
+      <c r="AS7" t="str">
         <f>_xll.NCDK_ChiChain(B7)</f>
         <v>0, 0, 0, 0.125, 0, 0, 0, 0, 0.125, 0</v>
       </c>
-      <c r="AS7" t="str">
+      <c r="AT7" t="str">
         <f>_xll.NCDK_ChiCluster(B7)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AT7" t="str">
+      <c r="AU7" t="str">
         <f>_xll.NCDK_ChiPathCluster(B7)</f>
         <v>0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AU7" t="str">
+      <c r="AV7" t="str">
         <f>_xll.NCDK_ChiPath(B7)</f>
         <v>4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0, 4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0</v>
       </c>
-      <c r="AV7" t="str">
+      <c r="AW7" t="str">
         <f>_xll.NCDK_CPSA(B7)</f>
         <v>#N/A</v>
       </c>
-      <c r="AW7">
+      <c r="AX7">
         <f>_xll.NCDK_EccentricConnectivityIndex(B7)</f>
         <v>36</v>
       </c>
-      <c r="AX7">
+      <c r="AY7">
         <f>_xll.NCDK_FMF(B7)</f>
         <v>1</v>
       </c>
-      <c r="AY7">
+      <c r="AZ7">
         <f>_xll.NCDK_FractionalPSA(B7)</f>
         <v>0</v>
       </c>
-      <c r="AZ7">
+      <c r="BA7">
         <f>_xll.NCDK_FragmentComplexity(B7)</f>
         <v>6</v>
       </c>
-      <c r="BA7" t="str">
+      <c r="BB7" t="str">
         <f>_xll.NCDK_GravitationalIndex(B7)</f>
         <v>#N/A</v>
       </c>
-      <c r="BB7">
+      <c r="BC7">
         <f>_xll.NCDK_HBondAcceptorCount(B7)</f>
         <v>0</v>
       </c>
-      <c r="BC7">
+      <c r="BD7">
         <f>_xll.NCDK_HBondDonorCount(B7)</f>
         <v>0</v>
       </c>
-      <c r="BD7">
+      <c r="BE7">
         <f>_xll.NCDK_HybridizationRatio(B7)</f>
         <v>1</v>
       </c>
-      <c r="BE7" t="str">
+      <c r="BF7" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B7)</f>
         <v>4.16666666666667, 2.22222222222222, 1.33333333333333</v>
       </c>
-      <c r="BF7" t="str">
+      <c r="BG7" t="str">
         <f>_xll.NCDK_KierHallSmarts(B7)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 6, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BG7">
+      <c r="BH7">
         <f>_xll.NCDK_LargestChain(B7)</f>
         <v>0</v>
       </c>
-      <c r="BH7">
+      <c r="BI7">
         <f>_xll.NCDK_LargestPiSystem(B7)</f>
         <v>0</v>
       </c>
-      <c r="BI7" t="str">
+      <c r="BJ7" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B7)</f>
         <v>#N/A</v>
       </c>
-      <c r="BJ7">
+      <c r="BK7">
         <f>_xll.NCDK_LongestAliphaticChain(B7)</f>
         <v>0</v>
       </c>
-      <c r="BK7" t="str">
+      <c r="BL7" t="str">
         <f>_xll.NCDK_MDE(B7)</f>
         <v>0, 0, 0, 0, 9.12546512839809, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BL7" t="str">
+      <c r="BM7" t="str">
         <f>_xll.NCDK_MomentOfInertia(B7)</f>
         <v>#N/A</v>
       </c>
-      <c r="BM7">
+      <c r="BN7">
         <f>_xll.NCDK_PetitjeanNumber(B7)</f>
         <v>0</v>
       </c>
-      <c r="BN7" t="str">
+      <c r="BO7" t="str">
         <f>_xll.NCDK_PetitjeanShapeIndex(B7)</f>
         <v>#N/A</v>
       </c>
-      <c r="BO7">
+      <c r="BP7">
         <f>_xll.NCDK_RotatableBondsCount(B7)</f>
         <v>0</v>
       </c>
-      <c r="BP7">
+      <c r="BQ7">
         <f>_xll.NCDK_RuleOfFive(B7)</f>
         <v>0</v>
       </c>
-      <c r="BQ7" t="str">
+      <c r="BR7" t="str">
         <f>_xll.NCDK_SmallRing(B7)</f>
         <v>1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0</v>
       </c>
-      <c r="BR7">
+      <c r="BS7">
         <f>_xll.NCDK_TPSA(B7)</f>
         <v>0</v>
       </c>
-      <c r="BS7">
+      <c r="BT7">
         <f>_xll.NCDK_VABC(B7)</f>
         <v>99.975907755200197</v>
       </c>
-      <c r="BT7">
+      <c r="BU7">
         <f>_xll.NCDK_VAdjMa(B7)</f>
         <v>3.5849625007211561</v>
       </c>
-      <c r="BU7" s="2">
+      <c r="BV7" s="2">
         <f>_xll.NCDK_MolecularWeight(B7)</f>
         <v>72.064415380728008</v>
       </c>
-      <c r="BV7" s="3">
+      <c r="BW7" s="3">
         <f>_xll.NCDK_ExactMass(B7)</f>
         <v>72</v>
       </c>
-      <c r="BW7" t="str">
+      <c r="BX7" t="str">
         <f>_xll.NCDK_WeightedPath(B7)</f>
         <v>11.8125, 1.96875, 0, 0, 0</v>
       </c>
-      <c r="BX7" t="str">
+      <c r="BY7" t="str">
         <f>_xll.NCDK_WHIM(B7)</f>
         <v>#N/A</v>
       </c>
-      <c r="BY7" t="str">
+      <c r="BZ7" t="str">
         <f>_xll.NCDK_WienerNumbers(B7)</f>
         <v>27, 3</v>
       </c>
-      <c r="BZ7">
+      <c r="CA7">
         <f>_xll.NCDK_ZagrebIndex(B7)</f>
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:78" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:79" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -4764,7 +4793,7 @@
         <v>XDTMQSROBMDMFD-UHFFFAOYSA-N</v>
       </c>
       <c r="D8">
-        <f>_xll.NCDK_Tanimoto($H8,$H9)</f>
+        <f>_xll.NCDK_Tanimoto($I8,$I9)</f>
         <v>1</v>
       </c>
       <c r="E8" t="str">
@@ -4772,299 +4801,303 @@
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000010000000000000000010000000000000001010</v>
       </c>
       <c r="F8" t="str">
+        <f>_xll.RDKit_MACCSFingerprint(B8)</f>
+        <v>00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="G8" t="str">
         <f>_xll.NCDK_ECFP0($B8)</f>
         <v>0000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="G8" t="str">
+      <c r="H8" t="str">
         <f>_xll.NCDK_ECFP2($B8)</f>
         <v>0000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="H8" t="str">
+      <c r="I8" t="str">
         <f>_xll.NCDK_ECFP4($B8)</f>
         <v>0000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="I8" t="str">
+      <c r="J8" t="str">
         <f>_xll.NCDK_ECFP6($B8)</f>
         <v>0000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="J8" t="str">
+      <c r="K8" t="str">
         <f>_xll.NCDK_FCFP0($B8)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="K8" t="str">
+      <c r="L8" t="str">
         <f>_xll.NCDK_FCFP2($B8)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="L8" t="str">
+      <c r="M8" t="str">
         <f>_xll.NCDK_FCFP4($B8)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="M8" t="str">
+      <c r="N8" t="str">
         <f>_xll.NCDK_FCFP0($B8)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="N8" t="str">
+      <c r="O8" t="str">
         <f>_xll.NCDK_AtomPairs2DFingerprinter($B8)</f>
         <v>100000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="O8" t="str">
+      <c r="P8" t="str">
         <f>_xll.NCDK_EStateFingerprinter($B8)</f>
         <v>0000000010000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="P8" t="str">
+      <c r="Q8" t="str">
         <f>_xll.NCDK_ExtendedFingerprinter($B8)</f>
         <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000001000000000000010001</v>
       </c>
-      <c r="Q8" t="str">
+      <c r="R8" t="str">
         <f>_xll.NCDK_CDKFingerprinter($B8)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000010000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="R8" t="str">
+      <c r="S8" t="str">
         <f>_xll.NCDK_KlekotaRothFingerprinter($B8)</f>
         <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000010000000000000100000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="S8" t="str">
+      <c r="T8" t="str">
         <f>_xll.NCDK_LingoFingerprinter($B8)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="T8" t="str">
+      <c r="U8" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($B8)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000010000000000000000010000000000000001010</v>
       </c>
-      <c r="U8" t="str">
+      <c r="V8" t="str">
         <f>_xll.NCDK_ShortestPathFingerprinter($B8)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="V8" t="str">
+      <c r="W8" t="str">
         <f>_xll.NCDK_SubstructureFingerprinter($B8)</f>
         <v>0100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="W8" t="str">
+      <c r="X8" t="str">
         <f>_xll.NCDK_PubchemFingerprinter($B8)</f>
         <v>00000000011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000100000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="X8" s="2">
+      <c r="Y8" s="2">
         <f>_xll.NCDK_MolecularWeight(B8)</f>
         <v>72.064415380728008</v>
       </c>
-      <c r="Y8" s="2">
+      <c r="Z8" s="2">
         <f>_xll.NCDK_ExactMass(B8)</f>
         <v>72</v>
       </c>
-      <c r="Z8">
+      <c r="AA8">
         <f>_xll.NCDK_AcidicGroupCount(B8)</f>
         <v>0</v>
       </c>
-      <c r="AA8" s="4">
+      <c r="AB8" s="4">
         <f>_xll.NCDK_ALogP(B8)</f>
         <v>2.7372000000000005</v>
       </c>
-      <c r="AB8" s="4">
+      <c r="AC8" s="4">
         <f>_xll.NCDK_XLogP(B8)</f>
         <v>3.4139999999999997</v>
       </c>
-      <c r="AC8" s="4">
+      <c r="AD8" s="4">
         <f>_xll.NCDK_MannholdLogP(B8)</f>
         <v>2.12</v>
       </c>
-      <c r="AD8" s="4">
+      <c r="AE8" s="4">
         <f>_xll.NCDK_JPlogP(B8)</f>
         <v>2.6952762459207973</v>
       </c>
-      <c r="AE8">
+      <c r="AF8">
         <f>_xll.NCDK_AMolarRefractivity(B8)</f>
         <v>27.606000000000002</v>
       </c>
-      <c r="AF8">
+      <c r="AG8">
         <f>_xll.NCDK_APol(B8)</f>
         <v>18.561516000000001</v>
       </c>
-      <c r="AG8">
+      <c r="AH8">
         <f>_xll.NCDK_AromaticAtomsCount(B8)</f>
         <v>0</v>
       </c>
-      <c r="AH8">
+      <c r="AI8">
         <f>_xll.NCDK_AromaticBondsCount(B8)</f>
         <v>0</v>
       </c>
-      <c r="AI8">
+      <c r="AJ8">
         <f>_xll.NCDK_AtomCount(B8)</f>
         <v>6</v>
       </c>
-      <c r="AJ8" t="str">
+      <c r="AK8" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B8)</f>
         <v>0, 0, 0, 0, 0</v>
       </c>
-      <c r="AK8" t="str">
+      <c r="AL8" t="str">
         <f>_xll.NCDK_AutocorrelationMass(B8)</f>
         <v>6, 6, 6, 3, 0</v>
       </c>
-      <c r="AL8" t="str">
+      <c r="AM8" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B8)</f>
         <v>257.709834375, 257.709834375, 257.709834375, 128.8549171875, 0</v>
       </c>
-      <c r="AM8">
+      <c r="AN8">
         <f>_xll.NCDK_BasicGroupCount(B8)</f>
         <v>0</v>
       </c>
-      <c r="AN8" t="str">
+      <c r="AO8" t="str">
         <f>_xll.NCDK_BCUT(B8)</f>
         <v>11.9, 12.1000824042221, -0.15279744210896, 0.0472849621131451, 6.45375, 6.65383240422211</v>
       </c>
-      <c r="AO8">
+      <c r="AP8">
         <f>_xll.NCDK_BondCount(B8)</f>
         <v>0</v>
       </c>
-      <c r="AP8">
+      <c r="AQ8">
         <f>_xll.NCDK_BPol(B8)</f>
         <v>0</v>
       </c>
-      <c r="AQ8" t="str">
+      <c r="AR8" t="str">
         <f>_xll.NCDK_CarbonTypes(B8)</f>
         <v>0, 0, 0, 0, 0, 0, 6, 0, 0</v>
       </c>
-      <c r="AR8" t="str">
+      <c r="AS8" t="str">
         <f>_xll.NCDK_ChiChain(B8)</f>
         <v>0, 0, 0, 0.125, 0, 0, 0, 0, 0.125, 0</v>
       </c>
-      <c r="AS8" t="str">
+      <c r="AT8" t="str">
         <f>_xll.NCDK_ChiCluster(B8)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AT8" t="str">
+      <c r="AU8" t="str">
         <f>_xll.NCDK_ChiPathCluster(B8)</f>
         <v>0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AU8" t="str">
+      <c r="AV8" t="str">
         <f>_xll.NCDK_ChiPath(B8)</f>
         <v>4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0, 4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0</v>
       </c>
-      <c r="AV8" t="str">
+      <c r="AW8" t="str">
         <f>_xll.NCDK_CPSA(B8)</f>
         <v>#N/A</v>
       </c>
-      <c r="AW8">
+      <c r="AX8">
         <f>_xll.NCDK_EccentricConnectivityIndex(B8)</f>
         <v>36</v>
       </c>
-      <c r="AX8">
+      <c r="AY8">
         <f>_xll.NCDK_FMF(B8)</f>
         <v>1</v>
       </c>
-      <c r="AY8">
+      <c r="AZ8">
         <f>_xll.NCDK_FractionalPSA(B8)</f>
         <v>0</v>
       </c>
-      <c r="AZ8">
+      <c r="BA8">
         <f>_xll.NCDK_FragmentComplexity(B8)</f>
         <v>294</v>
       </c>
-      <c r="BA8" t="str">
+      <c r="BB8" t="str">
         <f>_xll.NCDK_GravitationalIndex(B8)</f>
         <v>#N/A</v>
       </c>
-      <c r="BB8">
+      <c r="BC8">
         <f>_xll.NCDK_HBondAcceptorCount(B8)</f>
         <v>0</v>
       </c>
-      <c r="BC8">
+      <c r="BD8">
         <f>_xll.NCDK_HBondDonorCount(B8)</f>
         <v>0</v>
       </c>
-      <c r="BD8">
+      <c r="BE8">
         <f>_xll.NCDK_HybridizationRatio(B8)</f>
         <v>1</v>
       </c>
-      <c r="BE8" t="str">
+      <c r="BF8" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B8)</f>
         <v>4.16666666666667, 2.22222222222222, 1.33333333333333</v>
       </c>
-      <c r="BF8" t="str">
+      <c r="BG8" t="str">
         <f>_xll.NCDK_KierHallSmarts(B8)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BG8">
+      <c r="BH8">
         <f>_xll.NCDK_LargestChain(B8)</f>
         <v>0</v>
       </c>
-      <c r="BH8">
+      <c r="BI8">
         <f>_xll.NCDK_LargestPiSystem(B8)</f>
         <v>0</v>
       </c>
-      <c r="BI8" t="str">
+      <c r="BJ8" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B8)</f>
         <v>#N/A</v>
       </c>
-      <c r="BJ8">
+      <c r="BK8">
         <f>_xll.NCDK_LongestAliphaticChain(B8)</f>
         <v>0</v>
       </c>
-      <c r="BK8" t="str">
+      <c r="BL8" t="str">
         <f>_xll.NCDK_MDE(B8)</f>
         <v>0, 0, 0, 0, 9.12546512839809, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BL8" t="str">
+      <c r="BM8" t="str">
         <f>_xll.NCDK_MomentOfInertia(B8)</f>
         <v>#N/A</v>
       </c>
-      <c r="BM8">
+      <c r="BN8">
         <f>_xll.NCDK_PetitjeanNumber(B8)</f>
         <v>0</v>
       </c>
-      <c r="BN8" t="str">
+      <c r="BO8" t="str">
         <f>_xll.NCDK_PetitjeanShapeIndex(B8)</f>
         <v>#N/A</v>
       </c>
-      <c r="BO8">
+      <c r="BP8">
         <f>_xll.NCDK_RotatableBondsCount(B8)</f>
         <v>0</v>
       </c>
-      <c r="BP8">
+      <c r="BQ8">
         <f>_xll.NCDK_RuleOfFive(B8)</f>
         <v>0</v>
       </c>
-      <c r="BQ8" t="str">
+      <c r="BR8" t="str">
         <f>_xll.NCDK_SmallRing(B8)</f>
         <v>1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0</v>
       </c>
-      <c r="BR8">
+      <c r="BS8">
         <f>_xll.NCDK_TPSA(B8)</f>
         <v>0</v>
       </c>
-      <c r="BS8">
+      <c r="BT8">
         <f>_xll.NCDK_VABC(B8)</f>
         <v>99.975907755200197</v>
       </c>
-      <c r="BT8">
+      <c r="BU8">
         <f>_xll.NCDK_VAdjMa(B8)</f>
         <v>3.5849625007211561</v>
       </c>
-      <c r="BU8" s="2">
+      <c r="BV8" s="2">
         <f>_xll.NCDK_MolecularWeight(B8)</f>
         <v>72.064415380728008</v>
       </c>
-      <c r="BV8" s="3">
+      <c r="BW8" s="3">
         <f>_xll.NCDK_ExactMass(B8)</f>
         <v>72</v>
       </c>
-      <c r="BW8" t="str">
+      <c r="BX8" t="str">
         <f>_xll.NCDK_WeightedPath(B8)</f>
         <v>11.8125, 1.96875, 0, 0, 0</v>
       </c>
-      <c r="BX8" t="str">
+      <c r="BY8" t="str">
         <f>_xll.NCDK_WHIM(B8)</f>
         <v>#N/A</v>
       </c>
-      <c r="BY8" t="str">
+      <c r="BZ8" t="str">
         <f>_xll.NCDK_WienerNumbers(B8)</f>
         <v>27, 3</v>
       </c>
-      <c r="BZ8">
+      <c r="CA8">
         <f>_xll.NCDK_ZagrebIndex(B8)</f>
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:78" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:79" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -5076,7 +5109,7 @@
         <v>XDTMQSROBMDMFD-UHFFFAOYSA-N</v>
       </c>
       <c r="D9">
-        <f>_xll.NCDK_Tanimoto($H9,$H10)</f>
+        <f>_xll.NCDK_Tanimoto($I9,$I10)</f>
         <v>1.9607843137254902E-2</v>
       </c>
       <c r="E9" t="str">
@@ -5084,299 +5117,303 @@
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000010000000000000000010000000000000001010</v>
       </c>
       <c r="F9" t="str">
+        <f>_xll.RDKit_MACCSFingerprint(B9)</f>
+        <v>00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="G9" t="str">
         <f>_xll.NCDK_ECFP0($B9)</f>
         <v>0000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="G9" t="str">
+      <c r="H9" t="str">
         <f>_xll.NCDK_ECFP2($B9)</f>
         <v>0000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="H9" t="str">
+      <c r="I9" t="str">
         <f>_xll.NCDK_ECFP4($B9)</f>
         <v>0000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="I9" t="str">
+      <c r="J9" t="str">
         <f>_xll.NCDK_ECFP6($B9)</f>
         <v>0000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="J9" t="str">
+      <c r="K9" t="str">
         <f>_xll.NCDK_FCFP0($B9)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="K9" t="str">
+      <c r="L9" t="str">
         <f>_xll.NCDK_FCFP2($B9)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="L9" t="str">
+      <c r="M9" t="str">
         <f>_xll.NCDK_FCFP4($B9)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="M9" t="str">
+      <c r="N9" t="str">
         <f>_xll.NCDK_FCFP0($B9)</f>
         <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="N9" t="str">
+      <c r="O9" t="str">
         <f>_xll.NCDK_AtomPairs2DFingerprinter($B9)</f>
         <v>100000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="O9" t="str">
+      <c r="P9" t="str">
         <f>_xll.NCDK_EStateFingerprinter($B9)</f>
         <v>0000000010000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="P9" t="str">
+      <c r="Q9" t="str">
         <f>_xll.NCDK_ExtendedFingerprinter($B9)</f>
         <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000001000000000000010001</v>
       </c>
-      <c r="Q9" t="str">
+      <c r="R9" t="str">
         <f>_xll.NCDK_CDKFingerprinter($B9)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000010000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="R9" t="str">
+      <c r="S9" t="str">
         <f>_xll.NCDK_KlekotaRothFingerprinter($B9)</f>
         <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000010000000000000100000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="S9" t="str">
+      <c r="T9" t="str">
         <f>_xll.NCDK_LingoFingerprinter($B9)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="T9" t="str">
+      <c r="U9" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($B9)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000010000000000000000010000000000000001010</v>
       </c>
-      <c r="U9" t="str">
+      <c r="V9" t="str">
         <f>_xll.NCDK_ShortestPathFingerprinter($B9)</f>
         <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="V9" t="str">
+      <c r="W9" t="str">
         <f>_xll.NCDK_SubstructureFingerprinter($B9)</f>
         <v>0100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="W9" t="str">
+      <c r="X9" t="str">
         <f>_xll.NCDK_PubchemFingerprinter($B9)</f>
         <v>00000000011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000100000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="X9" s="2">
+      <c r="Y9" s="2">
         <f>_xll.NCDK_MolecularWeight(B9)</f>
         <v>72.064415380728008</v>
       </c>
-      <c r="Y9" s="2">
+      <c r="Z9" s="2">
         <f>_xll.NCDK_ExactMass(B9)</f>
         <v>72</v>
       </c>
-      <c r="Z9">
+      <c r="AA9">
         <f>_xll.NCDK_AcidicGroupCount(B9)</f>
         <v>0</v>
       </c>
-      <c r="AA9" s="4">
+      <c r="AB9" s="4">
         <f>_xll.NCDK_ALogP(B9)</f>
         <v>2.7372000000000005</v>
       </c>
-      <c r="AB9" s="4">
+      <c r="AC9" s="4">
         <f>_xll.NCDK_XLogP(B9)</f>
         <v>3.4139999999999997</v>
       </c>
-      <c r="AC9" s="4">
+      <c r="AD9" s="4">
         <f>_xll.NCDK_MannholdLogP(B9)</f>
         <v>2.12</v>
       </c>
-      <c r="AD9" s="4">
+      <c r="AE9" s="4">
         <f>_xll.NCDK_JPlogP(B9)</f>
         <v>2.6952762459207973</v>
       </c>
-      <c r="AE9">
+      <c r="AF9">
         <f>_xll.NCDK_AMolarRefractivity(B9)</f>
         <v>27.606000000000002</v>
       </c>
-      <c r="AF9">
+      <c r="AG9">
         <f>_xll.NCDK_APol(B9)</f>
         <v>18.561516000000001</v>
       </c>
-      <c r="AG9">
+      <c r="AH9">
         <f>_xll.NCDK_AromaticAtomsCount(B9)</f>
         <v>0</v>
       </c>
-      <c r="AH9">
+      <c r="AI9">
         <f>_xll.NCDK_AromaticBondsCount(B9)</f>
         <v>0</v>
       </c>
-      <c r="AI9">
+      <c r="AJ9">
         <f>_xll.NCDK_AtomCount(B9)</f>
         <v>6</v>
       </c>
-      <c r="AJ9" t="str">
+      <c r="AK9" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B9)</f>
         <v>0, 0, 0, 0, 0</v>
       </c>
-      <c r="AK9" t="str">
+      <c r="AL9" t="str">
         <f>_xll.NCDK_AutocorrelationMass(B9)</f>
         <v>6, 6, 6, 3, 0</v>
       </c>
-      <c r="AL9" t="str">
+      <c r="AM9" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B9)</f>
         <v>257.709834375, 257.709834375, 257.709834375, 128.8549171875, 0</v>
       </c>
-      <c r="AM9">
+      <c r="AN9">
         <f>_xll.NCDK_BasicGroupCount(B9)</f>
         <v>0</v>
       </c>
-      <c r="AN9" t="str">
+      <c r="AO9" t="str">
         <f>_xll.NCDK_BCUT(B9)</f>
         <v>11.9, 12.1000824042221, -0.15279744210896, 0.0472849621131451, 6.45375, 6.65383240422211</v>
       </c>
-      <c r="AO9">
+      <c r="AP9">
         <f>_xll.NCDK_BondCount(B9)</f>
         <v>0</v>
       </c>
-      <c r="AP9">
+      <c r="AQ9">
         <f>_xll.NCDK_BPol(B9)</f>
         <v>0</v>
       </c>
-      <c r="AQ9" t="str">
+      <c r="AR9" t="str">
         <f>_xll.NCDK_CarbonTypes(B9)</f>
         <v>0, 0, 0, 0, 0, 0, 6, 0, 0</v>
       </c>
-      <c r="AR9" t="str">
+      <c r="AS9" t="str">
         <f>_xll.NCDK_ChiChain(B9)</f>
         <v>0, 0, 0, 0.125, 0, 0, 0, 0, 0.125, 0</v>
       </c>
-      <c r="AS9" t="str">
+      <c r="AT9" t="str">
         <f>_xll.NCDK_ChiCluster(B9)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AT9" t="str">
+      <c r="AU9" t="str">
         <f>_xll.NCDK_ChiPathCluster(B9)</f>
         <v>0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="AU9" t="str">
+      <c r="AV9" t="str">
         <f>_xll.NCDK_ChiPath(B9)</f>
         <v>4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0, 4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0</v>
       </c>
-      <c r="AV9" t="str">
+      <c r="AW9" t="str">
         <f>_xll.NCDK_CPSA(B9)</f>
         <v>#N/A</v>
       </c>
-      <c r="AW9">
+      <c r="AX9">
         <f>_xll.NCDK_EccentricConnectivityIndex(B9)</f>
         <v>36</v>
       </c>
-      <c r="AX9">
+      <c r="AY9">
         <f>_xll.NCDK_FMF(B9)</f>
         <v>1</v>
       </c>
-      <c r="AY9">
+      <c r="AZ9">
         <f>_xll.NCDK_FractionalPSA(B9)</f>
         <v>0</v>
       </c>
-      <c r="AZ9">
+      <c r="BA9">
         <f>_xll.NCDK_FragmentComplexity(B9)</f>
         <v>294</v>
       </c>
-      <c r="BA9" t="str">
+      <c r="BB9" t="str">
         <f>_xll.NCDK_GravitationalIndex(B9)</f>
         <v>#N/A</v>
       </c>
-      <c r="BB9">
+      <c r="BC9">
         <f>_xll.NCDK_HBondAcceptorCount(B9)</f>
         <v>0</v>
       </c>
-      <c r="BC9">
+      <c r="BD9">
         <f>_xll.NCDK_HBondDonorCount(B9)</f>
         <v>0</v>
       </c>
-      <c r="BD9">
+      <c r="BE9">
         <f>_xll.NCDK_HybridizationRatio(B9)</f>
         <v>1</v>
       </c>
-      <c r="BE9" t="str">
+      <c r="BF9" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B9)</f>
         <v>4.16666666666667, 2.22222222222222, 1.33333333333333</v>
       </c>
-      <c r="BF9" t="str">
+      <c r="BG9" t="str">
         <f>_xll.NCDK_KierHallSmarts(B9)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BG9">
+      <c r="BH9">
         <f>_xll.NCDK_LargestChain(B9)</f>
         <v>0</v>
       </c>
-      <c r="BH9">
+      <c r="BI9">
         <f>_xll.NCDK_LargestPiSystem(B9)</f>
         <v>0</v>
       </c>
-      <c r="BI9" t="str">
+      <c r="BJ9" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B9)</f>
         <v>#N/A</v>
       </c>
-      <c r="BJ9">
+      <c r="BK9">
         <f>_xll.NCDK_LongestAliphaticChain(B9)</f>
         <v>0</v>
       </c>
-      <c r="BK9" t="str">
+      <c r="BL9" t="str">
         <f>_xll.NCDK_MDE(B9)</f>
         <v>0, 0, 0, 0, 9.12546512839809, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BL9" t="str">
+      <c r="BM9" t="str">
         <f>_xll.NCDK_MomentOfInertia(B9)</f>
         <v>#N/A</v>
       </c>
-      <c r="BM9">
+      <c r="BN9">
         <f>_xll.NCDK_PetitjeanNumber(B9)</f>
         <v>0</v>
       </c>
-      <c r="BN9" t="str">
+      <c r="BO9" t="str">
         <f>_xll.NCDK_PetitjeanShapeIndex(B9)</f>
         <v>#N/A</v>
       </c>
-      <c r="BO9">
+      <c r="BP9">
         <f>_xll.NCDK_RotatableBondsCount(B9)</f>
         <v>0</v>
       </c>
-      <c r="BP9">
+      <c r="BQ9">
         <f>_xll.NCDK_RuleOfFive(B9)</f>
         <v>0</v>
       </c>
-      <c r="BQ9" t="str">
+      <c r="BR9" t="str">
         <f>_xll.NCDK_SmallRing(B9)</f>
         <v>1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0</v>
       </c>
-      <c r="BR9">
+      <c r="BS9">
         <f>_xll.NCDK_TPSA(B9)</f>
         <v>0</v>
       </c>
-      <c r="BS9">
+      <c r="BT9">
         <f>_xll.NCDK_VABC(B9)</f>
         <v>99.975907755200197</v>
       </c>
-      <c r="BT9">
+      <c r="BU9">
         <f>_xll.NCDK_VAdjMa(B9)</f>
         <v>3.5849625007211561</v>
       </c>
-      <c r="BU9" s="2">
+      <c r="BV9" s="2">
         <f>_xll.NCDK_MolecularWeight(B9)</f>
         <v>72.064415380728008</v>
       </c>
-      <c r="BV9" s="3">
+      <c r="BW9" s="3">
         <f>_xll.NCDK_ExactMass(B9)</f>
         <v>72</v>
       </c>
-      <c r="BW9" t="str">
+      <c r="BX9" t="str">
         <f>_xll.NCDK_WeightedPath(B9)</f>
         <v>11.8125, 1.96875, 0, 0, 0</v>
       </c>
-      <c r="BX9" t="str">
+      <c r="BY9" t="str">
         <f>_xll.NCDK_WHIM(B9)</f>
         <v>#N/A</v>
       </c>
-      <c r="BY9" t="str">
+      <c r="BZ9" t="str">
         <f>_xll.NCDK_WienerNumbers(B9)</f>
         <v>27, 3</v>
       </c>
-      <c r="BZ9">
+      <c r="CA9">
         <f>_xll.NCDK_ZagrebIndex(B9)</f>
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:78" ht="19" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:79" ht="19" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -5388,7 +5425,7 @@
         <v>[C@@]12(C(C([C@](O[H])(C(C1=C(C([C@@]3([C@]2([H])C(C([C@]4([C@@]3([H])C(C([C@]4([H])[C@](C([H])([H])[H])(C(C(C(C(C([H])([H])[H])(C([H])([H])[H])[H])([H])[H])([H])[H])([H])[H])[H])([H])[H])([H])[H])C([H])([H])[H])([H])[H])([H])[H])[H])([H])[H])[H])([H])[H])[H])([H])[H])([H])[H])C([H])([H])[H]</v>
       </c>
       <c r="D10">
-        <f>_xll.NCDK_Tanimoto($H10,$H11)</f>
+        <f>_xll.NCDK_Tanimoto($I10,$I11)</f>
         <v>0.47761194029850745</v>
       </c>
       <c r="E10" t="str">
@@ -5396,299 +5433,303 @@
         <v>0000000000000000000000000100000000000000000000000100000000000000010000000101000000000000010000010010000110010001001101000000011110010000001010101010110100101001001110</v>
       </c>
       <c r="F10" t="str">
+        <f>_xll.RDKit_MACCSFingerprint(B10)</f>
+        <v>00000000000000000000000000100000000000000000000000100000000000000010000000101000000000000010000010010100110010001001101000000001110010000001010101010110100101001001110</v>
+      </c>
+      <c r="G10" t="str">
         <f>_xll.NCDK_ECFP0($B10)</f>
         <v>0000000000000010000000000100000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000100000000000000000010000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000100000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="G10" t="str">
+      <c r="H10" t="str">
         <f>_xll.NCDK_ECFP2($B10)</f>
         <v>0000000000000010000000001100000000000000000000001000000000000000000000000001000000001000100000000000000000000000000000000000000000000100000000000000000010000000000000000000000000000000000000000000000000000010000000000000010000000010000000000000000000000000000000000000000001000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000001000000000000000000000000000000000000000010000000000000000000000000100000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100010000000000001000001000000000000000000000001000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000010000000000000000000100000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="H10" t="str">
+      <c r="I10" t="str">
         <f>_xll.NCDK_ECFP4($B10)</f>
         <v>0000000000000010000000001100000000000000000100001000000000010000000000000001000000001010100000000000000000000000000000000000000000000100000000010000000010000000000000000000000000000000000000000000000000000010000000000000010000000010000000000000000000000000000000000000000001000000000010000000001000000000000000100000010000000000000000000000000000000010000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000001000100000000000100000000000000000000000010000000000000000000000000100000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000010100000000000000000000000000000000000000000000000000000000000000100010000000000001000001000000000000000000000011000000000000010100000000000000000000000000000000000000000100000000000000000000000000000100000000000001000010000000000000000000000000010000000000010000000000000000000100000001000000000000000100000000000000000000000000000000</v>
       </c>
-      <c r="I10" t="str">
+      <c r="J10" t="str">
         <f>_xll.NCDK_ECFP6($B10)</f>
         <v>0000000000001010001000001100000000000000000100001000000000010000000000000001000000001010100000000000000000000000000000000000000000000100000000010000000010000000000000000000000000000000000000000000000000001010000001100000011000000010000000000000000000000000000000000000000001000000000010000000001000000000000000110000010000000000000000000000000000000010000110000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000001000100000000000100000000000000000000000010000000000000000000000000100000000000000001000000000010000000000000000001000000000000100000000000000000000000000010000010000000000000000000000000000010100000001000000000000000000000000000000000000000000000000000000100010000000000001010001000000000000000000000011000000000000010100000000000000000000011000000010000000000100000000000000000000000000000100010000000001000010000000000000000000000000010000000000010000000000000001000100000001000000010000000100000000000000000000000000000000</v>
       </c>
-      <c r="J10" t="str">
+      <c r="K10" t="str">
         <f>_xll.NCDK_FCFP0($B10)</f>
         <v>1001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="K10" t="str">
+      <c r="L10" t="str">
         <f>_xll.NCDK_FCFP2($B10)</f>
         <v>1001000000000000000000010000000000000000000000000000000000000000000000000000000001000010000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="L10" t="str">
+      <c r="M10" t="str">
         <f>_xll.NCDK_FCFP4($B10)</f>
         <v>1001000000000000000000010000000000000000000000000000000000000000000000000000000001000010000000000000000000000000000000000000000000000000000000000000000100000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000100000000000000000000000001100000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000010000000000000000000000000000000000000000000000000001000100000000000000000000000000000000000000000000000000000000000000100000000001000000000010000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000100000000000010000000000000010000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000001000000000000000000000</v>
       </c>
-      <c r="M10" t="str">
+      <c r="N10" t="str">
         <f>_xll.NCDK_FCFP0($B10)</f>
         <v>1001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="N10" t="str">
+      <c r="O10" t="str">
         <f>_xll.NCDK_AtomPairs2DFingerprinter($B10)</f>
         <v>101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="O10" t="str">
+      <c r="P10" t="str">
         <f>_xll.NCDK_EStateFingerprinter($B10)</f>
         <v>0000000000000001001000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="P10" t="str">
+      <c r="Q10" t="str">
         <f>_xll.NCDK_ExtendedFingerprinter($B10)</f>
         <v>000000000000000000001000000010000000000000000000000000000000100001000000010000000000010000000010010001010000000110001110000000000000000010000000001000001001000000000000001010000000100000000000010000000000000000000000000000000000000100000010000000000010000001010000000000010000100001000000000000101000001000000000000000001000000000000011000000000000000000000000000000000000001000100000000000000000000000001100100100000000000010000001000000101000000000000100000000000000000101000000010000000000100000000001000000000000000000000010000000000000000000000000000000000000000000101000000000000000001000000000010000100010000000000000000000000000001000010000000000000000100001000001000000000010000100000000000000001010000000000000000000010000000000000000001000001000000000111000000010000000000000010000000010000010010010010000000000010000000000010000000000101000000000000000000001000000000010100100000010000010000000100000010000000000000100000000000000000010110000000001011000010010000000000000000010000001000000000000011111111</v>
       </c>
-      <c r="Q10" t="str">
+      <c r="R10" t="str">
         <f>_xll.NCDK_CDKFingerprinter($B10)</f>
         <v>0000010000000001001000000000000000000010000000000000000000100000000000000001100000000001000000000000000000000000000000000000000100001100000000000000110000000010000000000100100000110000000000000000000000000010000000000000000000000000000000000000000000000000010000000000000000000000001010000000000001001000000000000001100000000100000000000000000100000000000000000000010000000000000000000000000010000000000001001100000000000010000000000000000000010000000010000100000000000000001000000000010000000000011011100100101000000000001000000000011010000010010000000000000000000000001000100000000000001000000000000000000000000000011001000000000000000100000010000000000000011000000000000000010000000000000000000000000000010000000000011000000000000000000001110101000010000000000000000000000000000100000000000000000000001100000000000000000000000010000000001010001000100000000100010100000010000000000000000000000000000000000000000000000010000000010000000000000000000001000000000000000000010000000000000000000000000000000000000000001000000000</v>
       </c>
-      <c r="R10" t="str">
+      <c r="S10" t="str">
         <f>_xll.NCDK_KlekotaRothFingerprinter($B10)</f>
         <v>110000010000010011000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001111000000100000000000000000010000000000000011010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000010100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000010000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000011000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000001000000000000000000100000100000000000001000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000100000000000000001011000000010000000000000000000000010000000000000100000100000010010000100100000010000001000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="S10" t="str">
+      <c r="T10" t="str">
         <f>_xll.NCDK_LingoFingerprinter($B10)</f>
         <v>0000010000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000010000000000000000000000000000100000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000011000000000000000000000000000000010000000010000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000010000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000</v>
       </c>
-      <c r="T10" t="str">
+      <c r="U10" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($B10)</f>
         <v>0000000000000000000000000100000000000000000000000100000000000000010000000101000000000000010000010010000110010001001101000000011110010000001010101010110100101001001110</v>
       </c>
-      <c r="U10" t="str">
+      <c r="V10" t="str">
         <f>_xll.NCDK_ShortestPathFingerprinter($B10)</f>
         <v>1011001000010001010001111111000100000001000000000011011110010100101010100100000000001100000010100101000010010000011110100100000000010100010101000100000010000001000001010100000001100010000100000001100001000110100001000000001011000010101101010011010010001000010001000010001111000100011000000100101010110000110000010010110001100100010000000001000000010010110000000000010010111010010001101010010011000000101100000000100101101011000110100001100000100010010001010000000000010000010100001011001010001100010000010001111001100000101000010100010001001010000001000010011000111110010010000000110101011010001011001010000110000000000100000000010011000100000000011000010000000101000100000000100000000000010100000000010001000110100100000000000000010000001010000000010001000000101000010110000000101000011010011100011001110000000011100000001000000010101000001001001000010000111100010010010001110100100100001000010101000101000010010110010000000011001010010000000010011001101010100101001100000001011000001011001001101100000100100010000000000000</v>
       </c>
-      <c r="V10" t="str">
+      <c r="W10" t="str">
         <f>_xll.NCDK_SubstructureFingerprinter($B10)</f>
         <v>1111100000010110000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000001000000100001</v>
       </c>
-      <c r="W10" t="str">
+      <c r="X10" t="str">
         <f>_xll.NCDK_PubchemFingerprinter($B10)</f>
         <v>11110000011110000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000110000000000000000000000000000000001100100110000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001101000000000000000000000100000000000000000000000111100010100101000001000000000000010000000100000000000000000000000000000001000000000100000000000001000100000010000100000000000000000000000000000000000000000001000000000000000000000000000000000100000000000000000000000000000001000000000000001000000000010000000000000000100000000000000000100000000000000000001001100000000000000000010000000000000000011100000001100000011110000000011111000000000000000000000000000000000000000000000000000000000000000110000000000000000000100000000000000000000100000000000000000000100000000000000000000100000000000000000000</v>
       </c>
-      <c r="X10" s="2">
+      <c r="Y10" s="2">
         <f>_xll.NCDK_MolecularWeight(B10)</f>
         <v>386.65454881683121</v>
       </c>
-      <c r="Y10" s="2">
+      <c r="Z10" s="2">
         <f>_xll.NCDK_ExactMass(B10)</f>
         <v>386.35486609199995</v>
       </c>
-      <c r="Z10">
+      <c r="AA10">
         <f>_xll.NCDK_AcidicGroupCount(B10)</f>
         <v>0</v>
       </c>
-      <c r="AA10" s="4">
+      <c r="AB10" s="4">
         <f>_xll.NCDK_ALogP(B10)</f>
         <v>7.376100000000001</v>
       </c>
-      <c r="AB10" s="4">
+      <c r="AC10" s="4">
         <f>_xll.NCDK_XLogP(B10)</f>
         <v>10.518000000000004</v>
       </c>
-      <c r="AC10" s="4">
+      <c r="AD10" s="4">
         <f>_xll.NCDK_MannholdLogP(B10)</f>
         <v>4.3199999999999994</v>
       </c>
-      <c r="AD10" s="4">
+      <c r="AE10" s="4">
         <f>_xll.NCDK_JPlogP(B10)</f>
         <v>7.8290832169857083</v>
       </c>
-      <c r="AE10">
+      <c r="AF10">
         <f>_xll.NCDK_AMolarRefractivity(B10)</f>
         <v>120.6157</v>
       </c>
-      <c r="AF10">
+      <c r="AG10">
         <f>_xll.NCDK_APol(B10)</f>
         <v>78.99447799999993</v>
       </c>
-      <c r="AG10">
+      <c r="AH10">
         <f>_xll.NCDK_AromaticAtomsCount(B10)</f>
         <v>0</v>
       </c>
-      <c r="AH10">
+      <c r="AI10">
         <f>_xll.NCDK_AromaticBondsCount(B10)</f>
         <v>0</v>
       </c>
-      <c r="AI10">
+      <c r="AJ10">
         <f>_xll.NCDK_AtomCount(B10)</f>
         <v>74</v>
       </c>
-      <c r="AJ10" t="str">
+      <c r="AK10" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B10)</f>
         <v>0.0827991713427503, -0.0229631507285856, -0.0270969061556759, 0.00647128770548948, 0.00909713625645344</v>
       </c>
-      <c r="AK10" t="str">
+      <c r="AL10" t="str">
         <f>_xll.NCDK_AutocorrelationMass(B10)</f>
         <v>28.7744690355409, 31.3320919771326, 48.6641839542651, 54.6641839542651, 49.6641839542651</v>
       </c>
-      <c r="AL10" t="str">
+      <c r="AM10" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B10)</f>
         <v>2589.35165284459, 3179.06049775734, 4922.9791073968, 5328.87269506555, 4616.91714731414</v>
       </c>
-      <c r="AM10">
+      <c r="AN10">
         <f>_xll.NCDK_BasicGroupCount(B10)</f>
         <v>0</v>
       </c>
-      <c r="AN10" t="str">
+      <c r="AO10" t="str">
         <f>_xll.NCDK_BCUT(B10)</f>
         <v>11.89, 15.9949214370833, -0.392219399090072, 0.0596280868632924, 5.23875003301361, 12.6475909449557</v>
       </c>
-      <c r="AO10">
+      <c r="AP10">
         <f>_xll.NCDK_BondCount(B10)</f>
         <v>46</v>
       </c>
-      <c r="AP10">
+      <c r="AQ10">
         <f>_xll.NCDK_BPol(B10)</f>
         <v>50.287521999999989</v>
       </c>
-      <c r="AQ10" t="str">
+      <c r="AR10" t="str">
         <f>_xll.NCDK_CarbonTypes(B10)</f>
         <v>0, 0, 0, 1, 1, 5, 12, 6, 2</v>
       </c>
-      <c r="AR10" t="str">
+      <c r="AS10" t="str">
         <f>_xll.NCDK_ChiChain(B10)</f>
         <v>0, 0, 0.0833333333333333, 0.393634553260967, 0.976046921839545, 0, 0, 0.0833333333333333, 0.37164819290959, 0.863165765466815</v>
       </c>
-      <c r="AS10" t="str">
+      <c r="AT10" t="str">
         <f>_xll.NCDK_ChiCluster(B10)</f>
         <v>2.9521315814894, 0.235702260395516, 1.02234106177579, 0.203263132396285, 2.68481479020038, 0.219913202813724, 0.935219433730957, 0.179558378198271</v>
       </c>
-      <c r="AT10" t="str">
+      <c r="AU10" t="str">
         <f>_xll.NCDK_ChiPathCluster(B10)</f>
         <v>6.93012787723299, 11.9183161832455, 18.084244169983, 6.31056734345633, 10.8246614459309, 15.7948474414898</v>
       </c>
-      <c r="AU10" t="str">
+      <c r="AV10" t="str">
         <f>_xll.NCDK_ChiPath(B10)</f>
         <v>20.1040835277556, 13.2536913009629, 13.0668536638687, 11.1291235227258, 9.49703814548855, 7.69096408557495, 5.93907638185732, 4.4721666474432, 19.344190342069, 12.6298450216499, 12.1863667747532, 10.2790812759586, 8.6662445789686, 6.67875288189192, 5.16344144011131, 3.80610378452706</v>
       </c>
-      <c r="AV10" t="str">
+      <c r="AW10" t="str">
         <f>_xll.NCDK_CPSA(B10)</f>
         <v>740.518679745203, 1141.6281036277, 24.7477735904141, 216.516577646307, -333.794969260415, -24.5734427697376, 524.002102098896, 1475.42307288811, 49.3212163601517, 0.773763217212662, 1.19287988066324, 0.0258587898400593, 0.226236782787338, -0.348780221713257, -0.025676632684061, 708.702485273172, 1092.57834600072, 23.6844918679688, 207.213998617263, -319.453554322133, -23.5176511261314, 0.136302900713605, 0.25436791475781, 2.7228153119618, 9.4535627888125, 899.894129431074, 57.1411279604366, 0.940293602018195, 0.0597063979818049</v>
       </c>
-      <c r="AW10">
+      <c r="AX10">
         <f>_xll.NCDK_EccentricConnectivityIndex(B10)</f>
         <v>669</v>
       </c>
-      <c r="AX10">
+      <c r="AY10">
         <f>_xll.NCDK_FMF(B10)</f>
         <v>0.22972972972972974</v>
       </c>
-      <c r="AY10">
+      <c r="AZ10">
         <f>_xll.NCDK_FractionalPSA(B10)</f>
         <v>5.2361188574192148E-2</v>
       </c>
-      <c r="AZ10">
+      <c r="BA10">
         <f>_xll.NCDK_FragmentComplexity(B10)</f>
         <v>5173.01</v>
       </c>
-      <c r="BA10" t="str">
+      <c r="BB10" t="str">
         <f>_xll.NCDK_GravitationalIndex(B10)</f>
         <v>1941.85812139388, 44.0665192793109, 12.4759176252409, 2394.88950905792, 48.9376083299737, 13.37914910667, 4535.65140656394, 67.3472449812458, 16.5531209985441</v>
       </c>
-      <c r="BB10">
+      <c r="BC10">
         <f>_xll.NCDK_HBondAcceptorCount(B10)</f>
         <v>1</v>
       </c>
-      <c r="BC10">
+      <c r="BD10">
         <f>_xll.NCDK_HBondDonorCount(B10)</f>
         <v>1</v>
       </c>
-      <c r="BD10">
+      <c r="BE10">
         <f>_xll.NCDK_HybridizationRatio(B10)</f>
         <v>0.92592592592592593</v>
       </c>
-      <c r="BE10" t="str">
+      <c r="BF10" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B10)</f>
         <v>21.2403746097815, 7.921875, 3.65484429065744</v>
       </c>
-      <c r="BF10" t="str">
+      <c r="BG10" t="str">
         <f>_xll.NCDK_KierHallSmarts(B10)</f>
         <v>0, 0, 0, 0, 0, 0, 5, 0, 11, 0, 1, 0, 7, 0, 0, 1, 0, 0, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BG10">
+      <c r="BH10">
         <f>_xll.NCDK_LargestChain(B10)</f>
         <v>7</v>
       </c>
-      <c r="BH10">
+      <c r="BI10">
         <f>_xll.NCDK_LargestPiSystem(B10)</f>
         <v>2</v>
       </c>
-      <c r="BI10" t="str">
+      <c r="BJ10" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B10)</f>
         <v>3.502934717034, 3.502934717034</v>
       </c>
-      <c r="BJ10">
+      <c r="BK10">
         <f>_xll.NCDK_LongestAliphaticChain(B10)</f>
         <v>7</v>
       </c>
-      <c r="BK10" t="str">
+      <c r="BL10" t="str">
         <f>_xll.NCDK_MDE(B10)</f>
         <v>2.79346109096649, 16.5925259846737, 11.5560895487586, 3.39888423642021, 17.7527182855433, 29.2401176288661, 7.64127863367805, 8.77423090217006, 6.5802347918611, 0.5, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BL10" t="str">
+      <c r="BM10" t="str">
         <f>_xll.NCDK_MomentOfInertia(B10)</f>
         <v>10068.4095883237, 9731.07167302841, 773.613761142664, 1.03466606008362, 13.0147757111406, 12.5787210127379, 8.29661608019916</v>
       </c>
-      <c r="BM10">
+      <c r="BN10">
         <f>_xll.NCDK_PetitjeanNumber(B10)</f>
         <v>0.46666666666666667</v>
       </c>
-      <c r="BN10" t="str">
+      <c r="BO10" t="str">
         <f>_xll.NCDK_PetitjeanShapeIndex(B10)</f>
         <v>0.875, 0.940550174456362</v>
       </c>
-      <c r="BO10">
+      <c r="BP10">
         <f>_xll.NCDK_RotatableBondsCount(B10)</f>
         <v>5</v>
       </c>
-      <c r="BP10">
+      <c r="BQ10">
         <f>_xll.NCDK_RuleOfFive(B10)</f>
         <v>1</v>
       </c>
-      <c r="BQ10" t="str">
+      <c r="BR10" t="str">
         <f>_xll.NCDK_SmallRing(B10)</f>
         <v>4, 0, 1, 0, 0, 0, 1, 3, 0, 0, 0</v>
       </c>
-      <c r="BR10">
+      <c r="BS10">
         <f>_xll.NCDK_TPSA(B10)</f>
         <v>20.23</v>
       </c>
-      <c r="BS10">
+      <c r="BT10">
         <f>_xll.NCDK_VABC(B10)</f>
         <v>432.2759767957632</v>
       </c>
-      <c r="BT10">
+      <c r="BU10">
         <f>_xll.NCDK_VAdjMa(B10)</f>
         <v>5.9541963103868758</v>
       </c>
-      <c r="BU10" s="2">
+      <c r="BV10" s="2">
         <f>_xll.NCDK_MolecularWeight(B10)</f>
         <v>386.65454881683121</v>
       </c>
-      <c r="BV10" s="3">
+      <c r="BW10" s="3">
         <f>_xll.NCDK_ExactMass(B10)</f>
         <v>386.35486609199995</v>
       </c>
-      <c r="BW10" t="str">
+      <c r="BX10" t="str">
         <f>_xll.NCDK_WeightedPath(B10)</f>
         <v>57.2167299866347, 2.04345464237981, 2.54245315921217, 2.54245315921217, 0</v>
       </c>
-      <c r="BX10" t="str">
+      <c r="BY10" t="str">
         <f>_xll.NCDK_WHIM(B10)</f>
         <v>1.22231276339169, 2.17046945111189, 25.8559001988821, 0.0417903530188526, 0.0742074265238894, #N/A, #N/A, #N/A, 0.0962638773185697, 0.00388857657057473, 66.8991567190677, 29.2486824133857, 90.3764308473927, 188.22062289613, 0.413001665342944, #N/A, 66.9993091729568</v>
       </c>
-      <c r="BY10" t="str">
+      <c r="BZ10" t="str">
         <f>_xll.NCDK_WienerNumbers(B10)</f>
         <v>2022, 54</v>
       </c>
-      <c r="BZ10">
+      <c r="CA10">
         <f>_xll.NCDK_ZagrebIndex(B10)</f>
         <v>158</v>
       </c>
     </row>
-    <row r="11" spans="1:78" ht="19" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:79" ht="19" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -5704,294 +5745,298 @@
         <v>0000000000000000000000000100000000000000000000000100000000000000010000000101000000000000010000010010000110010001001101000000001110010000001010101010110100101001001110</v>
       </c>
       <c r="F11" t="str">
+        <f>_xll.RDKit_MACCSFingerprint(B11)</f>
+        <v>00000000000000000000000000100000000000000000000000100000000000000010000000101000000000000010000010010100110010001001101000000001110010000001010101010110100101001001110</v>
+      </c>
+      <c r="G11" t="str">
         <f>_xll.NCDK_ECFP0($B11)</f>
         <v>0000000000000010000000000100000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000100000000000000000010000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000100000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="G11" t="str">
+      <c r="H11" t="str">
         <f>_xll.NCDK_ECFP2($B11)</f>
         <v>0000000000000010000000001100000000000000000000001000000000000000000000000000000000000000100000000000000000000000000000000000000000000100000000000000000010000000000000000000000000000000000000000000000000000010000001000000010000000010000000000000000000000000000000000000000001000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000010000001000000000000000000000000000000000000000010000000000000000000000000100000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000001000001000000000000000000000001000100000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000010000000000000000000100000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="H11" t="str">
+      <c r="I11" t="str">
         <f>_xll.NCDK_ECFP4($B11)</f>
         <v>0000000000000010000000001100000000000000000100001000100000010000000000000000000000000000100000000000000000000000000000000000000000000100000000010000000010000000000000000000000000000000000000000000000000000010000001000000010000000010000000000000000000000000000000000000000001000000000010010000000000000000000000000000000000000010000000000000001000000010000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000100100000000000000000010000001000000000000000100000000000000000000000010000001000000000000000000100000000000000000001000000000000000000000000000000010000000100000000000000000000000000000000000000000000000000000000000000010000000100000000000000000000000000010000000000000000000000000000001000000000000001000001000100000000000010000001000100000000000100000000000000000000000000000000000000000000000000000001000000000000000000000000000001000000000000000000000000000000010000000000010000000000000000000100000000000000000000000100000000000000000000000000000000</v>
       </c>
-      <c r="I11" t="str">
+      <c r="J11" t="str">
         <f>_xll.NCDK_ECFP6($B11)</f>
         <v>0000000000001010000000001100000000000000000100001000100000010000000000000000000000000000100000000010000000000000001000000000000000000100000000010000000010000000000000000000000000000001000000000000000000001010000001000010010000000010000000000000000000000000000000000000100001000001000010010000000000000000000000000000000000000010001000000000001000000010000000000000000000000000000000000000100000000001000000000000000000000000000000000000000000000000000000000100000000000100100000000000000000010100001000000000000000100000000000000000000000010000001000000000000000000110000000000000000001000000000000000000000000000000010000000100000000000000000000000000000000000000000000000000000000000000010000010100000000000000000000000000011000000000000000000000000000001000000000000001000001000100000000001010000001000100000000000100010000000000000000000000000000000000000000000000000001000000001000000000000000000001000000000000000000000000000000010000000100010000000000001000000100000000000000000000000100000000000000000000000000000000</v>
       </c>
-      <c r="J11" t="str">
+      <c r="K11" t="str">
         <f>_xll.NCDK_FCFP0($B11)</f>
         <v>1001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="K11" t="str">
+      <c r="L11" t="str">
         <f>_xll.NCDK_FCFP2($B11)</f>
         <v>1001000000000000000000010000000000000000000000000000000000000000000000000000000001000010000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="L11" t="str">
+      <c r="M11" t="str">
         <f>_xll.NCDK_FCFP4($B11)</f>
         <v>1001000000000000000000010000000000000000000000000000000000000000000000000000000001000010000000000000000000000000000000000000000000000000000000000000000100000001010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000100000000000000000000000001100000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000010000000000000000000010000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000010000000000000000000000000100000000000010000000000000010000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="M11" t="str">
+      <c r="N11" t="str">
         <f>_xll.NCDK_FCFP0($B11)</f>
         <v>1001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="N11" t="str">
+      <c r="O11" t="str">
         <f>_xll.NCDK_AtomPairs2DFingerprinter($B11)</f>
         <v>101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000101000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="O11" t="str">
+      <c r="P11" t="str">
         <f>_xll.NCDK_EStateFingerprinter($B11)</f>
         <v>0000001010101001001000000000000001000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="P11" t="str">
+      <c r="Q11" t="str">
         <f>_xll.NCDK_ExtendedFingerprinter($B11)</f>
         <v>000000000000000000000000000000000000000000000000000000000000100001000000000000000000000000000010000000000000000000000110000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000001000001000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000001000000100000000000000000000000000101000000000000100000000000000000100000000010000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000010000100010000000000000000000000000000000000000000000000000000000000001000000000000000100000000000000000000000000000000000000000000000000000000001000001000000000010000000010000000000000010000000010000000000000010000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000110000000000001000010000000000000000000000000001000000000000011111111</v>
       </c>
-      <c r="Q11" t="str">
+      <c r="R11" t="str">
         <f>_xll.NCDK_CDKFingerprinter($B11)</f>
         <v>0000010000000000000000000000000000000010000000000000000000000000000000000001100000000001000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000001000100000000000010000000000000000000010000000000000000000000000000001000000000010000000000000000000000000000000000001000000000001000000010000000000000000000000000000000100000000000001000000000000000000000000000000001000000000000000100000010000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000001110001000010000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000001000100000000100010100000000000000000000000000000000000000000000000000000010000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000</v>
       </c>
-      <c r="R11" t="str">
+      <c r="S11" t="str">
         <f>_xll.NCDK_KlekotaRothFingerprinter($B11)</f>
         <v>110000010000010011000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001111000000100000000000000000010000000000000011010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000010100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000010000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000011000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000001000000000000000000100000100000000000001000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000100000000000000001011000000010000000000000000000000010000000000000100000100000010010000100100000010000001000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="S11" t="str">
+      <c r="T11" t="str">
         <f>_xll.NCDK_LingoFingerprinter($B11)</f>
         <v>0010000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000110000000100100000110000000000000000000000000000000000000000000000000000000000000000001000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000010001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000</v>
       </c>
-      <c r="T11" t="str">
+      <c r="U11" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($B11)</f>
         <v>0000000000000000000000000100000000000000000000000100000000000000010000000101000000000000010000010010000110010001001101000000001110010000001010101010110100101001001110</v>
       </c>
-      <c r="U11" t="str">
+      <c r="V11" t="str">
         <f>_xll.NCDK_ShortestPathFingerprinter($B11)</f>
         <v>0000000000000000000001100001000000000000000000000001011100000100101000100000000000001000000000000000000010000000010100000000000000010100000000000100000000000000000000000000000001000000000000000001100000000000000001000000000001000000001001000001000010000000000000000010000010000000001000000100101000100000100000000000100000000000000000000000000000000000000000000000000000000000000000000010000001000000100000000000000100001011000100000001000000100000010000000000000000000000000000000001001000000100000000010000010000100000100000000000000000001010000000000000000000010100000000000000100000000010000010001000000110000000000100000000010010000000000000000000010000000100000100000000100000000000000000000000000001000010000100000000000000000000000000000000000000000000001000000100000000000000000000000000010000000000000010000000000000000010100000000000000000000000001100000000000000100100000000000000010100000000000010000000010000000000001000000000000010000001100000000000000100000000000000000000000000000100000000100000000000000000</v>
       </c>
-      <c r="V11" t="str">
+      <c r="W11" t="str">
         <f>_xll.NCDK_SubstructureFingerprinter($B11)</f>
         <v>1111100000010100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000001000000100001</v>
       </c>
-      <c r="W11" t="str">
+      <c r="X11" t="str">
         <f>_xll.NCDK_PubchemFingerprinter($B11)</f>
         <v>00000000011110000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000110000000000000000000000000000000001100100110000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001101000000000000000000000100000000000000000000000111100010100101000001000000000000010000000100000000000000000000000000000001000000000100000000000001000100000010000100000000000000000000000000000000000000000001000000000000000000000000000000000100000000000000000000000000000001000000000000001000000000010000000000000000100000000000000000100000000000000000001001100000000000000000010000000000000000011100000001100000011110000000011111000000000000000000000000000000000000000000000000000000000000000110000000000000000000100000000000000000000100000000000000000000100000000000000000000100000000000000000000</v>
       </c>
-      <c r="X11" s="2">
+      <c r="Y11" s="2">
         <f>_xll.NCDK_MolecularWeight(B11)</f>
         <v>386.65454881683161</v>
       </c>
-      <c r="Y11" s="2">
+      <c r="Z11" s="2">
         <f>_xll.NCDK_ExactMass(B11)</f>
         <v>386.35486609199995</v>
       </c>
-      <c r="Z11">
+      <c r="AA11">
         <f>_xll.NCDK_AcidicGroupCount(B11)</f>
         <v>0</v>
       </c>
-      <c r="AA11" s="4">
+      <c r="AB11" s="4">
         <f>_xll.NCDK_ALogP(B11)</f>
         <v>7.376100000000001</v>
       </c>
-      <c r="AB11" s="4">
+      <c r="AC11" s="4">
         <f>_xll.NCDK_XLogP(B11)</f>
         <v>10.518000000000004</v>
       </c>
-      <c r="AC11" s="4">
+      <c r="AD11" s="4">
         <f>_xll.NCDK_MannholdLogP(B11)</f>
         <v>4.3199999999999994</v>
       </c>
-      <c r="AD11" s="4">
+      <c r="AE11" s="4">
         <f>_xll.NCDK_JPlogP(B11)</f>
         <v>7.8290832169857199</v>
       </c>
-      <c r="AE11">
+      <c r="AF11">
         <f>_xll.NCDK_AMolarRefractivity(B11)</f>
         <v>120.6157</v>
       </c>
-      <c r="AF11">
+      <c r="AG11">
         <f>_xll.NCDK_APol(B11)</f>
         <v>78.994478000000029</v>
       </c>
-      <c r="AG11">
+      <c r="AH11">
         <f>_xll.NCDK_AromaticAtomsCount(B11)</f>
         <v>0</v>
       </c>
-      <c r="AH11">
+      <c r="AI11">
         <f>_xll.NCDK_AromaticBondsCount(B11)</f>
         <v>0</v>
       </c>
-      <c r="AI11">
+      <c r="AJ11">
         <f>_xll.NCDK_AtomCount(B11)</f>
         <v>74</v>
       </c>
-      <c r="AJ11" t="str">
+      <c r="AK11" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B11)</f>
         <v>0.0827991713427503, -0.0229631507285856, -0.0270969061556759, 0.00647128770548948, 0.00909713625645344</v>
       </c>
-      <c r="AK11" t="str">
+      <c r="AL11" t="str">
         <f>_xll.NCDK_AutocorrelationMass(B11)</f>
         <v>28.7744690355409, 31.3320919771326, 48.6641839542651, 54.6641839542651, 49.6641839542651</v>
       </c>
-      <c r="AL11" t="str">
+      <c r="AM11" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B11)</f>
         <v>2589.35165284459, 3179.06049775734, 4922.9791073968, 5328.87269506555, 4616.91714731414</v>
       </c>
-      <c r="AM11">
+      <c r="AN11">
         <f>_xll.NCDK_BasicGroupCount(B11)</f>
         <v>0</v>
       </c>
-      <c r="AN11" t="str">
+      <c r="AO11" t="str">
         <f>_xll.NCDK_BCUT(B11)</f>
         <v>11.89, 15.9949214370832, -0.392219474278523, 0.0694748577202458, 5.23874992098634, 12.6503467270457</v>
       </c>
-      <c r="AO11">
+      <c r="AP11">
         <f>_xll.NCDK_BondCount(B11)</f>
         <v>0</v>
       </c>
-      <c r="AP11">
+      <c r="AQ11">
         <f>_xll.NCDK_BPol(B11)</f>
         <v>50.287521999999989</v>
       </c>
-      <c r="AQ11" t="str">
+      <c r="AR11" t="str">
         <f>_xll.NCDK_CarbonTypes(B11)</f>
         <v>0, 0, 0, 1, 1, 5, 12, 6, 2</v>
       </c>
-      <c r="AR11" t="str">
+      <c r="AS11" t="str">
         <f>_xll.NCDK_ChiChain(B11)</f>
         <v>0, 0, 0.0833333333333333, 0.393634553260967, 0.976046921839545, 0, 0, 0.0833333333333333, 0.37164819290959, 0.863165765466815</v>
       </c>
-      <c r="AS11" t="str">
+      <c r="AT11" t="str">
         <f>_xll.NCDK_ChiCluster(B11)</f>
         <v>2.9521315814894, 0.235702260395516, 1.02234106177579, 0.203263132396285, 2.68481479020038, 0.219913202813724, 0.935219433730957, 0.179558378198271</v>
       </c>
-      <c r="AT11" t="str">
+      <c r="AU11" t="str">
         <f>_xll.NCDK_ChiPathCluster(B11)</f>
         <v>6.93012787723299, 11.9183161832455, 18.084244169983, 6.31056734345633, 10.8246614459309, 15.7948474414898</v>
       </c>
-      <c r="AU11" t="str">
+      <c r="AV11" t="str">
         <f>_xll.NCDK_ChiPath(B11)</f>
         <v>20.1040835277556, 13.2536913009629, 13.0668536638687, 11.1291235227258, 9.49703814548855, 7.69096408557496, 5.93907638185732, 4.4721666474432, 19.344190342069, 12.6298450216499, 12.1863667747532, 10.2790812759586, 8.66624457896859, 6.67875288189192, 5.16344144011131, 3.80610378452706</v>
       </c>
-      <c r="AV11" t="str">
+      <c r="AW11" t="str">
         <f>_xll.NCDK_CPSA(B11)</f>
         <v>#N/A</v>
       </c>
-      <c r="AW11">
+      <c r="AX11">
         <f>_xll.NCDK_EccentricConnectivityIndex(B11)</f>
         <v>669</v>
       </c>
-      <c r="AX11">
+      <c r="AY11">
         <f>_xll.NCDK_FMF(B11)</f>
         <v>0.6071428571428571</v>
       </c>
-      <c r="AY11">
+      <c r="AZ11">
         <f>_xll.NCDK_FractionalPSA(B11)</f>
         <v>5.2361188524318612E-2</v>
       </c>
-      <c r="AZ11">
+      <c r="BA11">
         <f>_xll.NCDK_FragmentComplexity(B11)</f>
         <v>5173.01</v>
       </c>
-      <c r="BA11" t="str">
+      <c r="BB11" t="str">
         <f>_xll.NCDK_GravitationalIndex(B11)</f>
         <v>#N/A</v>
       </c>
-      <c r="BB11">
+      <c r="BC11">
         <f>_xll.NCDK_HBondAcceptorCount(B11)</f>
         <v>1</v>
       </c>
-      <c r="BC11">
+      <c r="BD11">
         <f>_xll.NCDK_HBondDonorCount(B11)</f>
         <v>1</v>
       </c>
-      <c r="BD11">
+      <c r="BE11">
         <f>_xll.NCDK_HybridizationRatio(B11)</f>
         <v>0.92592592592592593</v>
       </c>
-      <c r="BE11" t="str">
+      <c r="BF11" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B11)</f>
         <v>21.2403746097815, 7.921875, 3.65484429065744</v>
       </c>
-      <c r="BF11" t="str">
+      <c r="BG11" t="str">
         <f>_xll.NCDK_KierHallSmarts(B11)</f>
         <v>0, 0, 0, 0, 0, 0, 5, 0, 11, 0, 1, 0, 7, 0, 0, 1, 0, 0, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BG11">
+      <c r="BH11">
         <f>_xll.NCDK_LargestChain(B11)</f>
         <v>16</v>
       </c>
-      <c r="BH11">
+      <c r="BI11">
         <f>_xll.NCDK_LargestPiSystem(B11)</f>
         <v>2</v>
       </c>
-      <c r="BI11" t="str">
+      <c r="BJ11" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B11)</f>
         <v>#N/A</v>
       </c>
-      <c r="BJ11">
+      <c r="BK11">
         <f>_xll.NCDK_LongestAliphaticChain(B11)</f>
         <v>7</v>
       </c>
-      <c r="BK11" t="str">
+      <c r="BL11" t="str">
         <f>_xll.NCDK_MDE(B11)</f>
         <v>1.54697174276407, 11.0054221495714, 8.10399071027919, 2.24225976804296, 15.301585299106, 26.1301405209996, 7.46130267367364, 6.99912877305946, 5.73136198628621, 0.25, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BL11" t="str">
+      <c r="BM11" t="str">
         <f>_xll.NCDK_MomentOfInertia(B11)</f>
         <v>#N/A</v>
       </c>
-      <c r="BM11">
+      <c r="BN11">
         <f>_xll.NCDK_PetitjeanNumber(B11)</f>
         <v>0.46666666666666667</v>
       </c>
-      <c r="BN11" t="str">
+      <c r="BO11" t="str">
         <f>_xll.NCDK_PetitjeanShapeIndex(B11)</f>
         <v>#N/A</v>
       </c>
-      <c r="BO11">
+      <c r="BP11">
         <f>_xll.NCDK_RotatableBondsCount(B11)</f>
         <v>5</v>
       </c>
-      <c r="BP11">
+      <c r="BQ11">
         <f>_xll.NCDK_RuleOfFive(B11)</f>
         <v>1</v>
       </c>
-      <c r="BQ11" t="str">
+      <c r="BR11" t="str">
         <f>_xll.NCDK_SmallRing(B11)</f>
         <v>4, 0, 1, 0, 0, 0, 1, 3, 0, 0, 0</v>
       </c>
-      <c r="BR11">
+      <c r="BS11">
         <f>_xll.NCDK_TPSA(B11)</f>
         <v>20.23</v>
       </c>
-      <c r="BS11">
+      <c r="BT11">
         <f>_xll.NCDK_VABC(B11)</f>
         <v>432.27597679576252</v>
       </c>
-      <c r="BT11">
+      <c r="BU11">
         <f>_xll.NCDK_VAdjMa(B11)</f>
         <v>5.9541963103868758</v>
       </c>
-      <c r="BU11" s="2">
+      <c r="BV11" s="2">
         <f>_xll.NCDK_MolecularWeight(B11)</f>
         <v>386.65454881683161</v>
       </c>
-      <c r="BV11" s="3">
+      <c r="BW11" s="3">
         <f>_xll.NCDK_ExactMass(B11)</f>
         <v>386.35486609199995</v>
       </c>
-      <c r="BW11" t="str">
+      <c r="BX11" t="str">
         <f>_xll.NCDK_WeightedPath(B11)</f>
         <v>57.2167299866347, 2.04345464237981, 2.54245315921218, 2.54245315921218, 0</v>
       </c>
-      <c r="BX11" t="str">
+      <c r="BY11" t="str">
         <f>_xll.NCDK_WHIM(B11)</f>
         <v>#N/A</v>
       </c>
-      <c r="BY11" t="str">
+      <c r="BZ11" t="str">
         <f>_xll.NCDK_WienerNumbers(B11)</f>
         <v>2022, 54</v>
       </c>
-      <c r="BZ11">
+      <c r="CA11">
         <f>_xll.NCDK_ZagrebIndex(B11)</f>
         <v>158</v>
       </c>

</xml_diff>

<commit_message>
Update NCDK and use InChIToStructure to parse InChI.
</commit_message>
<xml_diff>
--- a/NCDK-Excel/ExcelNCDK-Test.xlsx
+++ b/NCDK-Excel/ExcelNCDK-Test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CD6713-5A36-4111-ACB7-D7EC90B0350E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D26D187-38B0-4E41-A312-378DB39C49E3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="407" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1988,10 +1988,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="NCDK-Picture 1">
+        <xdr:cNvPr id="3" name="NCDK-Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{903F7397-2E63-449D-A8C8-11D76A4BF2CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F0B3882-1633-42E3-9E57-415022A0CCF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2038,10 +2038,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="NCDK-Picture 2">
+        <xdr:cNvPr id="5" name="NCDK-Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03E5BB9A-4ED6-448A-850E-5FEAD9B2B35E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A56F313A-9F61-479D-80B5-646FE2765E88}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2088,10 +2088,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="NCDK-Picture 3">
+        <xdr:cNvPr id="7" name="NCDK-Picture 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C59F8C1F-B6F5-4F6F-9EA5-5C6932766028}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15B25713-3407-4776-87DC-92514CFE5334}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2138,10 +2138,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="NCDK-Picture 4">
+        <xdr:cNvPr id="9" name="NCDK-Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C792E8EB-24E6-428F-9CC6-A1D189560417}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07159D9B-4CBC-4038-8C7E-CB4F5A26D03F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2188,10 +2188,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="NCDK-Picture 5">
+        <xdr:cNvPr id="11" name="NCDK-Picture 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FD9CB53-4835-4BC4-BBF9-F3F5608F411B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD6D507F-8428-4709-91DD-4FAE9CFCF944}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2232,16 +2232,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>785927</xdr:colOff>
+      <xdr:colOff>786984</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="NCDK-Picture 6">
+        <xdr:cNvPr id="13" name="NCDK-Picture 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D91684F0-B66A-49F3-B2A6-7E727CB563C7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AD3AD25-9D5F-4877-BC0A-8EDD3FC11B52}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2250,7 +2250,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2264,7 +2264,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="857250" y="4286250"/>
-          <a:ext cx="785927" cy="889000"/>
+          <a:ext cx="786984" cy="889000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2288,10 +2288,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="NCDK-Picture 7">
+        <xdr:cNvPr id="15" name="NCDK-Picture 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DCA50D2-A590-4486-976A-47DFA5B535AA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2810D1FF-7C8E-46C7-9FBF-BF8B194B5E10}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2300,7 +2300,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2338,10 +2338,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="NCDK-Picture 8">
+        <xdr:cNvPr id="17" name="NCDK-Picture 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{088220FA-8133-4C24-A49F-CBAD89603F95}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B426472-EC50-432C-8E3C-8322AE333738}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2350,7 +2350,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2956,7 +2956,7 @@
       <c r="C2" t="str">
         <f>_xll.NCDK_MolText(B2)</f>
         <v xml:space="preserve">
-       CDK0816191014
+       CDK0818190722
  18 19  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 O   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -3084,7 +3084,7 @@
         <v>00000000000000000001000000000000000001000001000000100100000000100010000000001100100000000111100001110000001010101010011011000001110100001100001100110011001110111101110</v>
       </c>
       <c r="O2" t="b">
-        <f>($M2=MID($N2,2,166))</f>
+        <f t="shared" ref="O2:O11" si="0">($M2=MID($N2,2,166))</f>
         <v>1</v>
       </c>
       <c r="P2" t="str">
@@ -3325,7 +3325,7 @@
       </c>
       <c r="BW2">
         <f>_xll.NCDK_LargestChain(B2)</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="BX2">
         <f>_xll.NCDK_LargestPiSystem(B2)</f>
@@ -3414,7 +3414,7 @@
       <c r="C3" t="str">
         <f>_xll.NCDK_MolText(B3)</f>
         <v xml:space="preserve">
-       CDK0817191606
+       CDK0818190722
   1  0  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
 M  END
@@ -3446,7 +3446,7 @@
         <v>InChI=1S/CH4/h1H4</v>
       </c>
       <c r="I3" t="b">
-        <f t="shared" ref="I3:I11" si="0">($G3=$H3)</f>
+        <f t="shared" ref="I3:I11" si="1">($G3=$H3)</f>
         <v>1</v>
       </c>
       <c r="J3" t="str">
@@ -3470,7 +3470,7 @@
         <v>00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000</v>
       </c>
       <c r="O3" t="b">
-        <f>($M3=MID($N3,2,166))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="P3" t="str">
@@ -3800,7 +3800,7 @@
       <c r="C4" t="str">
         <f>_xll.NCDK_MolText(B4)</f>
         <v xml:space="preserve">
-       CDK0817191606
+       CDK0818190722
   4  3  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -3844,7 +3844,7 @@
         <v>InChI=1S/C2H4O2/c1-2(3)4/h1H3,(H,3,4)</v>
       </c>
       <c r="I4" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J4" t="str">
@@ -3868,7 +3868,7 @@
         <v>00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000001000000000000001001011000100</v>
       </c>
       <c r="O4" t="b">
-        <f>($M4=MID($N4,2,166))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="P4" t="str">
@@ -4198,7 +4198,7 @@
       <c r="C5" t="str">
         <f>_xll.NCDK_MolText(B5)</f>
         <v xml:space="preserve">
-       CDK0817191606
+       CDK0818190722
   6  6  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -4252,7 +4252,7 @@
         <v>InChI=1S/C6H6/c1-2-4-6-5-3-1/h1-6H</v>
       </c>
       <c r="I5" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J5" t="str">
@@ -4276,7 +4276,7 @@
         <v>00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000011010</v>
       </c>
       <c r="O5" t="b">
-        <f>($M5=MID($N5,2,166))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="P5" t="str">
@@ -4606,7 +4606,7 @@
       <c r="C6" t="str">
         <f>_xll.NCDK_MolText(B6)</f>
         <v xml:space="preserve">
-       CDK0817191606
+       CDK0818190722
   7  7  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -4664,7 +4664,7 @@
         <v>InChI=1S/C7H8/c1-7-5-3-2-4-6-7/h2-6H,1H3</v>
       </c>
       <c r="I6" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J6" t="str">
@@ -4688,7 +4688,7 @@
         <v>00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001011010</v>
       </c>
       <c r="O6" t="b">
-        <f>($M6=MID($N6,2,166))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="P6" t="str">
@@ -4929,7 +4929,7 @@
       </c>
       <c r="BW6">
         <f>_xll.NCDK_LargestChain(B6)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BX6">
         <f>_xll.NCDK_LargestPiSystem(B6)</f>
@@ -5018,7 +5018,7 @@
       <c r="C7" t="str">
         <f>_xll.NCDK_MolText(B7)</f>
         <v xml:space="preserve">
-       CDK0817191606
+       CDK0818190722
   6  6  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -5072,7 +5072,7 @@
         <v>InChI=1S/C6H6/c1-2-4-6-5-3-1/h1-6H</v>
       </c>
       <c r="I7" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J7" t="str">
@@ -5096,7 +5096,7 @@
         <v>00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000011010</v>
       </c>
       <c r="O7" t="b">
-        <f>($M7=MID($N7,2,166))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="P7" t="str">
@@ -5145,15 +5145,15 @@
       </c>
       <c r="AA7" t="str">
         <f>_xll.NCDK_FCFP2($B7)</f>
-        <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>0000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="AB7" t="str">
         <f>_xll.NCDK_FCFP4($B7)</f>
-        <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>0000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="AC7" t="str">
         <f>_xll.NCDK_FCFP0($B7)</f>
-        <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>0000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="AD7" t="str">
         <f>_xll.NCDK_AtomPairs2DFingerprinter($B7)</f>
@@ -5161,47 +5161,47 @@
       </c>
       <c r="AE7" t="str">
         <f>_xll.NCDK_EStateFingerprinter($B7)</f>
-        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>0000000000010000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="AF7" t="str">
         <f>_xll.NCDK_ExtendedFingerprinter($B7)</f>
-        <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000001000000000000010001</v>
+        <v>000000000000000000000000000000000000000000000000000001000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000010000000000000000000000000000000000000000000000000000000000010001</v>
       </c>
       <c r="AG7" t="str">
         <f>_xll.NCDK_CDKFingerprinter($B7)</f>
-        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000010000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="AH7" t="str">
         <f>_xll.NCDK_KlekotaRothFingerprinter($B7)</f>
-        <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000010000000000000100000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="AI7" t="str">
         <f>_xll.NCDK_LingoFingerprinter($B7)</f>
-        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>0000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000</v>
       </c>
       <c r="AJ7" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($B7)</f>
-        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001010</v>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000011010</v>
       </c>
       <c r="AK7" t="str">
         <f>_xll.NCDK_ShortestPathFingerprinter($B7)</f>
-        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
       </c>
       <c r="AL7" t="str">
         <f>_xll.NCDK_SubstructureFingerprinter($B7)</f>
-        <v>0100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000001</v>
       </c>
       <c r="AM7" t="str">
         <f>_xll.NCDK_PubchemFingerprinter($B7)</f>
-        <v>00000000011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000100000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>00000000011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000001100000000000000000000000000000000000000000000000100000000000100000000001000000000000001100000000000010000000000000000000000000000000100000000000000000100000010000100000000000000000000000100000000000000000001000000000000000000000000010001000100000000000000000000000000010001000000010000010000000100010100000000001000100010000100000000010000000000000001000001000000000000000000010001000100000000111000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="AN7" s="2">
         <f>_xll.NCDK_MolecularWeight(B7)</f>
-        <v>72.064415380728008</v>
+        <v>78.112059903682749</v>
       </c>
       <c r="AO7" s="2">
         <f>_xll.NCDK_ExactMass(B7)</f>
-        <v>72</v>
+        <v>78.046950191999997</v>
       </c>
       <c r="AP7">
         <f>_xll.NCDK_AcidicGroupCount(B7)</f>
@@ -5209,11 +5209,11 @@
       </c>
       <c r="AQ7" s="4">
         <f>_xll.NCDK_ALogP(B7)</f>
-        <v>2.7372000000000005</v>
+        <v>1.4033999999999995</v>
       </c>
       <c r="AR7" s="4">
         <f>_xll.NCDK_XLogP(B7)</f>
-        <v>3.4139999999999997</v>
+        <v>2.0819999999999999</v>
       </c>
       <c r="AS7" s="4">
         <f>_xll.NCDK_MannholdLogP(B7)</f>
@@ -5221,15 +5221,15 @@
       </c>
       <c r="AT7" s="4">
         <f>_xll.NCDK_JPlogP(B7)</f>
-        <v>2.6952762459207973</v>
+        <v>1.8466303941078017</v>
       </c>
       <c r="AU7">
         <f>_xll.NCDK_AMolarRefractivity(B7)</f>
-        <v>27.606000000000002</v>
+        <v>30.955799999999996</v>
       </c>
       <c r="AV7">
         <f>_xll.NCDK_APol(B7)</f>
-        <v>10.56</v>
+        <v>14.560758</v>
       </c>
       <c r="AW7">
         <f>_xll.NCDK_AromaticAtomsCount(B7)</f>
@@ -5241,7 +5241,7 @@
       </c>
       <c r="AY7">
         <f>_xll.NCDK_AtomCount(B7)</f>
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="AZ7" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B7)</f>
@@ -5253,7 +5253,7 @@
       </c>
       <c r="BB7" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B7)</f>
-        <v>257.709834375, 257.709834375, 257.709834375, 128.8549171875, 0</v>
+        <v>233.87838834375, 233.87838834375, 233.87838834375, 116.939194171875, 0</v>
       </c>
       <c r="BC7">
         <f>_xll.NCDK_BasicGroupCount(B7)</f>
@@ -5261,7 +5261,7 @@
       </c>
       <c r="BD7" t="str">
         <f>_xll.NCDK_BCUT(B7)</f>
-        <v>11.9, 12.1000824042221, -0.15279744210896, 0.0472849621131451, 6.45375, 6.65383240422211</v>
+        <v>11.9, 12.1000824042221, -0.161758152069243, 0.0383242521528618, 6.738375, 6.93845740422211</v>
       </c>
       <c r="BE7">
         <f>_xll.NCDK_BondCount(B7)</f>
@@ -5269,15 +5269,15 @@
       </c>
       <c r="BF7">
         <f>_xll.NCDK_BPol(B7)</f>
-        <v>13.118483999999999</v>
+        <v>6.5592419999999994</v>
       </c>
       <c r="BG7" t="str">
         <f>_xll.NCDK_CarbonTypes(B7)</f>
-        <v>0, 0, 0, 0, 0, 0, 6, 0, 0</v>
+        <v>0, 0, 0, 6, 0, 0, 0, 0, 0</v>
       </c>
       <c r="BH7" t="str">
         <f>_xll.NCDK_ChiChain(B7)</f>
-        <v>0, 0, 0, 0.125, 0, 0, 0, 0, 0.125, 0</v>
+        <v>0, 0, 0, 0.125, 0, 0, 0, 0, 0.037037037037037, 0</v>
       </c>
       <c r="BI7" t="str">
         <f>_xll.NCDK_ChiCluster(B7)</f>
@@ -5289,7 +5289,7 @@
       </c>
       <c r="BK7" t="str">
         <f>_xll.NCDK_ChiPath(B7)</f>
-        <v>4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0, 4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0</v>
+        <v>4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0, 3.46410161513775, 2, 1.15470053837925, 0.666666666666667, 0.384900179459751, 0.222222222222222, 0, 0</v>
       </c>
       <c r="BL7" t="str">
         <f>_xll.NCDK_CPSA(B7)</f>
@@ -5309,7 +5309,7 @@
       </c>
       <c r="BP7">
         <f>_xll.NCDK_FragmentComplexity(B7)</f>
-        <v>6</v>
+        <v>114</v>
       </c>
       <c r="BQ7" t="str">
         <f>_xll.NCDK_GravitationalIndex(B7)</f>
@@ -5325,7 +5325,7 @@
       </c>
       <c r="BT7">
         <f>_xll.NCDK_HybridizationRatio(B7)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU7" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B7)</f>
@@ -5333,15 +5333,15 @@
       </c>
       <c r="BV7" t="str">
         <f>_xll.NCDK_KierHallSmarts(B7)</f>
-        <v>0, 0, 0, 0, 0, 0, 0, 0, 6, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
+        <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 6, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
       <c r="BW7">
         <f>_xll.NCDK_LargestChain(B7)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BX7">
         <f>_xll.NCDK_LargestPiSystem(B7)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="BY7" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B7)</f>
@@ -5377,7 +5377,7 @@
       </c>
       <c r="CG7" t="str">
         <f>_xll.NCDK_SmallRing(B7)</f>
-        <v>1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0</v>
+        <v>1, 1, 1, 1, 0, 0, 0, 1, 0, 0, 0</v>
       </c>
       <c r="CH7">
         <f>_xll.NCDK_TPSA(B7)</f>
@@ -5385,7 +5385,7 @@
       </c>
       <c r="CI7">
         <f>_xll.NCDK_VABC(B7)</f>
-        <v>99.975907755200197</v>
+        <v>81.166531652800174</v>
       </c>
       <c r="CJ7">
         <f>_xll.NCDK_VAdjMa(B7)</f>
@@ -5393,11 +5393,11 @@
       </c>
       <c r="CK7" s="2">
         <f>_xll.NCDK_MolecularWeight(B7)</f>
-        <v>72.064415380728008</v>
+        <v>78.112059903682749</v>
       </c>
       <c r="CL7" s="3">
         <f>_xll.NCDK_ExactMass(B7)</f>
-        <v>72</v>
+        <v>78.046950191999997</v>
       </c>
       <c r="CM7" t="str">
         <f>_xll.NCDK_WeightedPath(B7)</f>
@@ -5426,7 +5426,7 @@
       <c r="C8" t="str">
         <f>_xll.NCDK_MolText(B8)</f>
         <v xml:space="preserve">
-       CDK0817191606
+       CDK0818190722
   6  6  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -5480,7 +5480,7 @@
         <v>InChI=1S/C6H6/c1-2-4-6-5-3-1/h1-6H</v>
       </c>
       <c r="I8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J8" t="str">
@@ -5504,7 +5504,7 @@
         <v>00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000011010</v>
       </c>
       <c r="O8" t="b">
-        <f>($M8=MID($N8,2,166))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="P8" t="str">
@@ -5553,15 +5553,15 @@
       </c>
       <c r="AA8" t="str">
         <f>_xll.NCDK_FCFP2($B8)</f>
-        <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>0000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="AB8" t="str">
         <f>_xll.NCDK_FCFP4($B8)</f>
-        <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>0000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="AC8" t="str">
         <f>_xll.NCDK_FCFP0($B8)</f>
-        <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>0000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="AD8" t="str">
         <f>_xll.NCDK_AtomPairs2DFingerprinter($B8)</f>
@@ -5569,47 +5569,47 @@
       </c>
       <c r="AE8" t="str">
         <f>_xll.NCDK_EStateFingerprinter($B8)</f>
-        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>0000000000010000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="AF8" t="str">
         <f>_xll.NCDK_ExtendedFingerprinter($B8)</f>
-        <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000001000000000000010001</v>
+        <v>000000000000000000000000000000000000000000000000000001000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000010000000000000000000000000000000000000000000000000000000000010001</v>
       </c>
       <c r="AG8" t="str">
         <f>_xll.NCDK_CDKFingerprinter($B8)</f>
-        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000010000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="AH8" t="str">
         <f>_xll.NCDK_KlekotaRothFingerprinter($B8)</f>
-        <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000010010100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000010000000000000100000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="AI8" t="str">
         <f>_xll.NCDK_LingoFingerprinter($B8)</f>
-        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>0000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000</v>
       </c>
       <c r="AJ8" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($B8)</f>
-        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001010</v>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000011010</v>
       </c>
       <c r="AK8" t="str">
         <f>_xll.NCDK_ShortestPathFingerprinter($B8)</f>
-        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
       </c>
       <c r="AL8" t="str">
         <f>_xll.NCDK_SubstructureFingerprinter($B8)</f>
-        <v>0100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000001</v>
       </c>
       <c r="AM8" t="str">
         <f>_xll.NCDK_PubchemFingerprinter($B8)</f>
-        <v>00000000011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000100000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>00000000011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000001100000000000000000000000000000000000000000000000100000000000100000000001000000000000001100000000000010000000000000000000000000000000100000000000000000100000010000100000000000000000000000100000000000000000001000000000000000000000000010001000100000000000000000000000000010001000000010000010000000100010100000000001000100010000100000000010000000000000001000001000000000000000000010001000100000000111000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="AN8" s="2">
         <f>_xll.NCDK_MolecularWeight(B8)</f>
-        <v>72.064415380728008</v>
+        <v>78.112059903682749</v>
       </c>
       <c r="AO8" s="2">
         <f>_xll.NCDK_ExactMass(B8)</f>
-        <v>72</v>
+        <v>78.046950191999997</v>
       </c>
       <c r="AP8">
         <f>_xll.NCDK_AcidicGroupCount(B8)</f>
@@ -5617,11 +5617,11 @@
       </c>
       <c r="AQ8" s="4">
         <f>_xll.NCDK_ALogP(B8)</f>
-        <v>2.7372000000000005</v>
+        <v>1.4033999999999995</v>
       </c>
       <c r="AR8" s="4">
         <f>_xll.NCDK_XLogP(B8)</f>
-        <v>3.4139999999999997</v>
+        <v>2.0819999999999999</v>
       </c>
       <c r="AS8" s="4">
         <f>_xll.NCDK_MannholdLogP(B8)</f>
@@ -5629,15 +5629,15 @@
       </c>
       <c r="AT8" s="4">
         <f>_xll.NCDK_JPlogP(B8)</f>
-        <v>2.6952762459207973</v>
+        <v>1.8466303941078017</v>
       </c>
       <c r="AU8">
         <f>_xll.NCDK_AMolarRefractivity(B8)</f>
-        <v>27.606000000000002</v>
+        <v>30.955799999999996</v>
       </c>
       <c r="AV8">
         <f>_xll.NCDK_APol(B8)</f>
-        <v>10.56</v>
+        <v>14.560758</v>
       </c>
       <c r="AW8">
         <f>_xll.NCDK_AromaticAtomsCount(B8)</f>
@@ -5649,7 +5649,7 @@
       </c>
       <c r="AY8">
         <f>_xll.NCDK_AtomCount(B8)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="AZ8" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B8)</f>
@@ -5661,7 +5661,7 @@
       </c>
       <c r="BB8" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B8)</f>
-        <v>257.709834375, 257.709834375, 257.709834375, 128.8549171875, 0</v>
+        <v>233.87838834375, 233.87838834375, 233.87838834375, 116.939194171875, 0</v>
       </c>
       <c r="BC8">
         <f>_xll.NCDK_BasicGroupCount(B8)</f>
@@ -5669,7 +5669,7 @@
       </c>
       <c r="BD8" t="str">
         <f>_xll.NCDK_BCUT(B8)</f>
-        <v>11.9, 12.1000824042221, -0.15279744210896, 0.0472849621131451, 6.45375, 6.65383240422211</v>
+        <v>11.9, 12.1000824042221, -0.161758152069243, 0.0383242521528618, 6.738375, 6.93845740422211</v>
       </c>
       <c r="BE8">
         <f>_xll.NCDK_BondCount(B8)</f>
@@ -5677,15 +5677,15 @@
       </c>
       <c r="BF8">
         <f>_xll.NCDK_BPol(B8)</f>
-        <v>0</v>
+        <v>6.5592419999999994</v>
       </c>
       <c r="BG8" t="str">
         <f>_xll.NCDK_CarbonTypes(B8)</f>
-        <v>0, 0, 0, 0, 0, 0, 6, 0, 0</v>
+        <v>0, 0, 0, 6, 0, 0, 0, 0, 0</v>
       </c>
       <c r="BH8" t="str">
         <f>_xll.NCDK_ChiChain(B8)</f>
-        <v>0, 0, 0, 0.125, 0, 0, 0, 0, 0.125, 0</v>
+        <v>0, 0, 0, 0.125, 0, 0, 0, 0, 0.037037037037037, 0</v>
       </c>
       <c r="BI8" t="str">
         <f>_xll.NCDK_ChiCluster(B8)</f>
@@ -5697,7 +5697,7 @@
       </c>
       <c r="BK8" t="str">
         <f>_xll.NCDK_ChiPath(B8)</f>
-        <v>4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0, 4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0</v>
+        <v>4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0, 3.46410161513775, 2, 1.15470053837925, 0.666666666666667, 0.384900179459751, 0.222222222222222, 0, 0</v>
       </c>
       <c r="BL8" t="str">
         <f>_xll.NCDK_CPSA(B8)</f>
@@ -5717,7 +5717,7 @@
       </c>
       <c r="BP8">
         <f>_xll.NCDK_FragmentComplexity(B8)</f>
-        <v>6</v>
+        <v>114</v>
       </c>
       <c r="BQ8" t="str">
         <f>_xll.NCDK_GravitationalIndex(B8)</f>
@@ -5733,7 +5733,7 @@
       </c>
       <c r="BT8">
         <f>_xll.NCDK_HybridizationRatio(B8)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU8" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B8)</f>
@@ -5741,15 +5741,15 @@
       </c>
       <c r="BV8" t="str">
         <f>_xll.NCDK_KierHallSmarts(B8)</f>
-        <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
+        <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 6, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
       <c r="BW8">
         <f>_xll.NCDK_LargestChain(B8)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BX8">
         <f>_xll.NCDK_LargestPiSystem(B8)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="BY8" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B8)</f>
@@ -5785,7 +5785,7 @@
       </c>
       <c r="CG8" t="str">
         <f>_xll.NCDK_SmallRing(B8)</f>
-        <v>1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0</v>
+        <v>1, 1, 1, 1, 0, 0, 0, 1, 0, 0, 0</v>
       </c>
       <c r="CH8">
         <f>_xll.NCDK_TPSA(B8)</f>
@@ -5793,7 +5793,7 @@
       </c>
       <c r="CI8">
         <f>_xll.NCDK_VABC(B8)</f>
-        <v>99.975907755200197</v>
+        <v>81.166531652800174</v>
       </c>
       <c r="CJ8">
         <f>_xll.NCDK_VAdjMa(B8)</f>
@@ -5801,11 +5801,11 @@
       </c>
       <c r="CK8" s="2">
         <f>_xll.NCDK_MolecularWeight(B8)</f>
-        <v>72.064415380728008</v>
+        <v>78.112059903682749</v>
       </c>
       <c r="CL8" s="3">
         <f>_xll.NCDK_ExactMass(B8)</f>
-        <v>72</v>
+        <v>78.046950191999997</v>
       </c>
       <c r="CM8" t="str">
         <f>_xll.NCDK_WeightedPath(B8)</f>
@@ -5834,7 +5834,7 @@
       <c r="C9" t="str">
         <f>_xll.NCDK_MolText(B9)</f>
         <v xml:space="preserve">
-       CDK0817191606
+       CDK0818190722
   6  6  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -5888,7 +5888,7 @@
         <v>InChI=1S/C6H6/c1-2-4-6-5-3-1/h1-6H</v>
       </c>
       <c r="I9" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J9" t="str">
@@ -5912,7 +5912,7 @@
         <v>00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000011010</v>
       </c>
       <c r="O9" t="b">
-        <f>($M9=MID($N9,2,166))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="P9" t="str">
@@ -5961,15 +5961,15 @@
       </c>
       <c r="AA9" t="str">
         <f>_xll.NCDK_FCFP2($B9)</f>
-        <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>0000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="AB9" t="str">
         <f>_xll.NCDK_FCFP4($B9)</f>
-        <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>0000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="AC9" t="str">
         <f>_xll.NCDK_FCFP0($B9)</f>
-        <v>1000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>0000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="AD9" t="str">
         <f>_xll.NCDK_AtomPairs2DFingerprinter($B9)</f>
@@ -5977,47 +5977,47 @@
       </c>
       <c r="AE9" t="str">
         <f>_xll.NCDK_EStateFingerprinter($B9)</f>
-        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>0000000000010000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="AF9" t="str">
         <f>_xll.NCDK_ExtendedFingerprinter($B9)</f>
-        <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000001000000000000010001</v>
+        <v>000000000000000000000000000000000000000000000000000001000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000010000000000000000000000000000000000000000000000000000000000010001</v>
       </c>
       <c r="AG9" t="str">
         <f>_xll.NCDK_CDKFingerprinter($B9)</f>
-        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000010000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="AH9" t="str">
         <f>_xll.NCDK_KlekotaRothFingerprinter($B9)</f>
-        <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000010010100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000010000000000000100000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="AI9" t="str">
         <f>_xll.NCDK_LingoFingerprinter($B9)</f>
-        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>0000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000</v>
       </c>
       <c r="AJ9" t="str">
         <f>_xll.NCDK_MACCSFingerprinter($B9)</f>
-        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001010</v>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000011010</v>
       </c>
       <c r="AK9" t="str">
         <f>_xll.NCDK_ShortestPathFingerprinter($B9)</f>
-        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
       </c>
       <c r="AL9" t="str">
         <f>_xll.NCDK_SubstructureFingerprinter($B9)</f>
-        <v>0100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000001</v>
       </c>
       <c r="AM9" t="str">
         <f>_xll.NCDK_PubchemFingerprinter($B9)</f>
-        <v>00000000011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000100000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+        <v>00000000011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001100000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000001100000000000000000000000000000000000000000000000100000000000100000000001000000000000001100000000000010000000000000000000000000000000100000000000000000100000010000100000000000000000000000100000000000000000001000000000000000000000000010001000100000000000000000000000000010001000000010000010000000100010100000000001000100010000100000000010000000000000001000001000000000000000000010001000100000000111000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
       <c r="AN9" s="2">
         <f>_xll.NCDK_MolecularWeight(B9)</f>
-        <v>72.064415380728008</v>
+        <v>78.112059903682749</v>
       </c>
       <c r="AO9" s="2">
         <f>_xll.NCDK_ExactMass(B9)</f>
-        <v>72</v>
+        <v>78.046950191999997</v>
       </c>
       <c r="AP9">
         <f>_xll.NCDK_AcidicGroupCount(B9)</f>
@@ -6025,11 +6025,11 @@
       </c>
       <c r="AQ9" s="4">
         <f>_xll.NCDK_ALogP(B9)</f>
-        <v>2.7372000000000005</v>
+        <v>1.4033999999999995</v>
       </c>
       <c r="AR9" s="4">
         <f>_xll.NCDK_XLogP(B9)</f>
-        <v>3.4139999999999997</v>
+        <v>2.0819999999999999</v>
       </c>
       <c r="AS9" s="4">
         <f>_xll.NCDK_MannholdLogP(B9)</f>
@@ -6037,15 +6037,15 @@
       </c>
       <c r="AT9" s="4">
         <f>_xll.NCDK_JPlogP(B9)</f>
-        <v>2.6952762459207973</v>
+        <v>1.8466303941078017</v>
       </c>
       <c r="AU9">
         <f>_xll.NCDK_AMolarRefractivity(B9)</f>
-        <v>27.606000000000002</v>
+        <v>30.955799999999996</v>
       </c>
       <c r="AV9">
         <f>_xll.NCDK_APol(B9)</f>
-        <v>10.56</v>
+        <v>14.560758</v>
       </c>
       <c r="AW9">
         <f>_xll.NCDK_AromaticAtomsCount(B9)</f>
@@ -6057,7 +6057,7 @@
       </c>
       <c r="AY9">
         <f>_xll.NCDK_AtomCount(B9)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="AZ9" t="str">
         <f>_xll.NCDK_AutocorrelationCharge(B9)</f>
@@ -6069,7 +6069,7 @@
       </c>
       <c r="BB9" t="str">
         <f>_xll.NCDK_AutocorrelationPolarizability(B9)</f>
-        <v>257.709834375, 257.709834375, 257.709834375, 128.8549171875, 0</v>
+        <v>233.87838834375, 233.87838834375, 233.87838834375, 116.939194171875, 0</v>
       </c>
       <c r="BC9">
         <f>_xll.NCDK_BasicGroupCount(B9)</f>
@@ -6077,7 +6077,7 @@
       </c>
       <c r="BD9" t="str">
         <f>_xll.NCDK_BCUT(B9)</f>
-        <v>11.9, 12.1000824042221, -0.15279744210896, 0.0472849621131451, 6.45375, 6.65383240422211</v>
+        <v>11.9, 12.1000824042221, -0.161758152069243, 0.0383242521528618, 6.738375, 6.93845740422211</v>
       </c>
       <c r="BE9">
         <f>_xll.NCDK_BondCount(B9)</f>
@@ -6085,15 +6085,15 @@
       </c>
       <c r="BF9">
         <f>_xll.NCDK_BPol(B9)</f>
-        <v>0</v>
+        <v>6.5592419999999994</v>
       </c>
       <c r="BG9" t="str">
         <f>_xll.NCDK_CarbonTypes(B9)</f>
-        <v>0, 0, 0, 0, 0, 0, 6, 0, 0</v>
+        <v>0, 0, 0, 6, 0, 0, 0, 0, 0</v>
       </c>
       <c r="BH9" t="str">
         <f>_xll.NCDK_ChiChain(B9)</f>
-        <v>0, 0, 0, 0.125, 0, 0, 0, 0, 0.125, 0</v>
+        <v>0, 0, 0, 0.125, 0, 0, 0, 0, 0.037037037037037, 0</v>
       </c>
       <c r="BI9" t="str">
         <f>_xll.NCDK_ChiCluster(B9)</f>
@@ -6105,7 +6105,7 @@
       </c>
       <c r="BK9" t="str">
         <f>_xll.NCDK_ChiPath(B9)</f>
-        <v>4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0, 4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0</v>
+        <v>4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0, 3.46410161513775, 2, 1.15470053837925, 0.666666666666667, 0.384900179459751, 0.222222222222222, 0, 0</v>
       </c>
       <c r="BL9" t="str">
         <f>_xll.NCDK_CPSA(B9)</f>
@@ -6125,7 +6125,7 @@
       </c>
       <c r="BP9">
         <f>_xll.NCDK_FragmentComplexity(B9)</f>
-        <v>6</v>
+        <v>114</v>
       </c>
       <c r="BQ9" t="str">
         <f>_xll.NCDK_GravitationalIndex(B9)</f>
@@ -6141,7 +6141,7 @@
       </c>
       <c r="BT9">
         <f>_xll.NCDK_HybridizationRatio(B9)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU9" t="str">
         <f>_xll.NCDK_KappaShapeIndices(B9)</f>
@@ -6149,15 +6149,15 @@
       </c>
       <c r="BV9" t="str">
         <f>_xll.NCDK_KierHallSmarts(B9)</f>
-        <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
+        <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 6, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
       <c r="BW9">
         <f>_xll.NCDK_LargestChain(B9)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BX9">
         <f>_xll.NCDK_LargestPiSystem(B9)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="BY9" t="str">
         <f>_xll.NCDK_LengthOverBreadth(B9)</f>
@@ -6193,7 +6193,7 @@
       </c>
       <c r="CG9" t="str">
         <f>_xll.NCDK_SmallRing(B9)</f>
-        <v>1, 0, 1, 0, 0, 0, 0, 1, 0, 0, 0</v>
+        <v>1, 1, 1, 1, 0, 0, 0, 1, 0, 0, 0</v>
       </c>
       <c r="CH9">
         <f>_xll.NCDK_TPSA(B9)</f>
@@ -6201,7 +6201,7 @@
       </c>
       <c r="CI9">
         <f>_xll.NCDK_VABC(B9)</f>
-        <v>99.975907755200197</v>
+        <v>81.166531652800174</v>
       </c>
       <c r="CJ9">
         <f>_xll.NCDK_VAdjMa(B9)</f>
@@ -6209,11 +6209,11 @@
       </c>
       <c r="CK9" s="2">
         <f>_xll.NCDK_MolecularWeight(B9)</f>
-        <v>72.064415380728008</v>
+        <v>78.112059903682749</v>
       </c>
       <c r="CL9" s="3">
         <f>_xll.NCDK_ExactMass(B9)</f>
-        <v>72</v>
+        <v>78.046950191999997</v>
       </c>
       <c r="CM9" t="str">
         <f>_xll.NCDK_WeightedPath(B9)</f>
@@ -6242,7 +6242,7 @@
       <c r="C10" t="str">
         <f>_xll.NCDK_MolText(B10)</f>
         <v xml:space="preserve">cholesterol 
-       CDK08171916063D
+       CDK08181907223D
  74 77  0  0  1  0  0  0  0  0999 V2000
    -4.4007   -0.4401    1.6251 C   0  0  2  0  0  0  0  0  0  0  0  0
    -5.4580   -1.0449    0.6688 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -6482,7 +6482,7 @@
         <v>InChI=1S/C27H46O/c1-18(2)7-6-8-19(3)23-11-12-24-22-10-9-20-17-21(28)13-15-26(20,4)25(22)14-16-27(23,24)5/h9,18-19,21-25,28H,6-8,10-17H2,1-5H3</v>
       </c>
       <c r="I10" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J10" t="str">
@@ -6506,7 +6506,7 @@
         <v>00000000000000000000000000100000000000000000000000100000000000000010000000101000000000000010000010010100110010001001101000000001110010000001010101010110100101001001110</v>
       </c>
       <c r="O10" t="b">
-        <f>($M10=MID($N10,2,166))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P10" t="str">
@@ -6836,7 +6836,7 @@
       <c r="C11" t="str">
         <f>_xll.NCDK_MolText(B11)</f>
         <v xml:space="preserve">
-       CDK0817191606
+       CDK0818190722
  28 31  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -6984,7 +6984,7 @@
         <v>InChI=1S/C27H46O/c1-18(2)7-6-8-19(3)23-11-12-24-22-10-9-20-17-21(28)13-15-26(20,4)25(22)14-16-27(23,24)5/h9,18-19,21-25,28H,6-8,10-17H2,1-5H3</v>
       </c>
       <c r="I11" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J11" t="str">
@@ -7008,7 +7008,7 @@
         <v>00000000000000000000000000100000000000000000000000100000000000000010000000101000000000000010000010010100110010001001101000000001110010000001010101010110100101001001110</v>
       </c>
       <c r="O11" t="b">
-        <f>($M11=MID($N11,2,166))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P11" t="str">
@@ -7249,7 +7249,7 @@
       </c>
       <c r="BW11">
         <f>_xll.NCDK_LargestChain(B11)</f>
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="BX11">
         <f>_xll.NCDK_LargestPiSystem(B11)</f>
@@ -7339,9 +7339,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D78F5C-B236-40D1-A056-FD195DD12728}">
   <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -8648,9 +8646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1647DD59-D041-4640-9111-9E35EC2330E5}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
-    </sheetView>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -8711,7 +8707,7 @@
         <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="236" customHeight="1" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
Cleanup and update documentation.
</commit_message>
<xml_diff>
--- a/NCDK-Excel/ExcelNCDK-Test.xlsx
+++ b/NCDK-Excel/ExcelNCDK-Test.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFF8FE9-8D74-4324-927C-2A4411C7BB31}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E19EB49-DFFB-48CB-A9FD-123B9A0C2A6E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="407" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2467" yWindow="2820" windowWidth="11431" windowHeight="10523" tabRatio="407" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Descriptors" sheetId="2" r:id="rId1"/>
-    <sheet name="SDF" sheetId="4" r:id="rId2"/>
-    <sheet name="SDF-RDKit" sheetId="6" r:id="rId3"/>
-    <sheet name="Picture" sheetId="5" r:id="rId4"/>
+    <sheet name="Picture" sheetId="5" r:id="rId1"/>
+    <sheet name="Descriptors" sheetId="2" r:id="rId2"/>
+    <sheet name="SDF" sheetId="4" r:id="rId3"/>
+    <sheet name="SDF-RDKit" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="741">
   <si>
     <t>CC(=O)O</t>
     <phoneticPr fontId="1"/>
@@ -3554,6 +3554,14 @@
   <si>
     <t>NCGC00261465-01</t>
   </si>
+  <si>
+    <t>SMILES</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MACCS</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
@@ -3636,16 +3644,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1870283</xdr:colOff>
+      <xdr:colOff>1865387</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="NCDK-Picture 2">
+        <xdr:cNvPr id="4" name="NCDK-Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F0B3882-1633-42E3-9E57-415022A0CCF0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4897602F-2152-4920-96EB-7572FA2742A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3668,7 +3676,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="857250" y="228600"/>
-          <a:ext cx="1870283" cy="1212850"/>
+          <a:ext cx="1865387" cy="1209675"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3686,16 +3694,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>543242</xdr:colOff>
+      <xdr:colOff>538638</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="NCDK-Picture 10">
+        <xdr:cNvPr id="8" name="NCDK-Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A56F313A-9F61-479D-80B5-646FE2765E88}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EE3003B-B168-4B20-AC9E-800BA33918A8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3717,8 +3725,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="857250" y="1441450"/>
-          <a:ext cx="543242" cy="374650"/>
+          <a:off x="857250" y="1438275"/>
+          <a:ext cx="538638" cy="371475"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3742,10 +3750,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="NCDK-Picture 11">
+        <xdr:cNvPr id="12" name="NCDK-Picture 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15B25713-3407-4776-87DC-92514CFE5334}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C88234B-A9D3-4265-8D61-C2F74D72D4AA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3767,7 +3775,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="857250" y="1816100"/>
+          <a:off x="857250" y="1809750"/>
           <a:ext cx="2136324" cy="762000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3786,16 +3794,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>652073</xdr:colOff>
+      <xdr:colOff>649262</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="NCDK-Picture 12">
+        <xdr:cNvPr id="16" name="NCDK-Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07159D9B-4CBC-4038-8C7E-CB4F5A26D03F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE35E0DC-D130-45CB-A6D8-151C0B562D2D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3817,8 +3825,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="857250" y="2578100"/>
-          <a:ext cx="652073" cy="736600"/>
+          <a:off x="857250" y="2571750"/>
+          <a:ext cx="649262" cy="733425"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3842,10 +3850,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="NCDK-Picture 13">
+        <xdr:cNvPr id="19" name="NCDK-Picture 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD6D507F-8428-4709-91DD-4FAE9CFCF944}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8C6232E-3AC3-4F2D-8DEA-B91BE76FEB6F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3867,7 +3875,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="857250" y="3314700"/>
+          <a:off x="857250" y="3305175"/>
           <a:ext cx="603031" cy="971550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3886,16 +3894,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>786984</xdr:colOff>
+      <xdr:colOff>784173</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="NCDK-Picture 14">
+        <xdr:cNvPr id="21" name="NCDK-Picture 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AD3AD25-9D5F-4877-BC0A-8EDD3FC11B52}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4665303D-23ED-4074-8024-13968C6B131C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3917,8 +3925,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="857250" y="4286250"/>
-          <a:ext cx="786984" cy="889000"/>
+          <a:off x="857250" y="4276725"/>
+          <a:ext cx="784173" cy="885825"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3938,14 +3946,14 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>1721782</xdr:rowOff>
+      <xdr:rowOff>1720914</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="NCDK-Picture 15">
+        <xdr:cNvPr id="23" name="NCDK-Picture 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2810D1FF-7C8E-46C7-9FBF-BF8B194B5E10}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EB0115C-AED4-4761-A332-8BDE380E6E24}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3967,8 +3975,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="857250" y="5175250"/>
-          <a:ext cx="3149600" cy="1721782"/>
+          <a:off x="857250" y="5162550"/>
+          <a:ext cx="3148013" cy="1720914"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3980,22 +3988,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2974428</xdr:colOff>
+      <xdr:colOff>2974427</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="NCDK-Picture 16">
+        <xdr:cNvPr id="25" name="NCDK-Picture 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B426472-EC50-432C-8E3C-8322AE333738}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{063C8F84-DF2E-4B42-B5CB-D95EF332E12E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4017,7 +4025,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="857251" y="8172450"/>
+          <a:off x="857250" y="8158163"/>
           <a:ext cx="2974427" cy="2133600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4292,31 +4300,276 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1647DD59-D041-4640-9111-9E35EC2330E5}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.7"/>
+  <cols>
+    <col min="1" max="1" width="11.25" customWidth="1"/>
+    <col min="2" max="2" width="41.3125" customWidth="1"/>
+    <col min="3" max="5" width="15.8125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>739</v>
+      </c>
+      <c r="D1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" t="s">
+        <v>740</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="95.55" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="str">
+        <f>_xll.RDKit_SMILES($B2)</f>
+        <v>CCC1(C2=CCCCCC2)C(=O)NC(=O)NC1=O</v>
+      </c>
+      <c r="D2" t="str">
+        <f>_xll.NCDK_ECFP4($B2)</f>
+        <v>0000000000000010000000001100000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000010010000000000000000000000000000000000000000000000000000000000000010001000000000000010000000100000000000000000000000000011000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000100000000000000000000000000000000101000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000010000010000000000000100000000000010100010000001000000000000000000000000000100</v>
+      </c>
+      <c r="E2" t="str">
+        <f>_xll.RDKit_MACCSFingerprint($B2)</f>
+        <v>00000000000000000001000000000000000001000001000000100100000000100010000000001100100000000111100001110000001010101010011011000001110100001100001100110011001110111101110</v>
+      </c>
+      <c r="F2" s="4">
+        <f>_xll.NCDK_XLogP($B2)</f>
+        <v>2.1759999999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="29.55" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="str">
+        <f>_xll.RDKit_SMILES($B3)</f>
+        <v>C</v>
+      </c>
+      <c r="D3" t="str">
+        <f>_xll.NCDK_ECFP4($B3)</f>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="E3" t="str">
+        <f>_xll.RDKit_MACCSFingerprint($B3)</f>
+        <v>00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000</v>
+      </c>
+      <c r="F3" s="4">
+        <f>_xll.NCDK_XLogP($B3)</f>
+        <v>0.73899999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C4" t="str">
+        <f>_xll.RDKit_SMILES($B4)</f>
+        <v>CCCCCC(=O)O</v>
+      </c>
+      <c r="D4" t="str">
+        <f>_xll.NCDK_ECFP4($B4)</f>
+        <v>0000000000000000000100000000000000000000000000000000000000000100000000000000000000000000000001000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000100000000001000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000100000000000000000000000001000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000001000000000000000001000000000000000000000000000000</v>
+      </c>
+      <c r="E4" t="str">
+        <f>_xll.RDKit_MACCSFingerprint($B4)</f>
+        <v>00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000011000000000000100010000011101000010000010010000001000000010000001101011000100</v>
+      </c>
+      <c r="F4" s="4">
+        <f>_xll.NCDK_XLogP($B4)</f>
+        <v>1.8800000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="58.05" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="str">
+        <f>_xll.RDKit_SMILES($B5)</f>
+        <v>c1ccccc1</v>
+      </c>
+      <c r="D5" t="str">
+        <f>_xll.NCDK_ECFP4($B5)</f>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="E5" t="str">
+        <f>_xll.RDKit_MACCSFingerprint($B5)</f>
+        <v>00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000011010</v>
+      </c>
+      <c r="F5" s="4">
+        <f>_xll.NCDK_XLogP($B5)</f>
+        <v>2.0220000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" t="str">
+        <f>_xll.RDKit_SMILES($B6)</f>
+        <v>Cc1ccccc1</v>
+      </c>
+      <c r="D6" t="str">
+        <f>_xll.NCDK_ECFP4($B6)</f>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000010000000000000000000100000000000000000000000000000010000000000000000000000000</v>
+      </c>
+      <c r="E6" t="str">
+        <f>_xll.RDKit_MACCSFingerprint($B6)</f>
+        <v>00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001011010</v>
+      </c>
+      <c r="F6" s="4">
+        <f>_xll.NCDK_XLogP($B6)</f>
+        <v>2.4590000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="70.05" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" t="str">
+        <f>_xll.RDKit_SMILES($B7)</f>
+        <v>c1ccccc1</v>
+      </c>
+      <c r="D7" t="str">
+        <f>_xll.NCDK_ECFP4($B7)</f>
+        <v>0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="E7" t="str">
+        <f>_xll.RDKit_MACCSFingerprint($B7)</f>
+        <v>00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000011010</v>
+      </c>
+      <c r="F7" s="4">
+        <f>_xll.NCDK_XLogP($B7)</f>
+        <v>2.0819999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="236" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" t="str">
+        <f>_xll.RDKit_SMILES($B8)</f>
+        <v>CC(C)CCCC(C)C1CCC2C3CC=C4CC(O)CCC4(C)C3CCC12C</v>
+      </c>
+      <c r="D8" t="str">
+        <f>_xll.NCDK_ECFP4($B8)</f>
+        <v>0000000000000010000000001100000000000000000100001000000000010000000000000001000000001010100000000000000000000000000000000000000000000100000000010000000010000000000000000000000000000000000000000000000000000010000000000000010000000010000000000000000000000000000000000000000001000000000010000000001000000000000000100000010000000000000000000000000000000010000010000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000100000000000000000000000001000100000000000100000000000000000000000010000000000000000000000000100000000000000000000000000000000000000000000000000000000000100000000000000000000000000000000000000000000000000000000000000010100000000000000000000000000000000000000000000000000000000000000100010000000000001000001000000000000000000000011000000000000010100000000000000000000000000000000000000000100000000000000000000000000000100000000000001000010000000000000000000000000010000000000010000000000000000000100000001000000000000000100000000000000000000000000000000</v>
+      </c>
+      <c r="E8" t="str">
+        <f>_xll.RDKit_MACCSFingerprint($B8)</f>
+        <v>00000000000000000000000000100000000000000000000000100000000000000010000000101000000000000010000010010100110010001001101000000001110010000001010101010110100101001001110</v>
+      </c>
+      <c r="F8" s="4">
+        <f>_xll.NCDK_XLogP($B8)</f>
+        <v>10.518000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="168" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" t="str">
+        <f>_xll.RDKit_SMILES($B9)</f>
+        <v>CC(C)CCCC(C)C1CCC2C3CC=C4CC(O)CCC4(C)C3CCC12C</v>
+      </c>
+      <c r="D9" t="str">
+        <f>_xll.NCDK_ECFP4($B9)</f>
+        <v>0000000000000010000000001100000000000000000100001000100000010000000000000000000000000000100000000000000000000000000000000000000000000100000000010000000010000000000000000000000000000000000000000000000000000010000001000000010000000010000000000000000000000000000000000000000001000000000010010000000000000000000000000000000000000010000000000000001000000010000000000000000000000000000000000000000000000001000000000000000000000000000000000000000000000000000000000000000000000100100000000000000000010000001000000000000000100000000000000000000000010000001000000000000000000100000000000000000001000000000000000000000000000000010000000100000000000000000000000000000000000000000000000000000000000000010000000100000000000000000000000000010000000000000000000000000000001000000000000001000001000100000000000010000001000100000000000100000000000000000000000000000000000000000000000000000001000000000000000000000000000001000000000000000000000000000000010000000000010000000000000000000100000000000000000000000100000000000000000000000000000000</v>
+      </c>
+      <c r="E9" t="str">
+        <f>_xll.RDKit_MACCSFingerprint($B9)</f>
+        <v>00000000000000000000000000100000000000000000000000100000000000000010000000101000000000000010000010010100110010001001101000000001110010000001010101010110100101001001110</v>
+      </c>
+      <c r="F9" s="4">
+        <f>_xll.NCDK_XLogP($B9)</f>
+        <v>10.518000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="F11" s="4"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B185B08-1BAB-4052-951E-1A2BC1F97D8F}">
   <dimension ref="A1:CP11"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>
   <cols>
     <col min="1" max="2" width="11.25" customWidth="1"/>
-    <col min="3" max="5" width="8.83203125" customWidth="1"/>
-    <col min="6" max="11" width="11.33203125" customWidth="1"/>
-    <col min="12" max="12" width="10.83203125" style="2" customWidth="1"/>
-    <col min="13" max="15" width="10.83203125" customWidth="1"/>
+    <col min="3" max="5" width="8.8125" customWidth="1"/>
+    <col min="6" max="11" width="11.3125" customWidth="1"/>
+    <col min="12" max="12" width="10.8125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="10.8125" customWidth="1"/>
+    <col min="14" max="14" width="32.3125" customWidth="1"/>
+    <col min="15" max="15" width="10.8125" customWidth="1"/>
     <col min="16" max="29" width="7.75" customWidth="1"/>
-    <col min="30" max="39" width="8.33203125" customWidth="1"/>
-    <col min="40" max="41" width="8.33203125" style="2" customWidth="1"/>
-    <col min="42" max="42" width="8.33203125" customWidth="1"/>
-    <col min="43" max="43" width="8.6640625" style="4" customWidth="1"/>
-    <col min="44" max="46" width="8.6640625" style="4"/>
-    <col min="47" max="47" width="8.6640625" customWidth="1"/>
-    <col min="69" max="69" width="14.83203125" customWidth="1"/>
-    <col min="89" max="89" width="8.6640625" style="2"/>
-    <col min="90" max="90" width="10.08203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="39" width="8.3125" customWidth="1"/>
+    <col min="40" max="41" width="8.3125" style="2" customWidth="1"/>
+    <col min="42" max="42" width="8.3125" customWidth="1"/>
+    <col min="43" max="43" width="8.6875" style="4" customWidth="1"/>
+    <col min="44" max="46" width="8.6875" style="4"/>
+    <col min="47" max="47" width="8.6875" customWidth="1"/>
+    <col min="69" max="69" width="14.8125" customWidth="1"/>
+    <col min="89" max="89" width="8.6875" style="2"/>
+    <col min="90" max="90" width="10.0625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:94" x14ac:dyDescent="0.7">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -4600,7 +4853,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:94" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:94" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -4854,7 +5107,7 @@
         <v>2.1996999999999991</v>
       </c>
       <c r="AR2" s="4">
-        <f>_xll.NCDK_XLogP(B2)</f>
+        <f>_xll.NCDK_XLogP($B2)</f>
         <v>2.1759999999999997</v>
       </c>
       <c r="AS2" s="4">
@@ -4990,7 +5243,7 @@
         <v>#N/A</v>
       </c>
       <c r="BZ2">
-        <f>_xll.NCDK_LongestAliphaticChain(B2)</f>
+        <f>_xll.NCDK_LongestAliphaticChain($B2)</f>
         <v>2</v>
       </c>
       <c r="CA2" t="str">
@@ -5058,7 +5311,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:94" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:94" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -5240,7 +5493,7 @@
         <v>0</v>
       </c>
       <c r="AR3" s="4">
-        <f>_xll.NCDK_XLogP(B3)</f>
+        <f>_xll.NCDK_XLogP($B3)</f>
         <v>0.73899999999999999</v>
       </c>
       <c r="AS3" s="4">
@@ -5376,7 +5629,7 @@
         <v>#N/A</v>
       </c>
       <c r="BZ3">
-        <f>_xll.NCDK_LongestAliphaticChain(B3)</f>
+        <f>_xll.NCDK_LongestAliphaticChain($B3)</f>
         <v>0</v>
       </c>
       <c r="CA3" t="str">
@@ -5444,7 +5697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:94" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:94" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -5638,7 +5891,7 @@
         <v>-0.22990000000000016</v>
       </c>
       <c r="AR4" s="4">
-        <f>_xll.NCDK_XLogP(B4)</f>
+        <f>_xll.NCDK_XLogP($B4)</f>
         <v>-0.08</v>
       </c>
       <c r="AS4" s="4">
@@ -5774,7 +6027,7 @@
         <v>#N/A</v>
       </c>
       <c r="BZ4">
-        <f>_xll.NCDK_LongestAliphaticChain(B4)</f>
+        <f>_xll.NCDK_LongestAliphaticChain($B4)</f>
         <v>2</v>
       </c>
       <c r="CA4" t="str">
@@ -5842,7 +6095,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:94" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:94" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -6046,7 +6299,7 @@
         <v>1.8299999999999996</v>
       </c>
       <c r="AR5" s="4">
-        <f>_xll.NCDK_XLogP(B5)</f>
+        <f>_xll.NCDK_XLogP($B5)</f>
         <v>2.0220000000000002</v>
       </c>
       <c r="AS5" s="4">
@@ -6182,7 +6435,7 @@
         <v>#N/A</v>
       </c>
       <c r="BZ5">
-        <f>_xll.NCDK_LongestAliphaticChain(B5)</f>
+        <f>_xll.NCDK_LongestAliphaticChain($B5)</f>
         <v>0</v>
       </c>
       <c r="CA5" t="str">
@@ -6250,7 +6503,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:94" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:94" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A6" t="s">
         <v>84</v>
       </c>
@@ -6458,7 +6711,7 @@
         <v>2.3162000000000003</v>
       </c>
       <c r="AR6" s="4">
-        <f>_xll.NCDK_XLogP(B6)</f>
+        <f>_xll.NCDK_XLogP($B6)</f>
         <v>2.4590000000000001</v>
       </c>
       <c r="AS6" s="4">
@@ -6594,7 +6847,7 @@
         <v>#N/A</v>
       </c>
       <c r="BZ6">
-        <f>_xll.NCDK_LongestAliphaticChain(B6)</f>
+        <f>_xll.NCDK_LongestAliphaticChain($B6)</f>
         <v>0</v>
       </c>
       <c r="CA6" t="str">
@@ -6662,7 +6915,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:94" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:94" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -6866,7 +7119,7 @@
         <v>1.4033999999999995</v>
       </c>
       <c r="AR7" s="4">
-        <f>_xll.NCDK_XLogP(B7)</f>
+        <f>_xll.NCDK_XLogP($B7)</f>
         <v>2.0819999999999999</v>
       </c>
       <c r="AS7" s="4">
@@ -7002,7 +7255,7 @@
         <v>#N/A</v>
       </c>
       <c r="BZ7">
-        <f>_xll.NCDK_LongestAliphaticChain(B7)</f>
+        <f>_xll.NCDK_LongestAliphaticChain($B7)</f>
         <v>0</v>
       </c>
       <c r="CA7" t="str">
@@ -7070,7 +7323,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:94" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:94" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -7274,7 +7527,7 @@
         <v>1.4033999999999995</v>
       </c>
       <c r="AR8" s="4">
-        <f>_xll.NCDK_XLogP(B8)</f>
+        <f>_xll.NCDK_XLogP($B8)</f>
         <v>2.0819999999999999</v>
       </c>
       <c r="AS8" s="4">
@@ -7410,7 +7663,7 @@
         <v>#N/A</v>
       </c>
       <c r="BZ8">
-        <f>_xll.NCDK_LongestAliphaticChain(B8)</f>
+        <f>_xll.NCDK_LongestAliphaticChain($B8)</f>
         <v>0</v>
       </c>
       <c r="CA8" t="str">
@@ -7478,7 +7731,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:94" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:94" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -7682,7 +7935,7 @@
         <v>1.4033999999999995</v>
       </c>
       <c r="AR9" s="4">
-        <f>_xll.NCDK_XLogP(B9)</f>
+        <f>_xll.NCDK_XLogP($B9)</f>
         <v>2.0819999999999999</v>
       </c>
       <c r="AS9" s="4">
@@ -7818,7 +8071,7 @@
         <v>#N/A</v>
       </c>
       <c r="BZ9">
-        <f>_xll.NCDK_LongestAliphaticChain(B9)</f>
+        <f>_xll.NCDK_LongestAliphaticChain($B9)</f>
         <v>0</v>
       </c>
       <c r="CA9" t="str">
@@ -7886,7 +8139,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:94" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:94" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -8276,7 +8529,7 @@
         <v>7.376100000000001</v>
       </c>
       <c r="AR10" s="4">
-        <f>_xll.NCDK_XLogP(B10)</f>
+        <f>_xll.NCDK_XLogP($B10)</f>
         <v>10.518000000000004</v>
       </c>
       <c r="AS10" s="4">
@@ -8412,7 +8665,7 @@
         <v>3.502934717034, 3.502934717034</v>
       </c>
       <c r="BZ10">
-        <f>_xll.NCDK_LongestAliphaticChain(B10)</f>
+        <f>_xll.NCDK_LongestAliphaticChain($B10)</f>
         <v>7</v>
       </c>
       <c r="CA10" t="str">
@@ -8480,7 +8733,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="11" spans="1:94" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:94" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -8778,7 +9031,7 @@
         <v>7.376100000000001</v>
       </c>
       <c r="AR11" s="4">
-        <f>_xll.NCDK_XLogP(B11)</f>
+        <f>_xll.NCDK_XLogP($B11)</f>
         <v>10.518000000000004</v>
       </c>
       <c r="AS11" s="4">
@@ -8914,7 +9167,7 @@
         <v>#N/A</v>
       </c>
       <c r="BZ11">
-        <f>_xll.NCDK_LongestAliphaticChain(B11)</f>
+        <f>_xll.NCDK_LongestAliphaticChain($B11)</f>
         <v>7</v>
       </c>
       <c r="CA11" t="str">
@@ -8989,19 +9242,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D78F5C-B236-40D1-A056-FD195DD12728}">
   <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>
   <cols>
-    <col min="7" max="18" width="4.83203125" customWidth="1"/>
-    <col min="20" max="20" width="8.6640625" style="4"/>
+    <col min="7" max="18" width="4.8125" customWidth="1"/>
+    <col min="20" max="20" width="8.6875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.7">
       <c r="A1" t="s">
         <v>86</v>
       </c>
@@ -9063,7 +9318,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A2" s="1" t="s">
         <v>88</v>
       </c>
@@ -9126,7 +9381,7 @@
         <v>-1.9040000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A3" s="1" t="s">
         <v>104</v>
       </c>
@@ -9174,7 +9429,7 @@
         <v>1.9170000000000009</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A4" s="1" t="s">
         <v>107</v>
       </c>
@@ -9222,7 +9477,7 @@
         <v>3.7249999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A5" s="1" t="s">
         <v>110</v>
       </c>
@@ -9288,7 +9543,7 @@
         <v>-1.6970000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A6" s="1" t="s">
         <v>114</v>
       </c>
@@ -9348,7 +9603,7 @@
         <v>1.413</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A7" s="1" t="s">
         <v>117</v>
       </c>
@@ -9414,7 +9669,7 @@
         <v>2.4140000000000006</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A8" s="1" t="s">
         <v>120</v>
       </c>
@@ -9477,7 +9732,7 @@
         <v>2.0469999999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A9" s="1" t="s">
         <v>123</v>
       </c>
@@ -9543,7 +9798,7 @@
         <v>0.17100000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A10" s="1" t="s">
         <v>126</v>
       </c>
@@ -9609,7 +9864,7 @@
         <v>3.8299999999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A11" s="1" t="s">
         <v>129</v>
       </c>
@@ -9663,7 +9918,7 @@
         <v>3.7529999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A12" s="1" t="s">
         <v>132</v>
       </c>
@@ -9729,7 +9984,7 @@
         <v>-2.601</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A13" s="1" t="s">
         <v>135</v>
       </c>
@@ -9792,7 +10047,7 @@
         <v>0.8670000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A14" s="1" t="s">
         <v>138</v>
       </c>
@@ -9858,7 +10113,7 @@
         <v>1.8070000000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A15" s="1" t="s">
         <v>141</v>
       </c>
@@ -9924,7 +10179,7 @@
         <v>3.24</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A16" s="1" t="s">
         <v>144</v>
       </c>
@@ -9990,7 +10245,7 @@
         <v>1.4250000000000014</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A17" s="1" t="s">
         <v>147</v>
       </c>
@@ -10056,7 +10311,7 @@
         <v>-4.3659999999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A18" s="1" t="s">
         <v>150</v>
       </c>
@@ -10104,7 +10359,7 @@
         <v>4.5600000000000005</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A19" s="1" t="s">
         <v>153</v>
       </c>
@@ -10167,7 +10422,7 @@
         <v>3.8220000000000005</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A20" s="1" t="s">
         <v>156</v>
       </c>
@@ -10224,7 +10479,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A21" s="1" t="s">
         <v>159</v>
       </c>
@@ -10296,7 +10551,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E5A51D-85D7-4C81-93AB-2292B6ADD80C}">
   <dimension ref="A1:P296"/>
   <sheetViews>
@@ -10304,9 +10559,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.7">
       <c r="A1" t="s">
         <v>87</v>
       </c>
@@ -10356,7 +10611,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -10403,7 +10658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A3" t="s">
         <v>105</v>
       </c>
@@ -10435,7 +10690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A4" t="s">
         <v>108</v>
       </c>
@@ -10467,7 +10722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A5" t="s">
         <v>111</v>
       </c>
@@ -10517,7 +10772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A6" t="s">
         <v>115</v>
       </c>
@@ -10561,7 +10816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A7" t="s">
         <v>118</v>
       </c>
@@ -10611,7 +10866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A8" t="s">
         <v>121</v>
       </c>
@@ -10658,7 +10913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A9" t="s">
         <v>124</v>
       </c>
@@ -10708,7 +10963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A10" t="s">
         <v>127</v>
       </c>
@@ -10758,7 +11013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A11" t="s">
         <v>130</v>
       </c>
@@ -10796,7 +11051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A12" t="s">
         <v>133</v>
       </c>
@@ -10846,7 +11101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A13" t="s">
         <v>136</v>
       </c>
@@ -10893,7 +11148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A14" t="s">
         <v>139</v>
       </c>
@@ -10943,7 +11198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A15" t="s">
         <v>142</v>
       </c>
@@ -10993,7 +11248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A16" t="s">
         <v>145</v>
       </c>
@@ -11043,7 +11298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A17" t="s">
         <v>148</v>
       </c>
@@ -11093,7 +11348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A18" t="s">
         <v>151</v>
       </c>
@@ -11125,7 +11380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A19" t="s">
         <v>154</v>
       </c>
@@ -11172,7 +11427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A20" t="s">
         <v>157</v>
       </c>
@@ -11213,7 +11468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A21" t="s">
         <v>160</v>
       </c>
@@ -11263,7 +11518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A22" t="s">
         <v>189</v>
       </c>
@@ -11313,7 +11568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A23" t="s">
         <v>191</v>
       </c>
@@ -11363,7 +11618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A24" t="s">
         <v>193</v>
       </c>
@@ -11410,7 +11665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A25" t="s">
         <v>195</v>
       </c>
@@ -11460,7 +11715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A26" t="s">
         <v>197</v>
       </c>
@@ -11501,7 +11756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A27" t="s">
         <v>199</v>
       </c>
@@ -11548,7 +11803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A28" t="s">
         <v>201</v>
       </c>
@@ -11598,7 +11853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A29" t="s">
         <v>203</v>
       </c>
@@ -11645,7 +11900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A30" t="s">
         <v>205</v>
       </c>
@@ -11695,7 +11950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A31" t="s">
         <v>207</v>
       </c>
@@ -11736,7 +11991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A32" t="s">
         <v>209</v>
       </c>
@@ -11786,7 +12041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A33" t="s">
         <v>211</v>
       </c>
@@ -11824,7 +12079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A34" t="s">
         <v>213</v>
       </c>
@@ -11871,7 +12126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A35" t="s">
         <v>215</v>
       </c>
@@ -11921,7 +12176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A36" t="s">
         <v>217</v>
       </c>
@@ -11968,7 +12223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A37" t="s">
         <v>219</v>
       </c>
@@ -12015,7 +12270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A38" t="s">
         <v>221</v>
       </c>
@@ -12053,7 +12308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A39" t="s">
         <v>223</v>
       </c>
@@ -12091,7 +12346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A40" t="s">
         <v>225</v>
       </c>
@@ -12135,7 +12390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A41" t="s">
         <v>227</v>
       </c>
@@ -12185,7 +12440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A42" t="s">
         <v>229</v>
       </c>
@@ -12235,7 +12490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A43" t="s">
         <v>231</v>
       </c>
@@ -12285,7 +12540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A44" t="s">
         <v>233</v>
       </c>
@@ -12335,7 +12590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A45" t="s">
         <v>235</v>
       </c>
@@ -12385,7 +12640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A46" t="s">
         <v>237</v>
       </c>
@@ -12429,7 +12684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A47" t="s">
         <v>239</v>
       </c>
@@ -12461,7 +12716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A48" t="s">
         <v>241</v>
       </c>
@@ -12502,7 +12757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A49" t="s">
         <v>243</v>
       </c>
@@ -12546,7 +12801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A50" t="s">
         <v>245</v>
       </c>
@@ -12584,7 +12839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A51" t="s">
         <v>247</v>
       </c>
@@ -12622,7 +12877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A52" t="s">
         <v>249</v>
       </c>
@@ -12663,7 +12918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A53" t="s">
         <v>251</v>
       </c>
@@ -12707,7 +12962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A54" t="s">
         <v>253</v>
       </c>
@@ -12757,7 +13012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A55" t="s">
         <v>255</v>
       </c>
@@ -12807,7 +13062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A56" t="s">
         <v>257</v>
       </c>
@@ -12842,7 +13097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A57" t="s">
         <v>259</v>
       </c>
@@ -12892,7 +13147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A58" t="s">
         <v>261</v>
       </c>
@@ -12942,7 +13197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A59" t="s">
         <v>263</v>
       </c>
@@ -12989,7 +13244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A60" t="s">
         <v>265</v>
       </c>
@@ -13033,7 +13288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A61" t="s">
         <v>267</v>
       </c>
@@ -13080,7 +13335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A62" t="s">
         <v>269</v>
       </c>
@@ -13118,7 +13373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A63" t="s">
         <v>271</v>
       </c>
@@ -13162,7 +13417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A64" t="s">
         <v>273</v>
       </c>
@@ -13206,7 +13461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A65" t="s">
         <v>275</v>
       </c>
@@ -13256,7 +13511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A66" t="s">
         <v>277</v>
       </c>
@@ -13306,7 +13561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A67" t="s">
         <v>279</v>
       </c>
@@ -13356,7 +13611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A68" t="s">
         <v>281</v>
       </c>
@@ -13403,7 +13658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A69" t="s">
         <v>283</v>
       </c>
@@ -13453,7 +13708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A70" t="s">
         <v>285</v>
       </c>
@@ -13503,7 +13758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A71" t="s">
         <v>287</v>
       </c>
@@ -13547,7 +13802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A72" t="s">
         <v>289</v>
       </c>
@@ -13594,7 +13849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A73" t="s">
         <v>291</v>
       </c>
@@ -13623,7 +13878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A74" t="s">
         <v>293</v>
       </c>
@@ -13673,7 +13928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A75" t="s">
         <v>295</v>
       </c>
@@ -13723,7 +13978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A76" t="s">
         <v>297</v>
       </c>
@@ -13773,7 +14028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A77" t="s">
         <v>299</v>
       </c>
@@ -13823,7 +14078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A78" t="s">
         <v>301</v>
       </c>
@@ -13873,7 +14128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A79" t="s">
         <v>303</v>
       </c>
@@ -13917,7 +14172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A80" t="s">
         <v>305</v>
       </c>
@@ -13967,7 +14222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A81" t="s">
         <v>307</v>
       </c>
@@ -14014,7 +14269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A82" t="s">
         <v>309</v>
       </c>
@@ -14064,7 +14319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A83" t="s">
         <v>311</v>
       </c>
@@ -14114,7 +14369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A84" t="s">
         <v>313</v>
       </c>
@@ -14164,7 +14419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A85" t="s">
         <v>315</v>
       </c>
@@ -14211,7 +14466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A86" t="s">
         <v>317</v>
       </c>
@@ -14258,7 +14513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A87" t="s">
         <v>319</v>
       </c>
@@ -14308,7 +14563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A88" t="s">
         <v>321</v>
       </c>
@@ -14346,7 +14601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A89" t="s">
         <v>323</v>
       </c>
@@ -14390,7 +14645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A90" t="s">
         <v>325</v>
       </c>
@@ -14440,7 +14695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A91" t="s">
         <v>327</v>
       </c>
@@ -14484,7 +14739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A92" t="s">
         <v>329</v>
       </c>
@@ -14531,7 +14786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A93" t="s">
         <v>331</v>
       </c>
@@ -14581,7 +14836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A94" t="s">
         <v>333</v>
       </c>
@@ -14631,7 +14886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A95" t="s">
         <v>335</v>
       </c>
@@ -14678,7 +14933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A96" t="s">
         <v>337</v>
       </c>
@@ -14728,7 +14983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A97" t="s">
         <v>339</v>
       </c>
@@ -14778,7 +15033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A98" t="s">
         <v>341</v>
       </c>
@@ -14828,7 +15083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A99" t="s">
         <v>343</v>
       </c>
@@ -14875,7 +15130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A100" t="s">
         <v>345</v>
       </c>
@@ -14925,7 +15180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A101" t="s">
         <v>347</v>
       </c>
@@ -14969,7 +15224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A102" t="s">
         <v>349</v>
       </c>
@@ -15016,7 +15271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A103" t="s">
         <v>351</v>
       </c>
@@ -15054,7 +15309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A104" t="s">
         <v>353</v>
       </c>
@@ -15080,7 +15335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A105" t="s">
         <v>355</v>
       </c>
@@ -15124,7 +15379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A106" t="s">
         <v>357</v>
       </c>
@@ -15174,7 +15429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A107" t="s">
         <v>359</v>
       </c>
@@ -15215,7 +15470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A108" t="s">
         <v>361</v>
       </c>
@@ -15265,7 +15520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A109" t="s">
         <v>363</v>
       </c>
@@ -15303,7 +15558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A110" t="s">
         <v>365</v>
       </c>
@@ -15350,7 +15605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A111" t="s">
         <v>367</v>
       </c>
@@ -15400,7 +15655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A112" t="s">
         <v>369</v>
       </c>
@@ -15435,7 +15690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A113" t="s">
         <v>371</v>
       </c>
@@ -15485,7 +15740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A114" t="s">
         <v>373</v>
       </c>
@@ -15535,7 +15790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A115" t="s">
         <v>375</v>
       </c>
@@ -15585,7 +15840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A116" t="s">
         <v>377</v>
       </c>
@@ -15617,7 +15872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A117" t="s">
         <v>379</v>
       </c>
@@ -15664,7 +15919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A118" t="s">
         <v>381</v>
       </c>
@@ -15711,7 +15966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A119" t="s">
         <v>383</v>
       </c>
@@ -15752,7 +16007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A120" t="s">
         <v>385</v>
       </c>
@@ -15799,7 +16054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A121" t="s">
         <v>387</v>
       </c>
@@ -15846,7 +16101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A122" t="s">
         <v>389</v>
       </c>
@@ -15896,7 +16151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A123" t="s">
         <v>391</v>
       </c>
@@ -15943,7 +16198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A124" t="s">
         <v>393</v>
       </c>
@@ -15990,7 +16245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A125" t="s">
         <v>395</v>
       </c>
@@ -16028,7 +16283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A126" t="s">
         <v>397</v>
       </c>
@@ -16057,7 +16312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A127" t="s">
         <v>399</v>
       </c>
@@ -16107,7 +16362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A128" t="s">
         <v>401</v>
       </c>
@@ -16154,7 +16409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A129" t="s">
         <v>403</v>
       </c>
@@ -16204,7 +16459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A130" t="s">
         <v>405</v>
       </c>
@@ -16254,7 +16509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A131" t="s">
         <v>407</v>
       </c>
@@ -16298,7 +16553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A132" t="s">
         <v>409</v>
       </c>
@@ -16345,7 +16600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A133" t="s">
         <v>411</v>
       </c>
@@ -16395,7 +16650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A134" t="s">
         <v>413</v>
       </c>
@@ -16427,7 +16682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A135" t="s">
         <v>415</v>
       </c>
@@ -16477,7 +16732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A136" t="s">
         <v>417</v>
       </c>
@@ -16527,7 +16782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A137" t="s">
         <v>419</v>
       </c>
@@ -16571,7 +16826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A138" t="s">
         <v>421</v>
       </c>
@@ -16621,7 +16876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A139" t="s">
         <v>423</v>
       </c>
@@ -16665,7 +16920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A140" t="s">
         <v>425</v>
       </c>
@@ -16706,7 +16961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A141" t="s">
         <v>427</v>
       </c>
@@ -16756,7 +17011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A142" t="s">
         <v>429</v>
       </c>
@@ -16803,7 +17058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A143" t="s">
         <v>431</v>
       </c>
@@ -16853,7 +17108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A144" t="s">
         <v>433</v>
       </c>
@@ -16903,7 +17158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A145" t="s">
         <v>435</v>
       </c>
@@ -16953,7 +17208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A146" t="s">
         <v>437</v>
       </c>
@@ -16994,7 +17249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A147" t="s">
         <v>439</v>
       </c>
@@ -17035,7 +17290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A148" t="s">
         <v>441</v>
       </c>
@@ -17085,7 +17340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A149" t="s">
         <v>443</v>
       </c>
@@ -17135,7 +17390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A150" t="s">
         <v>445</v>
       </c>
@@ -17185,7 +17440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A151" t="s">
         <v>447</v>
       </c>
@@ -17232,7 +17487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A152" t="s">
         <v>449</v>
       </c>
@@ -17279,7 +17534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A153" t="s">
         <v>451</v>
       </c>
@@ -17314,7 +17569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A154" t="s">
         <v>453</v>
       </c>
@@ -17352,7 +17607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A155" t="s">
         <v>455</v>
       </c>
@@ -17396,7 +17651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A156" t="s">
         <v>457</v>
       </c>
@@ -17443,7 +17698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A157" t="s">
         <v>459</v>
       </c>
@@ -17493,7 +17748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A158" t="s">
         <v>461</v>
       </c>
@@ -17543,7 +17798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A159" t="s">
         <v>463</v>
       </c>
@@ -17593,7 +17848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A160" t="s">
         <v>465</v>
       </c>
@@ -17643,7 +17898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A161" t="s">
         <v>467</v>
       </c>
@@ -17687,7 +17942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A162" t="s">
         <v>469</v>
       </c>
@@ -17737,7 +17992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A163" t="s">
         <v>471</v>
       </c>
@@ -17784,7 +18039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A164" t="s">
         <v>473</v>
       </c>
@@ -17834,7 +18089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A165" t="s">
         <v>475</v>
       </c>
@@ -17869,7 +18124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A166" t="s">
         <v>477</v>
       </c>
@@ -17913,7 +18168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A167" t="s">
         <v>479</v>
       </c>
@@ -17963,7 +18218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A168" t="s">
         <v>481</v>
       </c>
@@ -18013,7 +18268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A169" t="s">
         <v>483</v>
       </c>
@@ -18063,7 +18318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A170" t="s">
         <v>485</v>
       </c>
@@ -18113,7 +18368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A171" t="s">
         <v>487</v>
       </c>
@@ -18163,7 +18418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A172" t="s">
         <v>489</v>
       </c>
@@ -18210,7 +18465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A173" t="s">
         <v>491</v>
       </c>
@@ -18254,7 +18509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A174" t="s">
         <v>493</v>
       </c>
@@ -18283,7 +18538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A175" t="s">
         <v>495</v>
       </c>
@@ -18324,7 +18579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A176" t="s">
         <v>497</v>
       </c>
@@ -18371,7 +18626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A177" t="s">
         <v>499</v>
       </c>
@@ -18412,7 +18667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A178" t="s">
         <v>501</v>
       </c>
@@ -18462,7 +18717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A179" t="s">
         <v>503</v>
       </c>
@@ -18512,7 +18767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A180" t="s">
         <v>505</v>
       </c>
@@ -18550,7 +18805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A181" t="s">
         <v>507</v>
       </c>
@@ -18594,7 +18849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A182" t="s">
         <v>509</v>
       </c>
@@ -18635,7 +18890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A183" t="s">
         <v>511</v>
       </c>
@@ -18682,7 +18937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A184" t="s">
         <v>513</v>
       </c>
@@ -18732,7 +18987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A185" t="s">
         <v>515</v>
       </c>
@@ -18770,7 +19025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A186" t="s">
         <v>517</v>
       </c>
@@ -18817,7 +19072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A187" t="s">
         <v>519</v>
       </c>
@@ -18858,7 +19113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A188" t="s">
         <v>521</v>
       </c>
@@ -18905,7 +19160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A189" t="s">
         <v>523</v>
       </c>
@@ -18952,7 +19207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A190" t="s">
         <v>525</v>
       </c>
@@ -18984,7 +19239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A191" t="s">
         <v>527</v>
       </c>
@@ -19034,7 +19289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A192" t="s">
         <v>529</v>
       </c>
@@ -19081,7 +19336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A193" t="s">
         <v>531</v>
       </c>
@@ -19128,7 +19383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="194" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A194" t="s">
         <v>533</v>
       </c>
@@ -19178,7 +19433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="195" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A195" t="s">
         <v>535</v>
       </c>
@@ -19219,7 +19474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A196" t="s">
         <v>537</v>
       </c>
@@ -19266,7 +19521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A197" t="s">
         <v>539</v>
       </c>
@@ -19310,7 +19565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A198" t="s">
         <v>541</v>
       </c>
@@ -19345,7 +19600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="199" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A199" t="s">
         <v>543</v>
       </c>
@@ -19392,7 +19647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A200" t="s">
         <v>545</v>
       </c>
@@ -19439,7 +19694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="201" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A201" t="s">
         <v>547</v>
       </c>
@@ -19486,7 +19741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A202" t="s">
         <v>549</v>
       </c>
@@ -19536,7 +19791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="203" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A203" t="s">
         <v>551</v>
       </c>
@@ -19583,7 +19838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A204" t="s">
         <v>553</v>
       </c>
@@ -19627,7 +19882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A205" t="s">
         <v>555</v>
       </c>
@@ -19677,7 +19932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A206" t="s">
         <v>557</v>
       </c>
@@ -19724,7 +19979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A207" t="s">
         <v>559</v>
       </c>
@@ -19768,7 +20023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A208" t="s">
         <v>561</v>
       </c>
@@ -19815,7 +20070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="209" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A209" t="s">
         <v>563</v>
       </c>
@@ -19862,7 +20117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="210" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A210" t="s">
         <v>565</v>
       </c>
@@ -19912,7 +20167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A211" t="s">
         <v>567</v>
       </c>
@@ -19962,7 +20217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="212" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A212" t="s">
         <v>569</v>
       </c>
@@ -20006,7 +20261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="213" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A213" t="s">
         <v>571</v>
       </c>
@@ -20053,7 +20308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="214" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A214" t="s">
         <v>573</v>
       </c>
@@ -20103,7 +20358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="215" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A215" t="s">
         <v>575</v>
       </c>
@@ -20153,7 +20408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="216" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A216" t="s">
         <v>577</v>
       </c>
@@ -20188,7 +20443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="217" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A217" t="s">
         <v>579</v>
       </c>
@@ -20235,7 +20490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="218" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A218" t="s">
         <v>581</v>
       </c>
@@ -20282,7 +20537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="219" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A219" t="s">
         <v>583</v>
       </c>
@@ -20332,7 +20587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="220" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A220" t="s">
         <v>585</v>
       </c>
@@ -20379,7 +20634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="221" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A221" t="s">
         <v>587</v>
       </c>
@@ -20426,7 +20681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="222" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A222" t="s">
         <v>589</v>
       </c>
@@ -20473,7 +20728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="223" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A223" t="s">
         <v>591</v>
       </c>
@@ -20523,7 +20778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="224" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A224" t="s">
         <v>593</v>
       </c>
@@ -20564,7 +20819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="225" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A225" t="s">
         <v>595</v>
       </c>
@@ -20614,7 +20869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="226" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A226" t="s">
         <v>597</v>
       </c>
@@ -20655,7 +20910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="227" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A227" t="s">
         <v>599</v>
       </c>
@@ -20699,7 +20954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="228" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A228" t="s">
         <v>601</v>
       </c>
@@ -20749,7 +21004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="229" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A229" t="s">
         <v>603</v>
       </c>
@@ -20799,7 +21054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="230" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A230" t="s">
         <v>605</v>
       </c>
@@ -20846,7 +21101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="231" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A231" t="s">
         <v>607</v>
       </c>
@@ -20896,7 +21151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="232" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A232" t="s">
         <v>609</v>
       </c>
@@ -20943,7 +21198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="233" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A233" t="s">
         <v>611</v>
       </c>
@@ -20993,7 +21248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="234" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A234" t="s">
         <v>613</v>
       </c>
@@ -21043,7 +21298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="235" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A235" t="s">
         <v>615</v>
       </c>
@@ -21087,7 +21342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="236" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A236" t="s">
         <v>617</v>
       </c>
@@ -21128,7 +21383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="237" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A237" t="s">
         <v>619</v>
       </c>
@@ -21172,7 +21427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="238" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A238" t="s">
         <v>621</v>
       </c>
@@ -21222,7 +21477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="239" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A239" t="s">
         <v>623</v>
       </c>
@@ -21272,7 +21527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="240" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A240" t="s">
         <v>625</v>
       </c>
@@ -21304,7 +21559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="241" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A241" t="s">
         <v>627</v>
       </c>
@@ -21351,7 +21606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="242" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A242" t="s">
         <v>629</v>
       </c>
@@ -21401,7 +21656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="243" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A243" t="s">
         <v>631</v>
       </c>
@@ -21451,7 +21706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="244" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A244" t="s">
         <v>633</v>
       </c>
@@ -21495,7 +21750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="245" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A245" t="s">
         <v>635</v>
       </c>
@@ -21533,7 +21788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="246" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A246" t="s">
         <v>637</v>
       </c>
@@ -21583,7 +21838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="247" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A247" t="s">
         <v>639</v>
       </c>
@@ -21621,7 +21876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="248" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A248" t="s">
         <v>641</v>
       </c>
@@ -21668,7 +21923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="249" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A249" t="s">
         <v>643</v>
       </c>
@@ -21703,7 +21958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="250" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A250" t="s">
         <v>645</v>
       </c>
@@ -21744,7 +21999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="251" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A251" t="s">
         <v>647</v>
       </c>
@@ -21794,7 +22049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="252" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A252" t="s">
         <v>649</v>
       </c>
@@ -21844,7 +22099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="253" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A253" t="s">
         <v>651</v>
       </c>
@@ -21888,7 +22143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="254" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A254" t="s">
         <v>653</v>
       </c>
@@ -21938,7 +22193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="255" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A255" t="s">
         <v>655</v>
       </c>
@@ -21988,7 +22243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="256" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A256" t="s">
         <v>657</v>
       </c>
@@ -22032,7 +22287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="257" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A257" t="s">
         <v>659</v>
       </c>
@@ -22082,7 +22337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="258" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A258" t="s">
         <v>661</v>
       </c>
@@ -22132,7 +22387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="259" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A259" t="s">
         <v>663</v>
       </c>
@@ -22176,7 +22431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="260" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A260" t="s">
         <v>665</v>
       </c>
@@ -22223,7 +22478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="261" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A261" t="s">
         <v>667</v>
       </c>
@@ -22264,7 +22519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="262" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A262" t="s">
         <v>669</v>
       </c>
@@ -22314,7 +22569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="263" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A263" t="s">
         <v>671</v>
       </c>
@@ -22349,7 +22604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="264" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A264" t="s">
         <v>673</v>
       </c>
@@ -22399,7 +22654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="265" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A265" t="s">
         <v>675</v>
       </c>
@@ -22443,7 +22698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="266" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A266" t="s">
         <v>677</v>
       </c>
@@ -22490,7 +22745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="267" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A267" t="s">
         <v>679</v>
       </c>
@@ -22540,7 +22795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="268" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A268" t="s">
         <v>681</v>
       </c>
@@ -22584,7 +22839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="269" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A269" t="s">
         <v>683</v>
       </c>
@@ -22631,7 +22886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="270" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A270" t="s">
         <v>685</v>
       </c>
@@ -22672,7 +22927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="271" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A271" t="s">
         <v>687</v>
       </c>
@@ -22722,7 +22977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="272" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A272" t="s">
         <v>689</v>
       </c>
@@ -22772,7 +23027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="273" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A273" t="s">
         <v>691</v>
       </c>
@@ -22822,7 +23077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="274" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A274" t="s">
         <v>693</v>
       </c>
@@ -22863,7 +23118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="275" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A275" t="s">
         <v>695</v>
       </c>
@@ -22913,7 +23168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="276" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A276" t="s">
         <v>697</v>
       </c>
@@ -22960,7 +23215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="277" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A277" t="s">
         <v>699</v>
       </c>
@@ -22995,7 +23250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="278" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A278" t="s">
         <v>701</v>
       </c>
@@ -23042,7 +23297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="279" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A279" t="s">
         <v>703</v>
       </c>
@@ -23080,7 +23335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="280" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A280" t="s">
         <v>705</v>
       </c>
@@ -23124,7 +23379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="281" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A281" t="s">
         <v>707</v>
       </c>
@@ -23159,7 +23414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="282" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A282" t="s">
         <v>709</v>
       </c>
@@ -23203,7 +23458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="283" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A283" t="s">
         <v>711</v>
       </c>
@@ -23253,7 +23508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="284" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A284" t="s">
         <v>713</v>
       </c>
@@ -23303,7 +23558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="285" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A285" t="s">
         <v>715</v>
       </c>
@@ -23338,7 +23593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="286" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A286" t="s">
         <v>717</v>
       </c>
@@ -23388,7 +23643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="287" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A287" t="s">
         <v>719</v>
       </c>
@@ -23429,7 +23684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="288" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A288" t="s">
         <v>721</v>
       </c>
@@ -23476,7 +23731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="289" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A289" t="s">
         <v>723</v>
       </c>
@@ -23526,7 +23781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="290" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A290" t="s">
         <v>725</v>
       </c>
@@ -23576,7 +23831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="291" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A291" t="s">
         <v>727</v>
       </c>
@@ -23617,7 +23872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="292" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A292" t="s">
         <v>729</v>
       </c>
@@ -23667,7 +23922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="293" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A293" t="s">
         <v>731</v>
       </c>
@@ -23696,7 +23951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="294" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A294" t="s">
         <v>733</v>
       </c>
@@ -23746,7 +24001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="295" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A295" t="s">
         <v>735</v>
       </c>
@@ -23796,7 +24051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="296" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A296" t="s">
         <v>737</v>
       </c>
@@ -23848,96 +24103,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1647DD59-D041-4640-9111-9E35EC2330E5}">
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="1" max="1" width="11.25" customWidth="1"/>
-    <col min="2" max="2" width="41.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="95.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="29.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="58" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="76.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="70" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="236" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="168" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Move RDKit functions to separate project.
</commit_message>
<xml_diff>
--- a/NCDK-Excel/ExcelNCDK-Test.xlsx
+++ b/NCDK-Excel/ExcelNCDK-Test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AF528B-B1FB-407B-9184-6E5F80C2C587}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6235AA0F-3520-40A9-8FE0-EBD0B72D04DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" tabRatio="407" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20278,7 +20278,7 @@
   <dimension ref="A1:CT12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.25"/>
@@ -20598,7 +20598,7 @@
       <c r="C2" t="str">
         <f>_xll.NCDK_MolBlock(B2)</f>
         <v xml:space="preserve">
-       CDK1114192053
+       CDK1116191708
  18 19  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 O   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -21072,7 +21072,7 @@
       <c r="C3" t="str">
         <f>_xll.NCDK_MolBlock(B3)</f>
         <v xml:space="preserve">
-       CDK1114192053
+       CDK1116191708
   1  0  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
 M  END
@@ -21474,7 +21474,7 @@
       <c r="C4" t="str">
         <f>_xll.NCDK_MolBlock(B4)</f>
         <v xml:space="preserve">
-       CDK1114192053
+       CDK1116191708
   4  3  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -21888,7 +21888,7 @@
       <c r="C5" t="str">
         <f>_xll.NCDK_MolBlock(B5)</f>
         <v xml:space="preserve">
-       CDK1114192053
+       CDK1116191708
   6  6  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -22312,7 +22312,7 @@
       <c r="C6" t="str">
         <f>_xll.NCDK_MolBlock(B6)</f>
         <v xml:space="preserve">
-       CDK1114192053
+       CDK1116191708
   7  7  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -22740,7 +22740,7 @@
       <c r="C7" t="str">
         <f>_xll.NCDK_MolBlock(B7)</f>
         <v xml:space="preserve">
-       CDK1114192053
+       CDK1116191708
   6  6  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -23164,7 +23164,7 @@
       <c r="C8" t="str">
         <f>_xll.NCDK_MolBlock(B8)</f>
         <v xml:space="preserve">
-       CDK1114192053
+       CDK1116191708
   6  6  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -23588,7 +23588,7 @@
       <c r="C9" t="str">
         <f>_xll.NCDK_MolBlock(B9)</f>
         <v xml:space="preserve">
-       CDK1114192053
+       CDK1116191708
   6  6  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -24012,7 +24012,7 @@
       <c r="C10" t="str">
         <f>_xll.NCDK_MolBlock(B10)</f>
         <v xml:space="preserve">cholesterol 
-       CDK11141920533D
+       CDK11161917083D
  74 77  0  0  1  0  0  0  0  0999 V2000
    -4.4007   -0.4401    1.6251 C   0  0  2  0  0  0  0  0  0  0  0  0
    -5.4580   -1.0449    0.6688 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -24622,7 +24622,7 @@
       <c r="C11" t="str">
         <f>_xll.NCDK_MolBlock(B11)</f>
         <v xml:space="preserve">
-       CDK1114192053
+       CDK1116191708
  28 31  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -24781,13 +24781,13 @@
         <f>_xll.RDKit_InchiKey($B11)</f>
         <v>HVYWMOMLDIMFJA-UHFFFAOYSA-N</v>
       </c>
-      <c r="L11" s="7">
-        <f>_xll.NCDK_Tanimoto($AA11,$AA12)</f>
-        <v>7.9545454545454544E-2</v>
-      </c>
-      <c r="M11" s="7">
-        <f>_xll.RDKit_TanimotoSimilarity($AA11, $AA12)</f>
-        <v>7.9545454545454544E-2</v>
+      <c r="L11" s="7" t="e">
+        <f>_xll.NCDK_Tanimoto($AA11,#REF!)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M11" s="7" t="e">
+        <f>_xll.RDKit_TanimotoSimilarity($AA11,#REF!)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="N11" t="str">
         <f>_xll.NCDK(N$1,$B11)</f>
@@ -25140,7 +25140,7 @@
       <c r="C12" t="str">
         <f>_xll.NCDK_MolBlock(B12)</f>
         <v xml:space="preserve">
-       CDK1114192052
+       CDK1116191708
  24 27  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0

</xml_diff>

<commit_message>
Add Chem module functions in rdmolops.
</commit_message>
<xml_diff>
--- a/NCDK-Excel/ExcelNCDK-Test.xlsx
+++ b/NCDK-Excel/ExcelNCDK-Test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F852A07C-8C18-4D7F-B94D-7DBB7E7479D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726CD3BF-2B1C-42C7-A2B4-567EC56D26B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" tabRatio="407" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20277,8 +20277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B185B08-1BAB-4052-951E-1A2BC1F97D8F}">
   <dimension ref="A1:CT12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1:T1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.25"/>
@@ -20598,7 +20598,7 @@
       <c r="C2" t="str">
         <f>_xll.NCDK_MolBlock(B2)</f>
         <v xml:space="preserve">
-       CDK1117190132
+       CDK1118192118
  18 19  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 O   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -21072,7 +21072,7 @@
       <c r="C3" t="str">
         <f>_xll.NCDK_MolBlock(B3)</f>
         <v xml:space="preserve">
-       CDK1117190132
+       CDK1118192118
   1  0  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
 M  END
@@ -21474,7 +21474,7 @@
       <c r="C4" t="str">
         <f>_xll.NCDK_MolBlock(B4)</f>
         <v xml:space="preserve">
-       CDK1117190132
+       CDK1118192118
   4  3  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -21888,7 +21888,7 @@
       <c r="C5" t="str">
         <f>_xll.NCDK_MolBlock(B5)</f>
         <v xml:space="preserve">
-       CDK1117190132
+       CDK1118192118
   6  6  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -22312,7 +22312,7 @@
       <c r="C6" t="str">
         <f>_xll.NCDK_MolBlock(B6)</f>
         <v xml:space="preserve">
-       CDK1117190132
+       CDK1118192118
   7  7  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -22740,7 +22740,7 @@
       <c r="C7" t="str">
         <f>_xll.NCDK_MolBlock(B7)</f>
         <v xml:space="preserve">
-       CDK1117190132
+       CDK1118192118
   6  6  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -23164,7 +23164,7 @@
       <c r="C8" t="str">
         <f>_xll.NCDK_MolBlock(B8)</f>
         <v xml:space="preserve">
-       CDK1117190132
+       CDK1118192118
   6  6  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -23588,7 +23588,7 @@
       <c r="C9" t="str">
         <f>_xll.NCDK_MolBlock(B9)</f>
         <v xml:space="preserve">
-       CDK1117190132
+       CDK1118192118
   6  6  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -24012,7 +24012,7 @@
       <c r="C10" t="str">
         <f>_xll.NCDK_MolBlock(B10)</f>
         <v xml:space="preserve">cholesterol 
-       CDK11171901323D
+       CDK11181921183D
  74 77  0  0  1  0  0  0  0  0999 V2000
    -4.4007   -0.4401    1.6251 C   0  0  2  0  0  0  0  0  0  0  0  0
    -5.4580   -1.0449    0.6688 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -24622,7 +24622,7 @@
       <c r="C11" t="str">
         <f>_xll.NCDK_MolBlock(B11)</f>
         <v xml:space="preserve">
-       CDK1117190132
+       CDK1118192118
  28 31  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -25140,7 +25140,7 @@
       <c r="C12" t="str">
         <f>_xll.NCDK_MolBlock(B12)</f>
         <v xml:space="preserve">
-       CDK1117190132
+       CDK1118192118
  24 27  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0

</xml_diff>

<commit_message>
Add reaction SMILES features
</commit_message>
<xml_diff>
--- a/NCDK-Excel/ExcelNCDK-Test.xlsx
+++ b/NCDK-Excel/ExcelNCDK-Test.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CAEB19-F3D9-495C-A6B0-2AE10B80056A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E04C20F-59F0-4F99-AD2D-C7FD8218EC71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" tabRatio="407" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" tabRatio="407" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Picture" sheetId="5" r:id="rId1"/>
     <sheet name="Descriptors" sheetId="2" r:id="rId2"/>
     <sheet name="SDF" sheetId="4" r:id="rId3"/>
     <sheet name="SDF-RDKit" sheetId="7" r:id="rId4"/>
+    <sheet name="Reaction" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="1048">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="1054">
   <si>
     <t>CC(=O)O</t>
     <phoneticPr fontId="1"/>
@@ -19122,6 +19123,24 @@
   <si>
     <t>nHA</t>
   </si>
+  <si>
+    <t>SMILES</t>
+  </si>
+  <si>
+    <t>[C:1]&gt;&gt;[C:1]C</t>
+  </si>
+  <si>
+    <t>[c:1]&gt;&gt;[c:1]Cl</t>
+  </si>
+  <si>
+    <t>Cc1ccccc1</t>
+  </si>
+  <si>
+    <t>[c:1][Cl:2].[C:3]B&gt;&gt;[c:1][C:3]</t>
+  </si>
+  <si>
+    <t>c1ccccc1Cl.BCCCC</t>
+  </si>
 </sst>
 </file>
 
@@ -19133,7 +19152,7 @@
     <numFmt numFmtId="166" formatCode="0.0_ "/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -19147,6 +19166,12 @@
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="5"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -19169,7 +19194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -19180,6 +19205,9 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -19917,7 +19945,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1647DD59-D041-4640-9111-9E35EC2330E5}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1"/>
   <cols>
@@ -20291,16 +20321,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B185B08-1BAB-4052-951E-1A2BC1F97D8F}">
-  <dimension ref="A1:CU12"/>
+  <dimension ref="A1:CU17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C11:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="5" max="5" width="66.46484375" customWidth="1"/>
-    <col min="6" max="6" width="73.33203125" customWidth="1"/>
+    <col min="4" max="4" width="9.265625" customWidth="1"/>
+    <col min="5" max="6" width="10.06640625" customWidth="1"/>
     <col min="12" max="13" width="9.33203125" style="7"/>
     <col min="18" max="18" width="9.33203125" style="7"/>
     <col min="44" max="45" width="9.33203125" style="2"/>
@@ -20619,7 +20649,7 @@
       <c r="C2" t="str">
         <f>_xll.NCDK_MolBlock(B2)</f>
         <v xml:space="preserve">
-       CDK0323200417
+       CDK0411201431
  18 19  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 O   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -21008,7 +21038,7 @@
       </c>
       <c r="CB2">
         <f>_xll.NCDK_LargestChain(B2)</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="CC2">
         <f>_xll.NCDK_LargestPiSystem(B2)</f>
@@ -21097,7 +21127,7 @@
       <c r="C3" t="str">
         <f>_xll.NCDK_MolBlock(B3)</f>
         <v xml:space="preserve">
-       CDK0323200417
+       CDK0411201431
   1  0  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
 M  END
@@ -21503,7 +21533,7 @@
       <c r="C4" t="str">
         <f>_xll.NCDK_MolBlock(B4)</f>
         <v xml:space="preserve">
-       CDK0323200417
+       CDK0411201431
   4  3  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -21921,7 +21951,7 @@
       <c r="C5" t="str">
         <f>_xll.NCDK_MolBlock(B5)</f>
         <v xml:space="preserve">
-       CDK0323200417
+       CDK0411201431
   6  6  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -22260,7 +22290,7 @@
       </c>
       <c r="CB5">
         <f>_xll.NCDK_LargestChain(B5)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="CC5">
         <f>_xll.NCDK_LargestPiSystem(B5)</f>
@@ -22349,7 +22379,7 @@
       <c r="C6" t="str">
         <f>_xll.NCDK_MolBlock(B6)</f>
         <v xml:space="preserve">
-       CDK0323200417
+       CDK0411201431
   7  7  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -22692,7 +22722,7 @@
       </c>
       <c r="CB6">
         <f>_xll.NCDK_LargestChain(B6)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="CC6">
         <f>_xll.NCDK_LargestPiSystem(B6)</f>
@@ -22781,7 +22811,7 @@
       <c r="C7" t="str">
         <f>_xll.NCDK_MolBlock(B7)</f>
         <v xml:space="preserve">
-       CDK0323200417
+       CDK0411201431
   6  6  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -22992,11 +23022,11 @@
       </c>
       <c r="AV7" s="4">
         <f>_xll.NCDK_ALogP(B7)</f>
-        <v>1.8299999999999996</v>
+        <v>1.4033999999999995</v>
       </c>
       <c r="AW7" s="4">
         <f>_xll.NCDK_XLogP($B7)</f>
-        <v>2.0220000000000002</v>
+        <v>2.0819999999999999</v>
       </c>
       <c r="AX7" s="4">
         <f>_xll.NCDK_MannholdLogP(B7)</f>
@@ -23016,7 +23046,7 @@
       </c>
       <c r="BB7">
         <f>_xll.NCDK_AromaticAtomsCount(B7)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="BC7">
         <f>_xll.NCDK_AromaticBondsCount(B7)</f>
@@ -23120,7 +23150,7 @@
       </c>
       <c r="CB7">
         <f>_xll.NCDK_LargestChain(B7)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="CC7">
         <f>_xll.NCDK_LargestPiSystem(B7)</f>
@@ -23209,7 +23239,7 @@
       <c r="C8" t="str">
         <f>_xll.NCDK_MolBlock(B8)</f>
         <v xml:space="preserve">
-       CDK0323200417
+       CDK0411201431
   6  6  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -23637,7 +23667,7 @@
       <c r="C9" t="str">
         <f>_xll.NCDK_MolBlock(B9)</f>
         <v xml:space="preserve">
-       CDK0323200417
+       CDK0411201431
   6  6  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -24065,7 +24095,7 @@
       <c r="C10" t="str">
         <f>_xll.NCDK_MolBlock(B10)</f>
         <v xml:space="preserve">cholesterol 
-       CDK04062012303D
+       CDK04112014313D
  74 77  0  0  1  0  0  0  0  0999 V2000
    -4.4007   -0.4401    1.6251 C   0  0  2  0  0  0  0  0  0  0  0  0
    -5.4580   -1.0449    0.6688 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -24679,7 +24709,7 @@
       <c r="C11" t="str">
         <f>_xll.NCDK_MolBlock(B11)</f>
         <v xml:space="preserve">
-       CDK0323200417
+       CDK0411201431
  28 31  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -25112,7 +25142,7 @@
       </c>
       <c r="CB11">
         <f>_xll.NCDK_LargestChain(B11)</f>
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="CC11">
         <f>_xll.NCDK_LargestPiSystem(B11)</f>
@@ -25201,7 +25231,7 @@
       <c r="C12" t="str">
         <f>_xll.NCDK_MolBlock(B12)</f>
         <v xml:space="preserve">
-       CDK0323200417
+       CDK0411201431
  24 27  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -25697,6 +25727,12 @@
         <v>128</v>
       </c>
     </row>
+    <row r="17" spans="12:12">
+      <c r="L17" s="7" cm="1">
+        <f t="array" ref="L17">_xll.NCDK_Tanimoto(_xll.NCDK_ECFP4("c1ccccc1"), _xll.NCDK_ECFP4("c1(Cl)ccc(C)cc1"))</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -41451,4 +41487,128 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789F1525-30BC-430F-BD39-C5C8DD7E9E93}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="44.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.53125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="str" cm="1">
+        <f t="array" ref="B2">_xll.RDKit_RunReactionSmiles(B$1,$A2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C2" t="str" cm="1">
+        <f t="array" ref="C2">_xll.RDKit_RunReactionSmiles(C$1,$A2)</f>
+        <v>Clc1ccccc1</v>
+      </c>
+      <c r="D2" t="str" cm="1">
+        <f t="array" ref="D2">_xll.RDKit_RunReactionSmiles(D$1,$A2)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B3" t="str" cm="1">
+        <f t="array" ref="B3">_xll.RDKit_RunReactionSmiles(B$1,$A3)</f>
+        <v>CCc1ccccc1</v>
+      </c>
+      <c r="C3" t="str" cm="1">
+        <f t="array" ref="C3">_xll.RDKit_RunReactionSmiles(C$1,$A3)</f>
+        <v>Cc1(Cl)ccccc1</v>
+      </c>
+      <c r="D3" t="str" cm="1">
+        <f t="array" ref="D3">_xll.RDKit_RunReactionSmiles(D$1,$A3)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" t="str" cm="1">
+        <f t="array" ref="B4">_xll.RDKit_RunReactionSmiles(B$1,$A4)</f>
+        <v>CCC(C)CCCC(C)C1CCC2C3CC=C4CC(O)CCC4(C)C3CCC12C</v>
+      </c>
+      <c r="C4" t="str" cm="1">
+        <f t="array" ref="C4">_xll.RDKit_RunReactionSmiles(C$1,$A4)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D4" t="str" cm="1">
+        <f t="array" ref="D4">_xll.RDKit_RunReactionSmiles(D$1,$A4)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B5" t="str" cm="1">
+        <f t="array" ref="B5">_xll.RDKit_RunReactionSmiles(B$1,$A5)</f>
+        <v>CC1Oc2ccc(OCC3CNCCC3c3ccc(F)cc3)cc2O1</v>
+      </c>
+      <c r="C5" t="str" cm="1">
+        <f t="array" ref="C5">_xll.RDKit_RunReactionSmiles(C$1,$A5)</f>
+        <v>Fc1ccc(C2CCNCC2COc2cc3c(cc2Cl)OCO3)cc1</v>
+      </c>
+      <c r="D5" t="str" cm="1">
+        <f t="array" ref="D5">_xll.RDKit_RunReactionSmiles(D$1,$A5)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B6" t="str" cm="1">
+        <f t="array" ref="B6">_xll.RDKit_RunReactionSmiles(B$1,$A6)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C6" t="str" cm="1">
+        <f t="array" ref="C6">_xll.RDKit_RunReactionSmiles(C$1,$A6)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D6" t="str" cm="1">
+        <f t="array" ref="D6">_xll.RDKit_RunReactionSmiles(D$1,$A6)</f>
+        <v>CCCCc1ccccc1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="8"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add HasSubstructureMatch and return null rather than "#N/A" string
</commit_message>
<xml_diff>
--- a/NCDK-Excel/ExcelNCDK-Test.xlsx
+++ b/NCDK-Excel/ExcelNCDK-Test.xlsx
@@ -3,16 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E04C20F-59F0-4F99-AD2D-C7FD8218EC71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8CF026B-5FF9-4AB4-9068-7D771FDDCD6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" tabRatio="407" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" tabRatio="407" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Picture" sheetId="5" r:id="rId1"/>
     <sheet name="Descriptors" sheetId="2" r:id="rId2"/>
-    <sheet name="SDF" sheetId="4" r:id="rId3"/>
-    <sheet name="SDF-RDKit" sheetId="7" r:id="rId4"/>
-    <sheet name="Reaction" sheetId="8" r:id="rId5"/>
+    <sheet name="SMARTS" sheetId="9" r:id="rId3"/>
+    <sheet name="Reaction" sheetId="8" r:id="rId4"/>
+    <sheet name="SDF" sheetId="4" r:id="rId5"/>
+    <sheet name="SDF-RDKit" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="1054">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="1062">
   <si>
     <t>CC(=O)O</t>
     <phoneticPr fontId="1"/>
@@ -19141,6 +19142,30 @@
   <si>
     <t>c1ccccc1Cl.BCCCC</t>
   </si>
+  <si>
+    <t>C1CCCCC1</t>
+  </si>
+  <si>
+    <t>c1ccccc1</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>mol</t>
+  </si>
+  <si>
+    <t>cholesterol</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>eraogjoragjag</t>
+  </si>
+  <si>
+    <t>aewfj23faw</t>
+  </si>
 </sst>
 </file>
 
@@ -19152,7 +19177,7 @@
     <numFmt numFmtId="166" formatCode="0.0_ "/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -19166,12 +19191,6 @@
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="5"/>
-      <color rgb="FFD4D4D4"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -19194,7 +19213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -19205,9 +19224,6 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -20321,10 +20337,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B185B08-1BAB-4052-951E-1A2BC1F97D8F}">
-  <dimension ref="A1:CU17"/>
+  <dimension ref="A1:CU12"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C11:C12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.25"/>
@@ -20649,7 +20665,7 @@
       <c r="C2" t="str">
         <f>_xll.NCDK_MolBlock(B2)</f>
         <v xml:space="preserve">
-       CDK0411201431
+       CDK0412200502
  18 19  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 O   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -20992,9 +21008,9 @@
         <f>_xll.NCDK_ChiPath(B2)</f>
         <v>13.1733621074374, 8.60822612591632, 7.53308445980525, 6.57446305443147, 5.83502554474493, 3.66414268256136, 2.81639208561656, 1.24750715936873, 10.5447358277005, 6.47350942312757, 4.82495377161152, 3.84884458919458, 2.7963481600948, 1.78170696456175, 1.19223951604789, 0.520731228864019</v>
       </c>
-      <c r="BQ2" t="str">
+      <c r="BQ2" t="e">
         <f>_xll.NCDK_CPSA(B2)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="BR2">
         <f>_xll.NCDK_EccentricConnectivityIndex(B2)</f>
@@ -21012,9 +21028,9 @@
         <f>_xll.NCDK_FragmentComplexity(B2)</f>
         <v>1063.05</v>
       </c>
-      <c r="BV2" t="str">
+      <c r="BV2" t="e">
         <f>_xll.NCDK_GravitationalIndex(B2)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="BW2">
         <f>_xll.NCDK_HBondAcceptorCount(B2)</f>
@@ -21038,15 +21054,15 @@
       </c>
       <c r="CB2">
         <f>_xll.NCDK_LargestChain(B2)</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="CC2">
         <f>_xll.NCDK_LargestPiSystem(B2)</f>
         <v>8</v>
       </c>
-      <c r="CD2" t="str">
+      <c r="CD2" t="e">
         <f>_xll.NCDK_LengthOverBreadth(B2)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CE2">
         <f>_xll.NCDK_LongestAliphaticChain($B2)</f>
@@ -21056,17 +21072,17 @@
         <f>_xll.NCDK_MDE(B2)</f>
         <v>0, 1.78256861348341, 1.17348231572452, 0.5, 9.28105720195319, 8.27801156561087, 2.82326712400687, 2.67269615442102, 3.03934274260637, 0, 0.75, 0, 0, 0, 0, 0, 0.5, 0, 0</v>
       </c>
-      <c r="CG2" t="str">
+      <c r="CG2" t="e">
         <f>_xll.NCDK_MomentOfInertia(B2)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CH2">
         <f>_xll.NCDK_PetitjeanNumber(B2)</f>
         <v>0.5</v>
       </c>
-      <c r="CI2" t="str">
+      <c r="CI2" t="e">
         <f>_xll.NCDK_PetitjeanShapeIndex(B2)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CJ2">
         <f>_xll.NCDK_RotatableBondsCount(B2)</f>
@@ -21104,9 +21120,9 @@
         <f>_xll.NCDK_WeightedPath(B2)</f>
         <v>35.9822147160759, 1.99901192867088, 13.5466431850826, 7.60403910050065, 5.94260408458194</v>
       </c>
-      <c r="CS2" t="str">
+      <c r="CS2" t="e">
         <f>_xll.NCDK_WHIM(B2)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CT2" t="str">
         <f>_xll.NCDK_WienerNumbers(B2)</f>
@@ -21127,7 +21143,7 @@
       <c r="C3" t="str">
         <f>_xll.NCDK_MolBlock(B3)</f>
         <v xml:space="preserve">
-       CDK0411201431
+       CDK0412200501
   1  0  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
 M  END
@@ -21398,9 +21414,9 @@
         <f>_xll.NCDK_ChiPath(B3)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BQ3" t="str">
+      <c r="BQ3" t="e">
         <f>_xll.NCDK_CPSA(B3)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="BR3">
         <f>_xll.NCDK_EccentricConnectivityIndex(B3)</f>
@@ -21418,9 +21434,9 @@
         <f>_xll.NCDK_FragmentComplexity(B3)</f>
         <v>16</v>
       </c>
-      <c r="BV3" t="str">
+      <c r="BV3" t="e">
         <f>_xll.NCDK_GravitationalIndex(B3)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="BW3">
         <f>_xll.NCDK_HBondAcceptorCount(B3)</f>
@@ -21450,9 +21466,9 @@
         <f>_xll.NCDK_LargestPiSystem(B3)</f>
         <v>0</v>
       </c>
-      <c r="CD3" t="str">
+      <c r="CD3" t="e">
         <f>_xll.NCDK_LengthOverBreadth(B3)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CE3">
         <f>_xll.NCDK_LongestAliphaticChain($B3)</f>
@@ -21462,17 +21478,17 @@
         <f>_xll.NCDK_MDE(B3)</f>
         <v>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="CG3" t="str">
+      <c r="CG3" t="e">
         <f>_xll.NCDK_MomentOfInertia(B3)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CH3">
         <f>_xll.NCDK_PetitjeanNumber(B3)</f>
         <v>0</v>
       </c>
-      <c r="CI3" t="str">
+      <c r="CI3" t="e">
         <f>_xll.NCDK_PetitjeanShapeIndex(B3)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CJ3">
         <f>_xll.NCDK_RotatableBondsCount(B3)</f>
@@ -21510,9 +21526,9 @@
         <f>_xll.NCDK_WeightedPath(B3)</f>
         <v>1, 1, 0, 0, 0</v>
       </c>
-      <c r="CS3" t="str">
+      <c r="CS3" t="e">
         <f>_xll.NCDK_WHIM(B3)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CT3" t="str">
         <f>_xll.NCDK_WienerNumbers(B3)</f>
@@ -21533,7 +21549,7 @@
       <c r="C4" t="str">
         <f>_xll.NCDK_MolBlock(B4)</f>
         <v xml:space="preserve">
-       CDK0411201431
+       CDK0412200502
   4  3  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -21816,9 +21832,9 @@
         <f>_xll.NCDK_ChiPath(B4)</f>
         <v>3.57735026918963, 1.73205080756888, 1.73205080756888, 0, 0, 0, 0, 0, 2.35546188596382, 0.927730942981911, 0.519018035899438, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="BQ4" t="str">
+      <c r="BQ4" t="e">
         <f>_xll.NCDK_CPSA(B4)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="BR4">
         <f>_xll.NCDK_EccentricConnectivityIndex(B4)</f>
@@ -21836,9 +21852,9 @@
         <f>_xll.NCDK_FragmentComplexity(B4)</f>
         <v>37.020000000000003</v>
       </c>
-      <c r="BV4" t="str">
+      <c r="BV4" t="e">
         <f>_xll.NCDK_GravitationalIndex(B4)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="BW4">
         <f>_xll.NCDK_HBondAcceptorCount(B4)</f>
@@ -21868,9 +21884,9 @@
         <f>_xll.NCDK_LargestPiSystem(B4)</f>
         <v>2</v>
       </c>
-      <c r="CD4" t="str">
+      <c r="CD4" t="e">
         <f>_xll.NCDK_LengthOverBreadth(B4)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CE4">
         <f>_xll.NCDK_LongestAliphaticChain($B4)</f>
@@ -21880,17 +21896,17 @@
         <f>_xll.NCDK_MDE(B4)</f>
         <v>0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0.5, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="CG4" t="str">
+      <c r="CG4" t="e">
         <f>_xll.NCDK_MomentOfInertia(B4)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CH4">
         <f>_xll.NCDK_PetitjeanNumber(B4)</f>
         <v>0.5</v>
       </c>
-      <c r="CI4" t="str">
+      <c r="CI4" t="e">
         <f>_xll.NCDK_PetitjeanShapeIndex(B4)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CJ4">
         <f>_xll.NCDK_RotatableBondsCount(B4)</f>
@@ -21928,9 +21944,9 @@
         <f>_xll.NCDK_WeightedPath(B4)</f>
         <v>6.73205080756888, 1.68301270189222, 4.48803387171259, 4.48803387171259, 0</v>
       </c>
-      <c r="CS4" t="str">
+      <c r="CS4" t="e">
         <f>_xll.NCDK_WHIM(B4)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CT4" t="str">
         <f>_xll.NCDK_WienerNumbers(B4)</f>
@@ -21951,7 +21967,7 @@
       <c r="C5" t="str">
         <f>_xll.NCDK_MolBlock(B5)</f>
         <v xml:space="preserve">
-       CDK0411201431
+       CDK0412200502
   6  6  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -22244,9 +22260,9 @@
         <f>_xll.NCDK_ChiPath(B5)</f>
         <v>4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0, 3.46410161513775, 2, 1.15470053837925, 0.666666666666667, 0.384900179459751, 0.222222222222222, 0, 0</v>
       </c>
-      <c r="BQ5" t="str">
+      <c r="BQ5" t="e">
         <f>_xll.NCDK_CPSA(B5)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="BR5">
         <f>_xll.NCDK_EccentricConnectivityIndex(B5)</f>
@@ -22264,9 +22280,9 @@
         <f>_xll.NCDK_FragmentComplexity(B5)</f>
         <v>114</v>
       </c>
-      <c r="BV5" t="str">
+      <c r="BV5" t="e">
         <f>_xll.NCDK_GravitationalIndex(B5)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="BW5">
         <f>_xll.NCDK_HBondAcceptorCount(B5)</f>
@@ -22290,15 +22306,15 @@
       </c>
       <c r="CB5">
         <f>_xll.NCDK_LargestChain(B5)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="CC5">
         <f>_xll.NCDK_LargestPiSystem(B5)</f>
         <v>6</v>
       </c>
-      <c r="CD5" t="str">
+      <c r="CD5" t="e">
         <f>_xll.NCDK_LengthOverBreadth(B5)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CE5">
         <f>_xll.NCDK_LongestAliphaticChain($B5)</f>
@@ -22308,17 +22324,17 @@
         <f>_xll.NCDK_MDE(B5)</f>
         <v>0, 0, 0, 0, 9.12546512839809, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="CG5" t="str">
+      <c r="CG5" t="e">
         <f>_xll.NCDK_MomentOfInertia(B5)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CH5">
         <f>_xll.NCDK_PetitjeanNumber(B5)</f>
         <v>0</v>
       </c>
-      <c r="CI5" t="str">
+      <c r="CI5" t="e">
         <f>_xll.NCDK_PetitjeanShapeIndex(B5)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CJ5">
         <f>_xll.NCDK_RotatableBondsCount(B5)</f>
@@ -22356,9 +22372,9 @@
         <f>_xll.NCDK_WeightedPath(B5)</f>
         <v>11.8125, 1.96875, 0, 0, 0</v>
       </c>
-      <c r="CS5" t="str">
+      <c r="CS5" t="e">
         <f>_xll.NCDK_WHIM(B5)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CT5" t="str">
         <f>_xll.NCDK_WienerNumbers(B5)</f>
@@ -22379,7 +22395,7 @@
       <c r="C6" t="str">
         <f>_xll.NCDK_MolBlock(B6)</f>
         <v xml:space="preserve">
-       CDK0411201431
+       CDK0412200502
   7  7  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -22676,9 +22692,9 @@
         <f>_xll.NCDK_ChiPath(B6)</f>
         <v>5.11288417512236, 3.39384685011735, 2.74318215649199, 1.89384685011735, 1.30671282224753, 0.901047570290607, 0.204124145231932, 0, 4.38675134594813, 2.41068360252296, 1.65470053837925, 0.940455735015306, 0.534377897417612, 0.303561200840986, 0.0641500299099584, 0</v>
       </c>
-      <c r="BQ6" t="str">
+      <c r="BQ6" t="e">
         <f>_xll.NCDK_CPSA(B6)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="BR6">
         <f>_xll.NCDK_EccentricConnectivityIndex(B6)</f>
@@ -22696,9 +22712,9 @@
         <f>_xll.NCDK_FragmentComplexity(B6)</f>
         <v>183</v>
       </c>
-      <c r="BV6" t="str">
+      <c r="BV6" t="e">
         <f>_xll.NCDK_GravitationalIndex(B6)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="BW6">
         <f>_xll.NCDK_HBondAcceptorCount(B6)</f>
@@ -22722,15 +22738,15 @@
       </c>
       <c r="CB6">
         <f>_xll.NCDK_LargestChain(B6)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="CC6">
         <f>_xll.NCDK_LargestPiSystem(B6)</f>
         <v>6</v>
       </c>
-      <c r="CD6" t="str">
+      <c r="CD6" t="e">
         <f>_xll.NCDK_LengthOverBreadth(B6)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CE6">
         <f>_xll.NCDK_LongestAliphaticChain($B6)</f>
@@ -22740,17 +22756,17 @@
         <f>_xll.NCDK_MDE(B6)</f>
         <v>0, 1.85053586243577, 1, 0, 6.08364341893206, 3.04182170946603, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="CG6" t="str">
+      <c r="CG6" t="e">
         <f>_xll.NCDK_MomentOfInertia(B6)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CH6">
         <f>_xll.NCDK_PetitjeanNumber(B6)</f>
         <v>0.25</v>
       </c>
-      <c r="CI6" t="str">
+      <c r="CI6" t="e">
         <f>_xll.NCDK_PetitjeanShapeIndex(B6)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CJ6">
         <f>_xll.NCDK_RotatableBondsCount(B6)</f>
@@ -22788,9 +22804,9 @@
         <f>_xll.NCDK_WeightedPath(B6)</f>
         <v>13.6768253204364, 1.95383218863377, 0, 0, 0</v>
       </c>
-      <c r="CS6" t="str">
+      <c r="CS6" t="e">
         <f>_xll.NCDK_WHIM(B6)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CT6" t="str">
         <f>_xll.NCDK_WienerNumbers(B6)</f>
@@ -22811,7 +22827,7 @@
       <c r="C7" t="str">
         <f>_xll.NCDK_MolBlock(B7)</f>
         <v xml:space="preserve">
-       CDK0411201431
+       CDK0412200502
   6  6  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -23022,11 +23038,11 @@
       </c>
       <c r="AV7" s="4">
         <f>_xll.NCDK_ALogP(B7)</f>
-        <v>1.4033999999999995</v>
+        <v>1.8299999999999996</v>
       </c>
       <c r="AW7" s="4">
         <f>_xll.NCDK_XLogP($B7)</f>
-        <v>2.0819999999999999</v>
+        <v>2.0220000000000002</v>
       </c>
       <c r="AX7" s="4">
         <f>_xll.NCDK_MannholdLogP(B7)</f>
@@ -23046,7 +23062,7 @@
       </c>
       <c r="BB7">
         <f>_xll.NCDK_AromaticAtomsCount(B7)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="BC7">
         <f>_xll.NCDK_AromaticBondsCount(B7)</f>
@@ -23074,7 +23090,7 @@
       </c>
       <c r="BI7" t="str">
         <f>_xll.NCDK_BCUT(B7)</f>
-        <v>11.85, 12.1500544016358, -0.211758152069243, 0.0882962495665528, 6.093375, 6.3934294016358</v>
+        <v>11.9, 12.1000824042221, -0.161758152069243, 0.0383242521528618, 6.738375, 6.93845740422211</v>
       </c>
       <c r="BJ7">
         <f>_xll.NCDK_BondCount(B7)</f>
@@ -23104,9 +23120,9 @@
         <f>_xll.NCDK_ChiPath(B7)</f>
         <v>4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0, 3.46410161513775, 2, 1.15470053837925, 0.666666666666667, 0.384900179459751, 0.222222222222222, 0, 0</v>
       </c>
-      <c r="BQ7" t="str">
+      <c r="BQ7" t="e">
         <f>_xll.NCDK_CPSA(B7)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="BR7">
         <f>_xll.NCDK_EccentricConnectivityIndex(B7)</f>
@@ -23124,9 +23140,9 @@
         <f>_xll.NCDK_FragmentComplexity(B7)</f>
         <v>114</v>
       </c>
-      <c r="BV7" t="str">
+      <c r="BV7" t="e">
         <f>_xll.NCDK_GravitationalIndex(B7)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="BW7">
         <f>_xll.NCDK_HBondAcceptorCount(B7)</f>
@@ -23156,9 +23172,9 @@
         <f>_xll.NCDK_LargestPiSystem(B7)</f>
         <v>6</v>
       </c>
-      <c r="CD7" t="str">
+      <c r="CD7" t="e">
         <f>_xll.NCDK_LengthOverBreadth(B7)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CE7">
         <f>_xll.NCDK_LongestAliphaticChain($B7)</f>
@@ -23168,17 +23184,17 @@
         <f>_xll.NCDK_MDE(B7)</f>
         <v>0, 0, 0, 0, 9.12546512839809, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="CG7" t="str">
+      <c r="CG7" t="e">
         <f>_xll.NCDK_MomentOfInertia(B7)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CH7">
         <f>_xll.NCDK_PetitjeanNumber(B7)</f>
         <v>0</v>
       </c>
-      <c r="CI7" t="str">
+      <c r="CI7" t="e">
         <f>_xll.NCDK_PetitjeanShapeIndex(B7)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CJ7">
         <f>_xll.NCDK_RotatableBondsCount(B7)</f>
@@ -23216,9 +23232,9 @@
         <f>_xll.NCDK_WeightedPath(B7)</f>
         <v>11.8125, 1.96875, 0, 0, 0</v>
       </c>
-      <c r="CS7" t="str">
+      <c r="CS7" t="e">
         <f>_xll.NCDK_WHIM(B7)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CT7" t="str">
         <f>_xll.NCDK_WienerNumbers(B7)</f>
@@ -23239,7 +23255,7 @@
       <c r="C8" t="str">
         <f>_xll.NCDK_MolBlock(B8)</f>
         <v xml:space="preserve">
-       CDK0411201431
+       CDK0412200502
   6  6  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -23454,7 +23470,7 @@
       </c>
       <c r="AW8" s="4">
         <f>_xll.NCDK_XLogP($B8)</f>
-        <v>2.0220000000000002</v>
+        <v>2.0819999999999999</v>
       </c>
       <c r="AX8" s="4">
         <f>_xll.NCDK_MannholdLogP(B8)</f>
@@ -23532,9 +23548,9 @@
         <f>_xll.NCDK_ChiPath(B8)</f>
         <v>4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0, 3.46410161513775, 2, 1.15470053837925, 0.666666666666667, 0.384900179459751, 0.222222222222222, 0, 0</v>
       </c>
-      <c r="BQ8" t="str">
+      <c r="BQ8" t="e">
         <f>_xll.NCDK_CPSA(B8)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="BR8">
         <f>_xll.NCDK_EccentricConnectivityIndex(B8)</f>
@@ -23552,9 +23568,9 @@
         <f>_xll.NCDK_FragmentComplexity(B8)</f>
         <v>114</v>
       </c>
-      <c r="BV8" t="str">
+      <c r="BV8" t="e">
         <f>_xll.NCDK_GravitationalIndex(B8)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="BW8">
         <f>_xll.NCDK_HBondAcceptorCount(B8)</f>
@@ -23584,9 +23600,9 @@
         <f>_xll.NCDK_LargestPiSystem(B8)</f>
         <v>6</v>
       </c>
-      <c r="CD8" t="str">
+      <c r="CD8" t="e">
         <f>_xll.NCDK_LengthOverBreadth(B8)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CE8">
         <f>_xll.NCDK_LongestAliphaticChain($B8)</f>
@@ -23596,17 +23612,17 @@
         <f>_xll.NCDK_MDE(B8)</f>
         <v>0, 0, 0, 0, 9.12546512839809, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="CG8" t="str">
+      <c r="CG8" t="e">
         <f>_xll.NCDK_MomentOfInertia(B8)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CH8">
         <f>_xll.NCDK_PetitjeanNumber(B8)</f>
         <v>0</v>
       </c>
-      <c r="CI8" t="str">
+      <c r="CI8" t="e">
         <f>_xll.NCDK_PetitjeanShapeIndex(B8)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CJ8">
         <f>_xll.NCDK_RotatableBondsCount(B8)</f>
@@ -23644,9 +23660,9 @@
         <f>_xll.NCDK_WeightedPath(B8)</f>
         <v>11.8125, 1.96875, 0, 0, 0</v>
       </c>
-      <c r="CS8" t="str">
+      <c r="CS8" t="e">
         <f>_xll.NCDK_WHIM(B8)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CT8" t="str">
         <f>_xll.NCDK_WienerNumbers(B8)</f>
@@ -23667,7 +23683,7 @@
       <c r="C9" t="str">
         <f>_xll.NCDK_MolBlock(B9)</f>
         <v xml:space="preserve">
-       CDK0411201431
+       CDK0412200502
   6  6  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -23882,7 +23898,7 @@
       </c>
       <c r="AW9" s="4">
         <f>_xll.NCDK_XLogP($B9)</f>
-        <v>2.0220000000000002</v>
+        <v>2.0819999999999999</v>
       </c>
       <c r="AX9" s="4">
         <f>_xll.NCDK_MannholdLogP(B9)</f>
@@ -23960,9 +23976,9 @@
         <f>_xll.NCDK_ChiPath(B9)</f>
         <v>4.24264068711928, 3, 2.12132034355964, 1.5, 1.06066017177982, 0.75, 0, 0, 3.46410161513775, 2, 1.15470053837925, 0.666666666666667, 0.384900179459751, 0.222222222222222, 0, 0</v>
       </c>
-      <c r="BQ9" t="str">
+      <c r="BQ9" t="e">
         <f>_xll.NCDK_CPSA(B9)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="BR9">
         <f>_xll.NCDK_EccentricConnectivityIndex(B9)</f>
@@ -23980,9 +23996,9 @@
         <f>_xll.NCDK_FragmentComplexity(B9)</f>
         <v>114</v>
       </c>
-      <c r="BV9" t="str">
+      <c r="BV9" t="e">
         <f>_xll.NCDK_GravitationalIndex(B9)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="BW9">
         <f>_xll.NCDK_HBondAcceptorCount(B9)</f>
@@ -24012,9 +24028,9 @@
         <f>_xll.NCDK_LargestPiSystem(B9)</f>
         <v>6</v>
       </c>
-      <c r="CD9" t="str">
+      <c r="CD9" t="e">
         <f>_xll.NCDK_LengthOverBreadth(B9)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CE9">
         <f>_xll.NCDK_LongestAliphaticChain($B9)</f>
@@ -24024,17 +24040,17 @@
         <f>_xll.NCDK_MDE(B9)</f>
         <v>0, 0, 0, 0, 9.12546512839809, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="CG9" t="str">
+      <c r="CG9" t="e">
         <f>_xll.NCDK_MomentOfInertia(B9)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CH9">
         <f>_xll.NCDK_PetitjeanNumber(B9)</f>
         <v>0</v>
       </c>
-      <c r="CI9" t="str">
+      <c r="CI9" t="e">
         <f>_xll.NCDK_PetitjeanShapeIndex(B9)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CJ9">
         <f>_xll.NCDK_RotatableBondsCount(B9)</f>
@@ -24072,9 +24088,9 @@
         <f>_xll.NCDK_WeightedPath(B9)</f>
         <v>11.8125, 1.96875, 0, 0, 0</v>
       </c>
-      <c r="CS9" t="str">
+      <c r="CS9" t="e">
         <f>_xll.NCDK_WHIM(B9)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CT9" t="str">
         <f>_xll.NCDK_WienerNumbers(B9)</f>
@@ -24095,7 +24111,7 @@
       <c r="C10" t="str">
         <f>_xll.NCDK_MolBlock(B10)</f>
         <v xml:space="preserve">cholesterol 
-       CDK04112014313D
+       CDK04122005023D
  74 77  0  0  1  0  0  0  0  0999 V2000
    -4.4007   -0.4401    1.6251 C   0  0  2  0  0  0  0  0  0  0  0  0
    -5.4580   -1.0449    0.6688 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -24709,7 +24725,7 @@
       <c r="C11" t="str">
         <f>_xll.NCDK_MolBlock(B11)</f>
         <v xml:space="preserve">
-       CDK0411201431
+       CDK0412200502
  28 31  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -25096,9 +25112,9 @@
         <f>_xll.NCDK_ChiPath(B11)</f>
         <v>20.1040835277556, 13.2536913009629, 13.0668536638687, 11.1291235227258, 9.49703814548855, 7.69096408557496, 5.93907638185732, 4.4721666474432, 19.344190342069, 12.6298450216499, 12.1863667747532, 10.2790812759586, 8.66624457896859, 6.67875288189192, 5.16344144011131, 3.80610378452706</v>
       </c>
-      <c r="BQ11" t="str">
+      <c r="BQ11" t="e">
         <f>_xll.NCDK_CPSA(B11)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="BR11">
         <f>_xll.NCDK_EccentricConnectivityIndex(B11)</f>
@@ -25116,9 +25132,9 @@
         <f>_xll.NCDK_FragmentComplexity(B11)</f>
         <v>5173.01</v>
       </c>
-      <c r="BV11" t="str">
+      <c r="BV11" t="e">
         <f>_xll.NCDK_GravitationalIndex(B11)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="BW11">
         <f>_xll.NCDK_HBondAcceptorCount(B11)</f>
@@ -25148,9 +25164,9 @@
         <f>_xll.NCDK_LargestPiSystem(B11)</f>
         <v>2</v>
       </c>
-      <c r="CD11" t="str">
+      <c r="CD11" t="e">
         <f>_xll.NCDK_LengthOverBreadth(B11)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CE11">
         <f>_xll.NCDK_LongestAliphaticChain($B11)</f>
@@ -25160,17 +25176,17 @@
         <f>_xll.NCDK_MDE(B11)</f>
         <v>1.54697174276407, 11.0054221495714, 8.10399071027919, 2.24225976804296, 15.301585299106, 26.1301405209996, 7.46130267367363, 6.99912877305946, 5.73136198628621, 0.25, 0, 0, 0, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="CG11" t="str">
+      <c r="CG11" t="e">
         <f>_xll.NCDK_MomentOfInertia(B11)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CH11">
         <f>_xll.NCDK_PetitjeanNumber(B11)</f>
         <v>0.46666666666666667</v>
       </c>
-      <c r="CI11" t="str">
+      <c r="CI11" t="e">
         <f>_xll.NCDK_PetitjeanShapeIndex(B11)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CJ11">
         <f>_xll.NCDK_RotatableBondsCount(B11)</f>
@@ -25208,9 +25224,9 @@
         <f>_xll.NCDK_WeightedPath(B11)</f>
         <v>57.2167299866347, 2.04345464237981, 2.54245315921218, 2.54245315921218, 0</v>
       </c>
-      <c r="CS11" t="str">
+      <c r="CS11" t="e">
         <f>_xll.NCDK_WHIM(B11)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CT11" t="str">
         <f>_xll.NCDK_WienerNumbers(B11)</f>
@@ -25231,7 +25247,7 @@
       <c r="C12" t="str">
         <f>_xll.NCDK_MolBlock(B12)</f>
         <v xml:space="preserve">
-       CDK0411201431
+       CDK0412200502
  24 27  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -25375,12 +25391,12 @@
         <v>AHOUBRCZNHFOSL-UHFFFAOYSA-N</v>
       </c>
       <c r="L12" s="7" t="e">
-        <f>_xll.NCDK_Tanimoto($AB12,$AB13)</f>
-        <v>#NUM!</v>
+        <f>_xll.NCDK_Tanimoto($AB12,#REF!)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="M12" s="7" t="e">
-        <f>_xll.RDKit_TanimotoSimilarity($AB12, $AB13)</f>
-        <v>#NUM!</v>
+        <f>_xll.RDKit_TanimotoSimilarity($AB12,#REF!)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="N12" t="str">
         <f>_xll.NCDK(N$1,$B12)</f>
@@ -25602,9 +25618,9 @@
         <f>_xll.NCDK_ChiPath(B12)</f>
         <v>16.3551603833121, 11.7928263356837, 10.4358343986844, 8.97787455557224, 7.44109928106793, 6.0255800202926, 3.98584708544968, 2.87552775029882, 13.3343956730402, 8.28064127324963, 6.23699509774786, 4.7139481903526, 3.4167809845683, 2.36312961759525, 1.25968040045838, 0.791004433976926</v>
       </c>
-      <c r="BQ12" t="str">
+      <c r="BQ12" t="e">
         <f>_xll.NCDK_CPSA(B12)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="BR12">
         <f>_xll.NCDK_EccentricConnectivityIndex(B12)</f>
@@ -25622,9 +25638,9 @@
         <f>_xll.NCDK_FragmentComplexity(B12)</f>
         <v>1657.05</v>
       </c>
-      <c r="BV12" t="str">
+      <c r="BV12" t="e">
         <f>_xll.NCDK_GravitationalIndex(B12)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="BW12">
         <f>_xll.NCDK_HBondAcceptorCount(B12)</f>
@@ -25654,9 +25670,9 @@
         <f>_xll.NCDK_LargestPiSystem(B12)</f>
         <v>9</v>
       </c>
-      <c r="CD12" t="str">
+      <c r="CD12" t="e">
         <f>_xll.NCDK_LengthOverBreadth(B12)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CE12">
         <f>_xll.NCDK_LongestAliphaticChain($B12)</f>
@@ -25666,17 +25682,17 @@
         <f>_xll.NCDK_MDE(B12)</f>
         <v>0, 0, 0, 0, 14.6388564056411, 23.0332994066205, 0, 5.37507800602613, 0, 0, 0, 0, 0.87720532146386, 0, 0, 0, 0, 0, 0</v>
       </c>
-      <c r="CG12" t="str">
+      <c r="CG12" t="e">
         <f>_xll.NCDK_MomentOfInertia(B12)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CH12">
         <f>_xll.NCDK_PetitjeanNumber(B12)</f>
         <v>0.46153846153846156</v>
       </c>
-      <c r="CI12" t="str">
+      <c r="CI12" t="e">
         <f>_xll.NCDK_PetitjeanShapeIndex(B12)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CJ12">
         <f>_xll.NCDK_RotatableBondsCount(B12)</f>
@@ -25714,9 +25730,9 @@
         <f>_xll.NCDK_WeightedPath(B12)</f>
         <v>49.9996847695691, 2.08332019873205, 14.862766384289, 9.2783821135449, 3.05913677668983</v>
       </c>
-      <c r="CS12" t="str">
+      <c r="CS12" t="e">
         <f>_xll.NCDK_WHIM(B12)</f>
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
       <c r="CT12" t="str">
         <f>_xll.NCDK_WienerNumbers(B12)</f>
@@ -25725,12 +25741,6 @@
       <c r="CU12">
         <f>_xll.NCDK_ZagrebIndex(B12)</f>
         <v>128</v>
-      </c>
-    </row>
-    <row r="17" spans="12:12">
-      <c r="L17" s="7" cm="1">
-        <f t="array" ref="L17">_xll.NCDK_Tanimoto(_xll.NCDK_ECFP4("c1ccccc1"), _xll.NCDK_ECFP4("c1(Cl)ccc(C)cc1"))</f>
-        <v>6.6666666666666666E-2</v>
       </c>
     </row>
   </sheetData>
@@ -25741,6 +25751,238 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6AAC4A4-7166-488A-B8F2-19FDA50F99C9}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1054</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1055</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="b" cm="1">
+        <f t="array" ref="C2">_xll.RDKit_HasSubstructMatch($B2,C$1)</f>
+        <v>1</v>
+      </c>
+      <c r="D2" t="b" cm="1">
+        <f t="array" ref="D2">_xll.RDKit_HasSubstructMatch($B2,D$1)</f>
+        <v>0</v>
+      </c>
+      <c r="E2" t="e" cm="1">
+        <f t="array" ref="E2">_xll.RDKit_HasSubstructMatch($B2,E$1)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="b" cm="1">
+        <f t="array" ref="C3">_xll.RDKit_HasSubstructMatch($B3,C$1)</f>
+        <v>1</v>
+      </c>
+      <c r="D3" t="b" cm="1">
+        <f t="array" ref="D3">_xll.RDKit_HasSubstructMatch($B3,D$1)</f>
+        <v>0</v>
+      </c>
+      <c r="E3" t="e" cm="1">
+        <f t="array" ref="E3">_xll.RDKit_HasSubstructMatch($B3,E$1)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" t="b" cm="1">
+        <f t="array" ref="C4">_xll.RDKit_HasSubstructMatch($B4,C$1)</f>
+        <v>0</v>
+      </c>
+      <c r="D4" t="b" cm="1">
+        <f t="array" ref="D4">_xll.RDKit_HasSubstructMatch($B4,D$1)</f>
+        <v>1</v>
+      </c>
+      <c r="E4" t="e" cm="1">
+        <f t="array" ref="E4">_xll.RDKit_HasSubstructMatch($B4,E$1)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C5" t="e" cm="1">
+        <f t="array" ref="C5">_xll.RDKit_HasSubstructMatch($B5,C$1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="D5" t="e" cm="1">
+        <f t="array" ref="D5">_xll.RDKit_HasSubstructMatch($B5,D$1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="E5" t="e" cm="1">
+        <f t="array" ref="E5">_xll.RDKit_HasSubstructMatch($B5,E$1)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789F1525-30BC-430F-BD39-C5C8DD7E9E93}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="44.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.53125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="e" cm="1">
+        <f t="array" ref="B2">_xll.RDKit_RunReactionSmiles(B$1,$A2)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C2" t="str" cm="1">
+        <f t="array" ref="C2">_xll.RDKit_RunReactionSmiles(C$1,$A2)</f>
+        <v>Clc1ccccc1</v>
+      </c>
+      <c r="D2" t="e" cm="1">
+        <f t="array" ref="D2">_xll.RDKit_RunReactionSmiles(D$1,$A2)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B3" t="str" cm="1">
+        <f t="array" ref="B3">_xll.RDKit_RunReactionSmiles(B$1,$A3)</f>
+        <v>CCc1ccccc1</v>
+      </c>
+      <c r="C3" t="str" cm="1">
+        <f t="array" ref="C3">_xll.RDKit_RunReactionSmiles(C$1,$A3)</f>
+        <v>Cc1(Cl)ccccc1</v>
+      </c>
+      <c r="D3" t="e" cm="1">
+        <f t="array" ref="D3">_xll.RDKit_RunReactionSmiles(D$1,$A3)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" t="str" cm="1">
+        <f t="array" ref="B4">_xll.RDKit_RunReactionSmiles(B$1,$A4)</f>
+        <v>CCC(C)CCCC(C)C1CCC2C3CC=C4CC(O)CCC4(C)C3CCC12C</v>
+      </c>
+      <c r="C4" t="e" cm="1">
+        <f t="array" ref="C4">_xll.RDKit_RunReactionSmiles(C$1,$A4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="D4" t="e" cm="1">
+        <f t="array" ref="D4">_xll.RDKit_RunReactionSmiles(D$1,$A4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B5" t="str" cm="1">
+        <f t="array" ref="B5">_xll.RDKit_RunReactionSmiles(B$1,$A5)</f>
+        <v>CC1Oc2ccc(OCC3CNCCC3c3ccc(F)cc3)cc2O1</v>
+      </c>
+      <c r="C5" t="str" cm="1">
+        <f t="array" ref="C5">_xll.RDKit_RunReactionSmiles(C$1,$A5)</f>
+        <v>Fc1ccc(C2CCNCC2COc2cc3c(cc2Cl)OCO3)cc1</v>
+      </c>
+      <c r="D5" t="e" cm="1">
+        <f t="array" ref="D5">_xll.RDKit_RunReactionSmiles(D$1,$A5)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B6" t="e" cm="1">
+        <f t="array" ref="B6">_xll.RDKit_RunReactionSmiles(B$1,$A6)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C6" t="e" cm="1">
+        <f t="array" ref="C6">_xll.RDKit_RunReactionSmiles(C$1,$A6)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="D6" t="str" cm="1">
+        <f t="array" ref="D6">_xll.RDKit_RunReactionSmiles(D$1,$A6)</f>
+        <v>CCCCc1ccccc1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D78F5C-B236-40D1-A056-FD195DD12728}">
   <dimension ref="A1:T21"/>
   <sheetViews>
@@ -27049,7 +27291,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{852001DF-D8F4-4F73-A6C8-AC076D840020}">
   <dimension ref="A1:Q296"/>
   <sheetViews>
@@ -41487,128 +41729,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789F1525-30BC-430F-BD39-C5C8DD7E9E93}">
-  <dimension ref="A1:D12"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col min="1" max="1" width="44.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.53125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>1048</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1049</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1050</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1052</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" t="str" cm="1">
-        <f t="array" ref="B2">_xll.RDKit_RunReactionSmiles(B$1,$A2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C2" t="str" cm="1">
-        <f t="array" ref="C2">_xll.RDKit_RunReactionSmiles(C$1,$A2)</f>
-        <v>Clc1ccccc1</v>
-      </c>
-      <c r="D2" t="str" cm="1">
-        <f t="array" ref="D2">_xll.RDKit_RunReactionSmiles(D$1,$A2)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>1051</v>
-      </c>
-      <c r="B3" t="str" cm="1">
-        <f t="array" ref="B3">_xll.RDKit_RunReactionSmiles(B$1,$A3)</f>
-        <v>CCc1ccccc1</v>
-      </c>
-      <c r="C3" t="str" cm="1">
-        <f t="array" ref="C3">_xll.RDKit_RunReactionSmiles(C$1,$A3)</f>
-        <v>Cc1(Cl)ccccc1</v>
-      </c>
-      <c r="D3" t="str" cm="1">
-        <f t="array" ref="D3">_xll.RDKit_RunReactionSmiles(D$1,$A3)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" t="str" cm="1">
-        <f t="array" ref="B4">_xll.RDKit_RunReactionSmiles(B$1,$A4)</f>
-        <v>CCC(C)CCCC(C)C1CCC2C3CC=C4CC(O)CCC4(C)C3CCC12C</v>
-      </c>
-      <c r="C4" t="str" cm="1">
-        <f t="array" ref="C4">_xll.RDKit_RunReactionSmiles(C$1,$A4)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D4" t="str" cm="1">
-        <f t="array" ref="D4">_xll.RDKit_RunReactionSmiles(D$1,$A4)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>1034</v>
-      </c>
-      <c r="B5" t="str" cm="1">
-        <f t="array" ref="B5">_xll.RDKit_RunReactionSmiles(B$1,$A5)</f>
-        <v>CC1Oc2ccc(OCC3CNCCC3c3ccc(F)cc3)cc2O1</v>
-      </c>
-      <c r="C5" t="str" cm="1">
-        <f t="array" ref="C5">_xll.RDKit_RunReactionSmiles(C$1,$A5)</f>
-        <v>Fc1ccc(C2CCNCC2COc2cc3c(cc2Cl)OCO3)cc1</v>
-      </c>
-      <c r="D5" t="str" cm="1">
-        <f t="array" ref="D5">_xll.RDKit_RunReactionSmiles(D$1,$A5)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>1053</v>
-      </c>
-      <c r="B6" t="str" cm="1">
-        <f t="array" ref="B6">_xll.RDKit_RunReactionSmiles(B$1,$A6)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C6" t="str" cm="1">
-        <f t="array" ref="C6">_xll.RDKit_RunReactionSmiles(C$1,$A6)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D6" t="str" cm="1">
-        <f t="array" ref="D6">_xll.RDKit_RunReactionSmiles(D$1,$A6)</f>
-        <v>CCCCc1ccccc1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="8"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="8"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add NumAtoms and NumBonds function.
</commit_message>
<xml_diff>
--- a/NCDK-Excel/ExcelNCDK-Test.xlsx
+++ b/NCDK-Excel/ExcelNCDK-Test.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98EFF84-BE1A-4788-8DED-1A713642CEB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BE728B-38FF-4437-899D-44ABF83635EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" tabRatio="407" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="1065">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1472" uniqueCount="1067">
   <si>
     <t>CC(=O)O</t>
     <phoneticPr fontId="1"/>
@@ -19174,6 +19174,12 @@
   </si>
   <si>
     <t>Nc1ccccc1.CCC(=O)O</t>
+  </si>
+  <si>
+    <t>NumAtoms</t>
+  </si>
+  <si>
+    <t>NumBonds</t>
   </si>
 </sst>
 </file>
@@ -20346,11 +20352,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B185B08-1BAB-4052-951E-1A2BC1F97D8F}">
-  <dimension ref="A1:CU12"/>
+  <dimension ref="A1:CW12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.25"/>
   <cols>
@@ -20365,7 +20369,7 @@
     <col min="95" max="95" width="9.33203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99">
+    <row r="1" spans="1:101">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -20663,8 +20667,14 @@
       <c r="CU1" t="s">
         <v>46</v>
       </c>
+      <c r="CV1" t="s">
+        <v>1065</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>1066</v>
+      </c>
     </row>
-    <row r="2" spans="1:99" ht="18" customHeight="1">
+    <row r="2" spans="1:101" ht="18" customHeight="1">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -20674,7 +20684,7 @@
       <c r="C2" t="str">
         <f>_xll.NCDK_MolBlock(B2)</f>
         <v xml:space="preserve">
-       CDK0412200502
+       CDK0517200601
  18 19  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 O   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -21141,8 +21151,16 @@
         <f>_xll.NCDK_ZagrebIndex(B2)</f>
         <v>92</v>
       </c>
+      <c r="CV2">
+        <f>_xll.RDKit_NumAtoms(C2)</f>
+        <v>18</v>
+      </c>
+      <c r="CW2">
+        <f>_xll.RDKit_NumBonds(D2)</f>
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" spans="1:99" ht="18" customHeight="1">
+    <row r="3" spans="1:101" ht="18" customHeight="1">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -21152,7 +21170,7 @@
       <c r="C3" t="str">
         <f>_xll.NCDK_MolBlock(B3)</f>
         <v xml:space="preserve">
-       CDK0412200501
+       CDK0517200601
   1  0  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
 M  END
@@ -21547,8 +21565,16 @@
         <f>_xll.NCDK_ZagrebIndex(B3)</f>
         <v>0</v>
       </c>
+      <c r="CV3">
+        <f>_xll.RDKit_NumAtoms(C3)</f>
+        <v>1</v>
+      </c>
+      <c r="CW3">
+        <f>_xll.RDKit_NumBonds(D3)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:99" ht="18" customHeight="1">
+    <row r="4" spans="1:101" ht="18" customHeight="1">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -21558,7 +21584,7 @@
       <c r="C4" t="str">
         <f>_xll.NCDK_MolBlock(B4)</f>
         <v xml:space="preserve">
-       CDK0412200502
+       CDK0517200601
   4  3  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -21965,8 +21991,16 @@
         <f>_xll.NCDK_ZagrebIndex(B4)</f>
         <v>12</v>
       </c>
+      <c r="CV4">
+        <f>_xll.RDKit_NumAtoms(C4)</f>
+        <v>4</v>
+      </c>
+      <c r="CW4">
+        <f>_xll.RDKit_NumBonds(D4)</f>
+        <v>3</v>
+      </c>
     </row>
-    <row r="5" spans="1:99" ht="18" customHeight="1">
+    <row r="5" spans="1:101" ht="18" customHeight="1">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -21976,7 +22010,7 @@
       <c r="C5" t="str">
         <f>_xll.NCDK_MolBlock(B5)</f>
         <v xml:space="preserve">
-       CDK0412200502
+       CDK0517200601
   6  6  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -22315,7 +22349,7 @@
       </c>
       <c r="CB5">
         <f>_xll.NCDK_LargestChain(B5)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="CC5">
         <f>_xll.NCDK_LargestPiSystem(B5)</f>
@@ -22393,8 +22427,16 @@
         <f>_xll.NCDK_ZagrebIndex(B5)</f>
         <v>24</v>
       </c>
+      <c r="CV5">
+        <f>_xll.RDKit_NumAtoms(C5)</f>
+        <v>6</v>
+      </c>
+      <c r="CW5">
+        <f>_xll.RDKit_NumBonds(D5)</f>
+        <v>6</v>
+      </c>
     </row>
-    <row r="6" spans="1:99" ht="18" customHeight="1">
+    <row r="6" spans="1:101" ht="18" customHeight="1">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -22404,7 +22446,7 @@
       <c r="C6" t="str">
         <f>_xll.NCDK_MolBlock(B6)</f>
         <v xml:space="preserve">
-       CDK0412200502
+       CDK0517200601
   7  7  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -22825,8 +22867,16 @@
         <f>_xll.NCDK_ZagrebIndex(B6)</f>
         <v>30</v>
       </c>
+      <c r="CV6">
+        <f>_xll.RDKit_NumAtoms(C6)</f>
+        <v>7</v>
+      </c>
+      <c r="CW6">
+        <f>_xll.RDKit_NumBonds(D6)</f>
+        <v>7</v>
+      </c>
     </row>
-    <row r="7" spans="1:99" ht="18" customHeight="1">
+    <row r="7" spans="1:101" ht="18" customHeight="1">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -22836,7 +22886,7 @@
       <c r="C7" t="str">
         <f>_xll.NCDK_MolBlock(B7)</f>
         <v xml:space="preserve">
-       CDK0412200502
+       CDK0517200601
   6  6  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -23099,7 +23149,7 @@
       </c>
       <c r="BI7" t="str">
         <f>_xll.NCDK_BCUT(B7)</f>
-        <v>11.9, 12.1000824042221, -0.161758152069243, 0.0383242521528618, 6.738375, 6.93845740422211</v>
+        <v>11.85, 12.1500544016358, -0.211758152069243, 0.0882962495665528, 6.093375, 6.3934294016358</v>
       </c>
       <c r="BJ7">
         <f>_xll.NCDK_BondCount(B7)</f>
@@ -23253,8 +23303,16 @@
         <f>_xll.NCDK_ZagrebIndex(B7)</f>
         <v>24</v>
       </c>
+      <c r="CV7">
+        <f>_xll.RDKit_NumAtoms(C7)</f>
+        <v>6</v>
+      </c>
+      <c r="CW7">
+        <f>_xll.RDKit_NumBonds(D7)</f>
+        <v>6</v>
+      </c>
     </row>
-    <row r="8" spans="1:99" ht="18" customHeight="1">
+    <row r="8" spans="1:101" ht="18" customHeight="1">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -23264,7 +23322,7 @@
       <c r="C8" t="str">
         <f>_xll.NCDK_MolBlock(B8)</f>
         <v xml:space="preserve">
-       CDK0412200502
+       CDK0517200601
   6  6  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -23503,7 +23561,7 @@
       </c>
       <c r="BC8">
         <f>_xll.NCDK_AromaticBondsCount(B8)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="BD8">
         <f>_xll.NCDK_AtomCount(B8)</f>
@@ -23681,8 +23739,16 @@
         <f>_xll.NCDK_ZagrebIndex(B8)</f>
         <v>24</v>
       </c>
+      <c r="CV8">
+        <f>_xll.RDKit_NumAtoms(C8)</f>
+        <v>6</v>
+      </c>
+      <c r="CW8">
+        <f>_xll.RDKit_NumBonds(D8)</f>
+        <v>6</v>
+      </c>
     </row>
-    <row r="9" spans="1:99" ht="18" customHeight="1">
+    <row r="9" spans="1:101" ht="18" customHeight="1">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -23692,7 +23758,7 @@
       <c r="C9" t="str">
         <f>_xll.NCDK_MolBlock(B9)</f>
         <v xml:space="preserve">
-       CDK0412200502
+       CDK0517200601
   6  6  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -23931,7 +23997,7 @@
       </c>
       <c r="BC9">
         <f>_xll.NCDK_AromaticBondsCount(B9)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="BD9">
         <f>_xll.NCDK_AtomCount(B9)</f>
@@ -24109,8 +24175,16 @@
         <f>_xll.NCDK_ZagrebIndex(B9)</f>
         <v>24</v>
       </c>
+      <c r="CV9">
+        <f>_xll.RDKit_NumAtoms(C9)</f>
+        <v>6</v>
+      </c>
+      <c r="CW9">
+        <f>_xll.RDKit_NumBonds(D9)</f>
+        <v>6</v>
+      </c>
     </row>
-    <row r="10" spans="1:99" ht="20.65" customHeight="1">
+    <row r="10" spans="1:101" ht="20.65" customHeight="1">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -24120,7 +24194,7 @@
       <c r="C10" t="str">
         <f>_xll.NCDK_MolBlock(B10)</f>
         <v xml:space="preserve">cholesterol 
-       CDK04122005023D
+       CDK05172006013D
  74 77  0  0  1  0  0  0  0  0999 V2000
    -4.4007   -0.4401    1.6251 C   0  0  2  0  0  0  0  0  0  0  0  0
    -5.4580   -1.0449    0.6688 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -24723,8 +24797,16 @@
         <f>_xll.NCDK_ZagrebIndex(B10)</f>
         <v>158</v>
       </c>
+      <c r="CV10">
+        <f>_xll.RDKit_NumAtoms(C10)</f>
+        <v>28</v>
+      </c>
+      <c r="CW10">
+        <f>_xll.RDKit_NumBonds(D10)</f>
+        <v>31</v>
+      </c>
     </row>
-    <row r="11" spans="1:99" ht="18" customHeight="1">
+    <row r="11" spans="1:101" ht="18" customHeight="1">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -24734,7 +24816,7 @@
       <c r="C11" t="str">
         <f>_xll.NCDK_MolBlock(B11)</f>
         <v xml:space="preserve">
-       CDK0412200502
+       CDK0517200601
  28 31  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -25245,8 +25327,16 @@
         <f>_xll.NCDK_ZagrebIndex(B11)</f>
         <v>158</v>
       </c>
+      <c r="CV11">
+        <f>_xll.RDKit_NumAtoms(C11)</f>
+        <v>28</v>
+      </c>
+      <c r="CW11">
+        <f>_xll.RDKit_NumBonds(D11)</f>
+        <v>31</v>
+      </c>
     </row>
-    <row r="12" spans="1:99" ht="18" customHeight="1">
+    <row r="12" spans="1:101" ht="18" customHeight="1">
       <c r="A12" t="s">
         <v>1035</v>
       </c>
@@ -25256,7 +25346,7 @@
       <c r="C12" t="str">
         <f>_xll.NCDK_MolBlock(B12)</f>
         <v xml:space="preserve">
-       CDK0412200502
+       CDK0517200601
  24 27  0  0  0  0  0  0  0  0999 V2000
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
     0.0000    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
@@ -25751,6 +25841,14 @@
         <f>_xll.NCDK_ZagrebIndex(B12)</f>
         <v>128</v>
       </c>
+      <c r="CV12">
+        <f>_xll.RDKit_NumAtoms(C12)</f>
+        <v>24</v>
+      </c>
+      <c r="CW12">
+        <f>_xll.RDKit_NumBonds(D12)</f>
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>